<commit_message>
Fix some validation errors
- Time must be formatted as "hh:mm:ss"
- PWS Number must be exactly 9 characters
- Fixed element order
- Fixed namespace issue
</commit_message>
<xml_diff>
--- a/specs/Coliform-column-definitions.xlsx
+++ b/specs/Coliform-column-definitions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\xl-ese\specs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{158CFBB7-8F71-4215-A1FF-013F7CE5167C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F5E53E0-1982-4B9F-8299-AE6D783B3389}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2445" yWindow="930" windowWidth="17325" windowHeight="13410" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Coliform Sample" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="235">
   <si>
     <t>Optionality</t>
   </si>
@@ -96,9 +96,6 @@
   </si>
   <si>
     <t>B_COLLECTION_TIME</t>
-  </si>
-  <si>
-    <t>HHMM</t>
   </si>
   <si>
     <t>B_SAMPLE_TYPE</t>
@@ -783,6 +780,12 @@
     <t>OriginalSampleIdentification &gt; 
 OriginalSampleLabAccreditation &gt; 
 LabAccreditationIdentifier</t>
+  </si>
+  <si>
+    <t>HH:MM:SS</t>
+  </si>
+  <si>
+    <t>= 9</t>
   </si>
 </sst>
 </file>
@@ -869,10 +872,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="50">
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
+  <dxfs count="52">
     <dxf>
       <fill>
         <patternFill>
@@ -888,6 +888,57 @@
       </fill>
     </dxf>
     <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <bgColor theme="0" tint="-0.14996795556505021"/>
@@ -939,6 +990,20 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor theme="5" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
@@ -951,42 +1016,34 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
+      <alignment vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <fill>
@@ -1007,88 +1064,48 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1109,7 +1126,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{636125F0-68A9-4682-81D8-01BD3AB67D26}" name="Table1" displayName="Table1" ref="A1:O33" totalsRowShown="0" headerRowDxfId="49" dataDxfId="48">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{636125F0-68A9-4682-81D8-01BD3AB67D26}" name="Table1" displayName="Table1" ref="A1:O33" totalsRowShown="0" headerRowDxfId="46" dataDxfId="45">
   <autoFilter ref="A1:O33" xr:uid="{C224FB70-9F34-49CE-AC5D-FD58B7A283A8}">
     <filterColumn colId="6">
       <filters>
@@ -1120,47 +1137,47 @@
     </filterColumn>
   </autoFilter>
   <tableColumns count="15">
-    <tableColumn id="6" xr3:uid="{57EF6AB6-6C4C-4170-BD9B-BF376C46C5DF}" name="Title" dataDxfId="21"/>
-    <tableColumn id="12" xr3:uid="{BFDB40C3-C9ED-4560-81A1-344ECAE248C8}" name="Excel col #" dataDxfId="19"/>
-    <tableColumn id="1" xr3:uid="{3193A6D3-813B-4494-AEED-01D6509FCA0D}" name="CSV Column Name" dataDxfId="20"/>
-    <tableColumn id="11" xr3:uid="{057EA208-1889-4E3C-A179-F312337D9867}" name="CSV col #" dataDxfId="47"/>
-    <tableColumn id="16" xr3:uid="{1F4E7FF6-264D-41DA-AC14-BAA45F3439C7}" name="XML Element" dataDxfId="18"/>
-    <tableColumn id="2" xr3:uid="{5C52F15D-4AC8-44CE-A401-3402D3CD4152}" name="Data Type" dataDxfId="46"/>
-    <tableColumn id="3" xr3:uid="{FFD71D9C-951A-4BB1-9000-9A1C4C3F71D3}" name="Optionality" dataDxfId="45"/>
-    <tableColumn id="4" xr3:uid="{6FEED7B4-CF3F-4593-BB9F-5CFA5FA5B692}" name="Size" dataDxfId="44"/>
-    <tableColumn id="5" xr3:uid="{563427BF-63BA-491F-9B6F-4E02453C643B}" name="Business Rules" dataDxfId="43"/>
-    <tableColumn id="9" xr3:uid="{A9E34622-C2B4-476B-A018-EABC1256DC10}" name="User Editable" dataDxfId="42"/>
-    <tableColumn id="14" xr3:uid="{9DA3EF2F-E261-414A-B10C-F88F2052640F}" name="Generated" dataDxfId="41"/>
-    <tableColumn id="15" xr3:uid="{AA61284F-4409-4E18-9405-8F2EAA78028A}" name="Format" dataDxfId="40"/>
-    <tableColumn id="13" xr3:uid="{94BA7C53-9CFA-4072-B1A4-7E9CE9D9DDF7}" name="Conditional Formatting" dataDxfId="39"/>
-    <tableColumn id="7" xr3:uid="{22AE72C5-BA89-443A-81AF-BCF4B114454C}" name="Validation" dataDxfId="38"/>
-    <tableColumn id="8" xr3:uid="{5DE66E18-4141-4BDD-B41D-2782AC810F6E}" name="Validation Formula" dataDxfId="37"/>
+    <tableColumn id="6" xr3:uid="{57EF6AB6-6C4C-4170-BD9B-BF376C46C5DF}" name="Title" dataDxfId="44"/>
+    <tableColumn id="12" xr3:uid="{BFDB40C3-C9ED-4560-81A1-344ECAE248C8}" name="Excel col #" dataDxfId="43"/>
+    <tableColumn id="1" xr3:uid="{3193A6D3-813B-4494-AEED-01D6509FCA0D}" name="CSV Column Name" dataDxfId="42"/>
+    <tableColumn id="11" xr3:uid="{057EA208-1889-4E3C-A179-F312337D9867}" name="CSV col #" dataDxfId="41"/>
+    <tableColumn id="16" xr3:uid="{1F4E7FF6-264D-41DA-AC14-BAA45F3439C7}" name="XML Element" dataDxfId="40"/>
+    <tableColumn id="2" xr3:uid="{5C52F15D-4AC8-44CE-A401-3402D3CD4152}" name="Data Type" dataDxfId="39"/>
+    <tableColumn id="3" xr3:uid="{FFD71D9C-951A-4BB1-9000-9A1C4C3F71D3}" name="Optionality" dataDxfId="38"/>
+    <tableColumn id="4" xr3:uid="{6FEED7B4-CF3F-4593-BB9F-5CFA5FA5B692}" name="Size" dataDxfId="37"/>
+    <tableColumn id="5" xr3:uid="{563427BF-63BA-491F-9B6F-4E02453C643B}" name="Business Rules" dataDxfId="36"/>
+    <tableColumn id="9" xr3:uid="{A9E34622-C2B4-476B-A018-EABC1256DC10}" name="User Editable" dataDxfId="35"/>
+    <tableColumn id="14" xr3:uid="{9DA3EF2F-E261-414A-B10C-F88F2052640F}" name="Generated" dataDxfId="34"/>
+    <tableColumn id="15" xr3:uid="{AA61284F-4409-4E18-9405-8F2EAA78028A}" name="Format" dataDxfId="33"/>
+    <tableColumn id="13" xr3:uid="{94BA7C53-9CFA-4072-B1A4-7E9CE9D9DDF7}" name="Conditional Formatting" dataDxfId="32"/>
+    <tableColumn id="7" xr3:uid="{22AE72C5-BA89-443A-81AF-BCF4B114454C}" name="Validation" dataDxfId="31"/>
+    <tableColumn id="8" xr3:uid="{5DE66E18-4141-4BDD-B41D-2782AC810F6E}" name="Validation Formula" dataDxfId="30"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{05345577-AC31-4B6D-B899-55D66DEB1874}" name="Table2" displayName="Table2" ref="A1:O22" totalsRowShown="0" headerRowDxfId="36" dataDxfId="35">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{05345577-AC31-4B6D-B899-55D66DEB1874}" name="Table2" displayName="Table2" ref="A1:O22" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C2:O22">
     <sortCondition ref="D16:D22"/>
   </sortState>
   <tableColumns count="15">
-    <tableColumn id="7" xr3:uid="{9E32B24E-F549-442D-B6C5-5B5E67078170}" name="Title" dataDxfId="34"/>
-    <tableColumn id="12" xr3:uid="{023EA1AA-B7DF-4814-BFEF-5AB9B0752B95}" name="Excel col #" dataDxfId="17"/>
-    <tableColumn id="1" xr3:uid="{5687DF61-58A8-463A-A7F7-9B8B474466F3}" name="CSV Column Name" dataDxfId="33"/>
-    <tableColumn id="13" xr3:uid="{9E799E78-81C7-4788-BF70-799894A0FACA}" name="CSV col #" dataDxfId="32"/>
-    <tableColumn id="16" xr3:uid="{6872DDE9-C4EA-4656-AE08-1B51AE6AE7D6}" name="XML Element" dataDxfId="0"/>
-    <tableColumn id="2" xr3:uid="{E36A262F-69A4-4276-95F1-0FB7FCE8E2AD}" name="Data Type" dataDxfId="31"/>
-    <tableColumn id="3" xr3:uid="{B4F9F589-759B-40AB-BD12-81562C067103}" name="Optionality" dataDxfId="30"/>
-    <tableColumn id="4" xr3:uid="{29CBFF2E-DC73-4812-9BE8-505CDCED923B}" name="Size" dataDxfId="29"/>
-    <tableColumn id="5" xr3:uid="{2FBE4EBA-0896-4EA8-8E6A-9740D712F4CF}" name="Business Rules" dataDxfId="28"/>
-    <tableColumn id="14" xr3:uid="{F6A291D7-463E-4C10-AE63-F46C62F701F1}" name="User Editable" dataDxfId="27"/>
-    <tableColumn id="6" xr3:uid="{4A3A44E5-9909-437B-9914-BD7AF1AC2439}" name="Generated" dataDxfId="26"/>
-    <tableColumn id="15" xr3:uid="{30410F79-D89B-4BAE-852C-7ADB5287310A}" name="Format" dataDxfId="25"/>
-    <tableColumn id="8" xr3:uid="{23D225B6-A3A4-4446-9AD4-7762B64F46FE}" name="Conditional Formatting" dataDxfId="24"/>
-    <tableColumn id="9" xr3:uid="{27D08B50-8012-49E0-9C10-AEB67B99B91B}" name="Validation" dataDxfId="23"/>
-    <tableColumn id="10" xr3:uid="{A301C8EB-BB2A-4524-AF6E-20714C0D7DD5}" name="Validation Formula" dataDxfId="22"/>
+    <tableColumn id="7" xr3:uid="{9E32B24E-F549-442D-B6C5-5B5E67078170}" name="Title" dataDxfId="16"/>
+    <tableColumn id="12" xr3:uid="{023EA1AA-B7DF-4814-BFEF-5AB9B0752B95}" name="Excel col #" dataDxfId="15"/>
+    <tableColumn id="1" xr3:uid="{5687DF61-58A8-463A-A7F7-9B8B474466F3}" name="CSV Column Name" dataDxfId="14"/>
+    <tableColumn id="13" xr3:uid="{9E799E78-81C7-4788-BF70-799894A0FACA}" name="CSV col #" dataDxfId="13"/>
+    <tableColumn id="16" xr3:uid="{6872DDE9-C4EA-4656-AE08-1B51AE6AE7D6}" name="XML Element" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{E36A262F-69A4-4276-95F1-0FB7FCE8E2AD}" name="Data Type" dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{B4F9F589-759B-40AB-BD12-81562C067103}" name="Optionality" dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{29CBFF2E-DC73-4812-9BE8-505CDCED923B}" name="Size" dataDxfId="9"/>
+    <tableColumn id="5" xr3:uid="{2FBE4EBA-0896-4EA8-8E6A-9740D712F4CF}" name="Business Rules" dataDxfId="8"/>
+    <tableColumn id="14" xr3:uid="{F6A291D7-463E-4C10-AE63-F46C62F701F1}" name="User Editable" dataDxfId="7"/>
+    <tableColumn id="6" xr3:uid="{4A3A44E5-9909-437B-9914-BD7AF1AC2439}" name="Generated" dataDxfId="6"/>
+    <tableColumn id="15" xr3:uid="{30410F79-D89B-4BAE-852C-7ADB5287310A}" name="Format" dataDxfId="5"/>
+    <tableColumn id="8" xr3:uid="{23D225B6-A3A4-4446-9AD4-7762B64F46FE}" name="Conditional Formatting" dataDxfId="4"/>
+    <tableColumn id="9" xr3:uid="{27D08B50-8012-49E0-9C10-AEB67B99B91B}" name="Validation" dataDxfId="3"/>
+    <tableColumn id="10" xr3:uid="{A301C8EB-BB2A-4524-AF6E-20714C0D7DD5}" name="Validation Formula" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight14" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1435,7 +1452,7 @@
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="A31" sqref="A31"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1463,22 +1480,22 @@
   <sheetData>
     <row r="1" spans="1:15" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G1" s="6" t="s">
         <v>0</v>
@@ -1490,27 +1507,27 @@
         <v>2</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="K1" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="L1" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="M1" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="N1" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="O1" s="6" t="s">
         <v>55</v>
-      </c>
-      <c r="O1" s="6" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B2" s="7"/>
       <c r="C2" s="7" t="s">
@@ -1521,10 +1538,10 @@
       </c>
       <c r="E2" s="7"/>
       <c r="F2" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H2" s="8">
         <v>20</v>
@@ -1533,7 +1550,7 @@
         <v>4</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K2" s="7" t="s">
         <v>4</v>
@@ -1545,7 +1562,7 @@
     </row>
     <row r="3" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B3" s="2">
         <v>1</v>
@@ -1557,38 +1574,38 @@
         <v>2</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H3" s="3">
         <v>20</v>
       </c>
       <c r="I3" s="2"/>
       <c r="J3" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K3" s="2"/>
       <c r="L3" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="O3" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B4" s="2">
         <v>2</v>
@@ -1600,36 +1617,36 @@
         <v>3</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H4" s="3">
         <v>20</v>
       </c>
       <c r="I4" s="2"/>
       <c r="J4" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K4" s="2"/>
       <c r="L4" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="M4" s="2"/>
       <c r="N4" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="O4" s="2" t="s">
         <v>85</v>
-      </c>
-      <c r="O4" s="2" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B5" s="2">
         <v>3</v>
@@ -1641,40 +1658,40 @@
         <v>4</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H5" s="3">
         <v>9</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K5" s="2"/>
       <c r="L5" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="M5" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="O5" s="2" t="s">
-        <v>123</v>
+        <v>84</v>
+      </c>
+      <c r="O5" s="5" t="s">
+        <v>234</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B6" s="2">
         <v>4</v>
@@ -1686,38 +1703,38 @@
         <v>5</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H6" s="3">
         <v>1</v>
       </c>
       <c r="I6" s="2"/>
       <c r="J6" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="M6" s="2"/>
       <c r="N6" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="O6" s="5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2" t="s">
@@ -1727,23 +1744,23 @@
         <v>6</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H7" s="3">
         <v>10</v>
       </c>
       <c r="I7" s="2"/>
       <c r="J7" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
@@ -1752,7 +1769,7 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2" t="s">
@@ -1762,23 +1779,23 @@
         <v>7</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H8" s="3">
         <v>10</v>
       </c>
       <c r="I8" s="2"/>
       <c r="J8" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
@@ -1787,7 +1804,7 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B9" s="2">
         <v>5</v>
@@ -1799,40 +1816,40 @@
         <v>8</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H9" s="3">
         <v>10</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K9" s="2"/>
       <c r="L9" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="M9" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="N9" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="O9" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="10" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B10" s="2">
         <v>6</v>
@@ -1844,40 +1861,40 @@
         <v>9</v>
       </c>
       <c r="E10" s="13" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H10" s="3">
         <v>12</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K10" s="2"/>
       <c r="L10" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="M10" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="N10" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="O10" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="11" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2" t="s">
@@ -1887,23 +1904,23 @@
         <v>10</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H11" s="3">
         <v>40</v>
       </c>
       <c r="I11" s="2"/>
       <c r="J11" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K11" s="11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
@@ -1912,7 +1929,7 @@
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2" t="s">
@@ -1922,13 +1939,13 @@
         <v>11</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H12" s="3">
         <v>2</v>
@@ -1937,10 +1954,10 @@
         <v>15</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="L12" s="2"/>
       <c r="M12" s="2"/>
@@ -1949,7 +1966,7 @@
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B13" s="2">
         <v>7</v>
@@ -1961,13 +1978,13 @@
         <v>12</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H13" s="3">
         <v>1</v>
@@ -1976,25 +1993,25 @@
         <v>17</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K13" s="2"/>
       <c r="L13" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="M13" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="N13" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="O13" s="5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B14" s="2">
         <v>8</v>
@@ -2006,13 +2023,13 @@
         <v>13</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H14" s="3">
         <v>8</v>
@@ -2021,25 +2038,25 @@
         <v>19</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K14" s="2"/>
       <c r="L14" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="M14" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="N14" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="O14" s="5" t="s">
         <v>129</v>
-      </c>
-      <c r="N14" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="O14" s="5" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B15" s="2">
         <v>9</v>
@@ -2051,236 +2068,236 @@
         <v>14</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H15" s="3">
         <v>4</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>21</v>
+        <v>233</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K15" s="2"/>
       <c r="L15" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="M15" s="2"/>
       <c r="N15" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="O15" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B16" s="2">
         <v>10</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D16" s="7">
         <v>15</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H16" s="3">
         <v>2</v>
       </c>
       <c r="I16" s="2"/>
       <c r="J16" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K16" s="2"/>
       <c r="L16" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="M16" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="N16" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="O16" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="17" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B17" s="2">
         <v>11</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D17" s="2">
         <v>16</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H17" s="3">
         <v>2</v>
       </c>
       <c r="I17" s="2"/>
       <c r="J17" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K17" s="2"/>
       <c r="L17" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="M17" s="4" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="N17" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="O17" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B18" s="2">
         <v>12</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D18" s="7">
         <v>17</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H18" s="3">
         <v>8</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K18" s="2"/>
       <c r="L18" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="M18" s="2"/>
       <c r="N18" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="O18" s="5" t="s">
         <v>200</v>
-      </c>
-      <c r="O18" s="5" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="19" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B19" s="2">
         <v>13</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D19" s="2">
         <v>18</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H19" s="3">
         <v>40</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K19" s="2"/>
       <c r="L19" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="M19" s="2"/>
       <c r="N19" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="O19" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="20" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D20" s="7">
         <v>19</v>
       </c>
       <c r="E20" s="13" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H20" s="3">
         <v>9</v>
       </c>
       <c r="I20" s="2"/>
       <c r="J20" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K20" s="11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="L20" s="2"/>
       <c r="M20" s="2"/>
@@ -2289,33 +2306,33 @@
     </row>
     <row r="21" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D21" s="7">
         <v>20</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H21" s="3">
         <v>2</v>
       </c>
       <c r="I21" s="2"/>
       <c r="J21" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K21" s="11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="L21" s="2"/>
       <c r="M21" s="2"/>
@@ -2324,33 +2341,33 @@
     </row>
     <row r="22" spans="1:15" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D22" s="2">
         <v>21</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H22" s="3">
         <v>12</v>
       </c>
       <c r="I22" s="2"/>
       <c r="J22" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K22" s="11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="L22" s="2"/>
       <c r="M22" s="2"/>
@@ -2359,119 +2376,119 @@
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B23" s="2">
         <v>14</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D23" s="7">
         <v>22</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H23" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="I23" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="I23" s="2" t="s">
-        <v>36</v>
-      </c>
       <c r="J23" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K23" s="2"/>
       <c r="L23" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="M23" s="2"/>
       <c r="N23" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="O23" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B24" s="2">
         <v>15</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D24" s="2">
         <v>23</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K24" s="2"/>
       <c r="L24" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="M24" s="2"/>
       <c r="N24" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="O24" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="25" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D25" s="7">
         <v>24</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I25" s="2"/>
       <c r="J25" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K25" s="11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="L25" s="2"/>
       <c r="M25" s="2"/>
@@ -2480,31 +2497,31 @@
     </row>
     <row r="26" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D26" s="2">
         <v>25</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H26" s="3"/>
       <c r="I26" s="2"/>
       <c r="J26" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K26" s="11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="L26" s="2"/>
       <c r="M26" s="2"/>
@@ -2513,33 +2530,33 @@
     </row>
     <row r="27" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D27" s="7">
         <v>26</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I27" s="2"/>
       <c r="J27" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K27" s="11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="L27" s="2"/>
       <c r="M27" s="2"/>
@@ -2548,33 +2565,33 @@
     </row>
     <row r="28" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D28" s="2">
         <v>27</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I28" s="2"/>
       <c r="J28" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K28" s="11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="L28" s="2"/>
       <c r="M28" s="2"/>
@@ -2583,33 +2600,33 @@
     </row>
     <row r="29" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D29" s="7">
         <v>28</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H29" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I29" s="2"/>
       <c r="J29" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K29" s="11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="L29" s="2"/>
       <c r="M29" s="2"/>
@@ -2618,125 +2635,125 @@
     </row>
     <row r="30" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B30" s="2">
         <v>16</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D30" s="7">
         <v>29</v>
       </c>
       <c r="E30" s="13" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H30" s="3">
         <v>20</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K30" s="2"/>
       <c r="L30" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="M30" s="4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="N30" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="O30" s="5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="31" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B31" s="2">
         <v>17</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D31" s="2">
         <v>30</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H31" s="3">
         <v>8</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K31" s="2"/>
       <c r="L31" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="M31" s="4" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="N31" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="O31" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="32" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D32" s="7">
         <v>31</v>
       </c>
       <c r="E32" s="13" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H32" s="3">
         <v>10</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J32" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K32" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="L32" s="2"/>
       <c r="M32" s="2"/>
@@ -2745,35 +2762,35 @@
     </row>
     <row r="33" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D33" s="2">
         <v>32</v>
       </c>
       <c r="E33" s="13" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H33" s="3">
         <v>10</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J33" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K33" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="L33" s="2"/>
       <c r="M33" s="2"/>
@@ -2783,27 +2800,27 @@
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
   <conditionalFormatting sqref="D2:E33">
-    <cfRule type="expression" dxfId="16" priority="11">
+    <cfRule type="expression" dxfId="51" priority="11">
       <formula>LEN($D2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:A31 C15:N15 C2:O14 C16:O31 A32:O33">
-    <cfRule type="expression" dxfId="15" priority="12">
+    <cfRule type="expression" dxfId="50" priority="12">
       <formula>$J2="No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K33">
-    <cfRule type="expression" dxfId="14" priority="10">
+    <cfRule type="expression" dxfId="49" priority="10">
       <formula>AND($J2="No",LEN($K2)=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O15">
-    <cfRule type="expression" dxfId="13" priority="2">
+    <cfRule type="expression" dxfId="48" priority="2">
       <formula>$J15="No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B31">
-    <cfRule type="expression" dxfId="12" priority="1">
+    <cfRule type="expression" dxfId="47" priority="1">
       <formula>$J2="No"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2847,22 +2864,22 @@
   <sheetData>
     <row r="1" spans="1:15" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G1" s="6" t="s">
         <v>0</v>
@@ -2874,27 +2891,27 @@
         <v>2</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="K1" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="L1" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="M1" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="N1" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="O1" s="6" t="s">
         <v>55</v>
-      </c>
-      <c r="O1" s="6" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2" t="s">
@@ -2905,22 +2922,22 @@
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H2" s="2">
         <v>20</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
@@ -2929,7 +2946,7 @@
     </row>
     <row r="3" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B3" s="2">
         <v>1</v>
@@ -2942,37 +2959,37 @@
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H3" s="2">
         <v>20</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K3" s="2"/>
       <c r="L3" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="O3" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B4" s="2">
         <v>2</v>
@@ -2985,37 +3002,37 @@
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H4" s="2">
         <v>8</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K4" s="2"/>
       <c r="L4" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="M4" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="O4" s="5" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B5" s="2">
         <v>3</v>
@@ -3028,37 +3045,37 @@
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H5" s="2">
         <v>9</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K5" s="2"/>
       <c r="L5" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="M5" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="O5" s="2" t="s">
         <v>122</v>
-      </c>
-      <c r="N5" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="O5" s="2" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2" t="s">
@@ -3069,20 +3086,20 @@
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H6" s="2">
         <v>10</v>
       </c>
       <c r="I6" s="2"/>
       <c r="J6" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
@@ -3091,7 +3108,7 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2" t="s">
@@ -3102,20 +3119,20 @@
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H7" s="2">
         <v>10</v>
       </c>
       <c r="I7" s="2"/>
       <c r="J7" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
@@ -3124,241 +3141,241 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B8" s="2">
         <v>4</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D8" s="2">
         <v>7</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H8" s="2">
         <v>4</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K8" s="2"/>
       <c r="L8" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="M8" s="5" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="O8" s="5" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B9" s="2">
         <v>5</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D9" s="2">
         <v>8</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H9" s="2">
         <v>8</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K9" s="2"/>
       <c r="L9" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="M9" s="5"/>
       <c r="N9" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="O9" s="5" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B10" s="2">
         <v>6</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D10" s="2">
         <v>9</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H10" s="2">
         <v>4</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>21</v>
+        <v>233</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K10" s="2"/>
       <c r="L10" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="M10" s="2"/>
       <c r="N10" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="O10" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B11" s="2">
         <v>7</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D11" s="2">
         <v>10</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H11" s="2">
         <v>8</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K11" s="2"/>
       <c r="L11" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="M11" s="5"/>
       <c r="N11" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="O11" s="5" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B12" s="2">
         <v>8</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D12" s="2">
         <v>11</v>
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H12" s="2">
         <v>4</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>21</v>
+        <v>233</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K12" s="2"/>
       <c r="L12" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="M12" s="2"/>
       <c r="N12" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="O12" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B13" s="2">
         <v>9</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D13" s="2">
         <v>12</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H13" s="2">
         <v>8</v>
       </c>
       <c r="I13" s="2"/>
       <c r="J13" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K13" s="2"/>
       <c r="L13" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="M13" s="5"/>
       <c r="N13" s="2"/>
@@ -3366,33 +3383,33 @@
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D14" s="2">
         <v>13</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H14" s="2">
         <v>1</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="L14" s="2"/>
       <c r="M14" s="2"/>
@@ -3401,31 +3418,31 @@
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D15" s="2">
         <v>14</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H15" s="2">
         <v>2</v>
       </c>
       <c r="I15" s="2"/>
       <c r="J15" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K15" s="11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="L15" s="2"/>
       <c r="M15" s="2"/>
@@ -3434,36 +3451,36 @@
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B16" s="2">
         <v>10</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D16" s="2">
         <v>15</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H16" s="2">
         <v>30</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K16" s="2"/>
       <c r="L16" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="M16" s="2"/>
       <c r="N16" s="2"/>
@@ -3471,308 +3488,318 @@
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B17" s="2">
         <v>11</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D17" s="2">
         <v>16</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H17" s="2">
         <v>9</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K17" s="2"/>
       <c r="L17" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="M17" s="2"/>
       <c r="N17" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="O17" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B18" s="2">
         <v>12</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D18" s="2">
         <v>17</v>
       </c>
       <c r="E18" s="2"/>
       <c r="F18" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H18" s="2">
         <v>4</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K18" s="2"/>
       <c r="L18" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="M18" s="2"/>
       <c r="N18" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="O18" s="5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B19" s="2">
         <v>13</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D19" s="2">
         <v>18</v>
       </c>
       <c r="E19" s="2"/>
       <c r="F19" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H19" s="2">
         <v>1</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K19" s="2"/>
       <c r="L19" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="M19" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="N19" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="O19" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B20" s="2">
         <v>14</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D20" s="2">
         <v>20</v>
       </c>
       <c r="E20" s="2"/>
       <c r="F20" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H20" s="2">
         <v>10</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K20" s="2"/>
       <c r="L20" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="M20" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="N20" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="O20" s="5" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B21" s="2">
         <v>15</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D21" s="2">
         <v>27</v>
       </c>
       <c r="E21" s="2"/>
       <c r="F21" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H21" s="2">
         <v>9</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K21" s="2"/>
       <c r="L21" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="M21" s="5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="N21" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="O21" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B22" s="2">
         <v>16</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D22" s="2">
         <v>28</v>
       </c>
       <c r="E22" s="2"/>
       <c r="F22" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="I22" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="G22" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="H22" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="I22" s="2" t="s">
-        <v>140</v>
-      </c>
       <c r="J22" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K22" s="2"/>
       <c r="L22" s="2"/>
       <c r="M22" s="2"/>
       <c r="N22" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="O22" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="K2:K22">
-    <cfRule type="expression" dxfId="11" priority="9">
+    <cfRule type="expression" dxfId="29" priority="11">
       <formula>AND($J2="No",LEN($K2)=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:E22">
-    <cfRule type="expression" dxfId="10" priority="10">
+    <cfRule type="expression" dxfId="28" priority="12">
       <formula>LEN($D2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N3 N4:O4 N8:O8 N19:O19 A2:A22 C20:O22 C19:L19 C10:O18 C9:M9 C8:L8 C3:L5 C6:O7 C2:O2">
-    <cfRule type="expression" dxfId="9" priority="11">
+  <conditionalFormatting sqref="N3 N4:O4 N8:O8 N19:O19 A2:A22 C20:O22 C19:L19 C11:O11 C9:M9 C8:L8 C3:L5 C6:O7 C2:O2 C10:H10 J10:O10 C13:O18 C12:H12 J12:O12">
+    <cfRule type="expression" dxfId="27" priority="13">
       <formula>$J2="No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M3">
-    <cfRule type="expression" dxfId="8" priority="8">
+    <cfRule type="expression" dxfId="26" priority="10">
       <formula>$J3="No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O3">
-    <cfRule type="expression" dxfId="7" priority="7">
+    <cfRule type="expression" dxfId="25" priority="9">
       <formula>$J3="No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M4:M5">
-    <cfRule type="expression" dxfId="6" priority="6">
+    <cfRule type="expression" dxfId="24" priority="8">
       <formula>$J4="No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N5:O5">
-    <cfRule type="expression" dxfId="5" priority="5">
+    <cfRule type="expression" dxfId="23" priority="7">
       <formula>$J5="No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M8">
-    <cfRule type="expression" dxfId="4" priority="4">
+    <cfRule type="expression" dxfId="22" priority="6">
       <formula>$J8="No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N9:O9">
-    <cfRule type="expression" dxfId="3" priority="3">
+    <cfRule type="expression" dxfId="21" priority="5">
       <formula>$J9="No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M19">
-    <cfRule type="expression" dxfId="2" priority="2">
+    <cfRule type="expression" dxfId="20" priority="4">
       <formula>$J19="No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B22">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="19" priority="3">
       <formula>$J2="No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I10">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>$J10="No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I12">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>$J12="No"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Continue XML export work
- Start work on Results
</commit_message>
<xml_diff>
--- a/specs/Coliform-column-definitions.xlsx
+++ b/specs/Coliform-column-definitions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\xl-ese\specs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F5E53E0-1982-4B9F-8299-AE6D783B3389}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0790F9E3-5FE0-4FD5-BF45-05244B66CD2C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3195" yWindow="1365" windowWidth="18465" windowHeight="13410" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Coliform Sample" sheetId="1" r:id="rId1"/>
@@ -601,9 +601,6 @@
     <t>B_ANALYSIS_COMPLETE_TIME</t>
   </si>
   <si>
-    <t>Analysis Completion Time</t>
-  </si>
-  <si>
     <t>&gt;= MAX(RC2,RC5)</t>
   </si>
   <si>
@@ -612,9 +609,6 @@
   </si>
   <si>
     <t>B_ANALYSIS_COMPLETE_DATE</t>
-  </si>
-  <si>
-    <t>Analysis Completion Date</t>
   </si>
   <si>
     <t>B_ANALYSIS_START_TIME</t>
@@ -786,6 +780,12 @@
   </si>
   <si>
     <t>= 9</t>
+  </si>
+  <si>
+    <t>Analysis End Date</t>
+  </si>
+  <si>
+    <t>Analysis End Time</t>
   </si>
 </sst>
 </file>
@@ -874,6 +874,57 @@
   </cellStyles>
   <dxfs count="52">
     <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <bgColor theme="0" tint="-0.14996795556505021"/>
@@ -886,57 +937,6 @@
           <bgColor theme="0" tint="-0.14996795556505021"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <fill>
@@ -1158,26 +1158,26 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{05345577-AC31-4B6D-B899-55D66DEB1874}" name="Table2" displayName="Table2" ref="A1:O22" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{05345577-AC31-4B6D-B899-55D66DEB1874}" name="Table2" displayName="Table2" ref="A1:O22" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C2:O22">
     <sortCondition ref="D16:D22"/>
   </sortState>
   <tableColumns count="15">
-    <tableColumn id="7" xr3:uid="{9E32B24E-F549-442D-B6C5-5B5E67078170}" name="Title" dataDxfId="16"/>
-    <tableColumn id="12" xr3:uid="{023EA1AA-B7DF-4814-BFEF-5AB9B0752B95}" name="Excel col #" dataDxfId="15"/>
-    <tableColumn id="1" xr3:uid="{5687DF61-58A8-463A-A7F7-9B8B474466F3}" name="CSV Column Name" dataDxfId="14"/>
-    <tableColumn id="13" xr3:uid="{9E799E78-81C7-4788-BF70-799894A0FACA}" name="CSV col #" dataDxfId="13"/>
-    <tableColumn id="16" xr3:uid="{6872DDE9-C4EA-4656-AE08-1B51AE6AE7D6}" name="XML Element" dataDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{E36A262F-69A4-4276-95F1-0FB7FCE8E2AD}" name="Data Type" dataDxfId="11"/>
-    <tableColumn id="3" xr3:uid="{B4F9F589-759B-40AB-BD12-81562C067103}" name="Optionality" dataDxfId="10"/>
-    <tableColumn id="4" xr3:uid="{29CBFF2E-DC73-4812-9BE8-505CDCED923B}" name="Size" dataDxfId="9"/>
-    <tableColumn id="5" xr3:uid="{2FBE4EBA-0896-4EA8-8E6A-9740D712F4CF}" name="Business Rules" dataDxfId="8"/>
-    <tableColumn id="14" xr3:uid="{F6A291D7-463E-4C10-AE63-F46C62F701F1}" name="User Editable" dataDxfId="7"/>
-    <tableColumn id="6" xr3:uid="{4A3A44E5-9909-437B-9914-BD7AF1AC2439}" name="Generated" dataDxfId="6"/>
-    <tableColumn id="15" xr3:uid="{30410F79-D89B-4BAE-852C-7ADB5287310A}" name="Format" dataDxfId="5"/>
-    <tableColumn id="8" xr3:uid="{23D225B6-A3A4-4446-9AD4-7762B64F46FE}" name="Conditional Formatting" dataDxfId="4"/>
-    <tableColumn id="9" xr3:uid="{27D08B50-8012-49E0-9C10-AEB67B99B91B}" name="Validation" dataDxfId="3"/>
-    <tableColumn id="10" xr3:uid="{A301C8EB-BB2A-4524-AF6E-20714C0D7DD5}" name="Validation Formula" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{9E32B24E-F549-442D-B6C5-5B5E67078170}" name="Title" dataDxfId="14"/>
+    <tableColumn id="12" xr3:uid="{023EA1AA-B7DF-4814-BFEF-5AB9B0752B95}" name="Excel col #" dataDxfId="13"/>
+    <tableColumn id="1" xr3:uid="{5687DF61-58A8-463A-A7F7-9B8B474466F3}" name="CSV Column Name" dataDxfId="12"/>
+    <tableColumn id="13" xr3:uid="{9E799E78-81C7-4788-BF70-799894A0FACA}" name="CSV col #" dataDxfId="11"/>
+    <tableColumn id="16" xr3:uid="{6872DDE9-C4EA-4656-AE08-1B51AE6AE7D6}" name="XML Element" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{E36A262F-69A4-4276-95F1-0FB7FCE8E2AD}" name="Data Type" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{B4F9F589-759B-40AB-BD12-81562C067103}" name="Optionality" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{29CBFF2E-DC73-4812-9BE8-505CDCED923B}" name="Size" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{2FBE4EBA-0896-4EA8-8E6A-9740D712F4CF}" name="Business Rules" dataDxfId="6"/>
+    <tableColumn id="14" xr3:uid="{F6A291D7-463E-4C10-AE63-F46C62F701F1}" name="User Editable" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{4A3A44E5-9909-437B-9914-BD7AF1AC2439}" name="Generated" dataDxfId="4"/>
+    <tableColumn id="15" xr3:uid="{30410F79-D89B-4BAE-852C-7ADB5287310A}" name="Format" dataDxfId="3"/>
+    <tableColumn id="8" xr3:uid="{23D225B6-A3A4-4446-9AD4-7762B64F46FE}" name="Conditional Formatting" dataDxfId="2"/>
+    <tableColumn id="9" xr3:uid="{27D08B50-8012-49E0-9C10-AEB67B99B91B}" name="Validation" dataDxfId="1"/>
+    <tableColumn id="10" xr3:uid="{A301C8EB-BB2A-4524-AF6E-20714C0D7DD5}" name="Validation Formula" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight14" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1449,7 +1449,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:O33"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -1483,7 +1483,7 @@
         <v>53</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C1" s="6" t="s">
         <v>108</v>
@@ -1492,7 +1492,7 @@
         <v>119</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="F1" s="6" t="s">
         <v>115</v>
@@ -1574,7 +1574,7 @@
         <v>2</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>105</v>
@@ -1617,7 +1617,7 @@
         <v>3</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>105</v>
@@ -1658,7 +1658,7 @@
         <v>4</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>105</v>
@@ -1686,7 +1686,7 @@
         <v>84</v>
       </c>
       <c r="O5" s="5" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
@@ -1703,7 +1703,7 @@
         <v>5</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>105</v>
@@ -1744,7 +1744,7 @@
         <v>6</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>105</v>
@@ -1779,7 +1779,7 @@
         <v>7</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>105</v>
@@ -1816,7 +1816,7 @@
         <v>8</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>105</v>
@@ -1861,7 +1861,7 @@
         <v>9</v>
       </c>
       <c r="E10" s="13" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>105</v>
@@ -1904,7 +1904,7 @@
         <v>10</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>105</v>
@@ -1939,7 +1939,7 @@
         <v>11</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>105</v>
@@ -1978,7 +1978,7 @@
         <v>12</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>105</v>
@@ -2023,7 +2023,7 @@
         <v>13</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>92</v>
@@ -2068,7 +2068,7 @@
         <v>14</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>93</v>
@@ -2080,7 +2080,7 @@
         <v>4</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="J15" s="2" t="s">
         <v>82</v>
@@ -2111,7 +2111,7 @@
         <v>15</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>105</v>
@@ -2154,7 +2154,7 @@
         <v>16</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>105</v>
@@ -2174,7 +2174,7 @@
         <v>105</v>
       </c>
       <c r="M17" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="N17" s="2" t="s">
         <v>80</v>
@@ -2197,7 +2197,7 @@
         <v>17</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>92</v>
@@ -2220,10 +2220,10 @@
       </c>
       <c r="M18" s="2"/>
       <c r="N18" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="O18" s="5" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="19" spans="1:15" ht="30" x14ac:dyDescent="0.25">
@@ -2240,7 +2240,7 @@
         <v>18</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>105</v>
@@ -2281,7 +2281,7 @@
         <v>19</v>
       </c>
       <c r="E20" s="13" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>105</v>
@@ -2316,7 +2316,7 @@
         <v>20</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="F21" s="2" t="s">
         <v>105</v>
@@ -2351,7 +2351,7 @@
         <v>21</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="F22" s="2" t="s">
         <v>105</v>
@@ -2376,7 +2376,7 @@
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B23" s="2">
         <v>14</v>
@@ -2388,7 +2388,7 @@
         <v>22</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>103</v>
@@ -2419,7 +2419,7 @@
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B24" s="2">
         <v>15</v>
@@ -2431,7 +2431,7 @@
         <v>23</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="F24" s="2" t="s">
         <v>103</v>
@@ -2472,7 +2472,7 @@
         <v>24</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="F25" s="2" t="s">
         <v>103</v>
@@ -2507,7 +2507,7 @@
         <v>25</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="F26" s="2" t="s">
         <v>105</v>
@@ -2540,7 +2540,7 @@
         <v>26</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="F27" s="2" t="s">
         <v>103</v>
@@ -2575,7 +2575,7 @@
         <v>27</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="F28" s="2" t="s">
         <v>103</v>
@@ -2610,7 +2610,7 @@
         <v>28</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="F29" s="2" t="s">
         <v>103</v>
@@ -2647,7 +2647,7 @@
         <v>29</v>
       </c>
       <c r="E30" s="13" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="F30" s="2" t="s">
         <v>105</v>
@@ -2669,7 +2669,7 @@
         <v>105</v>
       </c>
       <c r="M30" s="4" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="N30" s="2" t="s">
         <v>78</v>
@@ -2692,7 +2692,7 @@
         <v>30</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="F31" s="2" t="s">
         <v>92</v>
@@ -2714,7 +2714,7 @@
         <v>97</v>
       </c>
       <c r="M31" s="4" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="N31" s="2" t="s">
         <v>78</v>
@@ -2735,7 +2735,7 @@
         <v>31</v>
       </c>
       <c r="E32" s="13" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="F32" s="2" t="s">
         <v>105</v>
@@ -2772,7 +2772,7 @@
         <v>32</v>
       </c>
       <c r="E33" s="13" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="F33" s="2" t="s">
         <v>105</v>
@@ -2837,7 +2837,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:O22"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -2867,7 +2867,7 @@
         <v>53</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C1" s="6" t="s">
         <v>108</v>
@@ -2876,7 +2876,7 @@
         <v>119</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="F1" s="6" t="s">
         <v>115</v>
@@ -2931,13 +2931,13 @@
         <v>20</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>81</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
@@ -2968,7 +2968,7 @@
         <v>20</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>82</v>
@@ -3011,7 +3011,7 @@
         <v>8</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="J4" s="2" t="s">
         <v>82</v>
@@ -3021,13 +3021,13 @@
         <v>97</v>
       </c>
       <c r="M4" s="5" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="N4" s="2" t="s">
         <v>78</v>
       </c>
       <c r="O4" s="5" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
@@ -3054,7 +3054,7 @@
         <v>9</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="J5" s="2" t="s">
         <v>82</v>
@@ -3141,13 +3141,13 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B8" s="2">
         <v>4</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D8" s="2">
         <v>7</v>
@@ -3163,7 +3163,7 @@
         <v>4</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="J8" s="2" t="s">
         <v>82</v>
@@ -3173,24 +3173,24 @@
         <v>105</v>
       </c>
       <c r="M8" s="5" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="N8" s="2" t="s">
         <v>80</v>
       </c>
       <c r="O8" s="5" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B9" s="2">
         <v>5</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D9" s="2">
         <v>8</v>
@@ -3206,7 +3206,7 @@
         <v>8</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="J9" s="2" t="s">
         <v>82</v>
@@ -3220,18 +3220,18 @@
         <v>92</v>
       </c>
       <c r="O9" s="5" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B10" s="2">
         <v>6</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D10" s="2">
         <v>9</v>
@@ -3247,7 +3247,7 @@
         <v>4</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="J10" s="2" t="s">
         <v>82</v>
@@ -3266,13 +3266,13 @@
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>181</v>
+        <v>233</v>
       </c>
       <c r="B11" s="2">
         <v>7</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D11" s="2">
         <v>10</v>
@@ -3288,7 +3288,7 @@
         <v>8</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="J11" s="2" t="s">
         <v>82</v>
@@ -3302,12 +3302,12 @@
         <v>92</v>
       </c>
       <c r="O11" s="5" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>177</v>
+        <v>234</v>
       </c>
       <c r="B12" s="2">
         <v>8</v>
@@ -3329,7 +3329,7 @@
         <v>4</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="J12" s="2" t="s">
         <v>82</v>
@@ -3793,12 +3793,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I10">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="18" priority="2">
       <formula>$J10="No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I12">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="17" priority="1">
       <formula>$J12="No"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Continue Results XML work
</commit_message>
<xml_diff>
--- a/specs/Coliform-column-definitions.xlsx
+++ b/specs/Coliform-column-definitions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\xl-ese\specs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0790F9E3-5FE0-4FD5-BF45-05244B66CD2C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA14635A-B649-4743-A2A7-138E2672ADF9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3195" yWindow="1365" windowWidth="18465" windowHeight="13410" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2840,7 +2840,7 @@
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Finish Results XML work
</commit_message>
<xml_diff>
--- a/specs/Coliform-column-definitions.xlsx
+++ b/specs/Coliform-column-definitions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\xl-ese\specs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA14635A-B649-4743-A2A7-138E2672ADF9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C812607-A283-49C7-9BD4-BADFD7B6E0E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3195" yWindow="1365" windowWidth="18465" windowHeight="13410" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Coliform Sample" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="249">
   <si>
     <t>Optionality</t>
   </si>
@@ -487,9 +487,6 @@
     <t>B_COUNT_UNITS</t>
   </si>
   <si>
-    <t>Result Count per</t>
-  </si>
-  <si>
     <t>=CountTypeList</t>
   </si>
   <si>
@@ -505,9 +502,6 @@
   </si>
   <si>
     <t>B_COUNT_TYPE</t>
-  </si>
-  <si>
-    <t>Result Count of</t>
   </si>
   <si>
     <t>=PresenceList</t>
@@ -570,9 +564,6 @@
     <t>B_ANALYSIS_METHOD_CODE</t>
   </si>
   <si>
-    <t>Sample Analytical Method</t>
-  </si>
-  <si>
     <t>B_DATA_QUALITY_REASON</t>
   </si>
   <si>
@@ -702,12 +693,6 @@
   </si>
   <si>
     <t>PWSFacilityIdentifier</t>
-  </si>
-  <si>
-    <t>LabAccreditationAuthorityName</t>
-  </si>
-  <si>
-    <t>LabAccreditationIdentifier</t>
   </si>
   <si>
     <t>SampleLocationName</t>
@@ -786,6 +771,72 @@
   </si>
   <si>
     <t>Analysis End Time</t>
+  </si>
+  <si>
+    <t>AnalysisResult &gt; Result &gt;
+MeasurementUnit</t>
+  </si>
+  <si>
+    <t>AnalysisResult &gt; Result &gt;
+MicrobialResultCountTypeCode</t>
+  </si>
+  <si>
+    <t>AnalysisResult &gt; Result &gt;
+MeasurementValue</t>
+  </si>
+  <si>
+    <t>Units</t>
+  </si>
+  <si>
+    <t>per Volume</t>
+  </si>
+  <si>
+    <t>LabAccreditation &gt;
+LabAccreditationAuthorityName</t>
+  </si>
+  <si>
+    <t>LabAccreditation &gt;
+LabAccreditationIdentifier</t>
+  </si>
+  <si>
+    <t>AnalyteIdentification &gt; 
+AnalyteCode</t>
+  </si>
+  <si>
+    <t>AnalysisStartDate</t>
+  </si>
+  <si>
+    <t>AnalysisStartTime</t>
+  </si>
+  <si>
+    <t>AnalysisEndDate</t>
+  </si>
+  <si>
+    <t>AnalysisEndTime</t>
+  </si>
+  <si>
+    <t>ResultStateNotificationDate</t>
+  </si>
+  <si>
+    <t>QAQCSummary &gt;
+DataQualityCode</t>
+  </si>
+  <si>
+    <t>SampleAnalyticalMethod &gt;
+MethodIdentifier</t>
+  </si>
+  <si>
+    <t>Analytical Method</t>
+  </si>
+  <si>
+    <t>SampleAnalyzedMeasure</t>
+  </si>
+  <si>
+    <t>AnalysisResult &gt; Result &gt;
+MeasurementQualifier</t>
+  </si>
+  <si>
+    <t>XML order #</t>
   </si>
 </sst>
 </file>
@@ -872,56 +923,14 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="52">
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
+  <dxfs count="56">
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -934,7 +943,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1004,6 +1013,20 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor theme="5" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
@@ -1014,6 +1037,95 @@
           <bgColor theme="7" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1071,41 +1183,6 @@
     </dxf>
     <dxf>
       <alignment vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1126,9 +1203,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{636125F0-68A9-4682-81D8-01BD3AB67D26}" name="Table1" displayName="Table1" ref="A1:O33" totalsRowShown="0" headerRowDxfId="46" dataDxfId="45">
-  <autoFilter ref="A1:O33" xr:uid="{C224FB70-9F34-49CE-AC5D-FD58B7A283A8}">
-    <filterColumn colId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{636125F0-68A9-4682-81D8-01BD3AB67D26}" name="Table1" displayName="Table1" ref="A1:P33" totalsRowShown="0" headerRowDxfId="55" dataDxfId="54">
+  <autoFilter ref="A1:P33" xr:uid="{C224FB70-9F34-49CE-AC5D-FD58B7A283A8}">
+    <filterColumn colId="7">
       <filters>
         <filter val="Conditional"/>
         <filter val="Mandatory"/>
@@ -1136,48 +1213,50 @@
       </filters>
     </filterColumn>
   </autoFilter>
-  <tableColumns count="15">
-    <tableColumn id="6" xr3:uid="{57EF6AB6-6C4C-4170-BD9B-BF376C46C5DF}" name="Title" dataDxfId="44"/>
-    <tableColumn id="12" xr3:uid="{BFDB40C3-C9ED-4560-81A1-344ECAE248C8}" name="Excel col #" dataDxfId="43"/>
-    <tableColumn id="1" xr3:uid="{3193A6D3-813B-4494-AEED-01D6509FCA0D}" name="CSV Column Name" dataDxfId="42"/>
-    <tableColumn id="11" xr3:uid="{057EA208-1889-4E3C-A179-F312337D9867}" name="CSV col #" dataDxfId="41"/>
-    <tableColumn id="16" xr3:uid="{1F4E7FF6-264D-41DA-AC14-BAA45F3439C7}" name="XML Element" dataDxfId="40"/>
-    <tableColumn id="2" xr3:uid="{5C52F15D-4AC8-44CE-A401-3402D3CD4152}" name="Data Type" dataDxfId="39"/>
-    <tableColumn id="3" xr3:uid="{FFD71D9C-951A-4BB1-9000-9A1C4C3F71D3}" name="Optionality" dataDxfId="38"/>
-    <tableColumn id="4" xr3:uid="{6FEED7B4-CF3F-4593-BB9F-5CFA5FA5B692}" name="Size" dataDxfId="37"/>
-    <tableColumn id="5" xr3:uid="{563427BF-63BA-491F-9B6F-4E02453C643B}" name="Business Rules" dataDxfId="36"/>
-    <tableColumn id="9" xr3:uid="{A9E34622-C2B4-476B-A018-EABC1256DC10}" name="User Editable" dataDxfId="35"/>
-    <tableColumn id="14" xr3:uid="{9DA3EF2F-E261-414A-B10C-F88F2052640F}" name="Generated" dataDxfId="34"/>
-    <tableColumn id="15" xr3:uid="{AA61284F-4409-4E18-9405-8F2EAA78028A}" name="Format" dataDxfId="33"/>
-    <tableColumn id="13" xr3:uid="{94BA7C53-9CFA-4072-B1A4-7E9CE9D9DDF7}" name="Conditional Formatting" dataDxfId="32"/>
-    <tableColumn id="7" xr3:uid="{22AE72C5-BA89-443A-81AF-BCF4B114454C}" name="Validation" dataDxfId="31"/>
-    <tableColumn id="8" xr3:uid="{5DE66E18-4141-4BDD-B41D-2782AC810F6E}" name="Validation Formula" dataDxfId="30"/>
+  <tableColumns count="16">
+    <tableColumn id="6" xr3:uid="{57EF6AB6-6C4C-4170-BD9B-BF376C46C5DF}" name="Title" dataDxfId="53"/>
+    <tableColumn id="12" xr3:uid="{BFDB40C3-C9ED-4560-81A1-344ECAE248C8}" name="Excel col #" dataDxfId="52"/>
+    <tableColumn id="1" xr3:uid="{3193A6D3-813B-4494-AEED-01D6509FCA0D}" name="CSV Column Name" dataDxfId="51"/>
+    <tableColumn id="11" xr3:uid="{057EA208-1889-4E3C-A179-F312337D9867}" name="CSV col #" dataDxfId="50"/>
+    <tableColumn id="16" xr3:uid="{1F4E7FF6-264D-41DA-AC14-BAA45F3439C7}" name="XML Element" dataDxfId="49"/>
+    <tableColumn id="10" xr3:uid="{F503FCB6-1F5D-4765-B4AB-F67230BC37A3}" name="XML order #" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{5C52F15D-4AC8-44CE-A401-3402D3CD4152}" name="Data Type" dataDxfId="48"/>
+    <tableColumn id="3" xr3:uid="{FFD71D9C-951A-4BB1-9000-9A1C4C3F71D3}" name="Optionality" dataDxfId="47"/>
+    <tableColumn id="4" xr3:uid="{6FEED7B4-CF3F-4593-BB9F-5CFA5FA5B692}" name="Size" dataDxfId="46"/>
+    <tableColumn id="5" xr3:uid="{563427BF-63BA-491F-9B6F-4E02453C643B}" name="Business Rules" dataDxfId="45"/>
+    <tableColumn id="9" xr3:uid="{A9E34622-C2B4-476B-A018-EABC1256DC10}" name="User Editable" dataDxfId="44"/>
+    <tableColumn id="14" xr3:uid="{9DA3EF2F-E261-414A-B10C-F88F2052640F}" name="Generated" dataDxfId="43"/>
+    <tableColumn id="15" xr3:uid="{AA61284F-4409-4E18-9405-8F2EAA78028A}" name="Format" dataDxfId="42"/>
+    <tableColumn id="13" xr3:uid="{94BA7C53-9CFA-4072-B1A4-7E9CE9D9DDF7}" name="Conditional Formatting" dataDxfId="41"/>
+    <tableColumn id="7" xr3:uid="{22AE72C5-BA89-443A-81AF-BCF4B114454C}" name="Validation" dataDxfId="40"/>
+    <tableColumn id="8" xr3:uid="{5DE66E18-4141-4BDD-B41D-2782AC810F6E}" name="Validation Formula" dataDxfId="39"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{05345577-AC31-4B6D-B899-55D66DEB1874}" name="Table2" displayName="Table2" ref="A1:O22" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C2:O22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{05345577-AC31-4B6D-B899-55D66DEB1874}" name="Table2" displayName="Table2" ref="A1:P22" totalsRowShown="0" headerRowDxfId="38" dataDxfId="37">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C2:P22">
     <sortCondition ref="D16:D22"/>
   </sortState>
-  <tableColumns count="15">
-    <tableColumn id="7" xr3:uid="{9E32B24E-F549-442D-B6C5-5B5E67078170}" name="Title" dataDxfId="14"/>
-    <tableColumn id="12" xr3:uid="{023EA1AA-B7DF-4814-BFEF-5AB9B0752B95}" name="Excel col #" dataDxfId="13"/>
-    <tableColumn id="1" xr3:uid="{5687DF61-58A8-463A-A7F7-9B8B474466F3}" name="CSV Column Name" dataDxfId="12"/>
-    <tableColumn id="13" xr3:uid="{9E799E78-81C7-4788-BF70-799894A0FACA}" name="CSV col #" dataDxfId="11"/>
-    <tableColumn id="16" xr3:uid="{6872DDE9-C4EA-4656-AE08-1B51AE6AE7D6}" name="XML Element" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{E36A262F-69A4-4276-95F1-0FB7FCE8E2AD}" name="Data Type" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{B4F9F589-759B-40AB-BD12-81562C067103}" name="Optionality" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{29CBFF2E-DC73-4812-9BE8-505CDCED923B}" name="Size" dataDxfId="7"/>
-    <tableColumn id="5" xr3:uid="{2FBE4EBA-0896-4EA8-8E6A-9740D712F4CF}" name="Business Rules" dataDxfId="6"/>
-    <tableColumn id="14" xr3:uid="{F6A291D7-463E-4C10-AE63-F46C62F701F1}" name="User Editable" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{4A3A44E5-9909-437B-9914-BD7AF1AC2439}" name="Generated" dataDxfId="4"/>
-    <tableColumn id="15" xr3:uid="{30410F79-D89B-4BAE-852C-7ADB5287310A}" name="Format" dataDxfId="3"/>
-    <tableColumn id="8" xr3:uid="{23D225B6-A3A4-4446-9AD4-7762B64F46FE}" name="Conditional Formatting" dataDxfId="2"/>
-    <tableColumn id="9" xr3:uid="{27D08B50-8012-49E0-9C10-AEB67B99B91B}" name="Validation" dataDxfId="1"/>
-    <tableColumn id="10" xr3:uid="{A301C8EB-BB2A-4524-AF6E-20714C0D7DD5}" name="Validation Formula" dataDxfId="0"/>
+  <tableColumns count="16">
+    <tableColumn id="7" xr3:uid="{9E32B24E-F549-442D-B6C5-5B5E67078170}" name="Title" dataDxfId="36"/>
+    <tableColumn id="12" xr3:uid="{023EA1AA-B7DF-4814-BFEF-5AB9B0752B95}" name="Excel col #" dataDxfId="35"/>
+    <tableColumn id="1" xr3:uid="{5687DF61-58A8-463A-A7F7-9B8B474466F3}" name="CSV Column Name" dataDxfId="34"/>
+    <tableColumn id="13" xr3:uid="{9E799E78-81C7-4788-BF70-799894A0FACA}" name="CSV col #" dataDxfId="33"/>
+    <tableColumn id="16" xr3:uid="{6872DDE9-C4EA-4656-AE08-1B51AE6AE7D6}" name="XML Element" dataDxfId="32"/>
+    <tableColumn id="11" xr3:uid="{F0D84552-7E57-4362-9DCD-EDC8E4E51415}" name="XML order #" dataDxfId="21"/>
+    <tableColumn id="2" xr3:uid="{E36A262F-69A4-4276-95F1-0FB7FCE8E2AD}" name="Data Type" dataDxfId="31"/>
+    <tableColumn id="3" xr3:uid="{B4F9F589-759B-40AB-BD12-81562C067103}" name="Optionality" dataDxfId="30"/>
+    <tableColumn id="4" xr3:uid="{29CBFF2E-DC73-4812-9BE8-505CDCED923B}" name="Size" dataDxfId="29"/>
+    <tableColumn id="5" xr3:uid="{2FBE4EBA-0896-4EA8-8E6A-9740D712F4CF}" name="Business Rules" dataDxfId="28"/>
+    <tableColumn id="14" xr3:uid="{F6A291D7-463E-4C10-AE63-F46C62F701F1}" name="User Editable" dataDxfId="27"/>
+    <tableColumn id="6" xr3:uid="{4A3A44E5-9909-437B-9914-BD7AF1AC2439}" name="Generated" dataDxfId="26"/>
+    <tableColumn id="15" xr3:uid="{30410F79-D89B-4BAE-852C-7ADB5287310A}" name="Format" dataDxfId="25"/>
+    <tableColumn id="8" xr3:uid="{23D225B6-A3A4-4446-9AD4-7762B64F46FE}" name="Conditional Formatting" dataDxfId="24"/>
+    <tableColumn id="9" xr3:uid="{27D08B50-8012-49E0-9C10-AEB67B99B91B}" name="Validation" dataDxfId="23"/>
+    <tableColumn id="10" xr3:uid="{A301C8EB-BB2A-4524-AF6E-20714C0D7DD5}" name="Validation Formula" dataDxfId="22"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight14" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1447,9 +1526,9 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:O33"/>
+  <dimension ref="A1:P33"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -1462,28 +1541,29 @@
     <col min="3" max="3" width="35" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5" customWidth="1"/>
     <col min="5" max="5" width="33.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.140625" customWidth="1"/>
-    <col min="7" max="7" width="11.28515625" customWidth="1"/>
-    <col min="8" max="8" width="4.85546875" customWidth="1"/>
-    <col min="9" max="9" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.140625" customWidth="1"/>
-    <col min="12" max="12" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="44" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="48.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="33.42578125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="28.5703125" customWidth="1"/>
-    <col min="19" max="19" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.140625" customWidth="1"/>
+    <col min="8" max="8" width="11.28515625" customWidth="1"/>
+    <col min="9" max="9" width="4.85546875" customWidth="1"/>
+    <col min="10" max="10" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.140625" customWidth="1"/>
+    <col min="13" max="13" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="44" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="48.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="33.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="28.5703125" customWidth="1"/>
+    <col min="20" max="20" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>53</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="C1" s="6" t="s">
         <v>108</v>
@@ -1492,40 +1572,43 @@
         <v>119</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="F1" s="6" t="s">
+        <v>248</v>
+      </c>
+      <c r="G1" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="H1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="I1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="J1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="K1" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="L1" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="M1" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="N1" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="O1" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="P1" s="6" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>120</v>
       </c>
@@ -1537,30 +1620,31 @@
         <v>1</v>
       </c>
       <c r="E2" s="7"/>
-      <c r="F2" s="7" t="s">
-        <v>105</v>
-      </c>
+      <c r="F2" s="7"/>
       <c r="G2" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="H2" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="H2" s="8">
+      <c r="I2" s="8">
         <v>20</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="J2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="K2" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="K2" s="7" t="s">
+      <c r="L2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="L2" s="7"/>
       <c r="M2" s="7"/>
       <c r="N2" s="7"/>
       <c r="O2" s="7"/>
-    </row>
-    <row r="3" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="P2" s="7"/>
+    </row>
+    <row r="3" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>56</v>
       </c>
@@ -1574,36 +1658,39 @@
         <v>2</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>105</v>
+        <v>201</v>
+      </c>
+      <c r="F3" s="2">
+        <v>4</v>
       </c>
       <c r="G3" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="H3" s="3">
+      <c r="I3" s="3">
         <v>20</v>
       </c>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2" t="s">
+      <c r="J3" s="2"/>
+      <c r="K3" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="M3" s="4" t="s">
+      <c r="L3" s="2"/>
+      <c r="M3" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="N3" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="N3" s="2" t="s">
+      <c r="O3" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="O3" s="5" t="s">
+      <c r="P3" s="5" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>59</v>
       </c>
@@ -1617,34 +1704,37 @@
         <v>3</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>205</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>105</v>
+        <v>202</v>
+      </c>
+      <c r="F4" s="7">
+        <v>3</v>
       </c>
       <c r="G4" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="H4" s="3">
+      <c r="I4" s="3">
         <v>20</v>
       </c>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2" t="s">
+      <c r="J4" s="2"/>
+      <c r="K4" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2" t="s">
+      <c r="L4" s="2"/>
+      <c r="M4" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="O4" s="2" t="s">
+      <c r="P4" s="2" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>60</v>
       </c>
@@ -1658,38 +1748,41 @@
         <v>4</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>105</v>
+        <v>203</v>
+      </c>
+      <c r="F5" s="2">
+        <v>5</v>
       </c>
       <c r="G5" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="H5" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="H5" s="3">
+      <c r="I5" s="3">
         <v>9</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="J5" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="J5" s="2" t="s">
+      <c r="K5" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="M5" s="5" t="s">
+      <c r="L5" s="2"/>
+      <c r="M5" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="N5" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="N5" s="2" t="s">
+      <c r="O5" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="O5" s="5" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P5" s="5" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>61</v>
       </c>
@@ -1703,36 +1796,39 @@
         <v>5</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>207</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>105</v>
+        <v>204</v>
+      </c>
+      <c r="F6" s="7">
+        <v>10</v>
       </c>
       <c r="G6" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="H6" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="H6" s="3">
+      <c r="I6" s="3">
         <v>1</v>
       </c>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2" t="s">
+      <c r="J6" s="2"/>
+      <c r="K6" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="K6" s="2" t="s">
+      <c r="L6" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="L6" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="M6" s="2"/>
-      <c r="N6" s="2" t="s">
+      <c r="M6" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="O6" s="5" t="s">
+      <c r="P6" s="5" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>62</v>
       </c>
@@ -1743,31 +1839,34 @@
       <c r="D7" s="2">
         <v>6</v>
       </c>
-      <c r="E7" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>105</v>
+      <c r="E7" s="6" t="s">
+        <v>235</v>
+      </c>
+      <c r="F7" s="6">
+        <v>1</v>
       </c>
       <c r="G7" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="H7" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="H7" s="3">
+      <c r="I7" s="3">
         <v>10</v>
       </c>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2" t="s">
+      <c r="J7" s="2"/>
+      <c r="K7" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="K7" s="2" t="s">
+      <c r="L7" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="L7" s="2"/>
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
       <c r="O7" s="2"/>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P7" s="2"/>
+    </row>
+    <row r="8" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>57</v>
       </c>
@@ -1778,31 +1877,34 @@
       <c r="D8" s="7">
         <v>7</v>
       </c>
-      <c r="E8" s="7" t="s">
-        <v>210</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>105</v>
+      <c r="E8" s="13" t="s">
+        <v>236</v>
+      </c>
+      <c r="F8" s="13">
+        <v>2</v>
       </c>
       <c r="G8" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="H8" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="H8" s="3">
+      <c r="I8" s="3">
         <v>10</v>
       </c>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2" t="s">
+      <c r="J8" s="2"/>
+      <c r="K8" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="K8" s="2" t="s">
+      <c r="L8" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="L8" s="2"/>
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
       <c r="O8" s="2"/>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P8" s="2"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>75</v>
       </c>
@@ -1816,38 +1918,41 @@
         <v>8</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>208</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>105</v>
+        <v>205</v>
+      </c>
+      <c r="F9" s="2">
+        <v>6</v>
       </c>
       <c r="G9" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="H9" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="H9" s="3">
+      <c r="I9" s="3">
         <v>10</v>
       </c>
-      <c r="I9" s="2" t="s">
+      <c r="J9" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="J9" s="2" t="s">
+      <c r="K9" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="K9" s="2"/>
-      <c r="L9" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="M9" s="5" t="s">
+      <c r="L9" s="2"/>
+      <c r="M9" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="N9" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="N9" s="2" t="s">
+      <c r="O9" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="O9" s="2" t="s">
+      <c r="P9" s="2" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>86</v>
       </c>
@@ -1861,38 +1966,41 @@
         <v>9</v>
       </c>
       <c r="E10" s="13" t="s">
-        <v>226</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>105</v>
+        <v>221</v>
+      </c>
+      <c r="F10" s="13">
+        <v>21</v>
       </c>
       <c r="G10" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="H10" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="H10" s="3">
+      <c r="I10" s="3">
         <v>12</v>
       </c>
-      <c r="I10" s="2" t="s">
+      <c r="J10" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="J10" s="2" t="s">
+      <c r="K10" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="M10" s="5" t="s">
+      <c r="L10" s="2"/>
+      <c r="M10" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="N10" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="N10" s="2" t="s">
+      <c r="O10" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="O10" s="2" t="s">
+      <c r="P10" s="2" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="11" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>106</v>
       </c>
@@ -1904,30 +2012,31 @@
         <v>10</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>105</v>
-      </c>
+        <v>206</v>
+      </c>
+      <c r="F11" s="2"/>
       <c r="G11" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="H11" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="H11" s="3">
+      <c r="I11" s="3">
         <v>40</v>
       </c>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2" t="s">
+      <c r="J11" s="2"/>
+      <c r="K11" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="K11" s="11" t="s">
+      <c r="L11" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="L11" s="2"/>
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
       <c r="O11" s="2"/>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P11" s="2"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>63</v>
       </c>
@@ -1939,32 +2048,35 @@
         <v>11</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>212</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>105</v>
+        <v>207</v>
+      </c>
+      <c r="F12" s="7">
+        <v>7</v>
       </c>
       <c r="G12" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="H12" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="H12" s="3">
+      <c r="I12" s="3">
         <v>2</v>
       </c>
-      <c r="I12" s="2" t="s">
+      <c r="J12" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J12" s="2" t="s">
+      <c r="K12" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="K12" s="2" t="s">
+      <c r="L12" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="L12" s="2"/>
       <c r="M12" s="2"/>
       <c r="N12" s="2"/>
       <c r="O12" s="2"/>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P12" s="2"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>89</v>
       </c>
@@ -1978,38 +2090,41 @@
         <v>12</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>105</v>
+        <v>208</v>
+      </c>
+      <c r="F13" s="2">
+        <v>9</v>
       </c>
       <c r="G13" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="H13" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="H13" s="3">
+      <c r="I13" s="3">
         <v>1</v>
       </c>
-      <c r="I13" s="2" t="s">
+      <c r="J13" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="J13" s="2" t="s">
+      <c r="K13" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="K13" s="2"/>
-      <c r="L13" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="M13" s="5" t="s">
+      <c r="L13" s="2"/>
+      <c r="M13" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="N13" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="N13" s="2" t="s">
+      <c r="O13" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="O13" s="5" t="s">
+      <c r="P13" s="5" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>90</v>
       </c>
@@ -2023,38 +2138,41 @@
         <v>13</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>214</v>
-      </c>
-      <c r="F14" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="F14" s="7">
+        <v>16</v>
+      </c>
+      <c r="G14" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="G14" s="2" t="s">
+      <c r="H14" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="H14" s="3">
+      <c r="I14" s="3">
         <v>8</v>
       </c>
-      <c r="I14" s="2" t="s">
+      <c r="J14" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="J14" s="2" t="s">
+      <c r="K14" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="K14" s="2"/>
-      <c r="L14" s="2" t="s">
+      <c r="L14" s="2"/>
+      <c r="M14" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="M14" s="5" t="s">
+      <c r="N14" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="N14" s="2" t="s">
+      <c r="O14" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="O14" s="5" t="s">
+      <c r="P14" s="5" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>91</v>
       </c>
@@ -2068,36 +2186,39 @@
         <v>14</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="F15" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="F15" s="2">
+        <v>17</v>
+      </c>
+      <c r="G15" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="G15" s="2" t="s">
+      <c r="H15" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="H15" s="3">
+      <c r="I15" s="3">
         <v>4</v>
       </c>
-      <c r="I15" s="2" t="s">
-        <v>231</v>
-      </c>
       <c r="J15" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="K15" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="K15" s="2"/>
-      <c r="L15" s="2" t="s">
+      <c r="L15" s="2"/>
+      <c r="M15" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="M15" s="2"/>
-      <c r="N15" s="2" t="s">
+      <c r="N15" s="2"/>
+      <c r="O15" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="O15" s="2" t="s">
+      <c r="P15" s="2" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>64</v>
       </c>
@@ -2111,36 +2232,39 @@
         <v>15</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>216</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>105</v>
+        <v>211</v>
+      </c>
+      <c r="F16" s="7">
+        <v>8</v>
       </c>
       <c r="G16" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="H16" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="H16" s="3">
+      <c r="I16" s="3">
         <v>2</v>
       </c>
-      <c r="I16" s="2"/>
-      <c r="J16" s="2" t="s">
+      <c r="J16" s="2"/>
+      <c r="K16" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="K16" s="2"/>
-      <c r="L16" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="M16" s="5" t="s">
+      <c r="L16" s="2"/>
+      <c r="M16" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="N16" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="N16" s="2" t="s">
+      <c r="O16" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="O16" s="5" t="s">
+      <c r="P16" s="5" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="17" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>65</v>
       </c>
@@ -2154,36 +2278,39 @@
         <v>16</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>225</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>105</v>
+        <v>220</v>
+      </c>
+      <c r="F17" s="6">
+        <v>22</v>
       </c>
       <c r="G17" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="H17" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="H17" s="3">
+      <c r="I17" s="3">
         <v>2</v>
       </c>
-      <c r="I17" s="2"/>
-      <c r="J17" s="2" t="s">
+      <c r="J17" s="2"/>
+      <c r="K17" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="K17" s="2"/>
-      <c r="L17" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="M17" s="4" t="s">
-        <v>200</v>
-      </c>
-      <c r="N17" s="2" t="s">
+      <c r="L17" s="2"/>
+      <c r="M17" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="N17" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="O17" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="O17" s="5" t="s">
+      <c r="P17" s="5" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>66</v>
       </c>
@@ -2197,36 +2324,39 @@
         <v>17</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>217</v>
-      </c>
-      <c r="F18" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="F18" s="7">
+        <v>18</v>
+      </c>
+      <c r="G18" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="G18" s="2" t="s">
+      <c r="H18" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="H18" s="3">
+      <c r="I18" s="3">
         <v>8</v>
       </c>
-      <c r="I18" s="2" t="s">
+      <c r="J18" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="J18" s="2" t="s">
+      <c r="K18" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="K18" s="2"/>
-      <c r="L18" s="2" t="s">
+      <c r="L18" s="2"/>
+      <c r="M18" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="M18" s="2"/>
-      <c r="N18" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="O18" s="5" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="N18" s="2"/>
+      <c r="O18" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="P18" s="5" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>107</v>
       </c>
@@ -2240,36 +2370,39 @@
         <v>18</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>222</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>105</v>
+        <v>217</v>
+      </c>
+      <c r="F19" s="6">
+        <v>15</v>
       </c>
       <c r="G19" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="H19" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="H19" s="3">
+      <c r="I19" s="3">
         <v>40</v>
       </c>
-      <c r="I19" s="2" t="s">
+      <c r="J19" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="J19" s="2" t="s">
+      <c r="K19" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="K19" s="2"/>
-      <c r="L19" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="M19" s="2"/>
-      <c r="N19" s="2" t="s">
+      <c r="L19" s="2"/>
+      <c r="M19" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="N19" s="2"/>
+      <c r="O19" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="O19" s="2" t="s">
+      <c r="P19" s="2" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="20" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>67</v>
       </c>
@@ -2281,30 +2414,31 @@
         <v>19</v>
       </c>
       <c r="E20" s="13" t="s">
-        <v>219</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>105</v>
-      </c>
+        <v>214</v>
+      </c>
+      <c r="F20" s="13"/>
       <c r="G20" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="H20" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="H20" s="3">
+      <c r="I20" s="3">
         <v>9</v>
       </c>
-      <c r="I20" s="2"/>
-      <c r="J20" s="2" t="s">
+      <c r="J20" s="2"/>
+      <c r="K20" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="K20" s="11" t="s">
+      <c r="L20" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="L20" s="2"/>
       <c r="M20" s="2"/>
       <c r="N20" s="2"/>
       <c r="O20" s="2"/>
-    </row>
-    <row r="21" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="P20" s="2"/>
+    </row>
+    <row r="21" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>68</v>
       </c>
@@ -2316,30 +2450,31 @@
         <v>20</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>218</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>105</v>
-      </c>
+        <v>213</v>
+      </c>
+      <c r="F21" s="7"/>
       <c r="G21" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="H21" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="H21" s="3">
+      <c r="I21" s="3">
         <v>2</v>
       </c>
-      <c r="I21" s="2"/>
-      <c r="J21" s="2" t="s">
+      <c r="J21" s="2"/>
+      <c r="K21" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="K21" s="11" t="s">
+      <c r="L21" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="L21" s="2"/>
       <c r="M21" s="2"/>
       <c r="N21" s="2"/>
       <c r="O21" s="2"/>
-    </row>
-    <row r="22" spans="1:15" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="P21" s="2"/>
+    </row>
+    <row r="22" spans="1:16" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>69</v>
       </c>
@@ -2351,32 +2486,33 @@
         <v>21</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>221</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>105</v>
-      </c>
+        <v>216</v>
+      </c>
+      <c r="F22" s="6"/>
       <c r="G22" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="H22" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="H22" s="3">
+      <c r="I22" s="3">
         <v>12</v>
       </c>
-      <c r="I22" s="2"/>
-      <c r="J22" s="2" t="s">
+      <c r="J22" s="2"/>
+      <c r="K22" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="K22" s="11" t="s">
+      <c r="L22" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="L22" s="2"/>
       <c r="M22" s="2"/>
       <c r="N22" s="2"/>
       <c r="O22" s="2"/>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P22" s="2"/>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="B23" s="2">
         <v>14</v>
@@ -2388,38 +2524,41 @@
         <v>22</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>220</v>
-      </c>
-      <c r="F23" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="F23" s="7">
+        <v>19</v>
+      </c>
+      <c r="G23" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="G23" s="2" t="s">
+      <c r="H23" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="H23" s="3" t="s">
+      <c r="I23" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="I23" s="2" t="s">
+      <c r="J23" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="J23" s="2" t="s">
+      <c r="K23" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="K23" s="2"/>
-      <c r="L23" s="2" t="s">
+      <c r="L23" s="2"/>
+      <c r="M23" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="M23" s="2"/>
-      <c r="N23" s="2" t="s">
+      <c r="N23" s="2"/>
+      <c r="O23" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="O23" s="2" t="s">
+      <c r="P23" s="2" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="B24" s="2">
         <v>15</v>
@@ -2431,36 +2570,39 @@
         <v>23</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>220</v>
-      </c>
-      <c r="F24" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="F24" s="7">
+        <v>20</v>
+      </c>
+      <c r="G24" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="G24" s="2" t="s">
+      <c r="H24" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="H24" s="3" t="s">
+      <c r="I24" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="I24" s="2" t="s">
+      <c r="J24" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="J24" s="2" t="s">
+      <c r="K24" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="K24" s="2"/>
-      <c r="L24" s="2" t="s">
+      <c r="L24" s="2"/>
+      <c r="M24" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="M24" s="2"/>
-      <c r="N24" s="2" t="s">
+      <c r="N24" s="2"/>
+      <c r="O24" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="O24" s="2" t="s">
+      <c r="P24" s="2" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="25" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>70</v>
       </c>
@@ -2472,30 +2614,31 @@
         <v>24</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>220</v>
-      </c>
-      <c r="F25" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="F25" s="7"/>
+      <c r="G25" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="G25" s="2" t="s">
+      <c r="H25" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="H25" s="3" t="s">
+      <c r="I25" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="I25" s="2"/>
-      <c r="J25" s="2" t="s">
+      <c r="J25" s="2"/>
+      <c r="K25" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="K25" s="11" t="s">
+      <c r="L25" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="L25" s="2"/>
       <c r="M25" s="2"/>
       <c r="N25" s="2"/>
       <c r="O25" s="2"/>
-    </row>
-    <row r="26" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="P25" s="2"/>
+    </row>
+    <row r="26" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>71</v>
       </c>
@@ -2507,28 +2650,29 @@
         <v>25</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>220</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>105</v>
-      </c>
+        <v>215</v>
+      </c>
+      <c r="F26" s="7"/>
       <c r="G26" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="H26" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="H26" s="3"/>
-      <c r="I26" s="2"/>
-      <c r="J26" s="2" t="s">
+      <c r="I26" s="3"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="K26" s="11" t="s">
+      <c r="L26" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="L26" s="2"/>
       <c r="M26" s="2"/>
       <c r="N26" s="2"/>
       <c r="O26" s="2"/>
-    </row>
-    <row r="27" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="P26" s="2"/>
+    </row>
+    <row r="27" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>72</v>
       </c>
@@ -2540,30 +2684,31 @@
         <v>26</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>220</v>
-      </c>
-      <c r="F27" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="F27" s="7"/>
+      <c r="G27" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="G27" s="2" t="s">
+      <c r="H27" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="H27" s="3" t="s">
+      <c r="I27" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="I27" s="2"/>
-      <c r="J27" s="2" t="s">
+      <c r="J27" s="2"/>
+      <c r="K27" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="K27" s="11" t="s">
+      <c r="L27" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="L27" s="2"/>
       <c r="M27" s="2"/>
       <c r="N27" s="2"/>
       <c r="O27" s="2"/>
-    </row>
-    <row r="28" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="P27" s="2"/>
+    </row>
+    <row r="28" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>76</v>
       </c>
@@ -2575,30 +2720,31 @@
         <v>27</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>220</v>
-      </c>
-      <c r="F28" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="F28" s="7"/>
+      <c r="G28" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="G28" s="2" t="s">
+      <c r="H28" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="H28" s="3" t="s">
+      <c r="I28" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="I28" s="2"/>
-      <c r="J28" s="2" t="s">
+      <c r="J28" s="2"/>
+      <c r="K28" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="K28" s="11" t="s">
+      <c r="L28" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="L28" s="2"/>
       <c r="M28" s="2"/>
       <c r="N28" s="2"/>
       <c r="O28" s="2"/>
-    </row>
-    <row r="29" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="P28" s="2"/>
+    </row>
+    <row r="29" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>73</v>
       </c>
@@ -2610,30 +2756,31 @@
         <v>28</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>220</v>
-      </c>
-      <c r="F29" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="F29" s="7"/>
+      <c r="G29" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="G29" s="2" t="s">
+      <c r="H29" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="H29" s="3" t="s">
+      <c r="I29" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="I29" s="2"/>
-      <c r="J29" s="2" t="s">
+      <c r="J29" s="2"/>
+      <c r="K29" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="K29" s="11" t="s">
+      <c r="L29" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="L29" s="2"/>
       <c r="M29" s="2"/>
       <c r="N29" s="2"/>
       <c r="O29" s="2"/>
-    </row>
-    <row r="30" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="P29" s="2"/>
+    </row>
+    <row r="30" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>104</v>
       </c>
@@ -2647,38 +2794,41 @@
         <v>29</v>
       </c>
       <c r="E30" s="13" t="s">
-        <v>223</v>
-      </c>
-      <c r="F30" s="2" t="s">
-        <v>105</v>
+        <v>218</v>
+      </c>
+      <c r="F30" s="13">
+        <v>11</v>
       </c>
       <c r="G30" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="H30" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="H30" s="3">
+      <c r="I30" s="3">
         <v>20</v>
       </c>
-      <c r="I30" s="2" t="s">
+      <c r="J30" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="J30" s="2" t="s">
+      <c r="K30" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="K30" s="2"/>
-      <c r="L30" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="M30" s="4" t="s">
-        <v>201</v>
-      </c>
-      <c r="N30" s="2" t="s">
+      <c r="L30" s="2"/>
+      <c r="M30" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="N30" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="O30" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="O30" s="5" t="s">
+      <c r="P30" s="5" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="31" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>133</v>
       </c>
@@ -2692,38 +2842,41 @@
         <v>30</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>224</v>
-      </c>
-      <c r="F31" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="F31" s="6">
+        <v>12</v>
+      </c>
+      <c r="G31" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="G31" s="2" t="s">
+      <c r="H31" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="H31" s="3">
+      <c r="I31" s="3">
         <v>8</v>
       </c>
-      <c r="I31" s="2" t="s">
+      <c r="J31" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="J31" s="2" t="s">
+      <c r="K31" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="K31" s="2"/>
-      <c r="L31" s="2" t="s">
+      <c r="L31" s="2"/>
+      <c r="M31" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="M31" s="4" t="s">
-        <v>202</v>
-      </c>
-      <c r="N31" s="2" t="s">
+      <c r="N31" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="O31" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="O31" s="5" t="s">
+      <c r="P31" s="5" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="32" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>74</v>
       </c>
@@ -2735,32 +2888,35 @@
         <v>31</v>
       </c>
       <c r="E32" s="13" t="s">
-        <v>229</v>
-      </c>
-      <c r="F32" s="2" t="s">
-        <v>105</v>
+        <v>224</v>
+      </c>
+      <c r="F32" s="13">
+        <v>13</v>
       </c>
       <c r="G32" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="H32" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="H32" s="3">
+      <c r="I32" s="3">
         <v>10</v>
       </c>
-      <c r="I32" s="2" t="s">
+      <c r="J32" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="J32" s="2" t="s">
+      <c r="K32" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="K32" s="2" t="s">
+      <c r="L32" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="L32" s="2"/>
       <c r="M32" s="2"/>
       <c r="N32" s="2"/>
       <c r="O32" s="2"/>
-    </row>
-    <row r="33" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+      <c r="P32" s="2"/>
+    </row>
+    <row r="33" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>58</v>
       </c>
@@ -2772,56 +2928,59 @@
         <v>32</v>
       </c>
       <c r="E33" s="13" t="s">
-        <v>230</v>
-      </c>
-      <c r="F33" s="2" t="s">
-        <v>105</v>
+        <v>225</v>
+      </c>
+      <c r="F33" s="13">
+        <v>14</v>
       </c>
       <c r="G33" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="H33" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="H33" s="3">
+      <c r="I33" s="3">
         <v>10</v>
       </c>
-      <c r="I33" s="2" t="s">
+      <c r="J33" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="J33" s="2" t="s">
+      <c r="K33" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="K33" s="2" t="s">
+      <c r="L33" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="L33" s="2"/>
       <c r="M33" s="2"/>
       <c r="N33" s="2"/>
       <c r="O33" s="2"/>
+      <c r="P33" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
-  <conditionalFormatting sqref="D2:E33">
-    <cfRule type="expression" dxfId="51" priority="11">
+  <conditionalFormatting sqref="D2:F33">
+    <cfRule type="expression" dxfId="20" priority="11">
       <formula>LEN($D2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:A31 C15:N15 C2:O14 C16:O31 A32:O33">
-    <cfRule type="expression" dxfId="50" priority="12">
-      <formula>$J2="No"</formula>
+  <conditionalFormatting sqref="A2:A31 C15:O15 C2:P14 C16:P31 A32:P33">
+    <cfRule type="expression" dxfId="19" priority="12">
+      <formula>$K2="No"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K2:K33">
-    <cfRule type="expression" dxfId="49" priority="10">
-      <formula>AND($J2="No",LEN($K2)=0)</formula>
+  <conditionalFormatting sqref="L2:L33">
+    <cfRule type="expression" dxfId="18" priority="10">
+      <formula>AND($K2="No",LEN($L2)=0)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O15">
-    <cfRule type="expression" dxfId="48" priority="2">
-      <formula>$J15="No"</formula>
+  <conditionalFormatting sqref="P15">
+    <cfRule type="expression" dxfId="17" priority="2">
+      <formula>$K15="No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B31">
-    <cfRule type="expression" dxfId="47" priority="1">
-      <formula>$J2="No"</formula>
+    <cfRule type="expression" dxfId="16" priority="1">
+      <formula>$K2="No"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2835,12 +2994,12 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15FEC0F5-029A-4987-81C0-EA7F2B314198}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:O22"/>
+  <dimension ref="A1:P22"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="C16" sqref="C16"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2849,25 +3008,26 @@
     <col min="2" max="2" width="5.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="35" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.28515625" customWidth="1"/>
-    <col min="7" max="7" width="11.28515625" customWidth="1"/>
-    <col min="8" max="8" width="5.42578125" customWidth="1"/>
-    <col min="9" max="9" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.5703125" customWidth="1"/>
-    <col min="12" max="12" width="25.140625" customWidth="1"/>
-    <col min="13" max="13" width="36.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.140625" customWidth="1"/>
-    <col min="15" max="15" width="31.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.28515625" customWidth="1"/>
+    <col min="8" max="8" width="11.28515625" customWidth="1"/>
+    <col min="9" max="9" width="5.42578125" customWidth="1"/>
+    <col min="10" max="10" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.5703125" customWidth="1"/>
+    <col min="13" max="13" width="25.140625" customWidth="1"/>
+    <col min="14" max="14" width="36.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.140625" customWidth="1"/>
+    <col min="16" max="16" width="31.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>53</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="C1" s="6" t="s">
         <v>108</v>
@@ -2876,40 +3036,43 @@
         <v>119</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="F1" s="6" t="s">
+        <v>248</v>
+      </c>
+      <c r="G1" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="H1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="I1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="K1" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="L1" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="M1" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="N1" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="O1" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="P1" s="6" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>120</v>
       </c>
@@ -2921,30 +3084,31 @@
         <v>1</v>
       </c>
       <c r="E2" s="2"/>
-      <c r="F2" s="2" t="s">
-        <v>105</v>
-      </c>
+      <c r="F2" s="2"/>
       <c r="G2" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="H2" s="2">
+      <c r="I2" s="2">
         <v>20</v>
       </c>
-      <c r="I2" s="2" t="s">
-        <v>196</v>
-      </c>
       <c r="J2" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="K2" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="K2" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="L2" s="2"/>
+      <c r="L2" s="2" t="s">
+        <v>193</v>
+      </c>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
-    </row>
-    <row r="3" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="P2" s="2"/>
+    </row>
+    <row r="3" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>56</v>
       </c>
@@ -2957,37 +3121,42 @@
       <c r="D3" s="2">
         <v>2</v>
       </c>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2" t="s">
-        <v>105</v>
+      <c r="E3" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="F3" s="2">
+        <v>1</v>
       </c>
       <c r="G3" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="H3" s="2">
+      <c r="I3" s="2">
         <v>20</v>
       </c>
-      <c r="I3" s="2" t="s">
-        <v>195</v>
-      </c>
       <c r="J3" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="K3" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="M3" s="4" t="s">
+      <c r="L3" s="2"/>
+      <c r="M3" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="N3" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="N3" s="2" t="s">
+      <c r="O3" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="O3" s="5" t="s">
+      <c r="P3" s="5" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>90</v>
       </c>
@@ -3000,37 +3169,42 @@
       <c r="D4" s="2">
         <v>3</v>
       </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2" t="s">
+      <c r="E4" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="F4" s="2">
+        <v>3</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="H4" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="H4" s="2">
+      <c r="I4" s="2">
         <v>8</v>
       </c>
-      <c r="I4" s="2" t="s">
-        <v>194</v>
-      </c>
       <c r="J4" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="K4" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2" t="s">
+      <c r="L4" s="2"/>
+      <c r="M4" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="M4" s="5" t="s">
-        <v>193</v>
-      </c>
-      <c r="N4" s="2" t="s">
+      <c r="N4" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="O4" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="O4" s="5" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P4" s="5" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>60</v>
       </c>
@@ -3043,37 +3217,42 @@
       <c r="D5" s="2">
         <v>4</v>
       </c>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2" t="s">
-        <v>105</v>
+      <c r="E5" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="F5" s="2">
+        <v>2</v>
       </c>
       <c r="G5" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="H5" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="H5" s="2">
+      <c r="I5" s="2">
         <v>9</v>
       </c>
-      <c r="I5" s="2" t="s">
-        <v>191</v>
-      </c>
       <c r="J5" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="K5" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="M5" s="5" t="s">
+      <c r="L5" s="2"/>
+      <c r="M5" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="N5" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="N5" s="2" t="s">
+      <c r="O5" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="O5" s="2" t="s">
+      <c r="P5" s="2" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>62</v>
       </c>
@@ -3084,29 +3263,34 @@
       <c r="D6" s="2">
         <v>5</v>
       </c>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2" t="s">
-        <v>105</v>
+      <c r="E6" s="6" t="s">
+        <v>235</v>
+      </c>
+      <c r="F6" s="6">
+        <v>4</v>
       </c>
       <c r="G6" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="H6" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="H6" s="2">
+      <c r="I6" s="2">
         <v>10</v>
       </c>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2" t="s">
+      <c r="J6" s="2"/>
+      <c r="K6" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="K6" s="2" t="s">
+      <c r="L6" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="L6" s="2"/>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
       <c r="O6" s="2"/>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P6" s="2"/>
+    </row>
+    <row r="7" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>57</v>
       </c>
@@ -3117,546 +3301,608 @@
       <c r="D7" s="2">
         <v>6</v>
       </c>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2" t="s">
-        <v>105</v>
+      <c r="E7" s="13" t="s">
+        <v>236</v>
+      </c>
+      <c r="F7" s="13">
+        <v>5</v>
       </c>
       <c r="G7" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="H7" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="H7" s="2">
+      <c r="I7" s="2">
         <v>10</v>
       </c>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2" t="s">
+      <c r="J7" s="2"/>
+      <c r="K7" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="K7" s="2" t="s">
+      <c r="L7" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="L7" s="2"/>
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
       <c r="O7" s="2"/>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P7" s="2"/>
+    </row>
+    <row r="8" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B8" s="2">
         <v>4</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="D8" s="2">
         <v>7</v>
       </c>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2" t="s">
-        <v>105</v>
+      <c r="E8" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="F8" s="6">
+        <v>12</v>
       </c>
       <c r="G8" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="H8" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="H8" s="2">
+      <c r="I8" s="2">
         <v>4</v>
       </c>
-      <c r="I8" s="2" t="s">
-        <v>188</v>
-      </c>
       <c r="J8" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="K8" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="M8" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="N8" s="2" t="s">
+      <c r="L8" s="2"/>
+      <c r="M8" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="N8" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="O8" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="O8" s="5" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P8" s="5" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B9" s="2">
         <v>5</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="D9" s="2">
         <v>8</v>
       </c>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2" t="s">
+      <c r="E9" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="F9" s="2">
+        <v>8</v>
+      </c>
+      <c r="G9" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="H9" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="H9" s="2">
+      <c r="I9" s="2">
         <v>8</v>
       </c>
-      <c r="I9" s="2" t="s">
-        <v>183</v>
-      </c>
       <c r="J9" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="K9" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="K9" s="2"/>
-      <c r="L9" s="2" t="s">
+      <c r="L9" s="2"/>
+      <c r="M9" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="M9" s="5"/>
-      <c r="N9" s="2" t="s">
+      <c r="N9" s="5"/>
+      <c r="O9" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="O9" s="5" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P9" s="5" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B10" s="2">
         <v>6</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="D10" s="2">
         <v>9</v>
       </c>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2" t="s">
+      <c r="E10" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="F10" s="2">
+        <v>9</v>
+      </c>
+      <c r="G10" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="G10" s="2" t="s">
+      <c r="H10" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="H10" s="2">
+      <c r="I10" s="2">
         <v>4</v>
       </c>
-      <c r="I10" s="2" t="s">
-        <v>231</v>
-      </c>
       <c r="J10" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="K10" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2" t="s">
+      <c r="L10" s="2"/>
+      <c r="M10" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="M10" s="2"/>
-      <c r="N10" s="2" t="s">
+      <c r="N10" s="2"/>
+      <c r="O10" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="O10" s="2" t="s">
+      <c r="P10" s="2" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="B11" s="2">
         <v>7</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="D11" s="2">
         <v>10</v>
       </c>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2" t="s">
+      <c r="E11" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="F11" s="2">
+        <v>10</v>
+      </c>
+      <c r="G11" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="G11" s="2" t="s">
+      <c r="H11" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="H11" s="2">
+      <c r="I11" s="2">
         <v>8</v>
       </c>
-      <c r="I11" s="2" t="s">
-        <v>178</v>
-      </c>
       <c r="J11" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="K11" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="K11" s="2"/>
-      <c r="L11" s="2" t="s">
+      <c r="L11" s="2"/>
+      <c r="M11" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="M11" s="5"/>
-      <c r="N11" s="2" t="s">
+      <c r="N11" s="5"/>
+      <c r="O11" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="O11" s="5" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P11" s="5" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="B12" s="2">
         <v>8</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D12" s="2">
         <v>11</v>
       </c>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2" t="s">
+      <c r="E12" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="F12" s="2">
+        <v>11</v>
+      </c>
+      <c r="G12" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="H12" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="H12" s="2">
+      <c r="I12" s="2">
         <v>4</v>
       </c>
-      <c r="I12" s="2" t="s">
-        <v>231</v>
-      </c>
       <c r="J12" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="K12" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="K12" s="2"/>
-      <c r="L12" s="2" t="s">
+      <c r="L12" s="2"/>
+      <c r="M12" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="M12" s="2"/>
-      <c r="N12" s="2" t="s">
+      <c r="N12" s="2"/>
+      <c r="O12" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="O12" s="2" t="s">
+      <c r="P12" s="2" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B13" s="2">
         <v>9</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="D13" s="2">
         <v>12</v>
       </c>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2" t="s">
+      <c r="E13" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="F13" s="2">
+        <v>17</v>
+      </c>
+      <c r="G13" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="G13" s="2" t="s">
+      <c r="H13" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="H13" s="2">
+      <c r="I13" s="2">
         <v>8</v>
       </c>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2" t="s">
+      <c r="J13" s="2"/>
+      <c r="K13" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="K13" s="2"/>
-      <c r="L13" s="2" t="s">
+      <c r="L13" s="2"/>
+      <c r="M13" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="M13" s="5"/>
-      <c r="N13" s="2"/>
-      <c r="O13" s="5"/>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N13" s="5"/>
+      <c r="O13" s="2"/>
+      <c r="P13" s="5"/>
+    </row>
+    <row r="14" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="D14" s="2">
         <v>13</v>
       </c>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2" t="s">
-        <v>105</v>
+      <c r="E14" s="6" t="s">
+        <v>243</v>
+      </c>
+      <c r="F14" s="6">
+        <v>18</v>
       </c>
       <c r="G14" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="H14" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="H14" s="2">
+      <c r="I14" s="2">
         <v>1</v>
       </c>
-      <c r="I14" s="2" t="s">
-        <v>171</v>
-      </c>
       <c r="J14" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="K14" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="K14" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="L14" s="2"/>
+      <c r="L14" s="2" t="s">
+        <v>167</v>
+      </c>
       <c r="M14" s="2"/>
       <c r="N14" s="2"/>
       <c r="O14" s="2"/>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P14" s="2"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="2" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="D15" s="2">
         <v>14</v>
       </c>
       <c r="E15" s="2"/>
-      <c r="F15" s="2" t="s">
-        <v>105</v>
-      </c>
+      <c r="F15" s="2"/>
       <c r="G15" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="H15" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="H15" s="2">
+      <c r="I15" s="2">
         <v>2</v>
       </c>
-      <c r="I15" s="2"/>
-      <c r="J15" s="2" t="s">
+      <c r="J15" s="2"/>
+      <c r="K15" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="K15" s="11" t="s">
+      <c r="L15" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="L15" s="2"/>
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
       <c r="O15" s="2"/>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P15" s="2"/>
+    </row>
+    <row r="16" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>167</v>
+        <v>245</v>
       </c>
       <c r="B16" s="2">
         <v>10</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D16" s="2">
         <v>15</v>
       </c>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2" t="s">
-        <v>105</v>
+      <c r="E16" s="6" t="s">
+        <v>244</v>
+      </c>
+      <c r="F16" s="6">
+        <v>6</v>
       </c>
       <c r="G16" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="H16" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="H16" s="2">
+      <c r="I16" s="2">
         <v>30</v>
       </c>
-      <c r="I16" s="2" t="s">
-        <v>165</v>
-      </c>
       <c r="J16" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="K16" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="K16" s="2"/>
-      <c r="L16" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="M16" s="2"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2" t="s">
+        <v>105</v>
+      </c>
       <c r="N16" s="2"/>
       <c r="O16" s="2"/>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P16" s="2"/>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B17" s="2">
         <v>11</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D17" s="2">
         <v>16</v>
       </c>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2" t="s">
-        <v>105</v>
+      <c r="E17" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="F17" s="2">
+        <v>7</v>
       </c>
       <c r="G17" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="H17" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="H17" s="2">
+      <c r="I17" s="2">
         <v>9</v>
       </c>
-      <c r="I17" s="2" t="s">
-        <v>162</v>
-      </c>
       <c r="J17" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="K17" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="K17" s="2"/>
-      <c r="L17" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="M17" s="2"/>
-      <c r="N17" s="2" t="s">
+      <c r="L17" s="2"/>
+      <c r="M17" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="N17" s="2"/>
+      <c r="O17" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="O17" s="5" t="s">
+      <c r="P17" s="5" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B18" s="2">
         <v>12</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D18" s="2">
         <v>17</v>
       </c>
       <c r="E18" s="2"/>
-      <c r="F18" s="2" t="s">
-        <v>105</v>
-      </c>
+      <c r="F18" s="2"/>
       <c r="G18" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="H18" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="H18" s="2">
+      <c r="I18" s="2">
         <v>4</v>
       </c>
-      <c r="I18" s="2" t="s">
-        <v>159</v>
-      </c>
       <c r="J18" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="K18" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="K18" s="2"/>
-      <c r="L18" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="M18" s="2"/>
-      <c r="N18" s="2" t="s">
+      <c r="L18" s="2"/>
+      <c r="M18" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="N18" s="2"/>
+      <c r="O18" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="O18" s="5" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P18" s="5" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B19" s="2">
         <v>13</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D19" s="2">
         <v>18</v>
       </c>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2" t="s">
-        <v>105</v>
+      <c r="E19" s="6" t="s">
+        <v>247</v>
+      </c>
+      <c r="F19" s="6">
+        <v>13</v>
       </c>
       <c r="G19" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="H19" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="H19" s="2">
+      <c r="I19" s="2">
         <v>1</v>
       </c>
-      <c r="I19" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="J19" s="2" t="s">
+      <c r="J19" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="K19" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="K19" s="2"/>
-      <c r="L19" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="M19" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="N19" s="2" t="s">
+      <c r="L19" s="2"/>
+      <c r="M19" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="N19" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="O19" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="O19" s="5" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P19" s="5" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>152</v>
+        <v>234</v>
       </c>
       <c r="B20" s="2">
         <v>14</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D20" s="2">
         <v>20</v>
       </c>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2" t="s">
-        <v>105</v>
+      <c r="E20" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="F20" s="6">
+        <v>15</v>
       </c>
       <c r="G20" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="H20" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="H20" s="2">
+      <c r="I20" s="2">
         <v>10</v>
       </c>
-      <c r="I20" s="2" t="s">
-        <v>150</v>
-      </c>
       <c r="J20" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="K20" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="K20" s="2"/>
-      <c r="L20" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="M20" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="N20" s="2" t="s">
+      <c r="L20" s="2"/>
+      <c r="M20" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="N20" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="O20" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="O20" s="5" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P20" s="5" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>147</v>
+        <v>233</v>
       </c>
       <c r="B21" s="2">
         <v>15</v>
@@ -3667,37 +3913,42 @@
       <c r="D21" s="2">
         <v>27</v>
       </c>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2" t="s">
-        <v>105</v>
+      <c r="E21" s="6" t="s">
+        <v>231</v>
+      </c>
+      <c r="F21" s="6">
+        <v>16</v>
       </c>
       <c r="G21" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="H21" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="H21" s="2">
+      <c r="I21" s="2">
         <v>9</v>
       </c>
-      <c r="I21" s="2" t="s">
+      <c r="J21" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="J21" s="2" t="s">
+      <c r="K21" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="K21" s="2"/>
-      <c r="L21" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="M21" s="5" t="s">
+      <c r="L21" s="2"/>
+      <c r="M21" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="N21" s="5" t="s">
         <v>144</v>
       </c>
-      <c r="N21" s="2" t="s">
+      <c r="O21" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="O21" s="5" t="s">
+      <c r="P21" s="5" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>142</v>
       </c>
@@ -3710,96 +3961,111 @@
       <c r="D22" s="2">
         <v>28</v>
       </c>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2" t="s">
+      <c r="E22" s="6" t="s">
+        <v>232</v>
+      </c>
+      <c r="F22" s="6">
+        <v>14</v>
+      </c>
+      <c r="G22" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="G22" s="2" t="s">
+      <c r="H22" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="H22" s="2" t="s">
+      <c r="I22" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="I22" s="2" t="s">
+      <c r="J22" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="J22" s="2" t="s">
+      <c r="K22" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="K22" s="2"/>
       <c r="L22" s="2"/>
       <c r="M22" s="2"/>
-      <c r="N22" s="2" t="s">
+      <c r="N22" s="2"/>
+      <c r="O22" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="O22" s="2" t="s">
+      <c r="P22" s="2" t="s">
         <v>137</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="K2:K22">
-    <cfRule type="expression" dxfId="29" priority="11">
-      <formula>AND($J2="No",LEN($K2)=0)</formula>
+  <conditionalFormatting sqref="L2:L22">
+    <cfRule type="expression" dxfId="15" priority="13">
+      <formula>AND($K2="No",LEN($L2)=0)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:E22">
-    <cfRule type="expression" dxfId="28" priority="12">
+  <conditionalFormatting sqref="D2:F5 D6:D7 D8:F22">
+    <cfRule type="expression" dxfId="14" priority="14">
       <formula>LEN($D2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N3 N4:O4 N8:O8 N19:O19 A2:A22 C20:O22 C19:L19 C11:O11 C9:M9 C8:L8 C3:L5 C6:O7 C2:O2 C10:H10 J10:O10 C13:O18 C12:H12 J12:O12">
-    <cfRule type="expression" dxfId="27" priority="13">
-      <formula>$J2="No"</formula>
+  <conditionalFormatting sqref="O3 O4:P4 O8:P8 O19:P19 A2:A22 C20:P22 C11:P11 C9:N9 C8:M8 C3:M5 C6:D7 C2:P2 C10:I10 K10:P10 C13:P18 C12:I12 K12:P12 G6:P7 C19:M19">
+    <cfRule type="expression" dxfId="13" priority="15">
+      <formula>$K2="No"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M3">
-    <cfRule type="expression" dxfId="26" priority="10">
-      <formula>$J3="No"</formula>
+  <conditionalFormatting sqref="N3">
+    <cfRule type="expression" dxfId="12" priority="12">
+      <formula>$K3="No"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O3">
-    <cfRule type="expression" dxfId="25" priority="9">
-      <formula>$J3="No"</formula>
+  <conditionalFormatting sqref="P3">
+    <cfRule type="expression" dxfId="11" priority="11">
+      <formula>$K3="No"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M4:M5">
-    <cfRule type="expression" dxfId="24" priority="8">
-      <formula>$J4="No"</formula>
+  <conditionalFormatting sqref="N4:N5">
+    <cfRule type="expression" dxfId="10" priority="10">
+      <formula>$K4="No"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N5:O5">
-    <cfRule type="expression" dxfId="23" priority="7">
-      <formula>$J5="No"</formula>
+  <conditionalFormatting sqref="O5:P5">
+    <cfRule type="expression" dxfId="9" priority="9">
+      <formula>$K5="No"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M8">
-    <cfRule type="expression" dxfId="22" priority="6">
-      <formula>$J8="No"</formula>
+  <conditionalFormatting sqref="N8">
+    <cfRule type="expression" dxfId="8" priority="8">
+      <formula>$K8="No"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N9:O9">
-    <cfRule type="expression" dxfId="21" priority="5">
-      <formula>$J9="No"</formula>
+  <conditionalFormatting sqref="O9:P9">
+    <cfRule type="expression" dxfId="7" priority="7">
+      <formula>$K9="No"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M19">
-    <cfRule type="expression" dxfId="20" priority="4">
-      <formula>$J19="No"</formula>
+  <conditionalFormatting sqref="N19">
+    <cfRule type="expression" dxfId="6" priority="6">
+      <formula>$K19="No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B22">
-    <cfRule type="expression" dxfId="19" priority="3">
-      <formula>$J2="No"</formula>
+    <cfRule type="expression" dxfId="5" priority="5">
+      <formula>$K2="No"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I10">
-    <cfRule type="expression" dxfId="18" priority="2">
-      <formula>$J10="No"</formula>
+  <conditionalFormatting sqref="J10">
+    <cfRule type="expression" dxfId="4" priority="4">
+      <formula>$K10="No"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I12">
-    <cfRule type="expression" dxfId="17" priority="1">
-      <formula>$J12="No"</formula>
+  <conditionalFormatting sqref="J12">
+    <cfRule type="expression" dxfId="3" priority="3">
+      <formula>$K12="No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E6:F7">
+    <cfRule type="expression" dxfId="2" priority="1">
+      <formula>LEN($D6)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E6:F7">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>$K6="No"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Confirm and fix data validation settings
Issues identified during initial QA

close #7
close #6
close #12
close #10
close #8
</commit_message>
<xml_diff>
--- a/specs/Coliform-column-definitions.xlsx
+++ b/specs/Coliform-column-definitions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\xl-ese\specs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C812607-A283-49C7-9BD4-BADFD7B6E0E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4CAE4DA-2CC6-4F33-A558-76C6A9CB9355}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Coliform Sample" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="248">
   <si>
     <t>Optionality</t>
   </si>
@@ -335,9 +335,6 @@
   </si>
   <si>
     <t>=RepeatLocationsList</t>
-  </si>
-  <si>
-    <t>=COUNTIF(R6C1:R6C1,RC)&lt;=1</t>
   </si>
   <si>
     <t>&lt;= 40</t>
@@ -656,9 +653,6 @@
     <t>"result"</t>
   </si>
   <si>
-    <t>Date between</t>
-  </si>
-  <si>
     <t>RC8 &lt;= x &lt;= TODAY()</t>
   </si>
   <si>
@@ -837,6 +831,9 @@
   </si>
   <si>
     <t>XML order #</t>
+  </si>
+  <si>
+    <t>1 &lt;= x &lt;= 20</t>
   </si>
 </sst>
 </file>
@@ -923,7 +920,203 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="56">
+  <dxfs count="57">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <alignment vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="none">
@@ -935,230 +1128,6 @@
     </dxf>
     <dxf>
       <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
           <bgColor indexed="65"/>
@@ -1183,6 +1152,41 @@
     </dxf>
     <dxf>
       <alignment vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1203,7 +1207,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{636125F0-68A9-4682-81D8-01BD3AB67D26}" name="Table1" displayName="Table1" ref="A1:P33" totalsRowShown="0" headerRowDxfId="55" dataDxfId="54">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{636125F0-68A9-4682-81D8-01BD3AB67D26}" name="Table1" displayName="Table1" ref="A1:P33" totalsRowShown="0" headerRowDxfId="51" dataDxfId="50">
   <autoFilter ref="A1:P33" xr:uid="{C224FB70-9F34-49CE-AC5D-FD58B7A283A8}">
     <filterColumn colId="7">
       <filters>
@@ -1214,49 +1218,49 @@
     </filterColumn>
   </autoFilter>
   <tableColumns count="16">
-    <tableColumn id="6" xr3:uid="{57EF6AB6-6C4C-4170-BD9B-BF376C46C5DF}" name="Title" dataDxfId="53"/>
-    <tableColumn id="12" xr3:uid="{BFDB40C3-C9ED-4560-81A1-344ECAE248C8}" name="Excel col #" dataDxfId="52"/>
-    <tableColumn id="1" xr3:uid="{3193A6D3-813B-4494-AEED-01D6509FCA0D}" name="CSV Column Name" dataDxfId="51"/>
-    <tableColumn id="11" xr3:uid="{057EA208-1889-4E3C-A179-F312337D9867}" name="CSV col #" dataDxfId="50"/>
-    <tableColumn id="16" xr3:uid="{1F4E7FF6-264D-41DA-AC14-BAA45F3439C7}" name="XML Element" dataDxfId="49"/>
-    <tableColumn id="10" xr3:uid="{F503FCB6-1F5D-4765-B4AB-F67230BC37A3}" name="XML order #" dataDxfId="0"/>
-    <tableColumn id="2" xr3:uid="{5C52F15D-4AC8-44CE-A401-3402D3CD4152}" name="Data Type" dataDxfId="48"/>
-    <tableColumn id="3" xr3:uid="{FFD71D9C-951A-4BB1-9000-9A1C4C3F71D3}" name="Optionality" dataDxfId="47"/>
-    <tableColumn id="4" xr3:uid="{6FEED7B4-CF3F-4593-BB9F-5CFA5FA5B692}" name="Size" dataDxfId="46"/>
-    <tableColumn id="5" xr3:uid="{563427BF-63BA-491F-9B6F-4E02453C643B}" name="Business Rules" dataDxfId="45"/>
-    <tableColumn id="9" xr3:uid="{A9E34622-C2B4-476B-A018-EABC1256DC10}" name="User Editable" dataDxfId="44"/>
-    <tableColumn id="14" xr3:uid="{9DA3EF2F-E261-414A-B10C-F88F2052640F}" name="Generated" dataDxfId="43"/>
-    <tableColumn id="15" xr3:uid="{AA61284F-4409-4E18-9405-8F2EAA78028A}" name="Format" dataDxfId="42"/>
-    <tableColumn id="13" xr3:uid="{94BA7C53-9CFA-4072-B1A4-7E9CE9D9DDF7}" name="Conditional Formatting" dataDxfId="41"/>
-    <tableColumn id="7" xr3:uid="{22AE72C5-BA89-443A-81AF-BCF4B114454C}" name="Validation" dataDxfId="40"/>
-    <tableColumn id="8" xr3:uid="{5DE66E18-4141-4BDD-B41D-2782AC810F6E}" name="Validation Formula" dataDxfId="39"/>
+    <tableColumn id="6" xr3:uid="{57EF6AB6-6C4C-4170-BD9B-BF376C46C5DF}" name="Title" dataDxfId="49"/>
+    <tableColumn id="12" xr3:uid="{BFDB40C3-C9ED-4560-81A1-344ECAE248C8}" name="Excel col #" dataDxfId="48"/>
+    <tableColumn id="1" xr3:uid="{3193A6D3-813B-4494-AEED-01D6509FCA0D}" name="CSV Column Name" dataDxfId="47"/>
+    <tableColumn id="11" xr3:uid="{057EA208-1889-4E3C-A179-F312337D9867}" name="CSV col #" dataDxfId="46"/>
+    <tableColumn id="16" xr3:uid="{1F4E7FF6-264D-41DA-AC14-BAA45F3439C7}" name="XML Element" dataDxfId="45"/>
+    <tableColumn id="10" xr3:uid="{F503FCB6-1F5D-4765-B4AB-F67230BC37A3}" name="XML order #" dataDxfId="44"/>
+    <tableColumn id="2" xr3:uid="{5C52F15D-4AC8-44CE-A401-3402D3CD4152}" name="Data Type" dataDxfId="43"/>
+    <tableColumn id="3" xr3:uid="{FFD71D9C-951A-4BB1-9000-9A1C4C3F71D3}" name="Optionality" dataDxfId="42"/>
+    <tableColumn id="4" xr3:uid="{6FEED7B4-CF3F-4593-BB9F-5CFA5FA5B692}" name="Size" dataDxfId="41"/>
+    <tableColumn id="5" xr3:uid="{563427BF-63BA-491F-9B6F-4E02453C643B}" name="Business Rules" dataDxfId="40"/>
+    <tableColumn id="9" xr3:uid="{A9E34622-C2B4-476B-A018-EABC1256DC10}" name="User Editable" dataDxfId="39"/>
+    <tableColumn id="14" xr3:uid="{9DA3EF2F-E261-414A-B10C-F88F2052640F}" name="Generated" dataDxfId="38"/>
+    <tableColumn id="15" xr3:uid="{AA61284F-4409-4E18-9405-8F2EAA78028A}" name="Format" dataDxfId="37"/>
+    <tableColumn id="13" xr3:uid="{94BA7C53-9CFA-4072-B1A4-7E9CE9D9DDF7}" name="Conditional Formatting" dataDxfId="36"/>
+    <tableColumn id="7" xr3:uid="{22AE72C5-BA89-443A-81AF-BCF4B114454C}" name="Validation" dataDxfId="35"/>
+    <tableColumn id="8" xr3:uid="{5DE66E18-4141-4BDD-B41D-2782AC810F6E}" name="Validation Formula" dataDxfId="34"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{05345577-AC31-4B6D-B899-55D66DEB1874}" name="Table2" displayName="Table2" ref="A1:P22" totalsRowShown="0" headerRowDxfId="38" dataDxfId="37">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{05345577-AC31-4B6D-B899-55D66DEB1874}" name="Table2" displayName="Table2" ref="A1:P22" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C2:P22">
     <sortCondition ref="D16:D22"/>
   </sortState>
   <tableColumns count="16">
-    <tableColumn id="7" xr3:uid="{9E32B24E-F549-442D-B6C5-5B5E67078170}" name="Title" dataDxfId="36"/>
-    <tableColumn id="12" xr3:uid="{023EA1AA-B7DF-4814-BFEF-5AB9B0752B95}" name="Excel col #" dataDxfId="35"/>
-    <tableColumn id="1" xr3:uid="{5687DF61-58A8-463A-A7F7-9B8B474466F3}" name="CSV Column Name" dataDxfId="34"/>
-    <tableColumn id="13" xr3:uid="{9E799E78-81C7-4788-BF70-799894A0FACA}" name="CSV col #" dataDxfId="33"/>
-    <tableColumn id="16" xr3:uid="{6872DDE9-C4EA-4656-AE08-1B51AE6AE7D6}" name="XML Element" dataDxfId="32"/>
-    <tableColumn id="11" xr3:uid="{F0D84552-7E57-4362-9DCD-EDC8E4E51415}" name="XML order #" dataDxfId="21"/>
-    <tableColumn id="2" xr3:uid="{E36A262F-69A4-4276-95F1-0FB7FCE8E2AD}" name="Data Type" dataDxfId="31"/>
-    <tableColumn id="3" xr3:uid="{B4F9F589-759B-40AB-BD12-81562C067103}" name="Optionality" dataDxfId="30"/>
-    <tableColumn id="4" xr3:uid="{29CBFF2E-DC73-4812-9BE8-505CDCED923B}" name="Size" dataDxfId="29"/>
-    <tableColumn id="5" xr3:uid="{2FBE4EBA-0896-4EA8-8E6A-9740D712F4CF}" name="Business Rules" dataDxfId="28"/>
-    <tableColumn id="14" xr3:uid="{F6A291D7-463E-4C10-AE63-F46C62F701F1}" name="User Editable" dataDxfId="27"/>
-    <tableColumn id="6" xr3:uid="{4A3A44E5-9909-437B-9914-BD7AF1AC2439}" name="Generated" dataDxfId="26"/>
-    <tableColumn id="15" xr3:uid="{30410F79-D89B-4BAE-852C-7ADB5287310A}" name="Format" dataDxfId="25"/>
-    <tableColumn id="8" xr3:uid="{23D225B6-A3A4-4446-9AD4-7762B64F46FE}" name="Conditional Formatting" dataDxfId="24"/>
-    <tableColumn id="9" xr3:uid="{27D08B50-8012-49E0-9C10-AEB67B99B91B}" name="Validation" dataDxfId="23"/>
-    <tableColumn id="10" xr3:uid="{A301C8EB-BB2A-4524-AF6E-20714C0D7DD5}" name="Validation Formula" dataDxfId="22"/>
+    <tableColumn id="7" xr3:uid="{9E32B24E-F549-442D-B6C5-5B5E67078170}" name="Title" dataDxfId="16"/>
+    <tableColumn id="12" xr3:uid="{023EA1AA-B7DF-4814-BFEF-5AB9B0752B95}" name="Excel col #" dataDxfId="15"/>
+    <tableColumn id="1" xr3:uid="{5687DF61-58A8-463A-A7F7-9B8B474466F3}" name="CSV Column Name" dataDxfId="14"/>
+    <tableColumn id="13" xr3:uid="{9E799E78-81C7-4788-BF70-799894A0FACA}" name="CSV col #" dataDxfId="13"/>
+    <tableColumn id="16" xr3:uid="{6872DDE9-C4EA-4656-AE08-1B51AE6AE7D6}" name="XML Element" dataDxfId="12"/>
+    <tableColumn id="11" xr3:uid="{F0D84552-7E57-4362-9DCD-EDC8E4E51415}" name="XML order #" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{E36A262F-69A4-4276-95F1-0FB7FCE8E2AD}" name="Data Type" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{B4F9F589-759B-40AB-BD12-81562C067103}" name="Optionality" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{29CBFF2E-DC73-4812-9BE8-505CDCED923B}" name="Size" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{2FBE4EBA-0896-4EA8-8E6A-9740D712F4CF}" name="Business Rules" dataDxfId="7"/>
+    <tableColumn id="14" xr3:uid="{F6A291D7-463E-4C10-AE63-F46C62F701F1}" name="User Editable" dataDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{4A3A44E5-9909-437B-9914-BD7AF1AC2439}" name="Generated" dataDxfId="5"/>
+    <tableColumn id="15" xr3:uid="{30410F79-D89B-4BAE-852C-7ADB5287310A}" name="Format" dataDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{23D225B6-A3A4-4446-9AD4-7762B64F46FE}" name="Conditional Formatting" dataDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{27D08B50-8012-49E0-9C10-AEB67B99B91B}" name="Validation" dataDxfId="2"/>
+    <tableColumn id="10" xr3:uid="{A301C8EB-BB2A-4524-AF6E-20714C0D7DD5}" name="Validation Formula" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight14" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1529,9 +1533,10 @@
   <dimension ref="A1:P33"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="E1" sqref="E1"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1563,22 +1568,22 @@
         <v>53</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H1" s="6" t="s">
         <v>0</v>
@@ -1590,7 +1595,7 @@
         <v>2</v>
       </c>
       <c r="K1" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="L1" s="6" t="s">
         <v>79</v>
@@ -1610,7 +1615,7 @@
     </row>
     <row r="2" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B2" s="7"/>
       <c r="C2" s="7" t="s">
@@ -1622,10 +1627,10 @@
       <c r="E2" s="7"/>
       <c r="F2" s="7"/>
       <c r="G2" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I2" s="8">
         <v>20</v>
@@ -1658,16 +1663,16 @@
         <v>2</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F3" s="2">
         <v>4</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I3" s="3">
         <v>20</v>
@@ -1678,16 +1683,16 @@
       </c>
       <c r="L3" s="2"/>
       <c r="M3" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="P3" s="5" t="s">
-        <v>100</v>
+        <v>247</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
@@ -1704,16 +1709,16 @@
         <v>3</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="F4" s="7">
         <v>3</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I4" s="3">
         <v>20</v>
@@ -1724,7 +1729,7 @@
       </c>
       <c r="L4" s="2"/>
       <c r="M4" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="N4" s="2"/>
       <c r="O4" s="2" t="s">
@@ -1748,16 +1753,16 @@
         <v>4</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="F5" s="2">
         <v>5</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I5" s="3">
         <v>9</v>
@@ -1770,16 +1775,16 @@
       </c>
       <c r="L5" s="2"/>
       <c r="M5" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="N5" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="O5" s="2" t="s">
         <v>84</v>
       </c>
       <c r="P5" s="5" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
@@ -1796,16 +1801,16 @@
         <v>5</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="F6" s="7">
         <v>10</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I6" s="3">
         <v>1</v>
@@ -1818,14 +1823,14 @@
         <v>94</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="N6" s="2"/>
       <c r="O6" s="2" t="s">
         <v>80</v>
       </c>
       <c r="P6" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="30" x14ac:dyDescent="0.25">
@@ -1840,16 +1845,16 @@
         <v>6</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="F7" s="6">
         <v>1</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I7" s="3">
         <v>10</v>
@@ -1859,7 +1864,7 @@
         <v>81</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
@@ -1878,16 +1883,16 @@
         <v>7</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="F8" s="13">
         <v>2</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I8" s="3">
         <v>10</v>
@@ -1918,16 +1923,16 @@
         <v>8</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="F9" s="2">
         <v>6</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I9" s="3">
         <v>10</v>
@@ -1940,16 +1945,16 @@
       </c>
       <c r="L9" s="2"/>
       <c r="M9" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="N9" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="O9" s="2" t="s">
         <v>84</v>
       </c>
       <c r="P9" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="30" x14ac:dyDescent="0.25">
@@ -1966,16 +1971,16 @@
         <v>9</v>
       </c>
       <c r="E10" s="13" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="F10" s="13">
         <v>21</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I10" s="3">
         <v>12</v>
@@ -1988,21 +1993,21 @@
       </c>
       <c r="L10" s="2"/>
       <c r="M10" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="N10" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="O10" s="2" t="s">
         <v>84</v>
       </c>
       <c r="P10" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="11" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2" t="s">
@@ -2012,14 +2017,14 @@
         <v>10</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I11" s="3">
         <v>40</v>
@@ -2048,16 +2053,16 @@
         <v>11</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="F12" s="7">
         <v>7</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I12" s="3">
         <v>2</v>
@@ -2090,16 +2095,16 @@
         <v>12</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="F13" s="2">
         <v>9</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I13" s="3">
         <v>1</v>
@@ -2112,16 +2117,16 @@
       </c>
       <c r="L13" s="2"/>
       <c r="M13" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="N13" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="O13" s="2" t="s">
         <v>80</v>
       </c>
       <c r="P13" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
@@ -2138,7 +2143,7 @@
         <v>13</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="F14" s="7">
         <v>16</v>
@@ -2147,7 +2152,7 @@
         <v>92</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I14" s="3">
         <v>8</v>
@@ -2163,13 +2168,13 @@
         <v>97</v>
       </c>
       <c r="N14" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="O14" s="2" t="s">
         <v>78</v>
       </c>
       <c r="P14" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
@@ -2186,7 +2191,7 @@
         <v>14</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="F15" s="2">
         <v>17</v>
@@ -2195,13 +2200,13 @@
         <v>93</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I15" s="3">
         <v>4</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="K15" s="2" t="s">
         <v>82</v>
@@ -2215,7 +2220,7 @@
         <v>93</v>
       </c>
       <c r="P15" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
@@ -2232,16 +2237,16 @@
         <v>15</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="F16" s="7">
         <v>8</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I16" s="3">
         <v>2</v>
@@ -2252,10 +2257,10 @@
       </c>
       <c r="L16" s="2"/>
       <c r="M16" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="N16" s="5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="O16" s="2" t="s">
         <v>80</v>
@@ -2278,16 +2283,16 @@
         <v>16</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="F17" s="6">
         <v>22</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I17" s="3">
         <v>2</v>
@@ -2298,10 +2303,10 @@
       </c>
       <c r="L17" s="2"/>
       <c r="M17" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="N17" s="4" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="O17" s="2" t="s">
         <v>80</v>
@@ -2324,7 +2329,7 @@
         <v>17</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="F18" s="7">
         <v>18</v>
@@ -2333,7 +2338,7 @@
         <v>92</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I18" s="3">
         <v>8</v>
@@ -2350,15 +2355,15 @@
       </c>
       <c r="N18" s="2"/>
       <c r="O18" s="2" t="s">
-        <v>194</v>
+        <v>92</v>
       </c>
       <c r="P18" s="5" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="19" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B19" s="2">
         <v>13</v>
@@ -2370,16 +2375,16 @@
         <v>18</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F19" s="6">
         <v>15</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I19" s="3">
         <v>40</v>
@@ -2392,14 +2397,14 @@
       </c>
       <c r="L19" s="2"/>
       <c r="M19" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="N19" s="2"/>
       <c r="O19" s="2" t="s">
         <v>84</v>
       </c>
       <c r="P19" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="20" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
@@ -2414,14 +2419,14 @@
         <v>19</v>
       </c>
       <c r="E20" s="13" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="F20" s="13"/>
       <c r="G20" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I20" s="3">
         <v>9</v>
@@ -2450,14 +2455,14 @@
         <v>20</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="F21" s="7"/>
       <c r="G21" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I21" s="3">
         <v>2</v>
@@ -2486,14 +2491,14 @@
         <v>21</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="F22" s="6"/>
       <c r="G22" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I22" s="3">
         <v>12</v>
@@ -2512,7 +2517,7 @@
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B23" s="2">
         <v>14</v>
@@ -2524,16 +2529,16 @@
         <v>22</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="F23" s="7">
         <v>19</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I23" s="3" t="s">
         <v>34</v>
@@ -2546,19 +2551,19 @@
       </c>
       <c r="L23" s="2"/>
       <c r="M23" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="N23" s="2"/>
       <c r="O23" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="P23" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B24" s="2">
         <v>15</v>
@@ -2570,16 +2575,16 @@
         <v>23</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="F24" s="7">
         <v>20</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I24" s="3" t="s">
         <v>34</v>
@@ -2592,14 +2597,14 @@
       </c>
       <c r="L24" s="2"/>
       <c r="M24" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="N24" s="2"/>
       <c r="O24" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="P24" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="25" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
@@ -2614,14 +2619,14 @@
         <v>24</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="F25" s="7"/>
       <c r="G25" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I25" s="3" t="s">
         <v>39</v>
@@ -2650,14 +2655,14 @@
         <v>25</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="F26" s="7"/>
       <c r="G26" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I26" s="3"/>
       <c r="J26" s="2"/>
@@ -2684,14 +2689,14 @@
         <v>26</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="F27" s="7"/>
       <c r="G27" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I27" s="3" t="s">
         <v>42</v>
@@ -2720,14 +2725,14 @@
         <v>27</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="F28" s="7"/>
       <c r="G28" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I28" s="3" t="s">
         <v>44</v>
@@ -2756,14 +2761,14 @@
         <v>28</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="F29" s="7"/>
       <c r="G29" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I29" s="3" t="s">
         <v>46</v>
@@ -2782,7 +2787,7 @@
     </row>
     <row r="30" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B30" s="2">
         <v>16</v>
@@ -2794,16 +2799,16 @@
         <v>29</v>
       </c>
       <c r="E30" s="13" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="F30" s="13">
         <v>11</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I30" s="3">
         <v>20</v>
@@ -2816,21 +2821,21 @@
       </c>
       <c r="L30" s="2"/>
       <c r="M30" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="N30" s="4" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="O30" s="2" t="s">
         <v>78</v>
       </c>
       <c r="P30" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="31" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B31" s="2">
         <v>17</v>
@@ -2842,7 +2847,7 @@
         <v>30</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="F31" s="6">
         <v>12</v>
@@ -2851,7 +2856,7 @@
         <v>92</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I31" s="3">
         <v>8</v>
@@ -2867,13 +2872,13 @@
         <v>97</v>
       </c>
       <c r="N31" s="4" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="O31" s="2" t="s">
         <v>78</v>
       </c>
       <c r="P31" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="32" spans="1:16" ht="45" x14ac:dyDescent="0.25">
@@ -2888,16 +2893,16 @@
         <v>31</v>
       </c>
       <c r="E32" s="13" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="F32" s="13">
         <v>13</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I32" s="3">
         <v>10</v>
@@ -2909,7 +2914,7 @@
         <v>81</v>
       </c>
       <c r="L32" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="M32" s="2"/>
       <c r="N32" s="2"/>
@@ -2928,16 +2933,16 @@
         <v>32</v>
       </c>
       <c r="E33" s="13" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="F33" s="13">
         <v>14</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I33" s="3">
         <v>10</v>
@@ -2949,7 +2954,7 @@
         <v>81</v>
       </c>
       <c r="L33" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="M33" s="2"/>
       <c r="N33" s="2"/>
@@ -2959,27 +2964,27 @@
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
   <conditionalFormatting sqref="D2:F33">
-    <cfRule type="expression" dxfId="20" priority="11">
+    <cfRule type="expression" dxfId="56" priority="11">
       <formula>LEN($D2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:A31 C15:O15 C2:P14 C16:P31 A32:P33">
-    <cfRule type="expression" dxfId="19" priority="12">
+    <cfRule type="expression" dxfId="55" priority="12">
       <formula>$K2="No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2:L33">
-    <cfRule type="expression" dxfId="18" priority="10">
+    <cfRule type="expression" dxfId="54" priority="10">
       <formula>AND($K2="No",LEN($L2)=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P15">
-    <cfRule type="expression" dxfId="17" priority="2">
+    <cfRule type="expression" dxfId="53" priority="2">
       <formula>$K15="No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B31">
-    <cfRule type="expression" dxfId="16" priority="1">
+    <cfRule type="expression" dxfId="52" priority="1">
       <formula>$K2="No"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2997,9 +3002,10 @@
   <dimension ref="A1:P22"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="E1" sqref="E1"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3027,22 +3033,22 @@
         <v>53</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H1" s="6" t="s">
         <v>0</v>
@@ -3054,7 +3060,7 @@
         <v>2</v>
       </c>
       <c r="K1" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="L1" s="6" t="s">
         <v>79</v>
@@ -3074,7 +3080,7 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2" t="s">
@@ -3086,22 +3092,22 @@
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I2" s="2">
         <v>20</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>81</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
@@ -3122,38 +3128,38 @@
         <v>2</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F3" s="2">
         <v>1</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I3" s="2">
         <v>20</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>82</v>
       </c>
       <c r="L3" s="2"/>
       <c r="M3" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="P3" s="5" t="s">
-        <v>100</v>
+        <v>247</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
@@ -3170,7 +3176,7 @@
         <v>3</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="F4" s="2">
         <v>3</v>
@@ -3179,13 +3185,13 @@
         <v>92</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I4" s="2">
         <v>8</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>82</v>
@@ -3195,13 +3201,13 @@
         <v>97</v>
       </c>
       <c r="N4" s="5" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="O4" s="2" t="s">
         <v>78</v>
       </c>
       <c r="P4" s="5" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
@@ -3218,38 +3224,38 @@
         <v>4</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="F5" s="2">
         <v>2</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I5" s="2">
         <v>9</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="K5" s="2" t="s">
         <v>82</v>
       </c>
       <c r="L5" s="2"/>
       <c r="M5" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="N5" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="O5" s="2" t="s">
         <v>84</v>
       </c>
       <c r="P5" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="45" x14ac:dyDescent="0.25">
@@ -3264,16 +3270,16 @@
         <v>5</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="F6" s="6">
         <v>4</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I6" s="2">
         <v>10</v>
@@ -3283,7 +3289,7 @@
         <v>81</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
@@ -3302,16 +3308,16 @@
         <v>6</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="F7" s="13">
         <v>5</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I7" s="2">
         <v>10</v>
@@ -3330,67 +3336,67 @@
     </row>
     <row r="8" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B8" s="2">
         <v>4</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D8" s="2">
         <v>7</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="F8" s="6">
         <v>12</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I8" s="2">
         <v>4</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="K8" s="2" t="s">
         <v>82</v>
       </c>
       <c r="L8" s="2"/>
       <c r="M8" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="N8" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="O8" s="2" t="s">
         <v>80</v>
       </c>
       <c r="P8" s="5" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B9" s="2">
         <v>5</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D9" s="2">
         <v>8</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="F9" s="2">
         <v>8</v>
@@ -3399,13 +3405,13 @@
         <v>92</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I9" s="2">
         <v>8</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="K9" s="2" t="s">
         <v>82</v>
@@ -3419,24 +3425,24 @@
         <v>92</v>
       </c>
       <c r="P9" s="5" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B10" s="2">
         <v>6</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D10" s="2">
         <v>9</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="F10" s="2">
         <v>9</v>
@@ -3445,13 +3451,13 @@
         <v>93</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I10" s="2">
         <v>4</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="K10" s="2" t="s">
         <v>82</v>
@@ -3465,24 +3471,24 @@
         <v>93</v>
       </c>
       <c r="P10" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B11" s="2">
         <v>7</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D11" s="2">
         <v>10</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="F11" s="2">
         <v>10</v>
@@ -3491,13 +3497,13 @@
         <v>92</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I11" s="2">
         <v>8</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="K11" s="2" t="s">
         <v>82</v>
@@ -3511,24 +3517,24 @@
         <v>92</v>
       </c>
       <c r="P11" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B12" s="2">
         <v>8</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D12" s="2">
         <v>11</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="F12" s="2">
         <v>11</v>
@@ -3537,13 +3543,13 @@
         <v>93</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I12" s="2">
         <v>4</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="K12" s="2" t="s">
         <v>82</v>
@@ -3557,24 +3563,24 @@
         <v>93</v>
       </c>
       <c r="P12" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B13" s="2">
         <v>9</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D13" s="2">
         <v>12</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="F13" s="2">
         <v>17</v>
@@ -3583,7 +3589,7 @@
         <v>92</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I13" s="2">
         <v>8</v>
@@ -3597,43 +3603,47 @@
         <v>97</v>
       </c>
       <c r="N13" s="5"/>
-      <c r="O13" s="2"/>
-      <c r="P13" s="5"/>
+      <c r="O13" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="P13" s="5" t="s">
+        <v>178</v>
+      </c>
     </row>
     <row r="14" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D14" s="2">
         <v>13</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="F14" s="6">
         <v>18</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I14" s="2">
         <v>1</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="K14" s="2" t="s">
         <v>81</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="M14" s="2"/>
       <c r="N14" s="2"/>
@@ -3642,11 +3652,11 @@
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D15" s="2">
         <v>14</v>
@@ -3654,10 +3664,10 @@
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
       <c r="G15" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I15" s="2">
         <v>2</v>
@@ -3676,41 +3686,41 @@
     </row>
     <row r="16" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B16" s="2">
         <v>10</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D16" s="2">
         <v>15</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="F16" s="6">
         <v>6</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I16" s="2">
         <v>30</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="K16" s="2" t="s">
         <v>82</v>
       </c>
       <c r="L16" s="2"/>
       <c r="M16" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="N16" s="2"/>
       <c r="O16" s="2"/>
@@ -3718,59 +3728,59 @@
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B17" s="2">
         <v>11</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D17" s="2">
         <v>16</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="F17" s="2">
         <v>7</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I17" s="2">
         <v>9</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K17" s="2" t="s">
         <v>82</v>
       </c>
       <c r="L17" s="2"/>
       <c r="M17" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="N17" s="2"/>
       <c r="O17" s="2" t="s">
         <v>80</v>
       </c>
       <c r="P17" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B18" s="2">
         <v>12</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D18" s="2">
         <v>17</v>
@@ -3778,206 +3788,206 @@
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I18" s="2">
         <v>4</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K18" s="2" t="s">
         <v>82</v>
       </c>
       <c r="L18" s="2"/>
       <c r="M18" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="N18" s="2"/>
       <c r="O18" s="2" t="s">
         <v>80</v>
       </c>
       <c r="P18" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="19" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B19" s="2">
         <v>13</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D19" s="2">
         <v>18</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="F19" s="6">
         <v>13</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I19" s="2">
         <v>1</v>
       </c>
       <c r="J19" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="K19" s="2" t="s">
         <v>82</v>
       </c>
       <c r="L19" s="2"/>
       <c r="M19" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="N19" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="O19" s="2" t="s">
         <v>80</v>
       </c>
       <c r="P19" s="5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="20" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B20" s="2">
         <v>14</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D20" s="2">
         <v>20</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="F20" s="6">
         <v>15</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I20" s="2">
         <v>10</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="K20" s="2" t="s">
         <v>82</v>
       </c>
       <c r="L20" s="2"/>
       <c r="M20" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="N20" s="5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="O20" s="2" t="s">
         <v>80</v>
       </c>
       <c r="P20" s="5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="21" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B21" s="2">
         <v>15</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D21" s="2">
         <v>27</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="F21" s="6">
         <v>16</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I21" s="2">
         <v>9</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="K21" s="2" t="s">
         <v>82</v>
       </c>
       <c r="L21" s="2"/>
       <c r="M21" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="N21" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="O21" s="2" t="s">
         <v>80</v>
       </c>
       <c r="P21" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="22" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B22" s="2">
         <v>16</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D22" s="2">
         <v>28</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="F22" s="6">
         <v>14</v>
       </c>
       <c r="G22" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="J22" s="2" t="s">
         <v>138</v>
-      </c>
-      <c r="H22" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="I22" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="J22" s="2" t="s">
-        <v>139</v>
       </c>
       <c r="K22" s="2" t="s">
         <v>82</v>
@@ -3986,86 +3996,86 @@
       <c r="M22" s="2"/>
       <c r="N22" s="2"/>
       <c r="O22" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="P22" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="L2:L22">
-    <cfRule type="expression" dxfId="15" priority="13">
+    <cfRule type="expression" dxfId="33" priority="14">
       <formula>AND($K2="No",LEN($L2)=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:F5 D6:D7 D8:F22">
-    <cfRule type="expression" dxfId="14" priority="14">
+    <cfRule type="expression" dxfId="32" priority="15">
       <formula>LEN($D2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O3 O4:P4 O8:P8 O19:P19 A2:A22 C20:P22 C11:P11 C9:N9 C8:M8 C3:M5 C6:D7 C2:P2 C10:I10 K10:P10 C13:P18 C12:I12 K12:P12 G6:P7 C19:M19">
-    <cfRule type="expression" dxfId="13" priority="15">
+  <conditionalFormatting sqref="O4:P4 O8:P8 O19:P19 A2:A22 C20:P22 C11:P11 C9:N9 C8:M8 C3:M5 C6:D7 C2:P2 C10:I10 K10:P10 C13:P18 C12:I12 K12:P12 G6:P7 C19:M19">
+    <cfRule type="expression" dxfId="31" priority="16">
       <formula>$K2="No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N3">
-    <cfRule type="expression" dxfId="12" priority="12">
-      <formula>$K3="No"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P3">
-    <cfRule type="expression" dxfId="11" priority="11">
+    <cfRule type="expression" dxfId="30" priority="13">
       <formula>$K3="No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N4:N5">
-    <cfRule type="expression" dxfId="10" priority="10">
+    <cfRule type="expression" dxfId="28" priority="11">
       <formula>$K4="No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O5:P5">
-    <cfRule type="expression" dxfId="9" priority="9">
+    <cfRule type="expression" dxfId="27" priority="10">
       <formula>$K5="No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N8">
-    <cfRule type="expression" dxfId="8" priority="8">
+    <cfRule type="expression" dxfId="26" priority="9">
       <formula>$K8="No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O9:P9">
-    <cfRule type="expression" dxfId="7" priority="7">
+    <cfRule type="expression" dxfId="25" priority="8">
       <formula>$K9="No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N19">
-    <cfRule type="expression" dxfId="6" priority="6">
+    <cfRule type="expression" dxfId="24" priority="7">
       <formula>$K19="No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B22">
-    <cfRule type="expression" dxfId="5" priority="5">
+    <cfRule type="expression" dxfId="23" priority="6">
       <formula>$K2="No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J10">
-    <cfRule type="expression" dxfId="4" priority="4">
+    <cfRule type="expression" dxfId="22" priority="5">
       <formula>$K10="No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J12">
-    <cfRule type="expression" dxfId="3" priority="3">
+    <cfRule type="expression" dxfId="21" priority="4">
       <formula>$K12="No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6:F7">
-    <cfRule type="expression" dxfId="2" priority="1">
+    <cfRule type="expression" dxfId="20" priority="2">
       <formula>LEN($D6)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6:F7">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="19" priority="3">
       <formula>$K6="No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O3:P3">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>$K3="No"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Clarify requirements for "Repeat" Sample Type
close #9
</commit_message>
<xml_diff>
--- a/specs/Coliform-column-definitions.xlsx
+++ b/specs/Coliform-column-definitions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\xl-ese\specs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4CAE4DA-2CC6-4F33-A558-76C6A9CB9355}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED10B97E-D3B4-4478-A7F0-4A62E610E0F4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Coliform Sample" sheetId="1" r:id="rId1"/>
@@ -920,7 +920,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="57">
+  <dxfs count="55">
     <dxf>
       <fill>
         <patternFill>
@@ -929,60 +929,6 @@
       </fill>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill>
           <bgColor theme="0" tint="-0.14996795556505021"/>
@@ -1069,6 +1015,34 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor theme="0" tint="-0.14996795556505021"/>
         </patternFill>
       </fill>
@@ -1081,11 +1055,58 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1152,41 +1173,6 @@
     </dxf>
     <dxf>
       <alignment vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1207,60 +1193,52 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{636125F0-68A9-4682-81D8-01BD3AB67D26}" name="Table1" displayName="Table1" ref="A1:P33" totalsRowShown="0" headerRowDxfId="51" dataDxfId="50">
-  <autoFilter ref="A1:P33" xr:uid="{C224FB70-9F34-49CE-AC5D-FD58B7A283A8}">
-    <filterColumn colId="7">
-      <filters>
-        <filter val="Conditional"/>
-        <filter val="Mandatory"/>
-        <filter val="Optional"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{636125F0-68A9-4682-81D8-01BD3AB67D26}" name="Table1" displayName="Table1" ref="A1:P33" totalsRowShown="0" headerRowDxfId="54" dataDxfId="53">
+  <autoFilter ref="A1:P33" xr:uid="{C224FB70-9F34-49CE-AC5D-FD58B7A283A8}"/>
   <tableColumns count="16">
-    <tableColumn id="6" xr3:uid="{57EF6AB6-6C4C-4170-BD9B-BF376C46C5DF}" name="Title" dataDxfId="49"/>
-    <tableColumn id="12" xr3:uid="{BFDB40C3-C9ED-4560-81A1-344ECAE248C8}" name="Excel col #" dataDxfId="48"/>
-    <tableColumn id="1" xr3:uid="{3193A6D3-813B-4494-AEED-01D6509FCA0D}" name="CSV Column Name" dataDxfId="47"/>
-    <tableColumn id="11" xr3:uid="{057EA208-1889-4E3C-A179-F312337D9867}" name="CSV col #" dataDxfId="46"/>
-    <tableColumn id="16" xr3:uid="{1F4E7FF6-264D-41DA-AC14-BAA45F3439C7}" name="XML Element" dataDxfId="45"/>
-    <tableColumn id="10" xr3:uid="{F503FCB6-1F5D-4765-B4AB-F67230BC37A3}" name="XML order #" dataDxfId="44"/>
-    <tableColumn id="2" xr3:uid="{5C52F15D-4AC8-44CE-A401-3402D3CD4152}" name="Data Type" dataDxfId="43"/>
-    <tableColumn id="3" xr3:uid="{FFD71D9C-951A-4BB1-9000-9A1C4C3F71D3}" name="Optionality" dataDxfId="42"/>
-    <tableColumn id="4" xr3:uid="{6FEED7B4-CF3F-4593-BB9F-5CFA5FA5B692}" name="Size" dataDxfId="41"/>
-    <tableColumn id="5" xr3:uid="{563427BF-63BA-491F-9B6F-4E02453C643B}" name="Business Rules" dataDxfId="40"/>
-    <tableColumn id="9" xr3:uid="{A9E34622-C2B4-476B-A018-EABC1256DC10}" name="User Editable" dataDxfId="39"/>
-    <tableColumn id="14" xr3:uid="{9DA3EF2F-E261-414A-B10C-F88F2052640F}" name="Generated" dataDxfId="38"/>
-    <tableColumn id="15" xr3:uid="{AA61284F-4409-4E18-9405-8F2EAA78028A}" name="Format" dataDxfId="37"/>
-    <tableColumn id="13" xr3:uid="{94BA7C53-9CFA-4072-B1A4-7E9CE9D9DDF7}" name="Conditional Formatting" dataDxfId="36"/>
-    <tableColumn id="7" xr3:uid="{22AE72C5-BA89-443A-81AF-BCF4B114454C}" name="Validation" dataDxfId="35"/>
-    <tableColumn id="8" xr3:uid="{5DE66E18-4141-4BDD-B41D-2782AC810F6E}" name="Validation Formula" dataDxfId="34"/>
+    <tableColumn id="6" xr3:uid="{57EF6AB6-6C4C-4170-BD9B-BF376C46C5DF}" name="Title" dataDxfId="52"/>
+    <tableColumn id="12" xr3:uid="{BFDB40C3-C9ED-4560-81A1-344ECAE248C8}" name="Excel col #" dataDxfId="51"/>
+    <tableColumn id="1" xr3:uid="{3193A6D3-813B-4494-AEED-01D6509FCA0D}" name="CSV Column Name" dataDxfId="50"/>
+    <tableColumn id="11" xr3:uid="{057EA208-1889-4E3C-A179-F312337D9867}" name="CSV col #" dataDxfId="49"/>
+    <tableColumn id="16" xr3:uid="{1F4E7FF6-264D-41DA-AC14-BAA45F3439C7}" name="XML Element" dataDxfId="48"/>
+    <tableColumn id="10" xr3:uid="{F503FCB6-1F5D-4765-B4AB-F67230BC37A3}" name="XML order #" dataDxfId="47"/>
+    <tableColumn id="2" xr3:uid="{5C52F15D-4AC8-44CE-A401-3402D3CD4152}" name="Data Type" dataDxfId="46"/>
+    <tableColumn id="3" xr3:uid="{FFD71D9C-951A-4BB1-9000-9A1C4C3F71D3}" name="Optionality" dataDxfId="45"/>
+    <tableColumn id="4" xr3:uid="{6FEED7B4-CF3F-4593-BB9F-5CFA5FA5B692}" name="Size" dataDxfId="44"/>
+    <tableColumn id="5" xr3:uid="{563427BF-63BA-491F-9B6F-4E02453C643B}" name="Business Rules" dataDxfId="43"/>
+    <tableColumn id="9" xr3:uid="{A9E34622-C2B4-476B-A018-EABC1256DC10}" name="User Editable" dataDxfId="42"/>
+    <tableColumn id="14" xr3:uid="{9DA3EF2F-E261-414A-B10C-F88F2052640F}" name="Generated" dataDxfId="41"/>
+    <tableColumn id="15" xr3:uid="{AA61284F-4409-4E18-9405-8F2EAA78028A}" name="Format" dataDxfId="40"/>
+    <tableColumn id="13" xr3:uid="{94BA7C53-9CFA-4072-B1A4-7E9CE9D9DDF7}" name="Conditional Formatting" dataDxfId="39"/>
+    <tableColumn id="7" xr3:uid="{22AE72C5-BA89-443A-81AF-BCF4B114454C}" name="Validation" dataDxfId="38"/>
+    <tableColumn id="8" xr3:uid="{5DE66E18-4141-4BDD-B41D-2782AC810F6E}" name="Validation Formula" dataDxfId="37"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{05345577-AC31-4B6D-B899-55D66DEB1874}" name="Table2" displayName="Table2" ref="A1:P22" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{05345577-AC31-4B6D-B899-55D66DEB1874}" name="Table2" displayName="Table2" ref="A1:P22" totalsRowShown="0" headerRowDxfId="36" dataDxfId="35">
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C2:P22">
     <sortCondition ref="D16:D22"/>
   </sortState>
   <tableColumns count="16">
-    <tableColumn id="7" xr3:uid="{9E32B24E-F549-442D-B6C5-5B5E67078170}" name="Title" dataDxfId="16"/>
-    <tableColumn id="12" xr3:uid="{023EA1AA-B7DF-4814-BFEF-5AB9B0752B95}" name="Excel col #" dataDxfId="15"/>
-    <tableColumn id="1" xr3:uid="{5687DF61-58A8-463A-A7F7-9B8B474466F3}" name="CSV Column Name" dataDxfId="14"/>
-    <tableColumn id="13" xr3:uid="{9E799E78-81C7-4788-BF70-799894A0FACA}" name="CSV col #" dataDxfId="13"/>
-    <tableColumn id="16" xr3:uid="{6872DDE9-C4EA-4656-AE08-1B51AE6AE7D6}" name="XML Element" dataDxfId="12"/>
-    <tableColumn id="11" xr3:uid="{F0D84552-7E57-4362-9DCD-EDC8E4E51415}" name="XML order #" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{E36A262F-69A4-4276-95F1-0FB7FCE8E2AD}" name="Data Type" dataDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{B4F9F589-759B-40AB-BD12-81562C067103}" name="Optionality" dataDxfId="9"/>
-    <tableColumn id="4" xr3:uid="{29CBFF2E-DC73-4812-9BE8-505CDCED923B}" name="Size" dataDxfId="8"/>
-    <tableColumn id="5" xr3:uid="{2FBE4EBA-0896-4EA8-8E6A-9740D712F4CF}" name="Business Rules" dataDxfId="7"/>
-    <tableColumn id="14" xr3:uid="{F6A291D7-463E-4C10-AE63-F46C62F701F1}" name="User Editable" dataDxfId="6"/>
-    <tableColumn id="6" xr3:uid="{4A3A44E5-9909-437B-9914-BD7AF1AC2439}" name="Generated" dataDxfId="5"/>
-    <tableColumn id="15" xr3:uid="{30410F79-D89B-4BAE-852C-7ADB5287310A}" name="Format" dataDxfId="4"/>
-    <tableColumn id="8" xr3:uid="{23D225B6-A3A4-4446-9AD4-7762B64F46FE}" name="Conditional Formatting" dataDxfId="3"/>
-    <tableColumn id="9" xr3:uid="{27D08B50-8012-49E0-9C10-AEB67B99B91B}" name="Validation" dataDxfId="2"/>
-    <tableColumn id="10" xr3:uid="{A301C8EB-BB2A-4524-AF6E-20714C0D7DD5}" name="Validation Formula" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{9E32B24E-F549-442D-B6C5-5B5E67078170}" name="Title" dataDxfId="34"/>
+    <tableColumn id="12" xr3:uid="{023EA1AA-B7DF-4814-BFEF-5AB9B0752B95}" name="Excel col #" dataDxfId="33"/>
+    <tableColumn id="1" xr3:uid="{5687DF61-58A8-463A-A7F7-9B8B474466F3}" name="CSV Column Name" dataDxfId="32"/>
+    <tableColumn id="13" xr3:uid="{9E799E78-81C7-4788-BF70-799894A0FACA}" name="CSV col #" dataDxfId="31"/>
+    <tableColumn id="16" xr3:uid="{6872DDE9-C4EA-4656-AE08-1B51AE6AE7D6}" name="XML Element" dataDxfId="30"/>
+    <tableColumn id="11" xr3:uid="{F0D84552-7E57-4362-9DCD-EDC8E4E51415}" name="XML order #" dataDxfId="29"/>
+    <tableColumn id="2" xr3:uid="{E36A262F-69A4-4276-95F1-0FB7FCE8E2AD}" name="Data Type" dataDxfId="28"/>
+    <tableColumn id="3" xr3:uid="{B4F9F589-759B-40AB-BD12-81562C067103}" name="Optionality" dataDxfId="27"/>
+    <tableColumn id="4" xr3:uid="{29CBFF2E-DC73-4812-9BE8-505CDCED923B}" name="Size" dataDxfId="26"/>
+    <tableColumn id="5" xr3:uid="{2FBE4EBA-0896-4EA8-8E6A-9740D712F4CF}" name="Business Rules" dataDxfId="25"/>
+    <tableColumn id="14" xr3:uid="{F6A291D7-463E-4C10-AE63-F46C62F701F1}" name="User Editable" dataDxfId="24"/>
+    <tableColumn id="6" xr3:uid="{4A3A44E5-9909-437B-9914-BD7AF1AC2439}" name="Generated" dataDxfId="23"/>
+    <tableColumn id="15" xr3:uid="{30410F79-D89B-4BAE-852C-7ADB5287310A}" name="Format" dataDxfId="22"/>
+    <tableColumn id="8" xr3:uid="{23D225B6-A3A4-4446-9AD4-7762B64F46FE}" name="Conditional Formatting" dataDxfId="21"/>
+    <tableColumn id="9" xr3:uid="{27D08B50-8012-49E0-9C10-AEB67B99B91B}" name="Validation" dataDxfId="20"/>
+    <tableColumn id="10" xr3:uid="{A301C8EB-BB2A-4524-AF6E-20714C0D7DD5}" name="Validation Formula" dataDxfId="19"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight14" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1541,7 +1519,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="35" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5" customWidth="1"/>
@@ -2005,7 +1983,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="11" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>105</v>
       </c>
@@ -2315,185 +2293,209 @@
         <v>99</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>66</v>
+        <v>103</v>
       </c>
       <c r="B18" s="2">
         <v>12</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="D18" s="7">
-        <v>17</v>
-      </c>
-      <c r="E18" s="7" t="s">
-        <v>210</v>
-      </c>
-      <c r="F18" s="7">
-        <v>18</v>
+        <v>29</v>
+      </c>
+      <c r="E18" s="13" t="s">
+        <v>216</v>
+      </c>
+      <c r="F18" s="13">
+        <v>11</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>92</v>
+        <v>104</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="I18" s="3">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="K18" s="2" t="s">
         <v>82</v>
       </c>
       <c r="L18" s="2"/>
       <c r="M18" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="N18" s="2"/>
+        <v>104</v>
+      </c>
+      <c r="N18" s="4" t="s">
+        <v>196</v>
+      </c>
       <c r="O18" s="2" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="P18" s="5" t="s">
-        <v>193</v>
+        <v>131</v>
       </c>
     </row>
     <row r="19" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>106</v>
+        <v>132</v>
       </c>
       <c r="B19" s="2">
         <v>13</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="D19" s="2">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="F19" s="6">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="I19" s="3">
-        <v>40</v>
+        <v>8</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="K19" s="2" t="s">
         <v>82</v>
       </c>
       <c r="L19" s="2"/>
       <c r="M19" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="N19" s="2"/>
+        <v>97</v>
+      </c>
+      <c r="N19" s="4" t="s">
+        <v>197</v>
+      </c>
       <c r="O19" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="P19" s="5" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B20" s="2">
+        <v>14</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D20" s="7">
+        <v>17</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="F20" s="7">
+        <v>18</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="I20" s="3">
+        <v>8</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="L20" s="2"/>
+      <c r="M20" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="N20" s="2"/>
+      <c r="O20" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="P20" s="5" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B21" s="2">
+        <v>15</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D21" s="2">
+        <v>18</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="F21" s="6">
+        <v>15</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="I21" s="3">
+        <v>40</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="K21" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="L21" s="2"/>
+      <c r="M21" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="N21" s="2"/>
+      <c r="O21" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="P19" s="2" t="s">
+      <c r="P21" s="2" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="20" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
         <v>67</v>
-      </c>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D20" s="7">
-        <v>19</v>
-      </c>
-      <c r="E20" s="13" t="s">
-        <v>212</v>
-      </c>
-      <c r="F20" s="13"/>
-      <c r="G20" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="H20" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="I20" s="3">
-        <v>9</v>
-      </c>
-      <c r="J20" s="2"/>
-      <c r="K20" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="L20" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="M20" s="2"/>
-      <c r="N20" s="2"/>
-      <c r="O20" s="2"/>
-      <c r="P20" s="2"/>
-    </row>
-    <row r="21" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D21" s="7">
-        <v>20</v>
-      </c>
-      <c r="E21" s="7" t="s">
-        <v>211</v>
-      </c>
-      <c r="F21" s="7"/>
-      <c r="G21" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="H21" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="I21" s="3">
-        <v>2</v>
-      </c>
-      <c r="J21" s="2"/>
-      <c r="K21" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="L21" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="M21" s="2"/>
-      <c r="N21" s="2"/>
-      <c r="O21" s="2"/>
-      <c r="P21" s="2"/>
-    </row>
-    <row r="22" spans="1:16" ht="30" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
-        <v>69</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D22" s="2">
-        <v>21</v>
-      </c>
-      <c r="E22" s="6" t="s">
-        <v>214</v>
-      </c>
-      <c r="F22" s="6"/>
+        <v>27</v>
+      </c>
+      <c r="D22" s="7">
+        <v>19</v>
+      </c>
+      <c r="E22" s="13" t="s">
+        <v>212</v>
+      </c>
+      <c r="F22" s="13"/>
       <c r="G22" s="2" t="s">
         <v>104</v>
       </c>
@@ -2501,7 +2503,7 @@
         <v>112</v>
       </c>
       <c r="I22" s="3">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="J22" s="2"/>
       <c r="K22" s="2" t="s">
@@ -2517,176 +2519,178 @@
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D23" s="7">
+        <v>20</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="F23" s="7"/>
+      <c r="G23" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="I23" s="3">
+        <v>2</v>
+      </c>
+      <c r="J23" s="2"/>
+      <c r="K23" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="L23" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="M23" s="2"/>
+      <c r="N23" s="2"/>
+      <c r="O23" s="2"/>
+      <c r="P23" s="2"/>
+    </row>
+    <row r="24" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D24" s="2">
+        <v>21</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="F24" s="6"/>
+      <c r="G24" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="I24" s="3">
+        <v>12</v>
+      </c>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="L24" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="M24" s="2"/>
+      <c r="N24" s="2"/>
+      <c r="O24" s="2"/>
+      <c r="P24" s="2"/>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="B23" s="2">
-        <v>14</v>
-      </c>
-      <c r="C23" s="2" t="s">
+      <c r="B25" s="2">
+        <v>16</v>
+      </c>
+      <c r="C25" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D23" s="7">
+      <c r="D25" s="7">
         <v>22</v>
-      </c>
-      <c r="E23" s="7" t="s">
-        <v>213</v>
-      </c>
-      <c r="F23" s="7">
-        <v>19</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="H23" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="I23" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="J23" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="K23" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="L23" s="2"/>
-      <c r="M23" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="N23" s="2"/>
-      <c r="O23" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="P23" s="2" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="B24" s="2">
-        <v>15</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D24" s="2">
-        <v>23</v>
-      </c>
-      <c r="E24" s="7" t="s">
-        <v>213</v>
-      </c>
-      <c r="F24" s="7">
-        <v>20</v>
-      </c>
-      <c r="G24" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="H24" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="I24" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="J24" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="K24" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="L24" s="2"/>
-      <c r="M24" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="N24" s="2"/>
-      <c r="O24" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="P24" s="2" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D25" s="7">
-        <v>24</v>
       </c>
       <c r="E25" s="7" t="s">
         <v>213</v>
       </c>
-      <c r="F25" s="7"/>
+      <c r="F25" s="7">
+        <v>19</v>
+      </c>
       <c r="G25" s="2" t="s">
         <v>102</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="I25" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="J25" s="2"/>
+        <v>34</v>
+      </c>
+      <c r="J25" s="2" t="s">
+        <v>35</v>
+      </c>
       <c r="K25" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="L25" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="M25" s="2"/>
+        <v>82</v>
+      </c>
+      <c r="L25" s="2"/>
+      <c r="M25" s="2" t="s">
+        <v>101</v>
+      </c>
       <c r="N25" s="2"/>
-      <c r="O25" s="2"/>
-      <c r="P25" s="2"/>
-    </row>
-    <row r="26" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+      <c r="O25" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="P25" s="2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="B26" s="2"/>
+        <v>221</v>
+      </c>
+      <c r="B26" s="2">
+        <v>17</v>
+      </c>
       <c r="C26" s="2" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D26" s="2">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E26" s="7" t="s">
         <v>213</v>
       </c>
-      <c r="F26" s="7"/>
+      <c r="F26" s="7">
+        <v>20</v>
+      </c>
       <c r="G26" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="I26" s="3"/>
-      <c r="J26" s="2"/>
+        <v>113</v>
+      </c>
+      <c r="I26" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="J26" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="K26" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="L26" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="M26" s="2"/>
+        <v>82</v>
+      </c>
+      <c r="L26" s="2"/>
+      <c r="M26" s="2" t="s">
+        <v>101</v>
+      </c>
       <c r="N26" s="2"/>
-      <c r="O26" s="2"/>
-      <c r="P26" s="2"/>
-    </row>
-    <row r="27" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+      <c r="O26" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="P26" s="2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D27" s="7">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E27" s="7" t="s">
         <v>213</v>
@@ -2699,7 +2703,7 @@
         <v>112</v>
       </c>
       <c r="I27" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="J27" s="2"/>
       <c r="K27" s="2" t="s">
@@ -2713,30 +2717,28 @@
       <c r="O27" s="2"/>
       <c r="P27" s="2"/>
     </row>
-    <row r="28" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D28" s="2">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E28" s="7" t="s">
         <v>213</v>
       </c>
       <c r="F28" s="7"/>
       <c r="G28" s="2" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="H28" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="I28" s="3" t="s">
-        <v>44</v>
-      </c>
+      <c r="I28" s="3"/>
       <c r="J28" s="2"/>
       <c r="K28" s="2" t="s">
         <v>81</v>
@@ -2749,16 +2751,16 @@
       <c r="O28" s="2"/>
       <c r="P28" s="2"/>
     </row>
-    <row r="29" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D29" s="7">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E29" s="7" t="s">
         <v>213</v>
@@ -2771,7 +2773,7 @@
         <v>112</v>
       </c>
       <c r="I29" s="3" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="J29" s="2"/>
       <c r="K29" s="2" t="s">
@@ -2785,101 +2787,77 @@
       <c r="O29" s="2"/>
       <c r="P29" s="2"/>
     </row>
-    <row r="30" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="B30" s="2">
-        <v>16</v>
-      </c>
+        <v>76</v>
+      </c>
+      <c r="B30" s="2"/>
       <c r="C30" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D30" s="7">
-        <v>29</v>
-      </c>
-      <c r="E30" s="13" t="s">
-        <v>216</v>
-      </c>
-      <c r="F30" s="13">
-        <v>11</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="D30" s="2">
+        <v>27</v>
+      </c>
+      <c r="E30" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="F30" s="7"/>
       <c r="G30" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="I30" s="3">
-        <v>20</v>
-      </c>
-      <c r="J30" s="2" t="s">
-        <v>31</v>
-      </c>
+        <v>112</v>
+      </c>
+      <c r="I30" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="J30" s="2"/>
       <c r="K30" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="L30" s="2"/>
-      <c r="M30" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="N30" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="O30" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="P30" s="5" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="31" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+      <c r="L30" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="M30" s="2"/>
+      <c r="N30" s="2"/>
+      <c r="O30" s="2"/>
+      <c r="P30" s="2"/>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="B31" s="2">
-        <v>17</v>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="B31" s="2"/>
       <c r="C31" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D31" s="2">
-        <v>30</v>
-      </c>
-      <c r="E31" s="6" t="s">
-        <v>217</v>
-      </c>
-      <c r="F31" s="6">
-        <v>12</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="D31" s="7">
+        <v>28</v>
+      </c>
+      <c r="E31" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="F31" s="7"/>
       <c r="G31" s="2" t="s">
-        <v>92</v>
+        <v>102</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="I31" s="3">
-        <v>8</v>
-      </c>
-      <c r="J31" s="2" t="s">
-        <v>31</v>
-      </c>
+        <v>112</v>
+      </c>
+      <c r="I31" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="J31" s="2"/>
       <c r="K31" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="L31" s="2"/>
-      <c r="M31" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="N31" s="4" t="s">
-        <v>197</v>
-      </c>
-      <c r="O31" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="P31" s="5" t="s">
-        <v>133</v>
-      </c>
+        <v>81</v>
+      </c>
+      <c r="L31" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="M31" s="2"/>
+      <c r="N31" s="2"/>
+      <c r="O31" s="2"/>
+      <c r="P31" s="2"/>
     </row>
     <row r="32" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
@@ -2964,28 +2942,23 @@
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
   <conditionalFormatting sqref="D2:F33">
-    <cfRule type="expression" dxfId="56" priority="11">
+    <cfRule type="expression" dxfId="18" priority="11">
       <formula>LEN($D2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:A31 C15:O15 C2:P14 C16:P31 A32:P33">
-    <cfRule type="expression" dxfId="55" priority="12">
+  <conditionalFormatting sqref="C15:O15 C2:P14 A32:P33 A2:B31 C16:P31">
+    <cfRule type="expression" dxfId="17" priority="12">
       <formula>$K2="No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2:L33">
-    <cfRule type="expression" dxfId="54" priority="10">
+    <cfRule type="expression" dxfId="16" priority="10">
       <formula>AND($K2="No",LEN($L2)=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P15">
-    <cfRule type="expression" dxfId="53" priority="2">
+    <cfRule type="expression" dxfId="15" priority="2">
       <formula>$K15="No"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B2:B31">
-    <cfRule type="expression" dxfId="52" priority="1">
-      <formula>$K2="No"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4004,72 +3977,72 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="L2:L22">
-    <cfRule type="expression" dxfId="33" priority="14">
+    <cfRule type="expression" dxfId="14" priority="14">
       <formula>AND($K2="No",LEN($L2)=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:F5 D6:D7 D8:F22">
-    <cfRule type="expression" dxfId="32" priority="15">
+    <cfRule type="expression" dxfId="13" priority="15">
       <formula>LEN($D2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O4:P4 O8:P8 O19:P19 A2:A22 C20:P22 C11:P11 C9:N9 C8:M8 C3:M5 C6:D7 C2:P2 C10:I10 K10:P10 C13:P18 C12:I12 K12:P12 G6:P7 C19:M19">
-    <cfRule type="expression" dxfId="31" priority="16">
+    <cfRule type="expression" dxfId="12" priority="16">
       <formula>$K2="No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N3">
-    <cfRule type="expression" dxfId="30" priority="13">
+    <cfRule type="expression" dxfId="11" priority="13">
       <formula>$K3="No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N4:N5">
-    <cfRule type="expression" dxfId="28" priority="11">
+    <cfRule type="expression" dxfId="10" priority="11">
       <formula>$K4="No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O5:P5">
-    <cfRule type="expression" dxfId="27" priority="10">
+    <cfRule type="expression" dxfId="9" priority="10">
       <formula>$K5="No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N8">
-    <cfRule type="expression" dxfId="26" priority="9">
+    <cfRule type="expression" dxfId="8" priority="9">
       <formula>$K8="No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O9:P9">
-    <cfRule type="expression" dxfId="25" priority="8">
+    <cfRule type="expression" dxfId="7" priority="8">
       <formula>$K9="No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N19">
-    <cfRule type="expression" dxfId="24" priority="7">
+    <cfRule type="expression" dxfId="6" priority="7">
       <formula>$K19="No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B22">
-    <cfRule type="expression" dxfId="23" priority="6">
+    <cfRule type="expression" dxfId="5" priority="6">
       <formula>$K2="No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J10">
-    <cfRule type="expression" dxfId="22" priority="5">
+    <cfRule type="expression" dxfId="4" priority="5">
       <formula>$K10="No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J12">
-    <cfRule type="expression" dxfId="21" priority="4">
+    <cfRule type="expression" dxfId="3" priority="4">
       <formula>$K12="No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6:F7">
-    <cfRule type="expression" dxfId="20" priority="2">
+    <cfRule type="expression" dxfId="2" priority="2">
       <formula>LEN($D6)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6:F7">
-    <cfRule type="expression" dxfId="19" priority="3">
+    <cfRule type="expression" dxfId="1" priority="3">
       <formula>$K6="No"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Confirm and fix required/unused cell highlighting
close #5
</commit_message>
<xml_diff>
--- a/specs/Coliform-column-definitions.xlsx
+++ b/specs/Coliform-column-definitions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\xl-ese\specs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED10B97E-D3B4-4478-A7F0-4A62E610E0F4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F5A2EBF-C74C-410C-BC30-42177F2FCCA2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="248">
   <si>
     <t>Optionality</t>
   </si>
@@ -319,9 +319,6 @@
     <t>Time</t>
   </si>
   <si>
-    <t>"N" if blank</t>
-  </si>
-  <si>
     <t>Format</t>
   </si>
   <si>
@@ -398,9 +395,6 @@
     <t>Record Type</t>
   </si>
   <si>
-    <t>=AND(LEN(RC1)&gt;0,LEN(RC3)=0)</t>
-  </si>
-  <si>
     <t>1 &lt;= x &lt;= 9</t>
   </si>
   <si>
@@ -410,24 +404,9 @@
     <t>1 &lt;= x &lt;= 12</t>
   </si>
   <si>
-    <t>=AND(LEN(RC1)&gt;0,LEN(RC5)=0)</t>
-  </si>
-  <si>
-    <t>=AND(LEN(RC1)&gt;0,LEN(RC6)=0)</t>
-  </si>
-  <si>
-    <t>=AND(LEN(RC1)&gt;0,LEN(RC7)=0)</t>
-  </si>
-  <si>
-    <t>=AND(LEN(RC1)&gt;0,LEN(RC8)=0)</t>
-  </si>
-  <si>
     <t>=AND(LEN(RC8)&gt;0,RC8&lt;=TODAY())</t>
   </si>
   <si>
-    <t>=AND(LEN(RC1)&gt;0,LEN(RC10)=0)</t>
-  </si>
-  <si>
     <t>Between 0.01 and 99.0</t>
   </si>
   <si>
@@ -465,9 +444,6 @@
   </si>
   <si>
     <t>=VolumeList</t>
-  </si>
-  <si>
-    <t>=AND(LEN(RC1)&gt;0,RC14&gt;0,LEN(RC16)=0)</t>
   </si>
   <si>
     <t xml:space="preserve"> Field must be valued if B_COUNT_TYPE is valued                                       
@@ -487,9 +463,6 @@
     <t>=CountTypeList</t>
   </si>
   <si>
-    <t>=AND(LEN(RC1)&gt;0,RC14&gt;0,LEN(RC15)=0)</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Field must be valued if B_COUNT &gt; 0           
 PVs:
 SPACES
@@ -502,9 +475,6 @@
   </si>
   <si>
     <t>=PresenceList</t>
-  </si>
-  <si>
-    <t>=AND(LEN(RC1)&gt;0,LEN(RC13)=0)</t>
   </si>
   <si>
     <t>--If not valued, B_LAB_REJECTION_REASON must be valued and B_COUNT must not be valued.
@@ -621,9 +591,6 @@
     <t>=AnalyteList</t>
   </si>
   <si>
-    <t>=AND(LEN(RC1)&gt;0,LEN(RC4)=0)</t>
-  </si>
-  <si>
     <t>3100 = Total Coliform
 3014 = E. Coli</t>
   </si>
@@ -640,9 +607,6 @@
     <t>=AND(LEN(RC2)&gt;0,RC2&lt;=TODAY())</t>
   </si>
   <si>
-    <t>=AND(LEN(RC1)&gt;0,LEN(RC2)=0)</t>
-  </si>
-  <si>
     <t>MM/DD/YYYY
  Reference field required to associate the result to the parent sample.  Must be same value as field B_PWS_NUMBER in Sample structure (documented in above rows) or result (and sample) will be rejected.</t>
   </si>
@@ -657,18 +621,6 @@
   </si>
   <si>
     <t>Excel col #</t>
-  </si>
-  <si>
-    <t>=AND(LEN(RC1)&gt;0,RC10="Repeat",LEN(RC11)=0)
-=AND(LEN(RC1)&gt;0,RC10&lt;&gt;"Repeat")</t>
-  </si>
-  <si>
-    <t>=AND(LEN(RC1)&gt;0,RC10="Repeat",LEN(RC16)=0)
-=AND(LEN(RC1)&gt;0,RC10&lt;&gt;"Repeat")</t>
-  </si>
-  <si>
-    <t>=AND(LEN(RC1)&gt;0,RC10="Repeat",LEN(RC17)=0)
-=AND(LEN(RC1)&gt;0,RC10&lt;&gt;"Repeat")</t>
   </si>
   <si>
     <t>XML Element</t>
@@ -834,6 +786,57 @@
   </si>
   <si>
     <t>1 &lt;= x &lt;= 20</t>
+  </si>
+  <si>
+    <t>=LEN(RC4)=0</t>
+  </si>
+  <si>
+    <t>=LEN(RC3)=0</t>
+  </si>
+  <si>
+    <t>=LEN(RC5)=0</t>
+  </si>
+  <si>
+    <t>=LEN(RC6)=0</t>
+  </si>
+  <si>
+    <t>=LEN(RC7)=0</t>
+  </si>
+  <si>
+    <t>=LEN(RC8)=0</t>
+  </si>
+  <si>
+    <t>=LEN(RC10)=0</t>
+  </si>
+  <si>
+    <t>=AND(RC10="Repeat",LEN(RC11)=0)
+=AND(RC10&lt;&gt;"Repeat")</t>
+  </si>
+  <si>
+    <t>=LEN(RC1)=0
+=COUNTIFS(R6C1:R6C1,RC1,R6C4:R6C4,RC4)&gt;1</t>
+  </si>
+  <si>
+    <t>=LEN(RC4)=0
+=COUNTIFS(R6C1:R6C1,RC1,R6C4:R6C4,RC4)&gt;1</t>
+  </si>
+  <si>
+    <t>=LEN(RC2)=0</t>
+  </si>
+  <si>
+    <t>=LEN(RC13)=0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+=RC13="Absent"</t>
+  </si>
+  <si>
+    <t>=AND(RC14&gt;0,LEN(RC15)=0)
+=RC13="Absent"</t>
+  </si>
+  <si>
+    <t>=AND(RC14&gt;0,LEN(RC16)=0)
+=RC13="Absent"</t>
   </si>
 </sst>
 </file>
@@ -920,7 +923,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="55">
+  <dxfs count="56">
     <dxf>
       <fill>
         <patternFill>
@@ -929,6 +932,60 @@
       </fill>
     </dxf>
     <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <bgColor theme="0" tint="-0.14996795556505021"/>
@@ -938,6 +995,13 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor theme="5" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
@@ -1025,88 +1089,6 @@
           <bgColor theme="7" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1173,6 +1155,34 @@
     </dxf>
     <dxf>
       <alignment vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1193,52 +1203,54 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{636125F0-68A9-4682-81D8-01BD3AB67D26}" name="Table1" displayName="Table1" ref="A1:P33" totalsRowShown="0" headerRowDxfId="54" dataDxfId="53">
-  <autoFilter ref="A1:P33" xr:uid="{C224FB70-9F34-49CE-AC5D-FD58B7A283A8}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{636125F0-68A9-4682-81D8-01BD3AB67D26}" name="Table1" displayName="Table1" ref="A1:P33" totalsRowShown="0" headerRowDxfId="51" dataDxfId="50">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:P33">
+    <sortCondition ref="B2:B33"/>
+  </sortState>
   <tableColumns count="16">
-    <tableColumn id="6" xr3:uid="{57EF6AB6-6C4C-4170-BD9B-BF376C46C5DF}" name="Title" dataDxfId="52"/>
-    <tableColumn id="12" xr3:uid="{BFDB40C3-C9ED-4560-81A1-344ECAE248C8}" name="Excel col #" dataDxfId="51"/>
-    <tableColumn id="1" xr3:uid="{3193A6D3-813B-4494-AEED-01D6509FCA0D}" name="CSV Column Name" dataDxfId="50"/>
-    <tableColumn id="11" xr3:uid="{057EA208-1889-4E3C-A179-F312337D9867}" name="CSV col #" dataDxfId="49"/>
-    <tableColumn id="16" xr3:uid="{1F4E7FF6-264D-41DA-AC14-BAA45F3439C7}" name="XML Element" dataDxfId="48"/>
-    <tableColumn id="10" xr3:uid="{F503FCB6-1F5D-4765-B4AB-F67230BC37A3}" name="XML order #" dataDxfId="47"/>
-    <tableColumn id="2" xr3:uid="{5C52F15D-4AC8-44CE-A401-3402D3CD4152}" name="Data Type" dataDxfId="46"/>
-    <tableColumn id="3" xr3:uid="{FFD71D9C-951A-4BB1-9000-9A1C4C3F71D3}" name="Optionality" dataDxfId="45"/>
-    <tableColumn id="4" xr3:uid="{6FEED7B4-CF3F-4593-BB9F-5CFA5FA5B692}" name="Size" dataDxfId="44"/>
-    <tableColumn id="5" xr3:uid="{563427BF-63BA-491F-9B6F-4E02453C643B}" name="Business Rules" dataDxfId="43"/>
-    <tableColumn id="9" xr3:uid="{A9E34622-C2B4-476B-A018-EABC1256DC10}" name="User Editable" dataDxfId="42"/>
-    <tableColumn id="14" xr3:uid="{9DA3EF2F-E261-414A-B10C-F88F2052640F}" name="Generated" dataDxfId="41"/>
-    <tableColumn id="15" xr3:uid="{AA61284F-4409-4E18-9405-8F2EAA78028A}" name="Format" dataDxfId="40"/>
-    <tableColumn id="13" xr3:uid="{94BA7C53-9CFA-4072-B1A4-7E9CE9D9DDF7}" name="Conditional Formatting" dataDxfId="39"/>
-    <tableColumn id="7" xr3:uid="{22AE72C5-BA89-443A-81AF-BCF4B114454C}" name="Validation" dataDxfId="38"/>
-    <tableColumn id="8" xr3:uid="{5DE66E18-4141-4BDD-B41D-2782AC810F6E}" name="Validation Formula" dataDxfId="37"/>
+    <tableColumn id="6" xr3:uid="{57EF6AB6-6C4C-4170-BD9B-BF376C46C5DF}" name="Title" dataDxfId="49"/>
+    <tableColumn id="12" xr3:uid="{BFDB40C3-C9ED-4560-81A1-344ECAE248C8}" name="Excel col #" dataDxfId="48"/>
+    <tableColumn id="1" xr3:uid="{3193A6D3-813B-4494-AEED-01D6509FCA0D}" name="CSV Column Name" dataDxfId="47"/>
+    <tableColumn id="11" xr3:uid="{057EA208-1889-4E3C-A179-F312337D9867}" name="CSV col #" dataDxfId="46"/>
+    <tableColumn id="16" xr3:uid="{1F4E7FF6-264D-41DA-AC14-BAA45F3439C7}" name="XML Element" dataDxfId="45"/>
+    <tableColumn id="10" xr3:uid="{F503FCB6-1F5D-4765-B4AB-F67230BC37A3}" name="XML order #" dataDxfId="44"/>
+    <tableColumn id="2" xr3:uid="{5C52F15D-4AC8-44CE-A401-3402D3CD4152}" name="Data Type" dataDxfId="43"/>
+    <tableColumn id="3" xr3:uid="{FFD71D9C-951A-4BB1-9000-9A1C4C3F71D3}" name="Optionality" dataDxfId="42"/>
+    <tableColumn id="4" xr3:uid="{6FEED7B4-CF3F-4593-BB9F-5CFA5FA5B692}" name="Size" dataDxfId="41"/>
+    <tableColumn id="5" xr3:uid="{563427BF-63BA-491F-9B6F-4E02453C643B}" name="Business Rules" dataDxfId="40"/>
+    <tableColumn id="9" xr3:uid="{A9E34622-C2B4-476B-A018-EABC1256DC10}" name="User Editable" dataDxfId="39"/>
+    <tableColumn id="14" xr3:uid="{9DA3EF2F-E261-414A-B10C-F88F2052640F}" name="Generated" dataDxfId="38"/>
+    <tableColumn id="15" xr3:uid="{AA61284F-4409-4E18-9405-8F2EAA78028A}" name="Format" dataDxfId="37"/>
+    <tableColumn id="13" xr3:uid="{94BA7C53-9CFA-4072-B1A4-7E9CE9D9DDF7}" name="Conditional Formatting" dataDxfId="36"/>
+    <tableColumn id="7" xr3:uid="{22AE72C5-BA89-443A-81AF-BCF4B114454C}" name="Validation" dataDxfId="35"/>
+    <tableColumn id="8" xr3:uid="{5DE66E18-4141-4BDD-B41D-2782AC810F6E}" name="Validation Formula" dataDxfId="34"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{05345577-AC31-4B6D-B899-55D66DEB1874}" name="Table2" displayName="Table2" ref="A1:P22" totalsRowShown="0" headerRowDxfId="36" dataDxfId="35">
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C2:P22">
-    <sortCondition ref="D16:D22"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{05345577-AC31-4B6D-B899-55D66DEB1874}" name="Table2" displayName="Table2" ref="A1:P22" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:P22">
+    <sortCondition ref="B2:B22"/>
   </sortState>
   <tableColumns count="16">
-    <tableColumn id="7" xr3:uid="{9E32B24E-F549-442D-B6C5-5B5E67078170}" name="Title" dataDxfId="34"/>
-    <tableColumn id="12" xr3:uid="{023EA1AA-B7DF-4814-BFEF-5AB9B0752B95}" name="Excel col #" dataDxfId="33"/>
-    <tableColumn id="1" xr3:uid="{5687DF61-58A8-463A-A7F7-9B8B474466F3}" name="CSV Column Name" dataDxfId="32"/>
-    <tableColumn id="13" xr3:uid="{9E799E78-81C7-4788-BF70-799894A0FACA}" name="CSV col #" dataDxfId="31"/>
-    <tableColumn id="16" xr3:uid="{6872DDE9-C4EA-4656-AE08-1B51AE6AE7D6}" name="XML Element" dataDxfId="30"/>
-    <tableColumn id="11" xr3:uid="{F0D84552-7E57-4362-9DCD-EDC8E4E51415}" name="XML order #" dataDxfId="29"/>
-    <tableColumn id="2" xr3:uid="{E36A262F-69A4-4276-95F1-0FB7FCE8E2AD}" name="Data Type" dataDxfId="28"/>
-    <tableColumn id="3" xr3:uid="{B4F9F589-759B-40AB-BD12-81562C067103}" name="Optionality" dataDxfId="27"/>
-    <tableColumn id="4" xr3:uid="{29CBFF2E-DC73-4812-9BE8-505CDCED923B}" name="Size" dataDxfId="26"/>
-    <tableColumn id="5" xr3:uid="{2FBE4EBA-0896-4EA8-8E6A-9740D712F4CF}" name="Business Rules" dataDxfId="25"/>
-    <tableColumn id="14" xr3:uid="{F6A291D7-463E-4C10-AE63-F46C62F701F1}" name="User Editable" dataDxfId="24"/>
-    <tableColumn id="6" xr3:uid="{4A3A44E5-9909-437B-9914-BD7AF1AC2439}" name="Generated" dataDxfId="23"/>
-    <tableColumn id="15" xr3:uid="{30410F79-D89B-4BAE-852C-7ADB5287310A}" name="Format" dataDxfId="22"/>
-    <tableColumn id="8" xr3:uid="{23D225B6-A3A4-4446-9AD4-7762B64F46FE}" name="Conditional Formatting" dataDxfId="21"/>
-    <tableColumn id="9" xr3:uid="{27D08B50-8012-49E0-9C10-AEB67B99B91B}" name="Validation" dataDxfId="20"/>
-    <tableColumn id="10" xr3:uid="{A301C8EB-BB2A-4524-AF6E-20714C0D7DD5}" name="Validation Formula" dataDxfId="19"/>
+    <tableColumn id="7" xr3:uid="{9E32B24E-F549-442D-B6C5-5B5E67078170}" name="Title" dataDxfId="16"/>
+    <tableColumn id="12" xr3:uid="{023EA1AA-B7DF-4814-BFEF-5AB9B0752B95}" name="Excel col #" dataDxfId="15"/>
+    <tableColumn id="1" xr3:uid="{5687DF61-58A8-463A-A7F7-9B8B474466F3}" name="CSV Column Name" dataDxfId="14"/>
+    <tableColumn id="13" xr3:uid="{9E799E78-81C7-4788-BF70-799894A0FACA}" name="CSV col #" dataDxfId="13"/>
+    <tableColumn id="16" xr3:uid="{6872DDE9-C4EA-4656-AE08-1B51AE6AE7D6}" name="XML Element" dataDxfId="12"/>
+    <tableColumn id="11" xr3:uid="{F0D84552-7E57-4362-9DCD-EDC8E4E51415}" name="XML order #" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{E36A262F-69A4-4276-95F1-0FB7FCE8E2AD}" name="Data Type" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{B4F9F589-759B-40AB-BD12-81562C067103}" name="Optionality" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{29CBFF2E-DC73-4812-9BE8-505CDCED923B}" name="Size" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{2FBE4EBA-0896-4EA8-8E6A-9740D712F4CF}" name="Business Rules" dataDxfId="7"/>
+    <tableColumn id="14" xr3:uid="{F6A291D7-463E-4C10-AE63-F46C62F701F1}" name="User Editable" dataDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{4A3A44E5-9909-437B-9914-BD7AF1AC2439}" name="Generated" dataDxfId="5"/>
+    <tableColumn id="15" xr3:uid="{30410F79-D89B-4BAE-852C-7ADB5287310A}" name="Format" dataDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{23D225B6-A3A4-4446-9AD4-7762B64F46FE}" name="Conditional Formatting" dataDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{27D08B50-8012-49E0-9C10-AEB67B99B91B}" name="Validation" dataDxfId="2"/>
+    <tableColumn id="10" xr3:uid="{A301C8EB-BB2A-4524-AF6E-20714C0D7DD5}" name="Validation Formula" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight14" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1532,7 +1544,7 @@
     <col min="11" max="11" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="16.140625" customWidth="1"/>
     <col min="13" max="13" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="44" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="33" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="48.85546875" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="10.140625" bestFit="1" customWidth="1"/>
@@ -1546,22 +1558,22 @@
         <v>53</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>194</v>
+        <v>182</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>246</v>
+        <v>231</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H1" s="6" t="s">
         <v>0</v>
@@ -1573,13 +1585,13 @@
         <v>2</v>
       </c>
       <c r="K1" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="L1" s="6" t="s">
         <v>79</v>
       </c>
       <c r="M1" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="N1" s="6" t="s">
         <v>77</v>
@@ -1591,66 +1603,76 @@
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7" t="s">
+    <row r="2" spans="1:16" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" s="2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="2">
+        <v>2</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="F2" s="2">
+        <v>4</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="I2" s="3">
+        <v>20</v>
+      </c>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="P2" s="5" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" s="2">
+        <v>2</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="7">
         <v>3</v>
       </c>
-      <c r="D2" s="7">
-        <v>1</v>
-      </c>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="I2" s="8">
-        <v>20</v>
-      </c>
-      <c r="J2" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="K2" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="L2" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="M2" s="7"/>
-      <c r="N2" s="7"/>
-      <c r="O2" s="7"/>
-      <c r="P2" s="7"/>
-    </row>
-    <row r="3" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B3" s="2">
-        <v>1</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="2">
-        <v>2</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="F3" s="2">
-        <v>4</v>
+      <c r="E3" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="F3" s="7">
+        <v>3</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="I3" s="3">
         <v>20</v>
@@ -1661,530 +1683,566 @@
       </c>
       <c r="L3" s="2"/>
       <c r="M3" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="N3" s="4" t="s">
-        <v>117</v>
-      </c>
+        <v>103</v>
+      </c>
+      <c r="N3" s="2"/>
       <c r="O3" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="P3" s="5" t="s">
-        <v>247</v>
+      <c r="P3" s="2" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B4" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="7">
-        <v>3</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>200</v>
-      </c>
-      <c r="F4" s="7">
-        <v>3</v>
+        <v>7</v>
+      </c>
+      <c r="D4" s="2">
+        <v>4</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="F4" s="2">
+        <v>5</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="I4" s="3">
-        <v>20</v>
-      </c>
-      <c r="J4" s="2"/>
+        <v>9</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>51</v>
+      </c>
       <c r="K4" s="2" t="s">
         <v>82</v>
       </c>
       <c r="L4" s="2"/>
       <c r="M4" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="N4" s="2"/>
+        <v>103</v>
+      </c>
+      <c r="N4" s="5" t="s">
+        <v>234</v>
+      </c>
       <c r="O4" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="P4" s="2" t="s">
-        <v>85</v>
+      <c r="P4" s="5" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B5" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="2">
-        <v>4</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="F5" s="2">
+        <v>8</v>
+      </c>
+      <c r="D5" s="7">
         <v>5</v>
       </c>
+      <c r="E5" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="F5" s="7">
+        <v>10</v>
+      </c>
       <c r="G5" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I5" s="3">
-        <v>9</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>51</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="J5" s="2"/>
       <c r="K5" s="2" t="s">
         <v>82</v>
       </c>
       <c r="L5" s="2"/>
       <c r="M5" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="N5" s="5" t="s">
-        <v>120</v>
+        <v>233</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="P5" s="5" t="s">
-        <v>225</v>
+        <v>127</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="B6" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="2">
         <v>8</v>
       </c>
-      <c r="D6" s="7">
-        <v>5</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>202</v>
-      </c>
-      <c r="F6" s="7">
+      <c r="E6" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="F6" s="2">
+        <v>6</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="I6" s="3">
         <v>10</v>
       </c>
-      <c r="G6" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="I6" s="3">
-        <v>1</v>
-      </c>
-      <c r="J6" s="2"/>
+      <c r="J6" s="2" t="s">
+        <v>52</v>
+      </c>
       <c r="K6" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="L6" s="2" t="s">
-        <v>94</v>
-      </c>
+      <c r="L6" s="2"/>
       <c r="M6" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="N6" s="2"/>
+        <v>103</v>
+      </c>
+      <c r="N6" s="5" t="s">
+        <v>235</v>
+      </c>
       <c r="O6" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="P6" s="5" t="s">
-        <v>134</v>
+        <v>84</v>
+      </c>
+      <c r="P6" s="2" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="B7" s="2"/>
+        <v>86</v>
+      </c>
+      <c r="B7" s="2">
+        <v>6</v>
+      </c>
       <c r="C7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="7">
         <v>9</v>
       </c>
-      <c r="D7" s="2">
-        <v>6</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>233</v>
-      </c>
-      <c r="F7" s="6">
+      <c r="E7" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="F7" s="13">
+        <v>21</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="I7" s="3">
+        <v>12</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="N7" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="O7" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="P7" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B8" s="2">
+        <v>7</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="2">
+        <v>12</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="F8" s="2">
+        <v>9</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="I8" s="3">
         <v>1</v>
       </c>
-      <c r="G7" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="I7" s="3">
-        <v>10</v>
-      </c>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="L7" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="M7" s="2"/>
-      <c r="N7" s="2"/>
-      <c r="O7" s="2"/>
-      <c r="P7" s="2"/>
-    </row>
-    <row r="8" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="7">
-        <v>7</v>
-      </c>
-      <c r="E8" s="13" t="s">
-        <v>234</v>
-      </c>
-      <c r="F8" s="13">
-        <v>2</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="I8" s="3">
-        <v>10</v>
-      </c>
-      <c r="J8" s="2"/>
+      <c r="J8" s="2" t="s">
+        <v>17</v>
+      </c>
       <c r="K8" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="L8" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="M8" s="2"/>
-      <c r="N8" s="2"/>
-      <c r="O8" s="2"/>
-      <c r="P8" s="2"/>
+        <v>82</v>
+      </c>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="N8" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="O8" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="P8" s="5" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>75</v>
+        <v>90</v>
       </c>
       <c r="B9" s="2">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" s="2">
+        <v>18</v>
+      </c>
+      <c r="D9" s="7">
+        <v>13</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="F9" s="7">
+        <v>16</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="I9" s="3">
         <v>8</v>
       </c>
-      <c r="E9" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="F9" s="2">
-        <v>6</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="I9" s="3">
-        <v>10</v>
-      </c>
       <c r="J9" s="2" t="s">
-        <v>52</v>
+        <v>19</v>
       </c>
       <c r="K9" s="2" t="s">
         <v>82</v>
       </c>
       <c r="L9" s="2"/>
       <c r="M9" s="2" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="N9" s="5" t="s">
-        <v>124</v>
+        <v>238</v>
       </c>
       <c r="O9" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="P9" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="P9" s="5" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="B10" s="2">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" s="7">
-        <v>9</v>
-      </c>
-      <c r="E10" s="13" t="s">
-        <v>219</v>
-      </c>
-      <c r="F10" s="13">
-        <v>21</v>
+        <v>20</v>
+      </c>
+      <c r="D10" s="2">
+        <v>14</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="F10" s="2">
+        <v>17</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="I10" s="3">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>51</v>
+        <v>209</v>
       </c>
       <c r="K10" s="2" t="s">
         <v>82</v>
       </c>
       <c r="L10" s="2"/>
       <c r="M10" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="N10" s="5" t="s">
-        <v>125</v>
-      </c>
+        <v>95</v>
+      </c>
+      <c r="N10" s="2"/>
       <c r="O10" s="2" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="P10" s="2" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="B11" s="2"/>
+        <v>64</v>
+      </c>
+      <c r="B11" s="2">
+        <v>10</v>
+      </c>
       <c r="C11" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D11" s="2">
-        <v>10</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="F11" s="2"/>
+        <v>21</v>
+      </c>
+      <c r="D11" s="7">
+        <v>15</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="F11" s="7">
+        <v>8</v>
+      </c>
       <c r="G11" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="I11" s="3">
-        <v>40</v>
+        <v>2</v>
       </c>
       <c r="J11" s="2"/>
       <c r="K11" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="L11" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="M11" s="2"/>
-      <c r="N11" s="2"/>
-      <c r="O11" s="2"/>
-      <c r="P11" s="2"/>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="N11" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="O11" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="P11" s="5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B12" s="2"/>
+        <v>65</v>
+      </c>
+      <c r="B12" s="2">
+        <v>11</v>
+      </c>
       <c r="C12" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D12" s="7">
-        <v>11</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>205</v>
-      </c>
-      <c r="F12" s="7">
-        <v>7</v>
+        <v>22</v>
+      </c>
+      <c r="D12" s="2">
+        <v>16</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="F12" s="6">
+        <v>22</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="I12" s="3">
         <v>2</v>
       </c>
-      <c r="J12" s="2" t="s">
-        <v>15</v>
-      </c>
+      <c r="J12" s="2"/>
       <c r="K12" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="L12" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="M12" s="2"/>
-      <c r="N12" s="2"/>
-      <c r="O12" s="2"/>
-      <c r="P12" s="2"/>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="N12" s="4" t="s">
+        <v>240</v>
+      </c>
+      <c r="O12" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="P12" s="5" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>89</v>
+        <v>102</v>
       </c>
       <c r="B13" s="2">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D13" s="2">
-        <v>12</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="F13" s="2">
-        <v>9</v>
+        <v>30</v>
+      </c>
+      <c r="D13" s="7">
+        <v>29</v>
+      </c>
+      <c r="E13" s="13" t="s">
+        <v>201</v>
+      </c>
+      <c r="F13" s="13">
+        <v>11</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="I13" s="3">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="K13" s="2" t="s">
         <v>82</v>
       </c>
       <c r="L13" s="2"/>
       <c r="M13" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="N13" s="5" t="s">
-        <v>126</v>
+        <v>103</v>
+      </c>
+      <c r="N13" s="4" t="s">
+        <v>240</v>
       </c>
       <c r="O13" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="P13" s="5" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>90</v>
+        <v>125</v>
       </c>
       <c r="B14" s="2">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D14" s="7">
-        <v>13</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>207</v>
-      </c>
-      <c r="F14" s="7">
-        <v>16</v>
+        <v>32</v>
+      </c>
+      <c r="D14" s="2">
+        <v>30</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="F14" s="6">
+        <v>12</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>92</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="I14" s="3">
         <v>8</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="K14" s="2" t="s">
         <v>82</v>
       </c>
       <c r="L14" s="2"/>
       <c r="M14" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="N14" s="5" t="s">
-        <v>127</v>
+        <v>96</v>
+      </c>
+      <c r="N14" s="4" t="s">
+        <v>240</v>
       </c>
       <c r="O14" s="2" t="s">
         <v>78</v>
       </c>
       <c r="P14" s="5" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>91</v>
+        <v>66</v>
       </c>
       <c r="B15" s="2">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D15" s="2">
-        <v>14</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>208</v>
-      </c>
-      <c r="F15" s="2">
+        <v>23</v>
+      </c>
+      <c r="D15" s="7">
         <v>17</v>
       </c>
+      <c r="E15" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="F15" s="7">
+        <v>18</v>
+      </c>
       <c r="G15" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I15" s="3">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>224</v>
+        <v>24</v>
       </c>
       <c r="K15" s="2" t="s">
         <v>82</v>
@@ -2195,515 +2253,477 @@
       </c>
       <c r="N15" s="2"/>
       <c r="O15" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="P15" s="2" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+      <c r="P15" s="5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>64</v>
+        <v>105</v>
       </c>
       <c r="B16" s="2">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D16" s="7">
+        <v>25</v>
+      </c>
+      <c r="D16" s="2">
+        <v>18</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="F16" s="6">
         <v>15</v>
       </c>
-      <c r="E16" s="7" t="s">
-        <v>209</v>
-      </c>
-      <c r="F16" s="7">
-        <v>8</v>
-      </c>
       <c r="G16" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="I16" s="3">
-        <v>2</v>
-      </c>
-      <c r="J16" s="2"/>
+        <v>40</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>26</v>
+      </c>
       <c r="K16" s="2" t="s">
         <v>82</v>
       </c>
       <c r="L16" s="2"/>
       <c r="M16" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="N16" s="5" t="s">
-        <v>129</v>
-      </c>
+        <v>103</v>
+      </c>
+      <c r="N16" s="2"/>
       <c r="O16" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="P16" s="5" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+      <c r="P16" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>65</v>
+        <v>205</v>
       </c>
       <c r="B17" s="2">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C17" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D17" s="7">
         <v>22</v>
       </c>
-      <c r="D17" s="2">
-        <v>16</v>
-      </c>
-      <c r="E17" s="6" t="s">
-        <v>218</v>
-      </c>
-      <c r="F17" s="6">
-        <v>22</v>
+      <c r="E17" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="F17" s="7">
+        <v>19</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="I17" s="3">
-        <v>2</v>
-      </c>
-      <c r="J17" s="2"/>
+        <v>112</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>35</v>
+      </c>
       <c r="K17" s="2" t="s">
         <v>82</v>
       </c>
       <c r="L17" s="2"/>
       <c r="M17" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="N17" s="4" t="s">
-        <v>195</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="N17" s="2"/>
       <c r="O17" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="P17" s="5" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+      <c r="P17" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>103</v>
+        <v>206</v>
       </c>
       <c r="B18" s="2">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D18" s="7">
-        <v>29</v>
-      </c>
-      <c r="E18" s="13" t="s">
-        <v>216</v>
-      </c>
-      <c r="F18" s="13">
-        <v>11</v>
+        <v>36</v>
+      </c>
+      <c r="D18" s="2">
+        <v>23</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="F18" s="7">
+        <v>20</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="I18" s="3">
-        <v>20</v>
+        <v>112</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>34</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="K18" s="2" t="s">
         <v>82</v>
       </c>
       <c r="L18" s="2"/>
       <c r="M18" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="N18" s="4" t="s">
-        <v>196</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="N18" s="2"/>
       <c r="O18" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="P18" s="5" t="s">
-        <v>131</v>
+        <v>101</v>
+      </c>
+      <c r="P18" s="2" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="19" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="B19" s="2">
-        <v>13</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="B19" s="2"/>
       <c r="C19" s="2" t="s">
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="D19" s="2">
-        <v>30</v>
+        <v>6</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="F19" s="6">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>92</v>
+        <v>103</v>
       </c>
       <c r="H19" s="2" t="s">
         <v>110</v>
       </c>
       <c r="I19" s="3">
-        <v>8</v>
-      </c>
-      <c r="J19" s="2" t="s">
-        <v>31</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="J19" s="2"/>
       <c r="K19" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="L19" s="2"/>
-      <c r="M19" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="N19" s="4" t="s">
-        <v>197</v>
-      </c>
-      <c r="O19" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="P19" s="5" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+      <c r="L19" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="M19" s="2"/>
+      <c r="N19" s="2"/>
+      <c r="O19" s="2"/>
+      <c r="P19" s="2"/>
+    </row>
+    <row r="20" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="B20" s="2">
+        <v>57</v>
+      </c>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" s="7">
+        <v>7</v>
+      </c>
+      <c r="E20" s="13" t="s">
+        <v>219</v>
+      </c>
+      <c r="F20" s="13">
+        <v>2</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="I20" s="3">
+        <v>10</v>
+      </c>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="L20" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="M20" s="2"/>
+      <c r="N20" s="2"/>
+      <c r="O20" s="2"/>
+      <c r="P20" s="2"/>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C20" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D20" s="7">
-        <v>17</v>
-      </c>
-      <c r="E20" s="7" t="s">
-        <v>210</v>
-      </c>
-      <c r="F20" s="7">
-        <v>18</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="H20" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="I20" s="3">
-        <v>8</v>
-      </c>
-      <c r="J20" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="K20" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="L20" s="2"/>
-      <c r="M20" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="N20" s="2"/>
-      <c r="O20" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="P20" s="5" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="B21" s="2">
+      <c r="D21" s="7">
+        <v>11</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="F21" s="7">
+        <v>7</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="I21" s="3">
+        <v>2</v>
+      </c>
+      <c r="J21" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C21" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D21" s="2">
-        <v>18</v>
-      </c>
-      <c r="E21" s="6" t="s">
-        <v>215</v>
-      </c>
-      <c r="F21" s="6">
-        <v>15</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="H21" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="I21" s="3">
-        <v>40</v>
-      </c>
-      <c r="J21" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="K21" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="L21" s="2"/>
-      <c r="M21" s="2" t="s">
-        <v>104</v>
-      </c>
+        <v>81</v>
+      </c>
+      <c r="L21" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="M21" s="2"/>
       <c r="N21" s="2"/>
-      <c r="O21" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="P21" s="2" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O21" s="2"/>
+      <c r="P21" s="2"/>
+    </row>
+    <row r="22" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" s="2" t="s">
-        <v>27</v>
+        <v>47</v>
       </c>
       <c r="D22" s="7">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="E22" s="13" t="s">
-        <v>212</v>
-      </c>
-      <c r="F22" s="13"/>
+        <v>207</v>
+      </c>
+      <c r="F22" s="13">
+        <v>13</v>
+      </c>
       <c r="G22" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="I22" s="3">
-        <v>9</v>
-      </c>
-      <c r="J22" s="2"/>
+        <v>10</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>50</v>
+      </c>
       <c r="K22" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="L22" s="11" t="s">
-        <v>87</v>
+      <c r="L22" s="2" t="s">
+        <v>114</v>
       </c>
       <c r="M22" s="2"/>
       <c r="N22" s="2"/>
       <c r="O22" s="2"/>
       <c r="P22" s="2"/>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D23" s="7">
-        <v>20</v>
-      </c>
-      <c r="E23" s="7" t="s">
-        <v>211</v>
-      </c>
-      <c r="F23" s="7"/>
+        <v>48</v>
+      </c>
+      <c r="D23" s="2">
+        <v>32</v>
+      </c>
+      <c r="E23" s="13" t="s">
+        <v>208</v>
+      </c>
+      <c r="F23" s="13">
+        <v>14</v>
+      </c>
       <c r="G23" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="I23" s="3">
-        <v>2</v>
-      </c>
-      <c r="J23" s="2"/>
+        <v>10</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>49</v>
+      </c>
       <c r="K23" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="L23" s="11" t="s">
-        <v>87</v>
+      <c r="L23" s="2" t="s">
+        <v>108</v>
       </c>
       <c r="M23" s="2"/>
       <c r="N23" s="2"/>
       <c r="O23" s="2"/>
       <c r="P23" s="2"/>
     </row>
-    <row r="24" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D24" s="2">
-        <v>21</v>
-      </c>
-      <c r="E24" s="6" t="s">
-        <v>214</v>
-      </c>
-      <c r="F24" s="6"/>
-      <c r="G24" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="H24" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="I24" s="3">
-        <v>12</v>
-      </c>
-      <c r="J24" s="2"/>
-      <c r="K24" s="2" t="s">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A24" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="B24" s="7"/>
+      <c r="C24" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D24" s="7">
+        <v>1</v>
+      </c>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="H24" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="I24" s="8">
+        <v>20</v>
+      </c>
+      <c r="J24" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="K24" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="L24" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="M24" s="2"/>
-      <c r="N24" s="2"/>
-      <c r="O24" s="2"/>
-      <c r="P24" s="2"/>
+      <c r="L24" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="M24" s="7"/>
+      <c r="N24" s="7"/>
+      <c r="O24" s="7"/>
+      <c r="P24" s="7"/>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="B25" s="2">
-        <v>16</v>
-      </c>
+        <v>104</v>
+      </c>
+      <c r="B25" s="2"/>
       <c r="C25" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D25" s="7">
-        <v>22</v>
-      </c>
-      <c r="E25" s="7" t="s">
-        <v>213</v>
-      </c>
-      <c r="F25" s="7">
-        <v>19</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="D25" s="2">
+        <v>10</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="F25" s="2"/>
       <c r="G25" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="I25" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="J25" s="2" t="s">
-        <v>35</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="I25" s="3">
+        <v>40</v>
+      </c>
+      <c r="J25" s="2"/>
       <c r="K25" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="L25" s="2"/>
-      <c r="M25" s="2" t="s">
-        <v>101</v>
-      </c>
+        <v>81</v>
+      </c>
+      <c r="L25" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="M25" s="2"/>
       <c r="N25" s="2"/>
-      <c r="O25" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="P25" s="2" t="s">
-        <v>130</v>
-      </c>
+      <c r="O25" s="2"/>
+      <c r="P25" s="2"/>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="B26" s="2">
-        <v>17</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="B26" s="2"/>
       <c r="C26" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D26" s="2">
-        <v>23</v>
-      </c>
-      <c r="E26" s="7" t="s">
-        <v>213</v>
-      </c>
-      <c r="F26" s="7">
-        <v>20</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="D26" s="7">
+        <v>19</v>
+      </c>
+      <c r="E26" s="13" t="s">
+        <v>197</v>
+      </c>
+      <c r="F26" s="13"/>
       <c r="G26" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="I26" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="J26" s="2" t="s">
-        <v>37</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="I26" s="3">
+        <v>9</v>
+      </c>
+      <c r="J26" s="2"/>
       <c r="K26" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="L26" s="2"/>
-      <c r="M26" s="2" t="s">
-        <v>101</v>
-      </c>
+        <v>81</v>
+      </c>
+      <c r="L26" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="M26" s="2"/>
       <c r="N26" s="2"/>
-      <c r="O26" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="P26" s="2" t="s">
-        <v>130</v>
-      </c>
+      <c r="O26" s="2"/>
+      <c r="P26" s="2"/>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" s="2" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="D27" s="7">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>213</v>
+        <v>196</v>
       </c>
       <c r="F27" s="7"/>
       <c r="G27" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="I27" s="3" t="s">
-        <v>39</v>
+        <v>111</v>
+      </c>
+      <c r="I27" s="3">
+        <v>2</v>
       </c>
       <c r="J27" s="2"/>
       <c r="K27" s="2" t="s">
@@ -2717,28 +2737,30 @@
       <c r="O27" s="2"/>
       <c r="P27" s="2"/>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" s="2" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="D28" s="2">
-        <v>25</v>
-      </c>
-      <c r="E28" s="7" t="s">
-        <v>213</v>
-      </c>
-      <c r="F28" s="7"/>
+        <v>21</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="F28" s="6"/>
       <c r="G28" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="I28" s="3"/>
+        <v>111</v>
+      </c>
+      <c r="I28" s="3">
+        <v>12</v>
+      </c>
       <c r="J28" s="2"/>
       <c r="K28" s="2" t="s">
         <v>81</v>
@@ -2753,27 +2775,27 @@
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D29" s="7">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>213</v>
+        <v>198</v>
       </c>
       <c r="F29" s="7"/>
       <c r="G29" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I29" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="J29" s="2"/>
       <c r="K29" s="2" t="s">
@@ -2789,28 +2811,26 @@
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D30" s="2">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>213</v>
+        <v>198</v>
       </c>
       <c r="F30" s="7"/>
       <c r="G30" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="I30" s="3" t="s">
-        <v>44</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="I30" s="3"/>
       <c r="J30" s="2"/>
       <c r="K30" s="2" t="s">
         <v>81</v>
@@ -2825,27 +2845,27 @@
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D31" s="7">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>213</v>
+        <v>198</v>
       </c>
       <c r="F31" s="7"/>
       <c r="G31" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I31" s="3" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="J31" s="2"/>
       <c r="K31" s="2" t="s">
@@ -2859,80 +2879,72 @@
       <c r="O31" s="2"/>
       <c r="P31" s="2"/>
     </row>
-    <row r="32" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D32" s="7">
-        <v>31</v>
-      </c>
-      <c r="E32" s="13" t="s">
-        <v>222</v>
-      </c>
-      <c r="F32" s="13">
-        <v>13</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="D32" s="2">
+        <v>27</v>
+      </c>
+      <c r="E32" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="F32" s="7"/>
       <c r="G32" s="2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="I32" s="3">
-        <v>10</v>
-      </c>
-      <c r="J32" s="2" t="s">
-        <v>50</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="I32" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="J32" s="2"/>
       <c r="K32" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="L32" s="2" t="s">
-        <v>115</v>
+      <c r="L32" s="11" t="s">
+        <v>87</v>
       </c>
       <c r="M32" s="2"/>
       <c r="N32" s="2"/>
       <c r="O32" s="2"/>
       <c r="P32" s="2"/>
     </row>
-    <row r="33" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>58</v>
+        <v>73</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D33" s="2">
-        <v>32</v>
-      </c>
-      <c r="E33" s="13" t="s">
-        <v>223</v>
-      </c>
-      <c r="F33" s="13">
-        <v>14</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="D33" s="7">
+        <v>28</v>
+      </c>
+      <c r="E33" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="F33" s="7"/>
       <c r="G33" s="2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="I33" s="3">
-        <v>10</v>
-      </c>
-      <c r="J33" s="2" t="s">
-        <v>49</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="I33" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="J33" s="2"/>
       <c r="K33" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="L33" s="2" t="s">
-        <v>109</v>
+      <c r="L33" s="11" t="s">
+        <v>87</v>
       </c>
       <c r="M33" s="2"/>
       <c r="N33" s="2"/>
@@ -2942,22 +2954,22 @@
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
   <conditionalFormatting sqref="D2:F33">
-    <cfRule type="expression" dxfId="18" priority="11">
+    <cfRule type="expression" dxfId="55" priority="11">
       <formula>LEN($D2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C15:O15 C2:P14 A32:P33 A2:B31 C16:P31">
-    <cfRule type="expression" dxfId="17" priority="12">
+  <conditionalFormatting sqref="C15:O15 A32:P33 A2:B31 C2:P14 C16:P31">
+    <cfRule type="expression" dxfId="54" priority="12">
       <formula>$K2="No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2:L33">
-    <cfRule type="expression" dxfId="16" priority="10">
+    <cfRule type="expression" dxfId="53" priority="10">
       <formula>AND($K2="No",LEN($L2)=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P15">
-    <cfRule type="expression" dxfId="15" priority="2">
+    <cfRule type="expression" dxfId="52" priority="2">
       <formula>$K15="No"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2996,7 +3008,7 @@
     <col min="11" max="11" width="8.28515625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10.5703125" customWidth="1"/>
     <col min="13" max="13" width="25.140625" customWidth="1"/>
-    <col min="14" max="14" width="36.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="41.85546875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="10.140625" customWidth="1"/>
     <col min="16" max="16" width="31.42578125" bestFit="1" customWidth="1"/>
   </cols>
@@ -3006,22 +3018,22 @@
         <v>53</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>194</v>
+        <v>182</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>246</v>
+        <v>231</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H1" s="6" t="s">
         <v>0</v>
@@ -3033,13 +3045,13 @@
         <v>2</v>
       </c>
       <c r="K1" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="L1" s="6" t="s">
         <v>79</v>
       </c>
       <c r="M1" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="N1" s="6" t="s">
         <v>77</v>
@@ -3051,387 +3063,411 @@
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="B2" s="2"/>
+        <v>56</v>
+      </c>
+      <c r="B2" s="2">
+        <v>1</v>
+      </c>
       <c r="C2" s="2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D2" s="2">
+        <v>2</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="F2" s="2">
         <v>1</v>
       </c>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
       <c r="G2" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I2" s="2">
         <v>20</v>
       </c>
       <c r="J2" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>241</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="P2" s="5" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B3" s="2">
+        <v>2</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="2">
+        <v>3</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="K2" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
-      <c r="O2" s="2"/>
-      <c r="P2" s="2"/>
-    </row>
-    <row r="3" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B3" s="2">
-        <v>1</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="2">
-        <v>2</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>199</v>
-      </c>
       <c r="F3" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="I3" s="2">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>191</v>
+        <v>178</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>82</v>
       </c>
       <c r="L3" s="2"/>
       <c r="M3" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="N3" s="4" t="s">
-        <v>117</v>
+        <v>96</v>
+      </c>
+      <c r="N3" s="5" t="s">
+        <v>243</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="P3" s="5" t="s">
-        <v>247</v>
+        <v>177</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="B4" s="2">
+        <v>3</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="2">
+        <v>4</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="F4" s="2">
         <v>2</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" s="2">
-        <v>3</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="F4" s="2">
-        <v>3</v>
-      </c>
       <c r="G4" s="2" t="s">
-        <v>92</v>
+        <v>103</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="I4" s="2">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>190</v>
+        <v>176</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>82</v>
       </c>
       <c r="L4" s="2"/>
       <c r="M4" s="2" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="N4" s="5" t="s">
-        <v>189</v>
+        <v>234</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="P4" s="5" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>60</v>
+        <v>175</v>
       </c>
       <c r="B5" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="D5" s="2">
         <v>7</v>
       </c>
-      <c r="D5" s="2">
+      <c r="E5" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="F5" s="6">
+        <v>12</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="I5" s="2">
         <v>4</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="F5" s="2">
-        <v>2</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="I5" s="2">
-        <v>9</v>
-      </c>
       <c r="J5" s="2" t="s">
-        <v>187</v>
+        <v>173</v>
       </c>
       <c r="K5" s="2" t="s">
         <v>82</v>
       </c>
       <c r="L5" s="2"/>
       <c r="M5" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="N5" s="5" t="s">
-        <v>120</v>
+        <v>103</v>
+      </c>
+      <c r="N5" s="4" t="s">
+        <v>242</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="P5" s="2" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+      <c r="P5" s="5" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="B6" s="2"/>
+        <v>171</v>
+      </c>
+      <c r="B6" s="2">
+        <v>5</v>
+      </c>
       <c r="C6" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="D6" s="2">
+        <v>8</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="F6" s="2">
+        <v>8</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="I6" s="2">
+        <v>8</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="N6" s="5"/>
+      <c r="O6" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="P6" s="5" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="B7" s="2">
+        <v>6</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="D7" s="2">
         <v>9</v>
       </c>
-      <c r="D6" s="2">
-        <v>5</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>233</v>
-      </c>
-      <c r="F6" s="6">
+      <c r="E7" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="F7" s="2">
+        <v>9</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="I7" s="2">
         <v>4</v>
       </c>
-      <c r="G6" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="I6" s="2">
+      <c r="J7" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="P7" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="B8" s="2">
+        <v>7</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="D8" s="2">
         <v>10</v>
       </c>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="L6" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="M6" s="2"/>
-      <c r="N6" s="2"/>
-      <c r="O6" s="2"/>
-      <c r="P6" s="2"/>
-    </row>
-    <row r="7" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2" t="s">
+      <c r="E8" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="F8" s="2">
         <v>10</v>
       </c>
-      <c r="D7" s="2">
-        <v>6</v>
-      </c>
-      <c r="E7" s="13" t="s">
-        <v>234</v>
-      </c>
-      <c r="F7" s="13">
-        <v>5</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="I7" s="2">
-        <v>10</v>
-      </c>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="L7" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="M7" s="2"/>
-      <c r="N7" s="2"/>
-      <c r="O7" s="2"/>
-      <c r="P7" s="2"/>
-    </row>
-    <row r="8" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="B8" s="2">
-        <v>4</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="D8" s="2">
-        <v>7</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>235</v>
-      </c>
-      <c r="F8" s="6">
-        <v>12</v>
-      </c>
       <c r="G8" s="2" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="I8" s="2">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>184</v>
+        <v>164</v>
       </c>
       <c r="K8" s="2" t="s">
         <v>82</v>
       </c>
       <c r="L8" s="2"/>
       <c r="M8" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="N8" s="5" t="s">
-        <v>183</v>
-      </c>
+        <v>96</v>
+      </c>
+      <c r="N8" s="5"/>
       <c r="O8" s="2" t="s">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="P8" s="5" t="s">
-        <v>182</v>
+        <v>163</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>181</v>
+        <v>212</v>
       </c>
       <c r="B9" s="2">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>180</v>
+        <v>162</v>
       </c>
       <c r="D9" s="2">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>236</v>
+        <v>224</v>
       </c>
       <c r="F9" s="2">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I9" s="2">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>179</v>
+        <v>209</v>
       </c>
       <c r="K9" s="2" t="s">
         <v>82</v>
       </c>
       <c r="L9" s="2"/>
       <c r="M9" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="N9" s="5"/>
+        <v>95</v>
+      </c>
+      <c r="N9" s="2"/>
       <c r="O9" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="P9" s="5" t="s">
-        <v>178</v>
+        <v>93</v>
+      </c>
+      <c r="P9" s="2" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>177</v>
+        <v>161</v>
       </c>
       <c r="B10" s="2">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>176</v>
+        <v>160</v>
       </c>
       <c r="D10" s="2">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>237</v>
+        <v>225</v>
       </c>
       <c r="F10" s="2">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I10" s="2">
-        <v>4</v>
-      </c>
-      <c r="J10" s="2" t="s">
-        <v>224</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="J10" s="2"/>
       <c r="K10" s="2" t="s">
         <v>82</v>
       </c>
@@ -3439,616 +3475,594 @@
       <c r="M10" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="N10" s="2"/>
+      <c r="N10" s="5"/>
       <c r="O10" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="P10" s="2" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+      <c r="P10" s="5" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="B11" s="2">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>175</v>
+        <v>153</v>
       </c>
       <c r="D11" s="2">
-        <v>10</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>238</v>
-      </c>
-      <c r="F11" s="2">
-        <v>10</v>
+        <v>15</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="F11" s="6">
+        <v>6</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>92</v>
+        <v>103</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I11" s="2">
-        <v>8</v>
+        <v>30</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>174</v>
+        <v>152</v>
       </c>
       <c r="K11" s="2" t="s">
         <v>82</v>
       </c>
       <c r="L11" s="2"/>
       <c r="M11" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="N11" s="5"/>
-      <c r="O11" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="P11" s="5" t="s">
-        <v>173</v>
-      </c>
+        <v>103</v>
+      </c>
+      <c r="N11" s="2"/>
+      <c r="O11" s="2"/>
+      <c r="P11" s="2"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>227</v>
+        <v>151</v>
       </c>
       <c r="B12" s="2">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>172</v>
+        <v>150</v>
       </c>
       <c r="D12" s="2">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>239</v>
+        <v>229</v>
       </c>
       <c r="F12" s="2">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>93</v>
+        <v>103</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I12" s="2">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>224</v>
+        <v>149</v>
       </c>
       <c r="K12" s="2" t="s">
         <v>82</v>
       </c>
       <c r="L12" s="2"/>
       <c r="M12" s="2" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="N12" s="2"/>
       <c r="O12" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="P12" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="P12" s="5" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>171</v>
+        <v>148</v>
       </c>
       <c r="B13" s="2">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>170</v>
+        <v>147</v>
       </c>
       <c r="D13" s="2">
-        <v>12</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="F13" s="2">
         <v>17</v>
       </c>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
       <c r="G13" s="2" t="s">
-        <v>92</v>
+        <v>103</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="I13" s="2">
-        <v>8</v>
-      </c>
-      <c r="J13" s="2"/>
+        <v>4</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>146</v>
+      </c>
       <c r="K13" s="2" t="s">
         <v>82</v>
       </c>
       <c r="L13" s="2"/>
       <c r="M13" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="N13" s="5"/>
+        <v>103</v>
+      </c>
+      <c r="N13" s="2"/>
       <c r="O13" s="2" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="P13" s="5" t="s">
-        <v>178</v>
+        <v>145</v>
       </c>
     </row>
     <row r="14" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="B14" s="2"/>
+        <v>144</v>
+      </c>
+      <c r="B14" s="2">
+        <v>13</v>
+      </c>
       <c r="C14" s="2" t="s">
-        <v>168</v>
+        <v>143</v>
       </c>
       <c r="D14" s="2">
+        <v>18</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="F14" s="6">
         <v>13</v>
       </c>
-      <c r="E14" s="6" t="s">
-        <v>241</v>
-      </c>
-      <c r="F14" s="6">
-        <v>18</v>
-      </c>
       <c r="G14" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="I14" s="2">
         <v>1</v>
       </c>
-      <c r="J14" s="2" t="s">
-        <v>167</v>
+      <c r="J14" s="5" t="s">
+        <v>142</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="L14" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="M14" s="2"/>
-      <c r="N14" s="2"/>
-      <c r="O14" s="2"/>
-      <c r="P14" s="2"/>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="N14" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="O14" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="P14" s="5" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="B15" s="2"/>
+        <v>134</v>
+      </c>
+      <c r="B15" s="2">
+        <v>14</v>
+      </c>
       <c r="C15" s="2" t="s">
-        <v>164</v>
+        <v>133</v>
       </c>
       <c r="D15" s="2">
+        <v>28</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="F15" s="6">
         <v>14</v>
       </c>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
       <c r="G15" s="2" t="s">
-        <v>104</v>
+        <v>130</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="I15" s="2">
-        <v>2</v>
-      </c>
-      <c r="J15" s="2"/>
+        <v>109</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>131</v>
+      </c>
       <c r="K15" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="L15" s="11" t="s">
-        <v>87</v>
-      </c>
+        <v>82</v>
+      </c>
+      <c r="L15" s="2"/>
       <c r="M15" s="2"/>
-      <c r="N15" s="2"/>
-      <c r="O15" s="2"/>
-      <c r="P15" s="2"/>
+      <c r="N15" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="O15" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="P15" s="2" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="16" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>243</v>
+        <v>216</v>
       </c>
       <c r="B16" s="2">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>163</v>
+        <v>137</v>
       </c>
       <c r="D16" s="2">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>242</v>
+        <v>214</v>
       </c>
       <c r="F16" s="6">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="I16" s="2">
-        <v>30</v>
+        <v>9</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>162</v>
+        <v>136</v>
       </c>
       <c r="K16" s="2" t="s">
         <v>82</v>
       </c>
       <c r="L16" s="2"/>
       <c r="M16" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="N16" s="2"/>
-      <c r="O16" s="2"/>
-      <c r="P16" s="2"/>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+      <c r="N16" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="O16" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="P16" s="5" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>161</v>
+        <v>217</v>
       </c>
       <c r="B17" s="2">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>160</v>
+        <v>140</v>
       </c>
       <c r="D17" s="2">
-        <v>16</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>244</v>
-      </c>
-      <c r="F17" s="2">
-        <v>7</v>
+        <v>20</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="F17" s="6">
+        <v>15</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="I17" s="2">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>159</v>
+        <v>139</v>
       </c>
       <c r="K17" s="2" t="s">
         <v>82</v>
       </c>
       <c r="L17" s="2"/>
       <c r="M17" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="N17" s="2"/>
+        <v>103</v>
+      </c>
+      <c r="N17" s="4" t="s">
+        <v>246</v>
+      </c>
       <c r="O17" s="2" t="s">
         <v>80</v>
       </c>
       <c r="P17" s="5" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="B18" s="2">
-        <v>12</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="B18" s="2"/>
       <c r="C18" s="2" t="s">
-        <v>157</v>
+        <v>9</v>
       </c>
       <c r="D18" s="2">
-        <v>17</v>
-      </c>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
+        <v>5</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="F18" s="6">
+        <v>4</v>
+      </c>
       <c r="G18" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H18" s="2" t="s">
         <v>110</v>
       </c>
       <c r="I18" s="2">
-        <v>4</v>
-      </c>
-      <c r="J18" s="2" t="s">
-        <v>156</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="J18" s="2"/>
       <c r="K18" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="L18" s="2"/>
-      <c r="M18" s="2" t="s">
-        <v>104</v>
-      </c>
+        <v>81</v>
+      </c>
+      <c r="L18" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="M18" s="2"/>
       <c r="N18" s="2"/>
-      <c r="O18" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="P18" s="5" t="s">
-        <v>155</v>
-      </c>
+      <c r="O18" s="2"/>
+      <c r="P18" s="2"/>
     </row>
     <row r="19" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="B19" s="2">
-        <v>13</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="B19" s="2"/>
       <c r="C19" s="2" t="s">
-        <v>153</v>
+        <v>10</v>
       </c>
       <c r="D19" s="2">
-        <v>18</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>245</v>
-      </c>
-      <c r="F19" s="6">
-        <v>13</v>
+        <v>6</v>
+      </c>
+      <c r="E19" s="13" t="s">
+        <v>219</v>
+      </c>
+      <c r="F19" s="13">
+        <v>5</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H19" s="2" t="s">
         <v>110</v>
       </c>
       <c r="I19" s="2">
-        <v>1</v>
-      </c>
-      <c r="J19" s="5" t="s">
-        <v>152</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="J19" s="2"/>
       <c r="K19" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="L19" s="2"/>
-      <c r="M19" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="N19" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="O19" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="P19" s="5" t="s">
-        <v>150</v>
-      </c>
+        <v>81</v>
+      </c>
+      <c r="L19" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="M19" s="2"/>
+      <c r="N19" s="2"/>
+      <c r="O19" s="2"/>
+      <c r="P19" s="2"/>
     </row>
     <row r="20" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="B20" s="2">
-        <v>14</v>
-      </c>
+        <v>159</v>
+      </c>
+      <c r="B20" s="2"/>
       <c r="C20" s="2" t="s">
-        <v>149</v>
+        <v>158</v>
       </c>
       <c r="D20" s="2">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="F20" s="6">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H20" s="2" t="s">
         <v>110</v>
       </c>
       <c r="I20" s="2">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>148</v>
+        <v>157</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="L20" s="2"/>
-      <c r="M20" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="N20" s="5" t="s">
-        <v>147</v>
-      </c>
-      <c r="O20" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="P20" s="5" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+      <c r="L20" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="M20" s="2"/>
+      <c r="N20" s="2"/>
+      <c r="O20" s="2"/>
+      <c r="P20" s="2"/>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>231</v>
-      </c>
-      <c r="B21" s="2">
-        <v>15</v>
-      </c>
+        <v>118</v>
+      </c>
+      <c r="B21" s="2"/>
       <c r="C21" s="2" t="s">
-        <v>145</v>
+        <v>3</v>
       </c>
       <c r="D21" s="2">
-        <v>27</v>
-      </c>
-      <c r="E21" s="6" t="s">
-        <v>229</v>
-      </c>
-      <c r="F21" s="6">
-        <v>16</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
       <c r="G21" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H21" s="2" t="s">
         <v>110</v>
       </c>
       <c r="I21" s="2">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>144</v>
+        <v>180</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="L21" s="2"/>
-      <c r="M21" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="N21" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="O21" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="P21" s="5" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+      <c r="L21" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="M21" s="2"/>
+      <c r="N21" s="2"/>
+      <c r="O21" s="2"/>
+      <c r="P21" s="2"/>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="B22" s="2">
-        <v>16</v>
-      </c>
+        <v>155</v>
+      </c>
+      <c r="B22" s="2"/>
       <c r="C22" s="2" t="s">
-        <v>140</v>
+        <v>154</v>
       </c>
       <c r="D22" s="2">
-        <v>28</v>
-      </c>
-      <c r="E22" s="6" t="s">
-        <v>230</v>
-      </c>
-      <c r="F22" s="6">
         <v>14</v>
       </c>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
       <c r="G22" s="2" t="s">
-        <v>137</v>
+        <v>103</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="I22" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="J22" s="2" t="s">
-        <v>138</v>
-      </c>
+        <v>109</v>
+      </c>
+      <c r="I22" s="2">
+        <v>2</v>
+      </c>
+      <c r="J22" s="2"/>
       <c r="K22" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="L22" s="2"/>
+        <v>81</v>
+      </c>
+      <c r="L22" s="11" t="s">
+        <v>87</v>
+      </c>
       <c r="M22" s="2"/>
       <c r="N22" s="2"/>
-      <c r="O22" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="P22" s="2" t="s">
-        <v>136</v>
-      </c>
+      <c r="O22" s="2"/>
+      <c r="P22" s="2"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="L2:L22">
-    <cfRule type="expression" dxfId="14" priority="14">
+    <cfRule type="expression" dxfId="33" priority="15">
       <formula>AND($K2="No",LEN($L2)=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:F5 D6:D7 D8:F22">
-    <cfRule type="expression" dxfId="13" priority="15">
+    <cfRule type="expression" dxfId="32" priority="16">
       <formula>LEN($D2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O4:P4 O8:P8 O19:P19 A2:A22 C20:P22 C11:P11 C9:N9 C8:M8 C3:M5 C6:D7 C2:P2 C10:I10 K10:P10 C13:P18 C12:I12 K12:P12 G6:P7 C19:M19">
-    <cfRule type="expression" dxfId="12" priority="16">
+    <cfRule type="expression" dxfId="31" priority="17">
       <formula>$K2="No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N3">
-    <cfRule type="expression" dxfId="11" priority="13">
+    <cfRule type="expression" dxfId="30" priority="14">
       <formula>$K3="No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N4:N5">
-    <cfRule type="expression" dxfId="10" priority="11">
+    <cfRule type="expression" dxfId="29" priority="12">
       <formula>$K4="No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O5:P5">
-    <cfRule type="expression" dxfId="9" priority="10">
+    <cfRule type="expression" dxfId="28" priority="11">
       <formula>$K5="No"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N8">
-    <cfRule type="expression" dxfId="8" priority="9">
-      <formula>$K8="No"</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="O9:P9">
-    <cfRule type="expression" dxfId="7" priority="8">
+    <cfRule type="expression" dxfId="26" priority="9">
       <formula>$K9="No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N19">
-    <cfRule type="expression" dxfId="6" priority="7">
+    <cfRule type="expression" dxfId="25" priority="8">
       <formula>$K19="No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B22">
-    <cfRule type="expression" dxfId="5" priority="6">
+    <cfRule type="expression" dxfId="24" priority="7">
       <formula>$K2="No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J10">
-    <cfRule type="expression" dxfId="4" priority="5">
+    <cfRule type="expression" dxfId="23" priority="6">
       <formula>$K10="No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J12">
-    <cfRule type="expression" dxfId="3" priority="4">
+    <cfRule type="expression" dxfId="22" priority="5">
       <formula>$K12="No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6:F7">
-    <cfRule type="expression" dxfId="2" priority="2">
+    <cfRule type="expression" dxfId="21" priority="3">
       <formula>LEN($D6)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6:F7">
-    <cfRule type="expression" dxfId="1" priority="3">
+    <cfRule type="expression" dxfId="20" priority="4">
       <formula>$K6="No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O3:P3">
+    <cfRule type="expression" dxfId="19" priority="2">
+      <formula>$K3="No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N8">
     <cfRule type="expression" dxfId="0" priority="1">
-      <formula>$K3="No"</formula>
+      <formula>$K8="No"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Reorder columns to group primary keys
Lab Sample ID, PWS Number, & 
Sample Collection Date
</commit_message>
<xml_diff>
--- a/specs/Coliform-column-definitions.xlsx
+++ b/specs/Coliform-column-definitions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\xl-ese\specs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F5A2EBF-C74C-410C-BC30-42177F2FCCA2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{934D5689-E15A-4313-BA5C-F0D674824DC7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Coliform Sample" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="245">
   <si>
     <t>Optionality</t>
   </si>
@@ -385,26 +385,16 @@
     <t>"000"</t>
   </si>
   <si>
-    <t>=LEN(R6C1)=0
-=COUNTIF(R6C1:R6C1)&gt;1</t>
-  </si>
-  <si>
     <t>CSV col #</t>
   </si>
   <si>
     <t>Record Type</t>
   </si>
   <si>
-    <t>1 &lt;= x &lt;= 9</t>
-  </si>
-  <si>
     <t>1 &lt;= x &lt;= 10</t>
   </si>
   <si>
     <t>1 &lt;= x &lt;= 12</t>
-  </si>
-  <si>
-    <t>=AND(LEN(RC8)&gt;0,RC8&lt;=TODAY())</t>
   </si>
   <si>
     <t>Between 0.01 and 99.0</t>
@@ -604,9 +594,6 @@
     <t xml:space="preserve"> Reference field required to associate the result to the parent sample.  Must be same value as field B_PWS_NUMBER in Sample structure (documented in above rows) or result (and sample) will be rejected.</t>
   </si>
   <si>
-    <t>=AND(LEN(RC2)&gt;0,RC2&lt;=TODAY())</t>
-  </si>
-  <si>
     <t>MM/DD/YYYY
  Reference field required to associate the result to the parent sample.  Must be same value as field B_PWS_NUMBER in Sample structure (documented in above rows) or result (and sample) will be rejected.</t>
   </si>
@@ -788,13 +775,7 @@
     <t>1 &lt;= x &lt;= 20</t>
   </si>
   <si>
-    <t>=LEN(RC4)=0</t>
-  </si>
-  <si>
     <t>=LEN(RC3)=0</t>
-  </si>
-  <si>
-    <t>=LEN(RC5)=0</t>
   </si>
   <si>
     <t>=LEN(RC6)=0</t>
@@ -837,6 +818,16 @@
   <si>
     <t>=AND(RC14&gt;0,LEN(RC16)=0)
 =RC13="Absent"</t>
+  </si>
+  <si>
+    <t>=AND(LEN(RC3)&gt;0,RC3&lt;=TODAY())</t>
+  </si>
+  <si>
+    <t>=LEN(RC9)=0</t>
+  </si>
+  <si>
+    <t>=LEN(RC1)=0
+=COUNTIF(R6C1:R6C1)&gt;1</t>
   </si>
 </sst>
 </file>
@@ -923,7 +914,61 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="56">
+  <dxfs count="53">
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -932,60 +977,6 @@
       </fill>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill>
           <bgColor theme="0" tint="-0.14996795556505021"/>
@@ -1002,13 +993,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor theme="0" tint="-0.14996795556505021"/>
         </patternFill>
       </fill>
@@ -1016,21 +1000,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1203,54 +1173,54 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{636125F0-68A9-4682-81D8-01BD3AB67D26}" name="Table1" displayName="Table1" ref="A1:P33" totalsRowShown="0" headerRowDxfId="51" dataDxfId="50">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{636125F0-68A9-4682-81D8-01BD3AB67D26}" name="Table1" displayName="Table1" ref="A1:P33" totalsRowShown="0" headerRowDxfId="48" dataDxfId="47">
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:P33">
     <sortCondition ref="B2:B33"/>
   </sortState>
   <tableColumns count="16">
-    <tableColumn id="6" xr3:uid="{57EF6AB6-6C4C-4170-BD9B-BF376C46C5DF}" name="Title" dataDxfId="49"/>
-    <tableColumn id="12" xr3:uid="{BFDB40C3-C9ED-4560-81A1-344ECAE248C8}" name="Excel col #" dataDxfId="48"/>
-    <tableColumn id="1" xr3:uid="{3193A6D3-813B-4494-AEED-01D6509FCA0D}" name="CSV Column Name" dataDxfId="47"/>
-    <tableColumn id="11" xr3:uid="{057EA208-1889-4E3C-A179-F312337D9867}" name="CSV col #" dataDxfId="46"/>
-    <tableColumn id="16" xr3:uid="{1F4E7FF6-264D-41DA-AC14-BAA45F3439C7}" name="XML Element" dataDxfId="45"/>
-    <tableColumn id="10" xr3:uid="{F503FCB6-1F5D-4765-B4AB-F67230BC37A3}" name="XML order #" dataDxfId="44"/>
-    <tableColumn id="2" xr3:uid="{5C52F15D-4AC8-44CE-A401-3402D3CD4152}" name="Data Type" dataDxfId="43"/>
-    <tableColumn id="3" xr3:uid="{FFD71D9C-951A-4BB1-9000-9A1C4C3F71D3}" name="Optionality" dataDxfId="42"/>
-    <tableColumn id="4" xr3:uid="{6FEED7B4-CF3F-4593-BB9F-5CFA5FA5B692}" name="Size" dataDxfId="41"/>
-    <tableColumn id="5" xr3:uid="{563427BF-63BA-491F-9B6F-4E02453C643B}" name="Business Rules" dataDxfId="40"/>
-    <tableColumn id="9" xr3:uid="{A9E34622-C2B4-476B-A018-EABC1256DC10}" name="User Editable" dataDxfId="39"/>
-    <tableColumn id="14" xr3:uid="{9DA3EF2F-E261-414A-B10C-F88F2052640F}" name="Generated" dataDxfId="38"/>
-    <tableColumn id="15" xr3:uid="{AA61284F-4409-4E18-9405-8F2EAA78028A}" name="Format" dataDxfId="37"/>
-    <tableColumn id="13" xr3:uid="{94BA7C53-9CFA-4072-B1A4-7E9CE9D9DDF7}" name="Conditional Formatting" dataDxfId="36"/>
-    <tableColumn id="7" xr3:uid="{22AE72C5-BA89-443A-81AF-BCF4B114454C}" name="Validation" dataDxfId="35"/>
-    <tableColumn id="8" xr3:uid="{5DE66E18-4141-4BDD-B41D-2782AC810F6E}" name="Validation Formula" dataDxfId="34"/>
+    <tableColumn id="6" xr3:uid="{57EF6AB6-6C4C-4170-BD9B-BF376C46C5DF}" name="Title" dataDxfId="46"/>
+    <tableColumn id="12" xr3:uid="{BFDB40C3-C9ED-4560-81A1-344ECAE248C8}" name="Excel col #" dataDxfId="45"/>
+    <tableColumn id="1" xr3:uid="{3193A6D3-813B-4494-AEED-01D6509FCA0D}" name="CSV Column Name" dataDxfId="44"/>
+    <tableColumn id="11" xr3:uid="{057EA208-1889-4E3C-A179-F312337D9867}" name="CSV col #" dataDxfId="43"/>
+    <tableColumn id="16" xr3:uid="{1F4E7FF6-264D-41DA-AC14-BAA45F3439C7}" name="XML Element" dataDxfId="42"/>
+    <tableColumn id="10" xr3:uid="{F503FCB6-1F5D-4765-B4AB-F67230BC37A3}" name="XML order #" dataDxfId="41"/>
+    <tableColumn id="2" xr3:uid="{5C52F15D-4AC8-44CE-A401-3402D3CD4152}" name="Data Type" dataDxfId="40"/>
+    <tableColumn id="3" xr3:uid="{FFD71D9C-951A-4BB1-9000-9A1C4C3F71D3}" name="Optionality" dataDxfId="39"/>
+    <tableColumn id="4" xr3:uid="{6FEED7B4-CF3F-4593-BB9F-5CFA5FA5B692}" name="Size" dataDxfId="38"/>
+    <tableColumn id="5" xr3:uid="{563427BF-63BA-491F-9B6F-4E02453C643B}" name="Business Rules" dataDxfId="37"/>
+    <tableColumn id="9" xr3:uid="{A9E34622-C2B4-476B-A018-EABC1256DC10}" name="User Editable" dataDxfId="36"/>
+    <tableColumn id="14" xr3:uid="{9DA3EF2F-E261-414A-B10C-F88F2052640F}" name="Generated" dataDxfId="35"/>
+    <tableColumn id="15" xr3:uid="{AA61284F-4409-4E18-9405-8F2EAA78028A}" name="Format" dataDxfId="34"/>
+    <tableColumn id="13" xr3:uid="{94BA7C53-9CFA-4072-B1A4-7E9CE9D9DDF7}" name="Conditional Formatting" dataDxfId="33"/>
+    <tableColumn id="7" xr3:uid="{22AE72C5-BA89-443A-81AF-BCF4B114454C}" name="Validation" dataDxfId="32"/>
+    <tableColumn id="8" xr3:uid="{5DE66E18-4141-4BDD-B41D-2782AC810F6E}" name="Validation Formula" dataDxfId="31"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{05345577-AC31-4B6D-B899-55D66DEB1874}" name="Table2" displayName="Table2" ref="A1:P22" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{05345577-AC31-4B6D-B899-55D66DEB1874}" name="Table2" displayName="Table2" ref="A1:P22" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:P22">
     <sortCondition ref="B2:B22"/>
   </sortState>
   <tableColumns count="16">
-    <tableColumn id="7" xr3:uid="{9E32B24E-F549-442D-B6C5-5B5E67078170}" name="Title" dataDxfId="16"/>
-    <tableColumn id="12" xr3:uid="{023EA1AA-B7DF-4814-BFEF-5AB9B0752B95}" name="Excel col #" dataDxfId="15"/>
-    <tableColumn id="1" xr3:uid="{5687DF61-58A8-463A-A7F7-9B8B474466F3}" name="CSV Column Name" dataDxfId="14"/>
-    <tableColumn id="13" xr3:uid="{9E799E78-81C7-4788-BF70-799894A0FACA}" name="CSV col #" dataDxfId="13"/>
-    <tableColumn id="16" xr3:uid="{6872DDE9-C4EA-4656-AE08-1B51AE6AE7D6}" name="XML Element" dataDxfId="12"/>
-    <tableColumn id="11" xr3:uid="{F0D84552-7E57-4362-9DCD-EDC8E4E51415}" name="XML order #" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{E36A262F-69A4-4276-95F1-0FB7FCE8E2AD}" name="Data Type" dataDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{B4F9F589-759B-40AB-BD12-81562C067103}" name="Optionality" dataDxfId="9"/>
-    <tableColumn id="4" xr3:uid="{29CBFF2E-DC73-4812-9BE8-505CDCED923B}" name="Size" dataDxfId="8"/>
-    <tableColumn id="5" xr3:uid="{2FBE4EBA-0896-4EA8-8E6A-9740D712F4CF}" name="Business Rules" dataDxfId="7"/>
-    <tableColumn id="14" xr3:uid="{F6A291D7-463E-4C10-AE63-F46C62F701F1}" name="User Editable" dataDxfId="6"/>
-    <tableColumn id="6" xr3:uid="{4A3A44E5-9909-437B-9914-BD7AF1AC2439}" name="Generated" dataDxfId="5"/>
-    <tableColumn id="15" xr3:uid="{30410F79-D89B-4BAE-852C-7ADB5287310A}" name="Format" dataDxfId="4"/>
-    <tableColumn id="8" xr3:uid="{23D225B6-A3A4-4446-9AD4-7762B64F46FE}" name="Conditional Formatting" dataDxfId="3"/>
-    <tableColumn id="9" xr3:uid="{27D08B50-8012-49E0-9C10-AEB67B99B91B}" name="Validation" dataDxfId="2"/>
-    <tableColumn id="10" xr3:uid="{A301C8EB-BB2A-4524-AF6E-20714C0D7DD5}" name="Validation Formula" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{9E32B24E-F549-442D-B6C5-5B5E67078170}" name="Title" dataDxfId="15"/>
+    <tableColumn id="12" xr3:uid="{023EA1AA-B7DF-4814-BFEF-5AB9B0752B95}" name="Excel col #" dataDxfId="14"/>
+    <tableColumn id="1" xr3:uid="{5687DF61-58A8-463A-A7F7-9B8B474466F3}" name="CSV Column Name" dataDxfId="13"/>
+    <tableColumn id="13" xr3:uid="{9E799E78-81C7-4788-BF70-799894A0FACA}" name="CSV col #" dataDxfId="12"/>
+    <tableColumn id="16" xr3:uid="{6872DDE9-C4EA-4656-AE08-1B51AE6AE7D6}" name="XML Element" dataDxfId="11"/>
+    <tableColumn id="11" xr3:uid="{F0D84552-7E57-4362-9DCD-EDC8E4E51415}" name="XML order #" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{E36A262F-69A4-4276-95F1-0FB7FCE8E2AD}" name="Data Type" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{B4F9F589-759B-40AB-BD12-81562C067103}" name="Optionality" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{29CBFF2E-DC73-4812-9BE8-505CDCED923B}" name="Size" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{2FBE4EBA-0896-4EA8-8E6A-9740D712F4CF}" name="Business Rules" dataDxfId="6"/>
+    <tableColumn id="14" xr3:uid="{F6A291D7-463E-4C10-AE63-F46C62F701F1}" name="User Editable" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{4A3A44E5-9909-437B-9914-BD7AF1AC2439}" name="Generated" dataDxfId="4"/>
+    <tableColumn id="15" xr3:uid="{30410F79-D89B-4BAE-852C-7ADB5287310A}" name="Format" dataDxfId="3"/>
+    <tableColumn id="8" xr3:uid="{23D225B6-A3A4-4446-9AD4-7762B64F46FE}" name="Conditional Formatting" dataDxfId="2"/>
+    <tableColumn id="9" xr3:uid="{27D08B50-8012-49E0-9C10-AEB67B99B91B}" name="Validation" dataDxfId="1"/>
+    <tableColumn id="10" xr3:uid="{A301C8EB-BB2A-4524-AF6E-20714C0D7DD5}" name="Validation Formula" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight14" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1558,19 +1528,19 @@
         <v>53</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="C1" s="6" t="s">
         <v>106</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="G1" s="6" t="s">
         <v>113</v>
@@ -1617,7 +1587,7 @@
         <v>2</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="F2" s="2">
         <v>4</v>
@@ -1640,44 +1610,46 @@
         <v>103</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>116</v>
+        <v>244</v>
       </c>
       <c r="O2" s="2" t="s">
         <v>84</v>
       </c>
       <c r="P2" s="5" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B3" s="2">
         <v>2</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="7">
-        <v>3</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>185</v>
-      </c>
-      <c r="F3" s="7">
-        <v>3</v>
+        <v>7</v>
+      </c>
+      <c r="D3" s="2">
+        <v>4</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="F3" s="2">
+        <v>5</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>103</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="I3" s="3">
-        <v>20</v>
-      </c>
-      <c r="J3" s="2"/>
+        <v>9</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>51</v>
+      </c>
       <c r="K3" s="2" t="s">
         <v>82</v>
       </c>
@@ -1685,139 +1657,139 @@
       <c r="M3" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="N3" s="2"/>
+      <c r="N3" s="5" t="s">
+        <v>237</v>
+      </c>
       <c r="O3" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="P3" s="2" t="s">
-        <v>85</v>
+      <c r="P3" s="5" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="B4" s="2">
         <v>3</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="2">
-        <v>4</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="F4" s="2">
-        <v>5</v>
+        <v>18</v>
+      </c>
+      <c r="D4" s="7">
+        <v>13</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="F4" s="7">
+        <v>16</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>110</v>
       </c>
       <c r="I4" s="3">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>51</v>
+        <v>19</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>82</v>
       </c>
       <c r="L4" s="2"/>
       <c r="M4" s="2" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="N4" s="5" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="P4" s="5" t="s">
-        <v>210</v>
+        <v>242</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>61</v>
+        <v>91</v>
       </c>
       <c r="B5" s="2">
         <v>4</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="7">
-        <v>5</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>187</v>
-      </c>
-      <c r="F5" s="7">
-        <v>10</v>
+        <v>20</v>
+      </c>
+      <c r="D5" s="2">
+        <v>14</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="F5" s="2">
+        <v>17</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="I5" s="3">
-        <v>1</v>
-      </c>
-      <c r="J5" s="2"/>
+        <v>4</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>205</v>
+      </c>
       <c r="K5" s="2" t="s">
         <v>82</v>
       </c>
       <c r="L5" s="2"/>
       <c r="M5" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="N5" s="5" t="s">
-        <v>233</v>
-      </c>
+        <v>95</v>
+      </c>
+      <c r="N5" s="2"/>
       <c r="O5" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="P5" s="5" t="s">
-        <v>127</v>
+        <v>93</v>
+      </c>
+      <c r="P5" s="2" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="B6" s="2">
         <v>5</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="2">
-        <v>8</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="F6" s="2">
         <v>6</v>
       </c>
+      <c r="D6" s="7">
+        <v>3</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="F6" s="7">
+        <v>3</v>
+      </c>
       <c r="G6" s="2" t="s">
         <v>103</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="I6" s="3">
-        <v>10</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>52</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="J6" s="2"/>
       <c r="K6" s="2" t="s">
         <v>82</v>
       </c>
@@ -1825,34 +1797,32 @@
       <c r="M6" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="N6" s="5" t="s">
-        <v>235</v>
-      </c>
+      <c r="N6" s="2"/>
       <c r="O6" s="2" t="s">
         <v>84</v>
       </c>
       <c r="P6" s="2" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>86</v>
+        <v>61</v>
       </c>
       <c r="B7" s="2">
         <v>6</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D7" s="7">
-        <v>9</v>
-      </c>
-      <c r="E7" s="13" t="s">
-        <v>204</v>
-      </c>
-      <c r="F7" s="13">
-        <v>21</v>
+        <v>5</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="F7" s="7">
+        <v>10</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>103</v>
@@ -1861,11 +1831,9 @@
         <v>110</v>
       </c>
       <c r="I7" s="3">
-        <v>12</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>51</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="J7" s="2"/>
       <c r="K7" s="2" t="s">
         <v>82</v>
       </c>
@@ -1874,33 +1842,33 @@
         <v>103</v>
       </c>
       <c r="N7" s="5" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="O7" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="P7" s="2" t="s">
-        <v>121</v>
+        <v>80</v>
+      </c>
+      <c r="P7" s="5" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="B8" s="2">
         <v>7</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D8" s="2">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="F8" s="2">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>103</v>
@@ -1909,10 +1877,10 @@
         <v>110</v>
       </c>
       <c r="I8" s="3">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>17</v>
+        <v>52</v>
       </c>
       <c r="K8" s="2" t="s">
         <v>82</v>
@@ -1922,107 +1890,109 @@
         <v>103</v>
       </c>
       <c r="N8" s="5" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="O8" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="P8" s="5" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+      <c r="P8" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B9" s="2">
         <v>8</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D9" s="7">
-        <v>13</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>192</v>
-      </c>
-      <c r="F9" s="7">
-        <v>16</v>
+        <v>9</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="F9" s="13">
+        <v>21</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>92</v>
+        <v>103</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>110</v>
       </c>
       <c r="I9" s="3">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>19</v>
+        <v>51</v>
       </c>
       <c r="K9" s="2" t="s">
         <v>82</v>
       </c>
       <c r="L9" s="2"/>
       <c r="M9" s="2" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="N9" s="5" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="O9" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="P9" s="5" t="s">
-        <v>122</v>
+        <v>84</v>
+      </c>
+      <c r="P9" s="2" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B10" s="2">
         <v>9</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D10" s="2">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="F10" s="2">
+        <v>9</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="I10" s="3">
+        <v>1</v>
+      </c>
+      <c r="J10" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="I10" s="3">
-        <v>4</v>
-      </c>
-      <c r="J10" s="2" t="s">
-        <v>209</v>
       </c>
       <c r="K10" s="2" t="s">
         <v>82</v>
       </c>
       <c r="L10" s="2"/>
       <c r="M10" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="N10" s="2"/>
+        <v>103</v>
+      </c>
+      <c r="N10" s="5" t="s">
+        <v>243</v>
+      </c>
       <c r="O10" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="P10" s="2" t="s">
-        <v>128</v>
+        <v>80</v>
+      </c>
+      <c r="P10" s="5" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
@@ -2039,7 +2009,7 @@
         <v>15</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="F11" s="7">
         <v>8</v>
@@ -2062,7 +2032,7 @@
         <v>103</v>
       </c>
       <c r="N11" s="5" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="O11" s="2" t="s">
         <v>80</v>
@@ -2085,7 +2055,7 @@
         <v>16</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="F12" s="6">
         <v>22</v>
@@ -2108,7 +2078,7 @@
         <v>103</v>
       </c>
       <c r="N12" s="4" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="O12" s="2" t="s">
         <v>80</v>
@@ -2131,7 +2101,7 @@
         <v>29</v>
       </c>
       <c r="E13" s="13" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="F13" s="13">
         <v>11</v>
@@ -2156,18 +2126,18 @@
         <v>103</v>
       </c>
       <c r="N13" s="4" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="O13" s="2" t="s">
         <v>78</v>
       </c>
       <c r="P13" s="5" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="14" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B14" s="2">
         <v>13</v>
@@ -2179,7 +2149,7 @@
         <v>30</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="F14" s="6">
         <v>12</v>
@@ -2204,13 +2174,13 @@
         <v>96</v>
       </c>
       <c r="N14" s="4" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="O14" s="2" t="s">
         <v>78</v>
       </c>
       <c r="P14" s="5" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
@@ -2227,7 +2197,7 @@
         <v>17</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="F15" s="7">
         <v>18</v>
@@ -2256,7 +2226,7 @@
         <v>92</v>
       </c>
       <c r="P15" s="5" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
     </row>
     <row r="16" spans="1:16" ht="30" x14ac:dyDescent="0.25">
@@ -2273,7 +2243,7 @@
         <v>18</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="F16" s="6">
         <v>15</v>
@@ -2307,7 +2277,7 @@
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="B17" s="2">
         <v>16</v>
@@ -2319,7 +2289,7 @@
         <v>22</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="F17" s="7">
         <v>19</v>
@@ -2348,12 +2318,12 @@
         <v>101</v>
       </c>
       <c r="P17" s="2" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="B18" s="2">
         <v>17</v>
@@ -2365,7 +2335,7 @@
         <v>23</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="F18" s="7">
         <v>20</v>
@@ -2394,7 +2364,7 @@
         <v>101</v>
       </c>
       <c r="P18" s="2" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="19" spans="1:16" ht="30" x14ac:dyDescent="0.25">
@@ -2409,7 +2379,7 @@
         <v>6</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="F19" s="6">
         <v>1</v>
@@ -2447,7 +2417,7 @@
         <v>7</v>
       </c>
       <c r="E20" s="13" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="F20" s="13">
         <v>2</v>
@@ -2485,7 +2455,7 @@
         <v>11</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="F21" s="7">
         <v>7</v>
@@ -2525,7 +2495,7 @@
         <v>31</v>
       </c>
       <c r="E22" s="13" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="F22" s="13">
         <v>13</v>
@@ -2565,7 +2535,7 @@
         <v>32</v>
       </c>
       <c r="E23" s="13" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="F23" s="13">
         <v>14</v>
@@ -2595,7 +2565,7 @@
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B24" s="7"/>
       <c r="C24" s="7" t="s">
@@ -2641,7 +2611,7 @@
         <v>10</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="F25" s="2"/>
       <c r="G25" s="2" t="s">
@@ -2677,7 +2647,7 @@
         <v>19</v>
       </c>
       <c r="E26" s="13" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="F26" s="13"/>
       <c r="G26" s="2" t="s">
@@ -2713,7 +2683,7 @@
         <v>20</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="F27" s="7"/>
       <c r="G27" s="2" t="s">
@@ -2749,7 +2719,7 @@
         <v>21</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="F28" s="6"/>
       <c r="G28" s="2" t="s">
@@ -2785,7 +2755,7 @@
         <v>24</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="F29" s="7"/>
       <c r="G29" s="2" t="s">
@@ -2821,7 +2791,7 @@
         <v>25</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="F30" s="7"/>
       <c r="G30" s="2" t="s">
@@ -2855,7 +2825,7 @@
         <v>26</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="F31" s="7"/>
       <c r="G31" s="2" t="s">
@@ -2891,7 +2861,7 @@
         <v>27</v>
       </c>
       <c r="E32" s="7" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="F32" s="7"/>
       <c r="G32" s="2" t="s">
@@ -2927,7 +2897,7 @@
         <v>28</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="F33" s="7"/>
       <c r="G33" s="2" t="s">
@@ -2954,22 +2924,22 @@
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
   <conditionalFormatting sqref="D2:F33">
-    <cfRule type="expression" dxfId="55" priority="11">
+    <cfRule type="expression" dxfId="52" priority="11">
       <formula>LEN($D2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C15:O15 A32:P33 A2:B31 C2:P14 C16:P31">
-    <cfRule type="expression" dxfId="54" priority="12">
+  <conditionalFormatting sqref="C15:O15 A32:P33 C16:P31 A11:B31 A2:P10 C11:P14">
+    <cfRule type="expression" dxfId="51" priority="12">
       <formula>$K2="No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2:L33">
-    <cfRule type="expression" dxfId="53" priority="10">
+    <cfRule type="expression" dxfId="50" priority="10">
       <formula>AND($K2="No",LEN($L2)=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P15">
-    <cfRule type="expression" dxfId="52" priority="2">
+    <cfRule type="expression" dxfId="49" priority="2">
       <formula>$K15="No"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3018,19 +2988,19 @@
         <v>53</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="C1" s="6" t="s">
         <v>106</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="G1" s="6" t="s">
         <v>113</v>
@@ -3077,7 +3047,7 @@
         <v>2</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="F2" s="2">
         <v>1</v>
@@ -3092,7 +3062,7 @@
         <v>20</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>82</v>
@@ -3102,126 +3072,126 @@
         <v>103</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="O2" s="2" t="s">
         <v>84</v>
       </c>
       <c r="P2" s="5" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="B3" s="2">
         <v>2</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="D3" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="F3" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>92</v>
+        <v>103</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="I3" s="2">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>82</v>
       </c>
       <c r="L3" s="2"/>
       <c r="M3" s="2" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="N3" s="5" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="P3" s="5" t="s">
-        <v>177</v>
+        <v>206</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="B4" s="2">
         <v>3</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="D4" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="F4" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="I4" s="2">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>82</v>
       </c>
       <c r="L4" s="2"/>
       <c r="M4" s="2" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="N4" s="5" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="P4" s="2" t="s">
-        <v>119</v>
+        <v>78</v>
+      </c>
+      <c r="P4" s="5" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B5" s="2">
         <v>4</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="D5" s="2">
         <v>7</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="F5" s="6">
         <v>12</v>
@@ -3236,7 +3206,7 @@
         <v>4</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="K5" s="2" t="s">
         <v>82</v>
@@ -3246,30 +3216,30 @@
         <v>103</v>
       </c>
       <c r="N5" s="4" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="O5" s="2" t="s">
         <v>80</v>
       </c>
       <c r="P5" s="5" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B6" s="2">
         <v>5</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="D6" s="2">
         <v>8</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="F6" s="2">
         <v>8</v>
@@ -3284,7 +3254,7 @@
         <v>8</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="K6" s="2" t="s">
         <v>82</v>
@@ -3298,24 +3268,24 @@
         <v>92</v>
       </c>
       <c r="P6" s="5" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B7" s="2">
         <v>6</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D7" s="2">
         <v>9</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="F7" s="2">
         <v>9</v>
@@ -3330,7 +3300,7 @@
         <v>4</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="K7" s="2" t="s">
         <v>82</v>
@@ -3344,24 +3314,24 @@
         <v>93</v>
       </c>
       <c r="P7" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="B8" s="2">
         <v>7</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D8" s="2">
         <v>10</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="F8" s="2">
         <v>10</v>
@@ -3376,7 +3346,7 @@
         <v>8</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="K8" s="2" t="s">
         <v>82</v>
@@ -3390,24 +3360,24 @@
         <v>92</v>
       </c>
       <c r="P8" s="5" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="B9" s="2">
         <v>8</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="D9" s="2">
         <v>11</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="F9" s="2">
         <v>11</v>
@@ -3422,7 +3392,7 @@
         <v>4</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="K9" s="2" t="s">
         <v>82</v>
@@ -3436,24 +3406,24 @@
         <v>93</v>
       </c>
       <c r="P9" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="B10" s="2">
         <v>9</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="D10" s="2">
         <v>12</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="F10" s="2">
         <v>17</v>
@@ -3480,24 +3450,24 @@
         <v>92</v>
       </c>
       <c r="P10" s="5" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="B11" s="2">
         <v>10</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="D11" s="2">
         <v>15</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="F11" s="6">
         <v>6</v>
@@ -3512,7 +3482,7 @@
         <v>30</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="K11" s="2" t="s">
         <v>82</v>
@@ -3527,19 +3497,19 @@
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B12" s="2">
         <v>11</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="D12" s="2">
         <v>16</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="F12" s="2">
         <v>7</v>
@@ -3554,7 +3524,7 @@
         <v>9</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="K12" s="2" t="s">
         <v>82</v>
@@ -3568,18 +3538,18 @@
         <v>80</v>
       </c>
       <c r="P12" s="5" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B13" s="2">
         <v>12</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="D13" s="2">
         <v>17</v>
@@ -3596,7 +3566,7 @@
         <v>4</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="K13" s="2" t="s">
         <v>82</v>
@@ -3610,24 +3580,24 @@
         <v>80</v>
       </c>
       <c r="P13" s="5" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="14" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B14" s="2">
         <v>13</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="D14" s="2">
         <v>18</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="F14" s="6">
         <v>13</v>
@@ -3642,7 +3612,7 @@
         <v>1</v>
       </c>
       <c r="J14" s="5" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="K14" s="2" t="s">
         <v>82</v>
@@ -3652,45 +3622,45 @@
         <v>103</v>
       </c>
       <c r="N14" s="5" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="O14" s="2" t="s">
         <v>80</v>
       </c>
       <c r="P14" s="5" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="15" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B15" s="2">
         <v>14</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D15" s="2">
         <v>28</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="F15" s="6">
         <v>14</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="H15" s="2" t="s">
         <v>109</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="K15" s="2" t="s">
         <v>82</v>
@@ -3698,30 +3668,30 @@
       <c r="L15" s="2"/>
       <c r="M15" s="2"/>
       <c r="N15" s="4" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="O15" s="2" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="P15" s="2" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="16" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="B16" s="2">
         <v>15</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D16" s="2">
         <v>27</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="F16" s="6">
         <v>16</v>
@@ -3736,7 +3706,7 @@
         <v>9</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="K16" s="2" t="s">
         <v>82</v>
@@ -3746,30 +3716,30 @@
         <v>103</v>
       </c>
       <c r="N16" s="4" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="O16" s="2" t="s">
         <v>80</v>
       </c>
       <c r="P16" s="5" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="17" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="B17" s="2">
         <v>16</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="D17" s="2">
         <v>20</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="F17" s="6">
         <v>15</v>
@@ -3784,7 +3754,7 @@
         <v>10</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="K17" s="2" t="s">
         <v>82</v>
@@ -3794,13 +3764,13 @@
         <v>103</v>
       </c>
       <c r="N17" s="4" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="O17" s="2" t="s">
         <v>80</v>
       </c>
       <c r="P17" s="5" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="18" spans="1:16" ht="45" x14ac:dyDescent="0.25">
@@ -3815,7 +3785,7 @@
         <v>5</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="F18" s="6">
         <v>4</v>
@@ -3853,7 +3823,7 @@
         <v>6</v>
       </c>
       <c r="E19" s="13" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="F19" s="13">
         <v>5</v>
@@ -3881,17 +3851,17 @@
     </row>
     <row r="20" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" s="2" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="D20" s="2">
         <v>13</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="F20" s="6">
         <v>18</v>
@@ -3906,13 +3876,13 @@
         <v>1</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="K20" s="2" t="s">
         <v>81</v>
       </c>
       <c r="L20" s="2" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="M20" s="2"/>
       <c r="N20" s="2"/>
@@ -3921,7 +3891,7 @@
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="2" t="s">
@@ -3942,13 +3912,13 @@
         <v>20</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="K21" s="2" t="s">
         <v>81</v>
       </c>
       <c r="L21" s="2" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="M21" s="2"/>
       <c r="N21" s="2"/>
@@ -3957,11 +3927,11 @@
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" s="2" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="D22" s="2">
         <v>14</v>
@@ -3991,78 +3961,68 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="L2:L22">
-    <cfRule type="expression" dxfId="33" priority="15">
+    <cfRule type="expression" dxfId="30" priority="16">
       <formula>AND($K2="No",LEN($L2)=0)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:F5 D6:D7 D8:F22">
-    <cfRule type="expression" dxfId="32" priority="16">
+  <conditionalFormatting sqref="D6:D7 D8:F22 D2:F5">
+    <cfRule type="expression" dxfId="29" priority="17">
       <formula>LEN($D2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O4:P4 O8:P8 O19:P19 A2:A22 C20:P22 C11:P11 C9:N9 C8:M8 C3:M5 C6:D7 C2:P2 C10:I10 K10:P10 C13:P18 C12:I12 K12:P12 G6:P7 C19:M19">
-    <cfRule type="expression" dxfId="31" priority="17">
+  <conditionalFormatting sqref="O8:P8 O19:P19 C20:P22 C11:P11 C9:N9 C8:M8 C6:D7 C10:I10 K10:P10 C13:P18 C12:I12 K12:P12 G6:P7 C19:M19 C5:N5 C2:P2 A2:B22 C3:M4 O3:P3">
+    <cfRule type="expression" dxfId="28" priority="18">
       <formula>$K2="No"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N3">
-    <cfRule type="expression" dxfId="30" priority="14">
-      <formula>$K3="No"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N4:N5">
-    <cfRule type="expression" dxfId="29" priority="12">
-      <formula>$K4="No"</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="O5:P5">
-    <cfRule type="expression" dxfId="28" priority="11">
+    <cfRule type="expression" dxfId="27" priority="12">
       <formula>$K5="No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O9:P9">
-    <cfRule type="expression" dxfId="26" priority="9">
+    <cfRule type="expression" dxfId="26" priority="10">
       <formula>$K9="No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N19">
-    <cfRule type="expression" dxfId="25" priority="8">
+    <cfRule type="expression" dxfId="25" priority="9">
       <formula>$K19="No"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:B22">
+  <conditionalFormatting sqref="J10">
     <cfRule type="expression" dxfId="24" priority="7">
-      <formula>$K2="No"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J10">
-    <cfRule type="expression" dxfId="23" priority="6">
       <formula>$K10="No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J12">
-    <cfRule type="expression" dxfId="22" priority="5">
+    <cfRule type="expression" dxfId="23" priority="6">
       <formula>$K12="No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6:F7">
-    <cfRule type="expression" dxfId="21" priority="3">
+    <cfRule type="expression" dxfId="22" priority="4">
       <formula>LEN($D6)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6:F7">
-    <cfRule type="expression" dxfId="20" priority="4">
+    <cfRule type="expression" dxfId="21" priority="5">
       <formula>$K6="No"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O3:P3">
-    <cfRule type="expression" dxfId="19" priority="2">
-      <formula>$K3="No"</formula>
+  <conditionalFormatting sqref="O4:P4">
+    <cfRule type="expression" dxfId="20" priority="3">
+      <formula>$K4="No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N8">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="19" priority="2">
       <formula>$K8="No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N3:N4">
+    <cfRule type="expression" dxfId="18" priority="1">
+      <formula>$K3="No"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Combine Sample & Result tables; Separate T. Coliform and E. coli columns
#16
</commit_message>
<xml_diff>
--- a/specs/Coliform-column-definitions.xlsx
+++ b/specs/Coliform-column-definitions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\xl-ese\specs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3140C3C9-AFE2-4D74-AEAB-B5315987C42A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B469741-0FE5-40BE-898D-8A7B910ED9D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="4305" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Coliform Sample" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="263">
   <si>
     <t>Optionality</t>
   </si>
@@ -549,9 +549,6 @@
     <t>B_ANALYSIS_COMPLETE_TIME</t>
   </si>
   <si>
-    <t>&gt;= MAX(RC2,RC5)</t>
-  </si>
-  <si>
     <t>MM/DD/YYYY
 Sample will be rejected if Analysis Completion Date is supplied but is prior to Sample Collection Date.  Sample will also be rejected if both Analysis Start and Completion Dates are supplied, but Completion Date is prior to Start Date.</t>
   </si>
@@ -578,9 +575,6 @@
     <t>Analysis Start Date</t>
   </si>
   <si>
-    <t>=AnalyteList</t>
-  </si>
-  <si>
     <t>3100 = Total Coliform
 3014 = E. Coli</t>
   </si>
@@ -602,9 +596,6 @@
   </si>
   <si>
     <t>"result"</t>
-  </si>
-  <si>
-    <t>RC8 &lt;= x &lt;= TODAY()</t>
   </si>
   <si>
     <t>Excel col #</t>
@@ -781,17 +772,6 @@
     <t>=LEN(RC6)=0</t>
   </si>
   <si>
-    <t>=LEN(RC10)=0</t>
-  </si>
-  <si>
-    <t>=LEN(RC1)=0
-=COUNTIFS(R6C1:R6C1,RC1,R6C4:R6C4,RC4)&gt;1</t>
-  </si>
-  <si>
-    <t>=LEN(RC4)=0
-=COUNTIFS(R6C1:R6C1,RC1,R6C4:R6C4,RC4)&gt;1</t>
-  </si>
-  <si>
     <t>=LEN(RC2)=0</t>
   </si>
   <si>
@@ -845,6 +825,63 @@
   <si>
     <t>=AND(RC6="Repeat",LEN(RC9)=0)
 =AND(RC6&lt;&gt;"",RC6&lt;&gt;"Repeat")</t>
+  </si>
+  <si>
+    <t>[1]</t>
+  </si>
+  <si>
+    <t>[2]</t>
+  </si>
+  <si>
+    <t>[3]</t>
+  </si>
+  <si>
+    <t>"3100" or "3014"</t>
+  </si>
+  <si>
+    <t>=LEN(RC14)=0</t>
+  </si>
+  <si>
+    <t>Required</t>
+  </si>
+  <si>
+    <t>=LEN(RC13)=0</t>
+  </si>
+  <si>
+    <t>Microbe Presence E</t>
+  </si>
+  <si>
+    <t>Analytical Method E</t>
+  </si>
+  <si>
+    <t>Analysis Start Date E</t>
+  </si>
+  <si>
+    <t>Analysis Start Time E</t>
+  </si>
+  <si>
+    <t>Analysis End Date E</t>
+  </si>
+  <si>
+    <t>Analysis End Time E</t>
+  </si>
+  <si>
+    <t>=AND(LEN(RC13)="Present",LEN(RC19)=0)</t>
+  </si>
+  <si>
+    <t>=AND(LEN(RC13)="Present",LEN(RC20)=0)</t>
+  </si>
+  <si>
+    <t>RC3 &lt;= x &lt;= TODAY()</t>
+  </si>
+  <si>
+    <t>&gt;= RC3</t>
+  </si>
+  <si>
+    <t>&gt;= MAX(RC3,RC15)</t>
+  </si>
+  <si>
+    <t>&gt;= MAX(RC3,RC21)</t>
   </si>
 </sst>
 </file>
@@ -931,7 +968,28 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="68">
+  <dxfs count="44">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -942,6 +1000,13 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor theme="0" tint="-0.14996795556505021"/>
         </patternFill>
       </fill>
@@ -956,203 +1021,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1295,54 +1164,54 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{636125F0-68A9-4682-81D8-01BD3AB67D26}" name="Table1" displayName="Table1" ref="A1:P33" totalsRowShown="0" headerRowDxfId="67" dataDxfId="66">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{636125F0-68A9-4682-81D8-01BD3AB67D26}" name="Table1" displayName="Table1" ref="A1:P33" totalsRowShown="0" headerRowDxfId="43" dataDxfId="42">
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:P33">
     <sortCondition ref="B2:B33"/>
   </sortState>
   <tableColumns count="16">
-    <tableColumn id="6" xr3:uid="{57EF6AB6-6C4C-4170-BD9B-BF376C46C5DF}" name="Title" dataDxfId="65"/>
-    <tableColumn id="12" xr3:uid="{BFDB40C3-C9ED-4560-81A1-344ECAE248C8}" name="Excel col #" dataDxfId="64"/>
-    <tableColumn id="1" xr3:uid="{3193A6D3-813B-4494-AEED-01D6509FCA0D}" name="CSV Column Name" dataDxfId="63"/>
-    <tableColumn id="11" xr3:uid="{057EA208-1889-4E3C-A179-F312337D9867}" name="CSV col #" dataDxfId="62"/>
-    <tableColumn id="16" xr3:uid="{1F4E7FF6-264D-41DA-AC14-BAA45F3439C7}" name="XML Element" dataDxfId="61"/>
-    <tableColumn id="10" xr3:uid="{F503FCB6-1F5D-4765-B4AB-F67230BC37A3}" name="XML order #" dataDxfId="60"/>
-    <tableColumn id="2" xr3:uid="{5C52F15D-4AC8-44CE-A401-3402D3CD4152}" name="Data Type" dataDxfId="59"/>
-    <tableColumn id="3" xr3:uid="{FFD71D9C-951A-4BB1-9000-9A1C4C3F71D3}" name="Optionality" dataDxfId="58"/>
-    <tableColumn id="4" xr3:uid="{6FEED7B4-CF3F-4593-BB9F-5CFA5FA5B692}" name="Size" dataDxfId="57"/>
-    <tableColumn id="5" xr3:uid="{563427BF-63BA-491F-9B6F-4E02453C643B}" name="Business Rules" dataDxfId="56"/>
-    <tableColumn id="9" xr3:uid="{A9E34622-C2B4-476B-A018-EABC1256DC10}" name="User Editable" dataDxfId="55"/>
-    <tableColumn id="14" xr3:uid="{9DA3EF2F-E261-414A-B10C-F88F2052640F}" name="Generated" dataDxfId="54"/>
-    <tableColumn id="15" xr3:uid="{AA61284F-4409-4E18-9405-8F2EAA78028A}" name="Format" dataDxfId="53"/>
-    <tableColumn id="13" xr3:uid="{94BA7C53-9CFA-4072-B1A4-7E9CE9D9DDF7}" name="Conditional Formatting" dataDxfId="52"/>
-    <tableColumn id="7" xr3:uid="{22AE72C5-BA89-443A-81AF-BCF4B114454C}" name="Validation" dataDxfId="51"/>
-    <tableColumn id="8" xr3:uid="{5DE66E18-4141-4BDD-B41D-2782AC810F6E}" name="Validation Formula" dataDxfId="50"/>
+    <tableColumn id="6" xr3:uid="{57EF6AB6-6C4C-4170-BD9B-BF376C46C5DF}" name="Title" dataDxfId="41"/>
+    <tableColumn id="12" xr3:uid="{BFDB40C3-C9ED-4560-81A1-344ECAE248C8}" name="Excel col #" dataDxfId="40"/>
+    <tableColumn id="1" xr3:uid="{3193A6D3-813B-4494-AEED-01D6509FCA0D}" name="CSV Column Name" dataDxfId="39"/>
+    <tableColumn id="11" xr3:uid="{057EA208-1889-4E3C-A179-F312337D9867}" name="CSV col #" dataDxfId="38"/>
+    <tableColumn id="16" xr3:uid="{1F4E7FF6-264D-41DA-AC14-BAA45F3439C7}" name="XML Element" dataDxfId="37"/>
+    <tableColumn id="10" xr3:uid="{F503FCB6-1F5D-4765-B4AB-F67230BC37A3}" name="XML order #" dataDxfId="36"/>
+    <tableColumn id="2" xr3:uid="{5C52F15D-4AC8-44CE-A401-3402D3CD4152}" name="Data Type" dataDxfId="35"/>
+    <tableColumn id="3" xr3:uid="{FFD71D9C-951A-4BB1-9000-9A1C4C3F71D3}" name="Optionality" dataDxfId="34"/>
+    <tableColumn id="4" xr3:uid="{6FEED7B4-CF3F-4593-BB9F-5CFA5FA5B692}" name="Size" dataDxfId="33"/>
+    <tableColumn id="5" xr3:uid="{563427BF-63BA-491F-9B6F-4E02453C643B}" name="Business Rules" dataDxfId="32"/>
+    <tableColumn id="9" xr3:uid="{A9E34622-C2B4-476B-A018-EABC1256DC10}" name="User Editable" dataDxfId="31"/>
+    <tableColumn id="14" xr3:uid="{9DA3EF2F-E261-414A-B10C-F88F2052640F}" name="Generated" dataDxfId="30"/>
+    <tableColumn id="15" xr3:uid="{AA61284F-4409-4E18-9405-8F2EAA78028A}" name="Format" dataDxfId="29"/>
+    <tableColumn id="13" xr3:uid="{94BA7C53-9CFA-4072-B1A4-7E9CE9D9DDF7}" name="Conditional Formatting" dataDxfId="28"/>
+    <tableColumn id="7" xr3:uid="{22AE72C5-BA89-443A-81AF-BCF4B114454C}" name="Validation" dataDxfId="27"/>
+    <tableColumn id="8" xr3:uid="{5DE66E18-4141-4BDD-B41D-2782AC810F6E}" name="Validation Formula" dataDxfId="26"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{05345577-AC31-4B6D-B899-55D66DEB1874}" name="Table2" displayName="Table2" ref="A1:P22" totalsRowShown="0" headerRowDxfId="49" dataDxfId="48">
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:P22">
-    <sortCondition ref="B2:B22"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{05345577-AC31-4B6D-B899-55D66DEB1874}" name="Table2" displayName="Table2" ref="A1:P28" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:P28">
+    <sortCondition ref="B2:B28"/>
   </sortState>
   <tableColumns count="16">
-    <tableColumn id="7" xr3:uid="{9E32B24E-F549-442D-B6C5-5B5E67078170}" name="Title" dataDxfId="47"/>
-    <tableColumn id="12" xr3:uid="{023EA1AA-B7DF-4814-BFEF-5AB9B0752B95}" name="Excel col #" dataDxfId="46"/>
-    <tableColumn id="1" xr3:uid="{5687DF61-58A8-463A-A7F7-9B8B474466F3}" name="CSV Column Name" dataDxfId="45"/>
-    <tableColumn id="13" xr3:uid="{9E799E78-81C7-4788-BF70-799894A0FACA}" name="CSV col #" dataDxfId="44"/>
-    <tableColumn id="16" xr3:uid="{6872DDE9-C4EA-4656-AE08-1B51AE6AE7D6}" name="XML Element" dataDxfId="43"/>
-    <tableColumn id="11" xr3:uid="{F0D84552-7E57-4362-9DCD-EDC8E4E51415}" name="XML order #" dataDxfId="42"/>
-    <tableColumn id="2" xr3:uid="{E36A262F-69A4-4276-95F1-0FB7FCE8E2AD}" name="Data Type" dataDxfId="41"/>
-    <tableColumn id="3" xr3:uid="{B4F9F589-759B-40AB-BD12-81562C067103}" name="Optionality" dataDxfId="40"/>
-    <tableColumn id="4" xr3:uid="{29CBFF2E-DC73-4812-9BE8-505CDCED923B}" name="Size" dataDxfId="39"/>
-    <tableColumn id="5" xr3:uid="{2FBE4EBA-0896-4EA8-8E6A-9740D712F4CF}" name="Business Rules" dataDxfId="38"/>
-    <tableColumn id="14" xr3:uid="{F6A291D7-463E-4C10-AE63-F46C62F701F1}" name="User Editable" dataDxfId="37"/>
-    <tableColumn id="6" xr3:uid="{4A3A44E5-9909-437B-9914-BD7AF1AC2439}" name="Generated" dataDxfId="36"/>
-    <tableColumn id="15" xr3:uid="{30410F79-D89B-4BAE-852C-7ADB5287310A}" name="Format" dataDxfId="35"/>
-    <tableColumn id="8" xr3:uid="{23D225B6-A3A4-4446-9AD4-7762B64F46FE}" name="Conditional Formatting" dataDxfId="34"/>
-    <tableColumn id="9" xr3:uid="{27D08B50-8012-49E0-9C10-AEB67B99B91B}" name="Validation" dataDxfId="33"/>
-    <tableColumn id="10" xr3:uid="{A301C8EB-BB2A-4524-AF6E-20714C0D7DD5}" name="Validation Formula" dataDxfId="32"/>
+    <tableColumn id="7" xr3:uid="{9E32B24E-F549-442D-B6C5-5B5E67078170}" name="Title" dataDxfId="23"/>
+    <tableColumn id="12" xr3:uid="{023EA1AA-B7DF-4814-BFEF-5AB9B0752B95}" name="Excel col #" dataDxfId="22"/>
+    <tableColumn id="1" xr3:uid="{5687DF61-58A8-463A-A7F7-9B8B474466F3}" name="CSV Column Name" dataDxfId="21"/>
+    <tableColumn id="13" xr3:uid="{9E799E78-81C7-4788-BF70-799894A0FACA}" name="CSV col #" dataDxfId="20"/>
+    <tableColumn id="16" xr3:uid="{6872DDE9-C4EA-4656-AE08-1B51AE6AE7D6}" name="XML Element" dataDxfId="19"/>
+    <tableColumn id="11" xr3:uid="{F0D84552-7E57-4362-9DCD-EDC8E4E51415}" name="XML order #" dataDxfId="18"/>
+    <tableColumn id="2" xr3:uid="{E36A262F-69A4-4276-95F1-0FB7FCE8E2AD}" name="Data Type" dataDxfId="17"/>
+    <tableColumn id="3" xr3:uid="{B4F9F589-759B-40AB-BD12-81562C067103}" name="Optionality" dataDxfId="16"/>
+    <tableColumn id="4" xr3:uid="{29CBFF2E-DC73-4812-9BE8-505CDCED923B}" name="Size" dataDxfId="15"/>
+    <tableColumn id="5" xr3:uid="{2FBE4EBA-0896-4EA8-8E6A-9740D712F4CF}" name="Business Rules" dataDxfId="14"/>
+    <tableColumn id="14" xr3:uid="{F6A291D7-463E-4C10-AE63-F46C62F701F1}" name="User Editable" dataDxfId="13"/>
+    <tableColumn id="6" xr3:uid="{4A3A44E5-9909-437B-9914-BD7AF1AC2439}" name="Generated" dataDxfId="12"/>
+    <tableColumn id="15" xr3:uid="{30410F79-D89B-4BAE-852C-7ADB5287310A}" name="Format" dataDxfId="11"/>
+    <tableColumn id="8" xr3:uid="{23D225B6-A3A4-4446-9AD4-7762B64F46FE}" name="Conditional Formatting" dataDxfId="10"/>
+    <tableColumn id="9" xr3:uid="{27D08B50-8012-49E0-9C10-AEB67B99B91B}" name="Validation" dataDxfId="9"/>
+    <tableColumn id="10" xr3:uid="{A301C8EB-BB2A-4524-AF6E-20714C0D7DD5}" name="Validation Formula" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight14" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1614,11 +1483,11 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:P33"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="N15" sqref="N15"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1650,7 +1519,7 @@
         <v>53</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C1" s="6" t="s">
         <v>106</v>
@@ -1659,10 +1528,10 @@
         <v>116</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="G1" s="6" t="s">
         <v>113</v>
@@ -1709,7 +1578,7 @@
         <v>2</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="F2" s="2">
         <v>4</v>
@@ -1732,13 +1601,13 @@
         <v>103</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="O2" s="2" t="s">
         <v>84</v>
       </c>
       <c r="P2" s="5" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
@@ -1755,7 +1624,7 @@
         <v>4</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="F3" s="2">
         <v>5</v>
@@ -1780,13 +1649,13 @@
         <v>103</v>
       </c>
       <c r="N3" s="5" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="O3" s="2" t="s">
         <v>84</v>
       </c>
       <c r="P3" s="5" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
@@ -1803,7 +1672,7 @@
         <v>13</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="F4" s="7">
         <v>16</v>
@@ -1828,13 +1697,13 @@
         <v>96</v>
       </c>
       <c r="N4" s="5" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="O4" s="2" t="s">
         <v>78</v>
       </c>
       <c r="P4" s="5" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
@@ -1851,7 +1720,7 @@
         <v>14</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="F5" s="2">
         <v>17</v>
@@ -1866,7 +1735,7 @@
         <v>4</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="K5" s="2" t="s">
         <v>82</v>
@@ -1895,7 +1764,7 @@
         <v>3</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="F6" s="7">
         <v>3</v>
@@ -1911,7 +1780,7 @@
       </c>
       <c r="J6" s="2"/>
       <c r="K6" s="2" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="L6" s="11" t="s">
         <v>87</v>
@@ -1939,7 +1808,7 @@
         <v>5</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="F7" s="7">
         <v>10</v>
@@ -1955,10 +1824,10 @@
       </c>
       <c r="J7" s="2"/>
       <c r="K7" s="2" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="M7" s="2" t="s">
         <v>103</v>
@@ -1983,7 +1852,7 @@
         <v>8</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="F8" s="2">
         <v>6</v>
@@ -2001,10 +1870,10 @@
         <v>52</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="L8" s="5" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="M8" s="2" t="s">
         <v>103</v>
@@ -2031,7 +1900,7 @@
         <v>9</v>
       </c>
       <c r="E9" s="13" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="F9" s="13">
         <v>21</v>
@@ -2056,7 +1925,7 @@
         <v>103</v>
       </c>
       <c r="N9" s="5" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="O9" s="2" t="s">
         <v>84</v>
@@ -2077,7 +1946,7 @@
         <v>12</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="F10" s="2">
         <v>9</v>
@@ -2095,10 +1964,10 @@
         <v>17</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="M10" s="2" t="s">
         <v>103</v>
@@ -2125,7 +1994,7 @@
         <v>15</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="F11" s="7">
         <v>8</v>
@@ -2148,7 +2017,7 @@
         <v>103</v>
       </c>
       <c r="N11" s="5" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="O11" s="2" t="s">
         <v>80</v>
@@ -2171,7 +2040,7 @@
         <v>16</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="F12" s="6">
         <v>22</v>
@@ -2194,7 +2063,7 @@
         <v>103</v>
       </c>
       <c r="N12" s="4" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="O12" s="2" t="s">
         <v>80</v>
@@ -2217,7 +2086,7 @@
         <v>29</v>
       </c>
       <c r="E13" s="13" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="F13" s="13">
         <v>11</v>
@@ -2242,7 +2111,7 @@
         <v>103</v>
       </c>
       <c r="N13" s="4" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="O13" s="2" t="s">
         <v>78</v>
@@ -2265,7 +2134,7 @@
         <v>30</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="F14" s="6">
         <v>12</v>
@@ -2290,7 +2159,7 @@
         <v>96</v>
       </c>
       <c r="N14" s="4" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="O14" s="2" t="s">
         <v>78</v>
@@ -2313,7 +2182,7 @@
         <v>17</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="F15" s="7">
         <v>18</v>
@@ -2342,7 +2211,7 @@
         <v>92</v>
       </c>
       <c r="P15" s="5" t="s">
-        <v>177</v>
+        <v>259</v>
       </c>
     </row>
     <row r="16" spans="1:16" ht="30" x14ac:dyDescent="0.25">
@@ -2359,7 +2228,7 @@
         <v>18</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="F16" s="6">
         <v>15</v>
@@ -2393,7 +2262,7 @@
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="B17" s="2">
         <v>12</v>
@@ -2405,7 +2274,7 @@
         <v>22</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="F17" s="7">
         <v>19</v>
@@ -2439,7 +2308,7 @@
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" s="2" t="s">
@@ -2449,7 +2318,7 @@
         <v>23</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="F18" s="7">
         <v>20</v>
@@ -2467,7 +2336,7 @@
         <v>37</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="L18" s="11" t="s">
         <v>87</v>
@@ -2495,7 +2364,7 @@
         <v>6</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="F19" s="6">
         <v>1</v>
@@ -2533,7 +2402,7 @@
         <v>7</v>
       </c>
       <c r="E20" s="13" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="F20" s="13">
         <v>2</v>
@@ -2571,7 +2440,7 @@
         <v>11</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="F21" s="7">
         <v>7</v>
@@ -2611,7 +2480,7 @@
         <v>31</v>
       </c>
       <c r="E22" s="13" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="F22" s="13">
         <v>13</v>
@@ -2651,7 +2520,7 @@
         <v>32</v>
       </c>
       <c r="E23" s="13" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="F23" s="13">
         <v>14</v>
@@ -2727,7 +2596,7 @@
         <v>10</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="F25" s="2"/>
       <c r="G25" s="2" t="s">
@@ -2763,7 +2632,7 @@
         <v>19</v>
       </c>
       <c r="E26" s="13" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="F26" s="13"/>
       <c r="G26" s="2" t="s">
@@ -2799,7 +2668,7 @@
         <v>20</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="F27" s="7"/>
       <c r="G27" s="2" t="s">
@@ -2835,7 +2704,7 @@
         <v>21</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="F28" s="6"/>
       <c r="G28" s="2" t="s">
@@ -2871,7 +2740,7 @@
         <v>24</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="F29" s="7"/>
       <c r="G29" s="2" t="s">
@@ -2907,7 +2776,7 @@
         <v>25</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="F30" s="7"/>
       <c r="G30" s="2" t="s">
@@ -2941,7 +2810,7 @@
         <v>26</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="F31" s="7"/>
       <c r="G31" s="2" t="s">
@@ -2977,7 +2846,7 @@
         <v>27</v>
       </c>
       <c r="E32" s="7" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="F32" s="7"/>
       <c r="G32" s="2" t="s">
@@ -3013,7 +2882,7 @@
         <v>28</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="F33" s="7"/>
       <c r="G33" s="2" t="s">
@@ -3040,20 +2909,20 @@
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
   <conditionalFormatting sqref="D2:F33">
-    <cfRule type="expression" dxfId="4" priority="12">
+    <cfRule type="expression" dxfId="7" priority="12">
       <formula>LEN($D2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:P33">
+    <cfRule type="expression" dxfId="6" priority="1">
+      <formula>$K2="Skip"</formula>
+    </cfRule>
     <cfRule type="expression" dxfId="5" priority="13">
       <formula>$K2="No"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="1">
-      <formula>$K2="Skip"</formula>
-    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2:L33">
-    <cfRule type="expression" dxfId="6" priority="11">
+    <cfRule type="expression" dxfId="4" priority="11">
       <formula>AND($K2&lt;&gt;"Yes",LEN($L2)=0)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3068,13 +2937,13 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15FEC0F5-029A-4987-81C0-EA7F2B314198}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:P22"/>
+  <dimension ref="A1:P28"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="N11" sqref="N11"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3088,9 +2957,9 @@
     <col min="7" max="7" width="8.28515625" customWidth="1"/>
     <col min="8" max="8" width="11.28515625" customWidth="1"/>
     <col min="9" max="9" width="5.42578125" customWidth="1"/>
-    <col min="10" max="10" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.5703125" customWidth="1"/>
     <col min="11" max="11" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.5703125" customWidth="1"/>
+    <col min="12" max="12" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="25.140625" customWidth="1"/>
     <col min="14" max="14" width="41.85546875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="10.140625" customWidth="1"/>
@@ -3102,7 +2971,7 @@
         <v>53</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C1" s="6" t="s">
         <v>106</v>
@@ -3111,10 +2980,10 @@
         <v>116</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="G1" s="6" t="s">
         <v>113</v>
@@ -3147,12 +3016,12 @@
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B2" s="2">
-        <v>1</v>
+      <c r="B2" s="3" t="s">
+        <v>244</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>5</v>
@@ -3161,7 +3030,7 @@
         <v>2</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="F2" s="2">
         <v>1</v>
@@ -3176,7 +3045,7 @@
         <v>20</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>82</v>
@@ -3185,22 +3054,16 @@
       <c r="M2" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="N2" s="4" t="s">
-        <v>232</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="P2" s="5" t="s">
-        <v>228</v>
-      </c>
+      <c r="N2" s="4"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="5"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B3" s="2">
-        <v>2</v>
+      <c r="B3" s="3" t="s">
+        <v>245</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>7</v>
@@ -3209,7 +3072,7 @@
         <v>4</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="F3" s="2">
         <v>2</v>
@@ -3224,7 +3087,7 @@
         <v>9</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>82</v>
@@ -3233,22 +3096,16 @@
       <c r="M3" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="N3" s="5" t="s">
-        <v>234</v>
-      </c>
-      <c r="O3" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="P3" s="5" t="s">
-        <v>206</v>
-      </c>
+      <c r="N3" s="5"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="5"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="B4" s="2">
-        <v>3</v>
+      <c r="B4" s="3" t="s">
+        <v>246</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>18</v>
@@ -3257,7 +3114,7 @@
         <v>3</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="F4" s="2">
         <v>3</v>
@@ -3272,7 +3129,7 @@
         <v>8</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>82</v>
@@ -3281,31 +3138,23 @@
       <c r="M4" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="N4" s="5" t="s">
-        <v>229</v>
-      </c>
-      <c r="O4" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="P4" s="5" t="s">
-        <v>238</v>
-      </c>
+      <c r="N4" s="5"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="5"/>
     </row>
     <row r="5" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="B5" s="2">
-        <v>4</v>
-      </c>
+        <v>170</v>
+      </c>
+      <c r="B5" s="2"/>
       <c r="C5" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D5" s="2">
         <v>7</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="F5" s="6">
         <v>12</v>
@@ -3319,136 +3168,132 @@
       <c r="I5" s="2">
         <v>4</v>
       </c>
-      <c r="J5" s="2" t="s">
-        <v>170</v>
+      <c r="J5" s="6" t="s">
+        <v>168</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="L5" s="2"/>
+        <v>81</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>247</v>
+      </c>
       <c r="M5" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="N5" s="4" t="s">
-        <v>233</v>
-      </c>
-      <c r="O5" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="P5" s="5" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N5" s="4"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="5"/>
+    </row>
+    <row r="6" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>168</v>
+        <v>141</v>
       </c>
       <c r="B6" s="2">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>167</v>
+        <v>140</v>
       </c>
       <c r="D6" s="2">
-        <v>8</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="F6" s="2">
-        <v>8</v>
+        <v>18</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>223</v>
+      </c>
+      <c r="F6" s="6">
+        <v>13</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>92</v>
+        <v>103</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="I6" s="2">
-        <v>8</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>166</v>
+        <v>1</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>139</v>
       </c>
       <c r="K6" s="2" t="s">
         <v>82</v>
       </c>
       <c r="L6" s="2"/>
       <c r="M6" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="N6" s="5"/>
+        <v>103</v>
+      </c>
+      <c r="N6" s="5" t="s">
+        <v>250</v>
+      </c>
       <c r="O6" s="2" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="P6" s="5" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>164</v>
+        <v>221</v>
       </c>
       <c r="B7" s="2">
+        <v>14</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="D7" s="2">
+        <v>15</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="F7" s="6">
         <v>6</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="D7" s="2">
-        <v>9</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="F7" s="2">
-        <v>9</v>
-      </c>
       <c r="G7" s="2" t="s">
-        <v>93</v>
+        <v>103</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>112</v>
+        <v>249</v>
       </c>
       <c r="I7" s="2">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>205</v>
+        <v>149</v>
       </c>
       <c r="K7" s="2" t="s">
         <v>82</v>
       </c>
       <c r="L7" s="2"/>
       <c r="M7" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="N7" s="2"/>
-      <c r="O7" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="P7" s="2" t="s">
-        <v>125</v>
-      </c>
+        <v>103</v>
+      </c>
+      <c r="N7" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>207</v>
+        <v>167</v>
       </c>
       <c r="B8" s="2">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="D8" s="2">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="F8" s="2">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>92</v>
@@ -3460,7 +3305,7 @@
         <v>8</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="K8" s="2" t="s">
         <v>82</v>
@@ -3474,27 +3319,27 @@
         <v>92</v>
       </c>
       <c r="P8" s="5" t="s">
-        <v>160</v>
+        <v>260</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>208</v>
+        <v>163</v>
       </c>
       <c r="B9" s="2">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="D9" s="2">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="F9" s="2">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>93</v>
@@ -3506,7 +3351,7 @@
         <v>4</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="K9" s="2" t="s">
         <v>82</v>
@@ -3525,20 +3370,22 @@
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="B10" s="2"/>
+        <v>204</v>
+      </c>
+      <c r="B10" s="2">
+        <v>17</v>
+      </c>
       <c r="C10" s="2" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="D10" s="2">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="F10" s="2">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>92</v>
@@ -3549,13 +3396,13 @@
       <c r="I10" s="2">
         <v>8</v>
       </c>
-      <c r="J10" s="2"/>
+      <c r="J10" s="2" t="s">
+        <v>160</v>
+      </c>
       <c r="K10" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="L10" s="5" t="s">
-        <v>244</v>
-      </c>
+        <v>82</v>
+      </c>
+      <c r="L10" s="2"/>
       <c r="M10" s="2" t="s">
         <v>96</v>
       </c>
@@ -3564,494 +3411,526 @@
         <v>92</v>
       </c>
       <c r="P10" s="5" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>224</v>
+        <v>205</v>
       </c>
       <c r="B11" s="2">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>150</v>
+        <v>159</v>
       </c>
       <c r="D11" s="2">
-        <v>15</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>223</v>
-      </c>
-      <c r="F11" s="6">
-        <v>6</v>
+        <v>11</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="F11" s="2">
+        <v>11</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>112</v>
       </c>
       <c r="I11" s="2">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>149</v>
+        <v>202</v>
       </c>
       <c r="K11" s="2" t="s">
         <v>82</v>
       </c>
       <c r="L11" s="2"/>
       <c r="M11" s="2" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="N11" s="2"/>
-      <c r="O11" s="2"/>
-      <c r="P11" s="2"/>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O11" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="P11" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="B12" s="2"/>
+        <v>251</v>
+      </c>
+      <c r="B12" s="2">
+        <v>19</v>
+      </c>
       <c r="C12" s="2" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="D12" s="2">
-        <v>16</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="F12" s="2">
-        <v>7</v>
+        <v>18</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>223</v>
+      </c>
+      <c r="F12" s="6">
+        <v>13</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>103</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="I12" s="2">
-        <v>9</v>
-      </c>
-      <c r="J12" s="2" t="s">
-        <v>146</v>
+        <v>1</v>
+      </c>
+      <c r="J12" s="5" t="s">
+        <v>139</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="L12" s="5" t="s">
-        <v>243</v>
-      </c>
+        <v>82</v>
+      </c>
+      <c r="L12" s="2"/>
       <c r="M12" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="N12" s="2"/>
+      <c r="N12" s="5" t="s">
+        <v>257</v>
+      </c>
       <c r="O12" s="2" t="s">
         <v>80</v>
       </c>
       <c r="P12" s="5" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="B13" s="2"/>
+        <v>252</v>
+      </c>
+      <c r="B13" s="2">
+        <v>20</v>
+      </c>
       <c r="C13" s="2" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="D13" s="2">
-        <v>17</v>
-      </c>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
+        <v>15</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="F13" s="6">
+        <v>6</v>
+      </c>
       <c r="G13" s="2" t="s">
         <v>103</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>109</v>
+        <v>249</v>
       </c>
       <c r="I13" s="2">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="L13" s="11" t="s">
-        <v>87</v>
-      </c>
+        <v>82</v>
+      </c>
+      <c r="L13" s="2"/>
       <c r="M13" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="N13" s="2"/>
-      <c r="O13" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="P13" s="5" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="N13" s="5" t="s">
+        <v>258</v>
+      </c>
+      <c r="O13" s="2"/>
+      <c r="P13" s="2"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>141</v>
+        <v>253</v>
       </c>
       <c r="B14" s="2">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>140</v>
+        <v>166</v>
       </c>
       <c r="D14" s="2">
-        <v>18</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>226</v>
-      </c>
-      <c r="F14" s="6">
-        <v>13</v>
+        <v>8</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="F14" s="2">
+        <v>8</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="I14" s="2">
-        <v>1</v>
-      </c>
-      <c r="J14" s="5" t="s">
-        <v>139</v>
+        <v>8</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>165</v>
       </c>
       <c r="K14" s="2" t="s">
         <v>82</v>
       </c>
       <c r="L14" s="2"/>
       <c r="M14" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="N14" s="5" t="s">
-        <v>231</v>
-      </c>
+        <v>96</v>
+      </c>
+      <c r="N14" s="5"/>
       <c r="O14" s="2" t="s">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="P14" s="5" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="B15" s="2"/>
+        <v>254</v>
+      </c>
+      <c r="B15" s="2">
+        <v>22</v>
+      </c>
       <c r="C15" s="2" t="s">
-        <v>130</v>
+        <v>162</v>
       </c>
       <c r="D15" s="2">
-        <v>28</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>211</v>
-      </c>
-      <c r="F15" s="6">
-        <v>14</v>
+        <v>9</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="F15" s="2">
+        <v>9</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>127</v>
+        <v>93</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="I15" s="2" t="s">
-        <v>129</v>
+        <v>112</v>
+      </c>
+      <c r="I15" s="2">
+        <v>4</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>128</v>
+        <v>202</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="L15" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="M15" s="2"/>
-      <c r="N15" s="4" t="s">
-        <v>235</v>
-      </c>
+        <v>82</v>
+      </c>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="N15" s="2"/>
       <c r="O15" s="2" t="s">
-        <v>127</v>
+        <v>93</v>
       </c>
       <c r="P15" s="2" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="B16" s="2"/>
+        <v>255</v>
+      </c>
+      <c r="B16" s="2">
+        <v>23</v>
+      </c>
       <c r="C16" s="2" t="s">
-        <v>134</v>
+        <v>161</v>
       </c>
       <c r="D16" s="2">
-        <v>27</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>210</v>
-      </c>
-      <c r="F16" s="6">
-        <v>16</v>
+        <v>10</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="F16" s="2">
+        <v>10</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="I16" s="2">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>133</v>
+        <v>160</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="L16" s="11" t="s">
-        <v>87</v>
-      </c>
+        <v>82</v>
+      </c>
+      <c r="L16" s="2"/>
       <c r="M16" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="N16" s="4" t="s">
-        <v>237</v>
-      </c>
+        <v>96</v>
+      </c>
+      <c r="N16" s="5"/>
       <c r="O16" s="2" t="s">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="P16" s="5" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="B17" s="2"/>
+        <v>256</v>
+      </c>
+      <c r="B17" s="2">
+        <v>24</v>
+      </c>
       <c r="C17" s="2" t="s">
-        <v>137</v>
+        <v>159</v>
       </c>
       <c r="D17" s="2">
-        <v>20</v>
-      </c>
-      <c r="E17" s="6" t="s">
-        <v>209</v>
-      </c>
-      <c r="F17" s="6">
-        <v>15</v>
+        <v>11</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="F17" s="2">
+        <v>11</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="I17" s="2">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>136</v>
+        <v>202</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="L17" s="11" t="s">
-        <v>87</v>
-      </c>
+        <v>82</v>
+      </c>
+      <c r="L17" s="2"/>
       <c r="M17" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="N17" s="4" t="s">
-        <v>236</v>
-      </c>
+        <v>95</v>
+      </c>
+      <c r="N17" s="2"/>
       <c r="O17" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="P17" s="5" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+      <c r="P17" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>62</v>
+        <v>158</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" s="2" t="s">
-        <v>9</v>
+        <v>157</v>
       </c>
       <c r="D18" s="2">
-        <v>5</v>
-      </c>
-      <c r="E18" s="6" t="s">
-        <v>214</v>
-      </c>
-      <c r="F18" s="6">
-        <v>4</v>
+        <v>12</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="F18" s="2">
+        <v>17</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="I18" s="2">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="J18" s="2"/>
       <c r="K18" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="L18" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="M18" s="2"/>
-      <c r="N18" s="2"/>
-      <c r="O18" s="2"/>
-      <c r="P18" s="2"/>
-    </row>
-    <row r="19" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+        <v>234</v>
+      </c>
+      <c r="L18" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="M18" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="N18" s="5"/>
+      <c r="O18" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="P18" s="5" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>57</v>
+        <v>148</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" s="2" t="s">
-        <v>10</v>
+        <v>147</v>
       </c>
       <c r="D19" s="2">
-        <v>6</v>
-      </c>
-      <c r="E19" s="13" t="s">
-        <v>215</v>
-      </c>
-      <c r="F19" s="13">
-        <v>5</v>
+        <v>16</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="F19" s="2">
+        <v>7</v>
       </c>
       <c r="G19" s="2" t="s">
         <v>103</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="I19" s="2">
-        <v>10</v>
-      </c>
-      <c r="J19" s="2"/>
+        <v>9</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>146</v>
+      </c>
       <c r="K19" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="L19" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="M19" s="2"/>
+        <v>234</v>
+      </c>
+      <c r="L19" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="M19" s="2" t="s">
+        <v>103</v>
+      </c>
       <c r="N19" s="2"/>
-      <c r="O19" s="2"/>
-      <c r="P19" s="2"/>
-    </row>
-    <row r="20" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="O19" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="P19" s="5" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" s="2" t="s">
-        <v>155</v>
+        <v>144</v>
       </c>
       <c r="D20" s="2">
-        <v>13</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>222</v>
-      </c>
-      <c r="F20" s="6">
-        <v>18</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
       <c r="G20" s="2" t="s">
         <v>103</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I20" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="L20" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="M20" s="2"/>
+        <v>234</v>
+      </c>
+      <c r="L20" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="M20" s="2" t="s">
+        <v>103</v>
+      </c>
       <c r="N20" s="2"/>
-      <c r="O20" s="2"/>
-      <c r="P20" s="2"/>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O20" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="P20" s="5" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>117</v>
+        <v>131</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="2" t="s">
-        <v>3</v>
+        <v>130</v>
       </c>
       <c r="D21" s="2">
-        <v>1</v>
-      </c>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
+        <v>28</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>208</v>
+      </c>
+      <c r="F21" s="6">
+        <v>14</v>
+      </c>
       <c r="G21" s="2" t="s">
-        <v>103</v>
+        <v>127</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="I21" s="2">
-        <v>20</v>
+        <v>109</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>129</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>176</v>
+        <v>128</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="L21" s="2" t="s">
-        <v>176</v>
+        <v>234</v>
+      </c>
+      <c r="L21" s="11" t="s">
+        <v>87</v>
       </c>
       <c r="M21" s="2"/>
-      <c r="N21" s="2"/>
-      <c r="O21" s="2"/>
-      <c r="P21" s="2"/>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N21" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="O21" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="P21" s="2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>152</v>
+        <v>209</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" s="2" t="s">
-        <v>151</v>
+        <v>134</v>
       </c>
       <c r="D22" s="2">
-        <v>14</v>
-      </c>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
+        <v>27</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="F22" s="6">
+        <v>16</v>
+      </c>
       <c r="G22" s="2" t="s">
         <v>103</v>
       </c>
@@ -4059,37 +3938,281 @@
         <v>109</v>
       </c>
       <c r="I22" s="2">
-        <v>2</v>
-      </c>
-      <c r="J22" s="2"/>
+        <v>9</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>133</v>
+      </c>
       <c r="K22" s="2" t="s">
-        <v>81</v>
+        <v>234</v>
       </c>
       <c r="L22" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="M22" s="2"/>
-      <c r="N22" s="2"/>
-      <c r="O22" s="2"/>
-      <c r="P22" s="2"/>
+      <c r="M22" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="N22" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="O22" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="P22" s="5" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="D23" s="2">
+        <v>20</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="F23" s="6">
+        <v>15</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="I23" s="2">
+        <v>10</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="K23" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="L23" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="M23" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="N23" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="O23" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="P23" s="5" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D24" s="2">
+        <v>5</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="F24" s="6">
+        <v>4</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="I24" s="2">
+        <v>10</v>
+      </c>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="L24" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="M24" s="2"/>
+      <c r="N24" s="2"/>
+      <c r="O24" s="2"/>
+      <c r="P24" s="2"/>
+    </row>
+    <row r="25" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D25" s="2">
+        <v>6</v>
+      </c>
+      <c r="E25" s="13" t="s">
+        <v>212</v>
+      </c>
+      <c r="F25" s="13">
+        <v>5</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="I25" s="2">
+        <v>10</v>
+      </c>
+      <c r="J25" s="2"/>
+      <c r="K25" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="L25" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="M25" s="2"/>
+      <c r="N25" s="2"/>
+      <c r="O25" s="2"/>
+      <c r="P25" s="2"/>
+    </row>
+    <row r="26" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="D26" s="2">
+        <v>13</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="F26" s="6">
+        <v>18</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="I26" s="2">
+        <v>1</v>
+      </c>
+      <c r="J26" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="K26" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="L26" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="M26" s="2"/>
+      <c r="N26" s="2"/>
+      <c r="O26" s="2"/>
+      <c r="P26" s="2"/>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D27" s="2">
+        <v>1</v>
+      </c>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="I27" s="2">
+        <v>20</v>
+      </c>
+      <c r="J27" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="K27" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="L27" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="M27" s="2"/>
+      <c r="N27" s="2"/>
+      <c r="O27" s="2"/>
+      <c r="P27" s="2"/>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="D28" s="2">
+        <v>14</v>
+      </c>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="I28" s="2">
+        <v>2</v>
+      </c>
+      <c r="J28" s="2"/>
+      <c r="K28" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="L28" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="M28" s="2"/>
+      <c r="N28" s="2"/>
+      <c r="O28" s="2"/>
+      <c r="P28" s="2"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="L2:L22">
-    <cfRule type="expression" dxfId="10" priority="17">
+  <conditionalFormatting sqref="L2:L28">
+    <cfRule type="expression" dxfId="3" priority="21">
       <formula>AND($K2&lt;&gt;"Yes",LEN($L2)=0)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:F22">
-    <cfRule type="expression" dxfId="7" priority="18">
+  <conditionalFormatting sqref="D2:F28">
+    <cfRule type="expression" dxfId="2" priority="22">
       <formula>LEN($D2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:P22">
-    <cfRule type="expression" dxfId="9" priority="19">
+  <conditionalFormatting sqref="A2:P28">
+    <cfRule type="expression" dxfId="1" priority="5">
+      <formula>$K2="Skip"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="23">
       <formula>$K2="No"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="8" priority="1">
-      <formula>$K2="Skip"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Adjust data validation severity levels
#16
</commit_message>
<xml_diff>
--- a/specs/Coliform-column-definitions.xlsx
+++ b/specs/Coliform-column-definitions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\xl-ese\specs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B469741-0FE5-40BE-898D-8A7B910ED9D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9212143-0466-47B1-977C-C3F6A85FDE8E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="613" uniqueCount="269">
   <si>
     <t>Optionality</t>
   </si>
@@ -882,6 +882,24 @@
   </si>
   <si>
     <t>&gt;= MAX(RC3,RC21)</t>
+  </si>
+  <si>
+    <t>Validation Severity</t>
+  </si>
+  <si>
+    <t>Warning</t>
+  </si>
+  <si>
+    <t>Stop</t>
+  </si>
+  <si>
+    <t>=LEN(R3C1)=0</t>
+  </si>
+  <si>
+    <t>[0]</t>
+  </si>
+  <si>
+    <t>Information</t>
   </si>
 </sst>
 </file>
@@ -968,7 +986,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="44">
+  <dxfs count="60">
     <dxf>
       <fill>
         <patternFill>
@@ -986,7 +1004,28 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1000,7 +1039,21 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1024,6 +1077,75 @@
           <bgColor theme="7" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1164,54 +1286,56 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{636125F0-68A9-4682-81D8-01BD3AB67D26}" name="Table1" displayName="Table1" ref="A1:P33" totalsRowShown="0" headerRowDxfId="43" dataDxfId="42">
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:P33">
-    <sortCondition ref="B2:B33"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{636125F0-68A9-4682-81D8-01BD3AB67D26}" name="Table1" displayName="Table1" ref="A1:Q33" totalsRowShown="0" headerRowDxfId="59" dataDxfId="58">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Q33">
+    <sortCondition ref="B18:B33"/>
   </sortState>
-  <tableColumns count="16">
-    <tableColumn id="6" xr3:uid="{57EF6AB6-6C4C-4170-BD9B-BF376C46C5DF}" name="Title" dataDxfId="41"/>
-    <tableColumn id="12" xr3:uid="{BFDB40C3-C9ED-4560-81A1-344ECAE248C8}" name="Excel col #" dataDxfId="40"/>
-    <tableColumn id="1" xr3:uid="{3193A6D3-813B-4494-AEED-01D6509FCA0D}" name="CSV Column Name" dataDxfId="39"/>
-    <tableColumn id="11" xr3:uid="{057EA208-1889-4E3C-A179-F312337D9867}" name="CSV col #" dataDxfId="38"/>
-    <tableColumn id="16" xr3:uid="{1F4E7FF6-264D-41DA-AC14-BAA45F3439C7}" name="XML Element" dataDxfId="37"/>
-    <tableColumn id="10" xr3:uid="{F503FCB6-1F5D-4765-B4AB-F67230BC37A3}" name="XML order #" dataDxfId="36"/>
-    <tableColumn id="2" xr3:uid="{5C52F15D-4AC8-44CE-A401-3402D3CD4152}" name="Data Type" dataDxfId="35"/>
-    <tableColumn id="3" xr3:uid="{FFD71D9C-951A-4BB1-9000-9A1C4C3F71D3}" name="Optionality" dataDxfId="34"/>
-    <tableColumn id="4" xr3:uid="{6FEED7B4-CF3F-4593-BB9F-5CFA5FA5B692}" name="Size" dataDxfId="33"/>
-    <tableColumn id="5" xr3:uid="{563427BF-63BA-491F-9B6F-4E02453C643B}" name="Business Rules" dataDxfId="32"/>
-    <tableColumn id="9" xr3:uid="{A9E34622-C2B4-476B-A018-EABC1256DC10}" name="User Editable" dataDxfId="31"/>
-    <tableColumn id="14" xr3:uid="{9DA3EF2F-E261-414A-B10C-F88F2052640F}" name="Generated" dataDxfId="30"/>
-    <tableColumn id="15" xr3:uid="{AA61284F-4409-4E18-9405-8F2EAA78028A}" name="Format" dataDxfId="29"/>
-    <tableColumn id="13" xr3:uid="{94BA7C53-9CFA-4072-B1A4-7E9CE9D9DDF7}" name="Conditional Formatting" dataDxfId="28"/>
-    <tableColumn id="7" xr3:uid="{22AE72C5-BA89-443A-81AF-BCF4B114454C}" name="Validation" dataDxfId="27"/>
-    <tableColumn id="8" xr3:uid="{5DE66E18-4141-4BDD-B41D-2782AC810F6E}" name="Validation Formula" dataDxfId="26"/>
+  <tableColumns count="17">
+    <tableColumn id="6" xr3:uid="{57EF6AB6-6C4C-4170-BD9B-BF376C46C5DF}" name="Title" dataDxfId="57"/>
+    <tableColumn id="12" xr3:uid="{BFDB40C3-C9ED-4560-81A1-344ECAE248C8}" name="Excel col #" dataDxfId="56"/>
+    <tableColumn id="1" xr3:uid="{3193A6D3-813B-4494-AEED-01D6509FCA0D}" name="CSV Column Name" dataDxfId="55"/>
+    <tableColumn id="11" xr3:uid="{057EA208-1889-4E3C-A179-F312337D9867}" name="CSV col #" dataDxfId="54"/>
+    <tableColumn id="16" xr3:uid="{1F4E7FF6-264D-41DA-AC14-BAA45F3439C7}" name="XML Element" dataDxfId="53"/>
+    <tableColumn id="10" xr3:uid="{F503FCB6-1F5D-4765-B4AB-F67230BC37A3}" name="XML order #" dataDxfId="52"/>
+    <tableColumn id="2" xr3:uid="{5C52F15D-4AC8-44CE-A401-3402D3CD4152}" name="Data Type" dataDxfId="51"/>
+    <tableColumn id="3" xr3:uid="{FFD71D9C-951A-4BB1-9000-9A1C4C3F71D3}" name="Optionality" dataDxfId="50"/>
+    <tableColumn id="4" xr3:uid="{6FEED7B4-CF3F-4593-BB9F-5CFA5FA5B692}" name="Size" dataDxfId="49"/>
+    <tableColumn id="5" xr3:uid="{563427BF-63BA-491F-9B6F-4E02453C643B}" name="Business Rules" dataDxfId="48"/>
+    <tableColumn id="9" xr3:uid="{A9E34622-C2B4-476B-A018-EABC1256DC10}" name="User Editable" dataDxfId="47"/>
+    <tableColumn id="14" xr3:uid="{9DA3EF2F-E261-414A-B10C-F88F2052640F}" name="Generated" dataDxfId="46"/>
+    <tableColumn id="15" xr3:uid="{AA61284F-4409-4E18-9405-8F2EAA78028A}" name="Format" dataDxfId="45"/>
+    <tableColumn id="13" xr3:uid="{94BA7C53-9CFA-4072-B1A4-7E9CE9D9DDF7}" name="Conditional Formatting" dataDxfId="44"/>
+    <tableColumn id="7" xr3:uid="{22AE72C5-BA89-443A-81AF-BCF4B114454C}" name="Validation" dataDxfId="43"/>
+    <tableColumn id="8" xr3:uid="{5DE66E18-4141-4BDD-B41D-2782AC810F6E}" name="Validation Formula" dataDxfId="42"/>
+    <tableColumn id="17" xr3:uid="{3088A6C0-DDC9-48B3-825B-006B2A52B333}" name="Validation Severity" dataDxfId="23"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{05345577-AC31-4B6D-B899-55D66DEB1874}" name="Table2" displayName="Table2" ref="A1:P28" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24">
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:P28">
-    <sortCondition ref="B2:B28"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{05345577-AC31-4B6D-B899-55D66DEB1874}" name="Table2" displayName="Table2" ref="A1:Q28" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Q28">
+    <sortCondition ref="B25:B28"/>
   </sortState>
-  <tableColumns count="16">
-    <tableColumn id="7" xr3:uid="{9E32B24E-F549-442D-B6C5-5B5E67078170}" name="Title" dataDxfId="23"/>
-    <tableColumn id="12" xr3:uid="{023EA1AA-B7DF-4814-BFEF-5AB9B0752B95}" name="Excel col #" dataDxfId="22"/>
-    <tableColumn id="1" xr3:uid="{5687DF61-58A8-463A-A7F7-9B8B474466F3}" name="CSV Column Name" dataDxfId="21"/>
-    <tableColumn id="13" xr3:uid="{9E799E78-81C7-4788-BF70-799894A0FACA}" name="CSV col #" dataDxfId="20"/>
-    <tableColumn id="16" xr3:uid="{6872DDE9-C4EA-4656-AE08-1B51AE6AE7D6}" name="XML Element" dataDxfId="19"/>
-    <tableColumn id="11" xr3:uid="{F0D84552-7E57-4362-9DCD-EDC8E4E51415}" name="XML order #" dataDxfId="18"/>
-    <tableColumn id="2" xr3:uid="{E36A262F-69A4-4276-95F1-0FB7FCE8E2AD}" name="Data Type" dataDxfId="17"/>
-    <tableColumn id="3" xr3:uid="{B4F9F589-759B-40AB-BD12-81562C067103}" name="Optionality" dataDxfId="16"/>
-    <tableColumn id="4" xr3:uid="{29CBFF2E-DC73-4812-9BE8-505CDCED923B}" name="Size" dataDxfId="15"/>
-    <tableColumn id="5" xr3:uid="{2FBE4EBA-0896-4EA8-8E6A-9740D712F4CF}" name="Business Rules" dataDxfId="14"/>
-    <tableColumn id="14" xr3:uid="{F6A291D7-463E-4C10-AE63-F46C62F701F1}" name="User Editable" dataDxfId="13"/>
-    <tableColumn id="6" xr3:uid="{4A3A44E5-9909-437B-9914-BD7AF1AC2439}" name="Generated" dataDxfId="12"/>
-    <tableColumn id="15" xr3:uid="{30410F79-D89B-4BAE-852C-7ADB5287310A}" name="Format" dataDxfId="11"/>
-    <tableColumn id="8" xr3:uid="{23D225B6-A3A4-4446-9AD4-7762B64F46FE}" name="Conditional Formatting" dataDxfId="10"/>
-    <tableColumn id="9" xr3:uid="{27D08B50-8012-49E0-9C10-AEB67B99B91B}" name="Validation" dataDxfId="9"/>
-    <tableColumn id="10" xr3:uid="{A301C8EB-BB2A-4524-AF6E-20714C0D7DD5}" name="Validation Formula" dataDxfId="8"/>
+  <tableColumns count="17">
+    <tableColumn id="7" xr3:uid="{9E32B24E-F549-442D-B6C5-5B5E67078170}" name="Title" dataDxfId="39"/>
+    <tableColumn id="12" xr3:uid="{023EA1AA-B7DF-4814-BFEF-5AB9B0752B95}" name="Excel col #" dataDxfId="38"/>
+    <tableColumn id="1" xr3:uid="{5687DF61-58A8-463A-A7F7-9B8B474466F3}" name="CSV Column Name" dataDxfId="37"/>
+    <tableColumn id="13" xr3:uid="{9E799E78-81C7-4788-BF70-799894A0FACA}" name="CSV col #" dataDxfId="36"/>
+    <tableColumn id="16" xr3:uid="{6872DDE9-C4EA-4656-AE08-1B51AE6AE7D6}" name="XML Element" dataDxfId="35"/>
+    <tableColumn id="11" xr3:uid="{F0D84552-7E57-4362-9DCD-EDC8E4E51415}" name="XML order #" dataDxfId="34"/>
+    <tableColumn id="2" xr3:uid="{E36A262F-69A4-4276-95F1-0FB7FCE8E2AD}" name="Data Type" dataDxfId="33"/>
+    <tableColumn id="3" xr3:uid="{B4F9F589-759B-40AB-BD12-81562C067103}" name="Optionality" dataDxfId="32"/>
+    <tableColumn id="4" xr3:uid="{29CBFF2E-DC73-4812-9BE8-505CDCED923B}" name="Size" dataDxfId="31"/>
+    <tableColumn id="5" xr3:uid="{2FBE4EBA-0896-4EA8-8E6A-9740D712F4CF}" name="Business Rules" dataDxfId="30"/>
+    <tableColumn id="14" xr3:uid="{F6A291D7-463E-4C10-AE63-F46C62F701F1}" name="User Editable" dataDxfId="29"/>
+    <tableColumn id="6" xr3:uid="{4A3A44E5-9909-437B-9914-BD7AF1AC2439}" name="Generated" dataDxfId="28"/>
+    <tableColumn id="15" xr3:uid="{30410F79-D89B-4BAE-852C-7ADB5287310A}" name="Format" dataDxfId="27"/>
+    <tableColumn id="8" xr3:uid="{23D225B6-A3A4-4446-9AD4-7762B64F46FE}" name="Conditional Formatting" dataDxfId="26"/>
+    <tableColumn id="9" xr3:uid="{27D08B50-8012-49E0-9C10-AEB67B99B91B}" name="Validation" dataDxfId="25"/>
+    <tableColumn id="10" xr3:uid="{A301C8EB-BB2A-4524-AF6E-20714C0D7DD5}" name="Validation Formula" dataDxfId="24"/>
+    <tableColumn id="17" xr3:uid="{BAA62FBF-6DD1-4BE3-944E-A7C12DBF01CD}" name="Validation Severity" dataDxfId="22"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight14" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1481,7 +1605,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:P33"/>
+  <dimension ref="A1:Q33"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -1514,7 +1638,7 @@
     <col min="20" max="20" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>53</v>
       </c>
@@ -1563,25 +1687,28 @@
       <c r="P1" s="6" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="Q1" s="6" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B2" s="2">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="7">
+        <v>7</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>212</v>
+      </c>
+      <c r="F2" s="13">
         <v>1</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="2">
-        <v>2</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="F2" s="2">
-        <v>4</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>103</v>
@@ -1590,7 +1717,7 @@
         <v>110</v>
       </c>
       <c r="I2" s="3">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="J2" s="2"/>
       <c r="K2" s="2" t="s">
@@ -1600,34 +1727,37 @@
       <c r="M2" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="N2" s="4" t="s">
-        <v>233</v>
+      <c r="N2" s="5" t="s">
+        <v>266</v>
       </c>
       <c r="O2" s="2" t="s">
         <v>84</v>
       </c>
       <c r="P2" s="5" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B3" s="2">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="2">
         <v>2</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="2">
+      <c r="E3" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="F3" s="2">
         <v>4</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="F3" s="2">
-        <v>5</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>103</v>
@@ -1636,11 +1766,9 @@
         <v>110</v>
       </c>
       <c r="I3" s="3">
-        <v>9</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>51</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="J3" s="2"/>
       <c r="K3" s="2" t="s">
         <v>82</v>
       </c>
@@ -1648,170 +1776,188 @@
       <c r="M3" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="N3" s="5" t="s">
-        <v>228</v>
+      <c r="N3" s="4" t="s">
+        <v>233</v>
       </c>
       <c r="O3" s="2" t="s">
         <v>84</v>
       </c>
       <c r="P3" s="5" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+        <v>225</v>
+      </c>
+      <c r="Q3" s="7" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="B4" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" s="7">
-        <v>13</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>185</v>
-      </c>
-      <c r="F4" s="7">
-        <v>16</v>
+        <v>7</v>
+      </c>
+      <c r="D4" s="2">
+        <v>4</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="F4" s="2">
+        <v>5</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>92</v>
+        <v>103</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>110</v>
       </c>
       <c r="I4" s="3">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>19</v>
+        <v>51</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>82</v>
       </c>
       <c r="L4" s="2"/>
       <c r="M4" s="2" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="N4" s="5" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="P4" s="5" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+        <v>203</v>
+      </c>
+      <c r="Q4" s="2" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B5" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" s="2">
-        <v>14</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="F5" s="2">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="D5" s="7">
+        <v>13</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="F5" s="7">
+        <v>16</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="I5" s="3">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>202</v>
+        <v>19</v>
       </c>
       <c r="K5" s="2" t="s">
         <v>82</v>
       </c>
       <c r="L5" s="2"/>
       <c r="M5" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="N5" s="2"/>
+        <v>96</v>
+      </c>
+      <c r="N5" s="5" t="s">
+        <v>226</v>
+      </c>
       <c r="O5" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="P5" s="5" t="s">
+        <v>232</v>
+      </c>
+      <c r="Q5" s="2" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B6" s="2">
+        <v>4</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="2">
+        <v>14</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="F6" s="2">
+        <v>17</v>
+      </c>
+      <c r="G6" s="2" t="s">
         <v>93</v>
-      </c>
-      <c r="P5" s="2" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" s="7">
-        <v>3</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>178</v>
-      </c>
-      <c r="F6" s="7">
-        <v>3</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>103</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>112</v>
       </c>
       <c r="I6" s="3">
-        <v>20</v>
-      </c>
-      <c r="J6" s="2"/>
+        <v>4</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>202</v>
+      </c>
       <c r="K6" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="L6" s="11" t="s">
-        <v>87</v>
-      </c>
+        <v>82</v>
+      </c>
+      <c r="L6" s="2"/>
       <c r="M6" s="2" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="N6" s="2"/>
       <c r="O6" s="2" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="P6" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+        <v>125</v>
+      </c>
+      <c r="Q6" s="2" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="B7" s="2"/>
+        <v>86</v>
+      </c>
+      <c r="B7" s="2">
+        <v>5</v>
+      </c>
       <c r="C7" s="2" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D7" s="7">
-        <v>5</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>180</v>
-      </c>
-      <c r="F7" s="7">
-        <v>10</v>
+        <v>9</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>197</v>
+      </c>
+      <c r="F7" s="13">
+        <v>21</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>103</v>
@@ -1820,42 +1966,49 @@
         <v>110</v>
       </c>
       <c r="I7" s="3">
-        <v>1</v>
-      </c>
-      <c r="J7" s="2"/>
+        <v>12</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>51</v>
+      </c>
       <c r="K7" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="L7" s="2" t="s">
-        <v>239</v>
-      </c>
+        <v>82</v>
+      </c>
+      <c r="L7" s="2"/>
       <c r="M7" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="N7" s="5"/>
+      <c r="N7" s="5" t="s">
+        <v>240</v>
+      </c>
       <c r="O7" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="P7" s="5" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+      <c r="P7" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q7" s="2" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="B8" s="2"/>
+        <v>64</v>
+      </c>
+      <c r="B8" s="2">
+        <v>6</v>
+      </c>
       <c r="C8" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="2">
+        <v>21</v>
+      </c>
+      <c r="D8" s="7">
+        <v>15</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="F8" s="7">
         <v>8</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="F8" s="2">
-        <v>6</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>103</v>
@@ -1864,59 +2017,58 @@
         <v>110</v>
       </c>
       <c r="I8" s="3">
-        <v>10</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>52</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="J8" s="2"/>
       <c r="K8" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="L8" s="5" t="s">
-        <v>235</v>
-      </c>
+        <v>82</v>
+      </c>
+      <c r="L8" s="2"/>
       <c r="M8" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="N8" s="5"/>
+      <c r="N8" s="5" t="s">
+        <v>227</v>
+      </c>
       <c r="O8" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="P8" s="2" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+      <c r="P8" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="Q8" s="2" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>86</v>
+        <v>65</v>
       </c>
       <c r="B9" s="2">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" s="7">
-        <v>9</v>
-      </c>
-      <c r="E9" s="13" t="s">
-        <v>197</v>
-      </c>
-      <c r="F9" s="13">
-        <v>21</v>
+        <v>22</v>
+      </c>
+      <c r="D9" s="2">
+        <v>16</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>196</v>
+      </c>
+      <c r="F9" s="6">
+        <v>22</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>103</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="I9" s="3">
-        <v>12</v>
-      </c>
-      <c r="J9" s="2" t="s">
-        <v>51</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="J9" s="2"/>
       <c r="K9" s="2" t="s">
         <v>82</v>
       </c>
@@ -1924,184 +2076,200 @@
       <c r="M9" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="N9" s="5" t="s">
-        <v>240</v>
+      <c r="N9" s="4" t="s">
+        <v>241</v>
       </c>
       <c r="O9" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="P9" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+      <c r="P9" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q9" s="2" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="B10" s="2"/>
+        <v>102</v>
+      </c>
+      <c r="B10" s="2">
+        <v>8</v>
+      </c>
       <c r="C10" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D10" s="2">
+        <v>30</v>
+      </c>
+      <c r="D10" s="7">
+        <v>29</v>
+      </c>
+      <c r="E10" s="13" t="s">
+        <v>194</v>
+      </c>
+      <c r="F10" s="13">
+        <v>11</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="I10" s="3">
+        <v>20</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="N10" s="4" t="s">
+        <v>242</v>
+      </c>
+      <c r="O10" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="P10" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="Q10" s="2" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B11" s="2">
+        <v>9</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="2">
+        <v>30</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>195</v>
+      </c>
+      <c r="F11" s="6">
         <v>12</v>
       </c>
-      <c r="E10" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="F10" s="2">
-        <v>9</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="I10" s="3">
-        <v>1</v>
-      </c>
-      <c r="J10" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K10" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="L10" s="2" t="s">
-        <v>236</v>
-      </c>
-      <c r="M10" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="N10" s="5"/>
-      <c r="O10" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="P10" s="5" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B11" s="2">
-        <v>6</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D11" s="7">
-        <v>15</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>187</v>
-      </c>
-      <c r="F11" s="7">
+      <c r="G11" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="I11" s="3">
         <v>8</v>
       </c>
-      <c r="G11" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="I11" s="3">
-        <v>2</v>
-      </c>
-      <c r="J11" s="2"/>
+      <c r="J11" s="2" t="s">
+        <v>31</v>
+      </c>
       <c r="K11" s="2" t="s">
         <v>82</v>
       </c>
       <c r="L11" s="2"/>
       <c r="M11" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="N11" s="5" t="s">
-        <v>227</v>
+        <v>96</v>
+      </c>
+      <c r="N11" s="4" t="s">
+        <v>243</v>
       </c>
       <c r="O11" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="P11" s="5" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+        <v>123</v>
+      </c>
+      <c r="Q11" s="2" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B12" s="2">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D12" s="2">
-        <v>16</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>196</v>
-      </c>
-      <c r="F12" s="6">
-        <v>22</v>
+        <v>23</v>
+      </c>
+      <c r="D12" s="7">
+        <v>17</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="F12" s="7">
+        <v>18</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="H12" s="2" t="s">
         <v>112</v>
       </c>
       <c r="I12" s="3">
-        <v>2</v>
-      </c>
-      <c r="J12" s="2"/>
+        <v>8</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>24</v>
+      </c>
       <c r="K12" s="2" t="s">
         <v>82</v>
       </c>
       <c r="L12" s="2"/>
       <c r="M12" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="N12" s="4" t="s">
-        <v>241</v>
-      </c>
+        <v>96</v>
+      </c>
+      <c r="N12" s="2"/>
       <c r="O12" s="2" t="s">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="P12" s="5" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+        <v>259</v>
+      </c>
+      <c r="Q12" s="2" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="B13" s="2">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D13" s="7">
-        <v>29</v>
-      </c>
-      <c r="E13" s="13" t="s">
-        <v>194</v>
-      </c>
-      <c r="F13" s="13">
-        <v>11</v>
+        <v>25</v>
+      </c>
+      <c r="D13" s="2">
+        <v>18</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="F13" s="6">
+        <v>15</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>103</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="I13" s="3">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="K13" s="2" t="s">
         <v>82</v>
@@ -2110,128 +2278,119 @@
       <c r="M13" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="N13" s="4" t="s">
-        <v>242</v>
-      </c>
+      <c r="N13" s="2"/>
       <c r="O13" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="P13" s="5" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+      <c r="P13" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="Q13" s="2" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>122</v>
+        <v>198</v>
       </c>
       <c r="B14" s="2">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D14" s="2">
-        <v>30</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>195</v>
-      </c>
-      <c r="F14" s="6">
-        <v>12</v>
+        <v>33</v>
+      </c>
+      <c r="D14" s="7">
+        <v>22</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="F14" s="7">
+        <v>19</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="I14" s="3">
-        <v>8</v>
+        <v>112</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>34</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="K14" s="2" t="s">
         <v>82</v>
       </c>
       <c r="L14" s="2"/>
       <c r="M14" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="N14" s="4" t="s">
-        <v>243</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="N14" s="2"/>
       <c r="O14" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="P14" s="5" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="B15" s="2">
-        <v>10</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>23</v>
+        <v>101</v>
+      </c>
+      <c r="P14" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q14" s="2" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7" t="s">
+        <v>3</v>
       </c>
       <c r="D15" s="7">
-        <v>17</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>188</v>
-      </c>
-      <c r="F15" s="7">
-        <v>18</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="I15" s="3">
-        <v>8</v>
-      </c>
-      <c r="J15" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="K15" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="L15" s="2"/>
-      <c r="M15" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="N15" s="2"/>
-      <c r="O15" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="P15" s="5" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="H15" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="I15" s="8">
+        <v>20</v>
+      </c>
+      <c r="J15" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="K15" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="L15" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="M15" s="7"/>
+      <c r="N15" s="7"/>
+      <c r="O15" s="7"/>
+      <c r="P15" s="7"/>
+      <c r="Q15" s="2"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="B16" s="2">
-        <v>11</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="B16" s="2"/>
       <c r="C16" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D16" s="2">
-        <v>18</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>193</v>
-      </c>
-      <c r="F16" s="6">
-        <v>15</v>
+        <v>6</v>
+      </c>
+      <c r="D16" s="7">
+        <v>3</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="F16" s="7">
+        <v>3</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>103</v>
@@ -2240,15 +2399,15 @@
         <v>112</v>
       </c>
       <c r="I16" s="3">
-        <v>40</v>
-      </c>
-      <c r="J16" s="2" t="s">
-        <v>26</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="J16" s="2"/>
       <c r="K16" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="L16" s="2"/>
+        <v>234</v>
+      </c>
+      <c r="L16" s="11" t="s">
+        <v>87</v>
+      </c>
       <c r="M16" s="2" t="s">
         <v>103</v>
       </c>
@@ -2257,117 +2416,110 @@
         <v>84</v>
       </c>
       <c r="P16" s="2" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+      <c r="Q16" s="2"/>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="B17" s="2">
-        <v>12</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="B17" s="2"/>
       <c r="C17" s="2" t="s">
-        <v>33</v>
+        <v>8</v>
       </c>
       <c r="D17" s="7">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>191</v>
+        <v>180</v>
       </c>
       <c r="F17" s="7">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="I17" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="J17" s="2" t="s">
-        <v>35</v>
-      </c>
+        <v>110</v>
+      </c>
+      <c r="I17" s="3">
+        <v>1</v>
+      </c>
+      <c r="J17" s="2"/>
       <c r="K17" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="L17" s="2"/>
+        <v>234</v>
+      </c>
+      <c r="L17" s="2" t="s">
+        <v>239</v>
+      </c>
       <c r="M17" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="N17" s="2"/>
+        <v>103</v>
+      </c>
+      <c r="N17" s="5"/>
       <c r="O17" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="P17" s="2" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+      <c r="P17" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="Q17" s="2"/>
+    </row>
+    <row r="18" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>199</v>
+        <v>62</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" s="2" t="s">
-        <v>36</v>
+        <v>9</v>
       </c>
       <c r="D18" s="2">
-        <v>23</v>
-      </c>
-      <c r="E18" s="7" t="s">
-        <v>191</v>
-      </c>
-      <c r="F18" s="7">
-        <v>20</v>
+        <v>6</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="F18" s="6">
+        <v>2</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="I18" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="J18" s="2" t="s">
-        <v>37</v>
-      </c>
+        <v>110</v>
+      </c>
+      <c r="I18" s="3">
+        <v>10</v>
+      </c>
+      <c r="J18" s="2"/>
       <c r="K18" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="L18" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="M18" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="N18" s="2"/>
-      <c r="O18" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="P18" s="2" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+      <c r="L18" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="M18" s="2"/>
+      <c r="N18" s="5"/>
+      <c r="O18" s="2"/>
+      <c r="P18" s="5"/>
+      <c r="Q18" s="2"/>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D19" s="2">
+        <v>8</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="F19" s="2">
         <v>6</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>211</v>
-      </c>
-      <c r="F19" s="6">
-        <v>1</v>
       </c>
       <c r="G19" s="2" t="s">
         <v>103</v>
@@ -2378,57 +2530,65 @@
       <c r="I19" s="3">
         <v>10</v>
       </c>
-      <c r="J19" s="2"/>
+      <c r="J19" s="2" t="s">
+        <v>52</v>
+      </c>
       <c r="K19" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="L19" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="M19" s="2"/>
-      <c r="N19" s="2"/>
-      <c r="O19" s="2"/>
-      <c r="P19" s="2"/>
-    </row>
-    <row r="20" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+        <v>234</v>
+      </c>
+      <c r="L19" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="M19" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="N19" s="5"/>
+      <c r="O19" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="P19" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="Q19" s="2"/>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>57</v>
+        <v>104</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D20" s="2">
         <v>10</v>
       </c>
-      <c r="D20" s="7">
-        <v>7</v>
-      </c>
-      <c r="E20" s="13" t="s">
-        <v>212</v>
-      </c>
-      <c r="F20" s="13">
-        <v>2</v>
-      </c>
+      <c r="E20" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="F20" s="2"/>
       <c r="G20" s="2" t="s">
         <v>103</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="I20" s="3">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="J20" s="2"/>
       <c r="K20" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="L20" s="2" t="s">
-        <v>83</v>
+      <c r="L20" s="11" t="s">
+        <v>87</v>
       </c>
       <c r="M20" s="2"/>
       <c r="N20" s="2"/>
       <c r="O20" s="2"/>
       <c r="P20" s="2"/>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q20" s="2"/>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>63</v>
       </c>
@@ -2467,138 +2627,144 @@
       <c r="N21" s="2"/>
       <c r="O21" s="2"/>
       <c r="P21" s="2"/>
-    </row>
-    <row r="22" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+      <c r="Q21" s="2"/>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>74</v>
+        <v>89</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D22" s="7">
-        <v>31</v>
-      </c>
-      <c r="E22" s="13" t="s">
-        <v>200</v>
-      </c>
-      <c r="F22" s="13">
-        <v>13</v>
+        <v>16</v>
+      </c>
+      <c r="D22" s="2">
+        <v>12</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="F22" s="2">
+        <v>9</v>
       </c>
       <c r="G22" s="2" t="s">
         <v>103</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="I22" s="3">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>50</v>
+        <v>17</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>81</v>
+        <v>234</v>
       </c>
       <c r="L22" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="M22" s="2"/>
-      <c r="N22" s="2"/>
-      <c r="O22" s="2"/>
-      <c r="P22" s="2"/>
-    </row>
-    <row r="23" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+        <v>236</v>
+      </c>
+      <c r="M22" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="N22" s="5"/>
+      <c r="O22" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="P22" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="Q22" s="2"/>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D23" s="2">
-        <v>32</v>
+        <v>27</v>
+      </c>
+      <c r="D23" s="7">
+        <v>19</v>
       </c>
       <c r="E23" s="13" t="s">
-        <v>201</v>
-      </c>
-      <c r="F23" s="13">
-        <v>14</v>
-      </c>
+        <v>190</v>
+      </c>
+      <c r="F23" s="13"/>
       <c r="G23" s="2" t="s">
         <v>103</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="I23" s="3">
-        <v>10</v>
-      </c>
-      <c r="J23" s="2" t="s">
-        <v>49</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="J23" s="2"/>
       <c r="K23" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="L23" s="2" t="s">
-        <v>108</v>
+      <c r="L23" s="11" t="s">
+        <v>87</v>
       </c>
       <c r="M23" s="2"/>
       <c r="N23" s="2"/>
       <c r="O23" s="2"/>
       <c r="P23" s="2"/>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A24" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="B24" s="7"/>
-      <c r="C24" s="7" t="s">
-        <v>3</v>
+      <c r="Q23" s="2"/>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2" t="s">
+        <v>28</v>
       </c>
       <c r="D24" s="7">
-        <v>1</v>
-      </c>
-      <c r="E24" s="7"/>
+        <v>20</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>189</v>
+      </c>
       <c r="F24" s="7"/>
-      <c r="G24" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="H24" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="I24" s="8">
-        <v>20</v>
-      </c>
-      <c r="J24" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="K24" s="7" t="s">
+      <c r="G24" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="I24" s="3">
+        <v>2</v>
+      </c>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="L24" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="M24" s="7"/>
-      <c r="N24" s="7"/>
-      <c r="O24" s="7"/>
-      <c r="P24" s="7"/>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="L24" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="M24" s="2"/>
+      <c r="N24" s="2"/>
+      <c r="O24" s="2"/>
+      <c r="P24" s="2"/>
+      <c r="Q24" s="2"/>
+    </row>
+    <row r="25" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>104</v>
+        <v>69</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" s="2" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="D25" s="2">
-        <v>10</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="F25" s="2"/>
+        <v>21</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="F25" s="6"/>
       <c r="G25" s="2" t="s">
         <v>103</v>
       </c>
@@ -2606,7 +2772,7 @@
         <v>111</v>
       </c>
       <c r="I25" s="3">
-        <v>40</v>
+        <v>12</v>
       </c>
       <c r="J25" s="2"/>
       <c r="K25" s="2" t="s">
@@ -2619,66 +2785,78 @@
       <c r="N25" s="2"/>
       <c r="O25" s="2"/>
       <c r="P25" s="2"/>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q25" s="2"/>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>67</v>
+        <v>199</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D26" s="7">
-        <v>19</v>
-      </c>
-      <c r="E26" s="13" t="s">
-        <v>190</v>
-      </c>
-      <c r="F26" s="13"/>
+        <v>36</v>
+      </c>
+      <c r="D26" s="2">
+        <v>23</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="F26" s="7">
+        <v>20</v>
+      </c>
       <c r="G26" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="I26" s="3">
-        <v>9</v>
-      </c>
-      <c r="J26" s="2"/>
+        <v>112</v>
+      </c>
+      <c r="I26" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="J26" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="K26" s="2" t="s">
-        <v>81</v>
+        <v>234</v>
       </c>
       <c r="L26" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="M26" s="2"/>
+      <c r="M26" s="2" t="s">
+        <v>100</v>
+      </c>
       <c r="N26" s="2"/>
-      <c r="O26" s="2"/>
-      <c r="P26" s="2"/>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O26" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="P26" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q26" s="2"/>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" s="2" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="D27" s="7">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="F27" s="7"/>
       <c r="G27" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H27" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="I27" s="3">
-        <v>2</v>
+      <c r="I27" s="3" t="s">
+        <v>39</v>
       </c>
       <c r="J27" s="2"/>
       <c r="K27" s="2" t="s">
@@ -2691,31 +2869,30 @@
       <c r="N27" s="2"/>
       <c r="O27" s="2"/>
       <c r="P27" s="2"/>
-    </row>
-    <row r="28" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="Q27" s="2"/>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" s="2" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="D28" s="2">
-        <v>21</v>
-      </c>
-      <c r="E28" s="6" t="s">
-        <v>192</v>
-      </c>
-      <c r="F28" s="6"/>
+        <v>25</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="F28" s="7"/>
       <c r="G28" s="2" t="s">
         <v>103</v>
       </c>
       <c r="H28" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="I28" s="3">
-        <v>12</v>
-      </c>
+      <c r="I28" s="3"/>
       <c r="J28" s="2"/>
       <c r="K28" s="2" t="s">
         <v>81</v>
@@ -2727,17 +2904,18 @@
       <c r="N28" s="2"/>
       <c r="O28" s="2"/>
       <c r="P28" s="2"/>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q28" s="2"/>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" s="2" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D29" s="7">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E29" s="7" t="s">
         <v>191</v>
@@ -2750,7 +2928,7 @@
         <v>111</v>
       </c>
       <c r="I29" s="3" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="J29" s="2"/>
       <c r="K29" s="2" t="s">
@@ -2763,29 +2941,32 @@
       <c r="N29" s="2"/>
       <c r="O29" s="2"/>
       <c r="P29" s="2"/>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q29" s="2"/>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" s="2" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="D30" s="2">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E30" s="7" t="s">
         <v>191</v>
       </c>
       <c r="F30" s="7"/>
       <c r="G30" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H30" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="I30" s="3"/>
+      <c r="I30" s="3" t="s">
+        <v>44</v>
+      </c>
       <c r="J30" s="2"/>
       <c r="K30" s="2" t="s">
         <v>81</v>
@@ -2797,17 +2978,18 @@
       <c r="N30" s="2"/>
       <c r="O30" s="2"/>
       <c r="P30" s="2"/>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q30" s="2"/>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" s="2" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="D31" s="7">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E31" s="7" t="s">
         <v>191</v>
@@ -2820,7 +3002,7 @@
         <v>111</v>
       </c>
       <c r="I31" s="3" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="J31" s="2"/>
       <c r="K31" s="2" t="s">
@@ -2833,97 +3015,108 @@
       <c r="N31" s="2"/>
       <c r="O31" s="2"/>
       <c r="P31" s="2"/>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q31" s="2"/>
+    </row>
+    <row r="32" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D32" s="2">
-        <v>27</v>
-      </c>
-      <c r="E32" s="7" t="s">
-        <v>191</v>
-      </c>
-      <c r="F32" s="7"/>
+        <v>47</v>
+      </c>
+      <c r="D32" s="7">
+        <v>31</v>
+      </c>
+      <c r="E32" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="F32" s="13">
+        <v>13</v>
+      </c>
       <c r="G32" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="I32" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="J32" s="2"/>
+        <v>109</v>
+      </c>
+      <c r="I32" s="3">
+        <v>10</v>
+      </c>
+      <c r="J32" s="2" t="s">
+        <v>50</v>
+      </c>
       <c r="K32" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="L32" s="11" t="s">
-        <v>87</v>
+      <c r="L32" s="2" t="s">
+        <v>114</v>
       </c>
       <c r="M32" s="2"/>
       <c r="N32" s="2"/>
       <c r="O32" s="2"/>
       <c r="P32" s="2"/>
-    </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q32" s="2"/>
+    </row>
+    <row r="33" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D33" s="7">
-        <v>28</v>
-      </c>
-      <c r="E33" s="7" t="s">
-        <v>191</v>
-      </c>
-      <c r="F33" s="7"/>
+        <v>48</v>
+      </c>
+      <c r="D33" s="2">
+        <v>32</v>
+      </c>
+      <c r="E33" s="13" t="s">
+        <v>201</v>
+      </c>
+      <c r="F33" s="13">
+        <v>14</v>
+      </c>
       <c r="G33" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="I33" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="J33" s="2"/>
+        <v>109</v>
+      </c>
+      <c r="I33" s="3">
+        <v>10</v>
+      </c>
+      <c r="J33" s="2" t="s">
+        <v>49</v>
+      </c>
       <c r="K33" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="L33" s="11" t="s">
-        <v>87</v>
+      <c r="L33" s="2" t="s">
+        <v>108</v>
       </c>
       <c r="M33" s="2"/>
       <c r="N33" s="2"/>
       <c r="O33" s="2"/>
       <c r="P33" s="2"/>
+      <c r="Q33" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
   <conditionalFormatting sqref="D2:F33">
-    <cfRule type="expression" dxfId="7" priority="12">
+    <cfRule type="expression" dxfId="3" priority="14">
       <formula>LEN($D2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:P33">
-    <cfRule type="expression" dxfId="6" priority="1">
+  <conditionalFormatting sqref="L2:L33">
+    <cfRule type="expression" dxfId="2" priority="13">
+      <formula>AND($K2&lt;&gt;"Yes",LEN($L2)=0)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A2:Q33">
+    <cfRule type="expression" dxfId="1" priority="3">
       <formula>$K2="Skip"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="13">
+    <cfRule type="expression" dxfId="0" priority="15">
       <formula>$K2="No"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L2:L33">
-    <cfRule type="expression" dxfId="4" priority="11">
-      <formula>AND($K2&lt;&gt;"Yes",LEN($L2)=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2937,7 +3130,7 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15FEC0F5-029A-4987-81C0-EA7F2B314198}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:P28"/>
+  <dimension ref="A1:Q28"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -2964,9 +3157,10 @@
     <col min="14" max="14" width="41.85546875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="10.140625" customWidth="1"/>
     <col min="16" max="16" width="31.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>53</v>
       </c>
@@ -3015,25 +3209,28 @@
       <c r="P1" s="6" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q1" s="6" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>244</v>
+        <v>267</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="2">
+        <v>6</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>212</v>
+      </c>
+      <c r="F2" s="13">
         <v>5</v>
-      </c>
-      <c r="D2" s="2">
-        <v>2</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="F2" s="2">
-        <v>1</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>103</v>
@@ -3042,11 +3239,9 @@
         <v>110</v>
       </c>
       <c r="I2" s="2">
-        <v>20</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>173</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="J2" s="2"/>
       <c r="K2" s="2" t="s">
         <v>82</v>
       </c>
@@ -3054,28 +3249,29 @@
       <c r="M2" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="N2" s="4"/>
+      <c r="N2" s="2"/>
       <c r="O2" s="2"/>
-      <c r="P2" s="5"/>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D3" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="F3" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>103</v>
@@ -3084,10 +3280,10 @@
         <v>110</v>
       </c>
       <c r="I3" s="2">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>82</v>
@@ -3096,95 +3292,98 @@
       <c r="M3" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="N3" s="5"/>
+      <c r="N3" s="4"/>
       <c r="O3" s="2"/>
       <c r="P3" s="5"/>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q3" s="2"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="D4" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="F4" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>92</v>
+        <v>103</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="I4" s="2">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>82</v>
       </c>
       <c r="L4" s="2"/>
       <c r="M4" s="2" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="N4" s="5"/>
       <c r="O4" s="2"/>
       <c r="P4" s="5"/>
-    </row>
-    <row r="5" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="Q4" s="2"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="B5" s="2"/>
+        <v>90</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>246</v>
+      </c>
       <c r="C5" s="2" t="s">
-        <v>169</v>
+        <v>18</v>
       </c>
       <c r="D5" s="2">
-        <v>7</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="F5" s="6">
-        <v>12</v>
+        <v>3</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="F5" s="2">
+        <v>3</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="I5" s="2">
-        <v>4</v>
-      </c>
-      <c r="J5" s="6" t="s">
-        <v>168</v>
+        <v>8</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>172</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="L5" s="2" t="s">
-        <v>247</v>
-      </c>
+        <v>82</v>
+      </c>
+      <c r="L5" s="2"/>
       <c r="M5" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="N5" s="4"/>
+        <v>96</v>
+      </c>
+      <c r="N5" s="5"/>
       <c r="O5" s="2"/>
       <c r="P5" s="5"/>
-    </row>
-    <row r="6" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="Q5" s="2"/>
+    </row>
+    <row r="6" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>141</v>
       </c>
@@ -3231,8 +3430,11 @@
       <c r="P6" s="5" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="7" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="Q6" s="2" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>221</v>
       </c>
@@ -3275,8 +3477,11 @@
       </c>
       <c r="O7" s="2"/>
       <c r="P7" s="2"/>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q7" s="2" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>167</v>
       </c>
@@ -3321,8 +3526,11 @@
       <c r="P8" s="5" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q8" s="2" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>163</v>
       </c>
@@ -3367,8 +3575,11 @@
       <c r="P9" s="2" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q9" s="2" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>204</v>
       </c>
@@ -3413,8 +3624,11 @@
       <c r="P10" s="5" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q10" s="2" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>205</v>
       </c>
@@ -3459,8 +3673,11 @@
       <c r="P11" s="2" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="12" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="Q11" s="2" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>251</v>
       </c>
@@ -3507,8 +3724,11 @@
       <c r="P12" s="5" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="13" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="Q12" s="2" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>252</v>
       </c>
@@ -3551,8 +3771,11 @@
       </c>
       <c r="O13" s="2"/>
       <c r="P13" s="2"/>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q13" s="2" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>253</v>
       </c>
@@ -3597,8 +3820,11 @@
       <c r="P14" s="5" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q14" s="2" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>254</v>
       </c>
@@ -3643,8 +3869,11 @@
       <c r="P15" s="2" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q15" s="2" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>255</v>
       </c>
@@ -3689,8 +3918,11 @@
       <c r="P16" s="5" t="s">
         <v>262</v>
       </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q16" s="2" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>256</v>
       </c>
@@ -3735,250 +3967,228 @@
       <c r="P17" s="2" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q17" s="2" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>158</v>
+        <v>117</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" s="2" t="s">
-        <v>157</v>
+        <v>3</v>
       </c>
       <c r="D18" s="2">
-        <v>12</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="F18" s="2">
-        <v>17</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
       <c r="G18" s="2" t="s">
-        <v>92</v>
+        <v>103</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="I18" s="2">
-        <v>8</v>
-      </c>
-      <c r="J18" s="2"/>
+        <v>20</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>174</v>
+      </c>
       <c r="K18" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="L18" s="5" t="s">
-        <v>238</v>
-      </c>
-      <c r="M18" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="N18" s="5"/>
-      <c r="O18" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="P18" s="5" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+      <c r="L18" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="M18" s="2"/>
+      <c r="N18" s="2"/>
+      <c r="O18" s="2"/>
+      <c r="P18" s="2"/>
+      <c r="Q18" s="2"/>
+    </row>
+    <row r="19" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>148</v>
+        <v>62</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" s="2" t="s">
-        <v>147</v>
+        <v>9</v>
       </c>
       <c r="D19" s="2">
-        <v>16</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="F19" s="2">
-        <v>7</v>
+        <v>5</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="F19" s="6">
+        <v>4</v>
       </c>
       <c r="G19" s="2" t="s">
         <v>103</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="I19" s="2">
-        <v>9</v>
-      </c>
-      <c r="J19" s="2" t="s">
-        <v>146</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="J19" s="2"/>
       <c r="K19" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="L19" s="5" t="s">
-        <v>237</v>
-      </c>
-      <c r="M19" s="2" t="s">
-        <v>103</v>
-      </c>
+        <v>81</v>
+      </c>
+      <c r="L19" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="M19" s="2"/>
       <c r="N19" s="2"/>
-      <c r="O19" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="P19" s="5" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O19" s="2"/>
+      <c r="P19" s="2"/>
+      <c r="Q19" s="2"/>
+    </row>
+    <row r="20" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>145</v>
+        <v>170</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" s="2" t="s">
-        <v>144</v>
+        <v>169</v>
       </c>
       <c r="D20" s="2">
-        <v>17</v>
-      </c>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
+        <v>7</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="F20" s="6">
+        <v>12</v>
+      </c>
       <c r="G20" s="2" t="s">
         <v>103</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="I20" s="2">
         <v>4</v>
       </c>
-      <c r="J20" s="2" t="s">
-        <v>143</v>
+      <c r="J20" s="6" t="s">
+        <v>168</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="L20" s="11" t="s">
-        <v>87</v>
+        <v>81</v>
+      </c>
+      <c r="L20" s="2" t="s">
+        <v>247</v>
       </c>
       <c r="M20" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="N20" s="2"/>
-      <c r="O20" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="P20" s="5" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="N20" s="4"/>
+      <c r="O20" s="2"/>
+      <c r="P20" s="5"/>
+      <c r="Q20" s="2"/>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>131</v>
+        <v>158</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="2" t="s">
-        <v>130</v>
+        <v>157</v>
       </c>
       <c r="D21" s="2">
-        <v>28</v>
-      </c>
-      <c r="E21" s="6" t="s">
-        <v>208</v>
-      </c>
-      <c r="F21" s="6">
-        <v>14</v>
+        <v>12</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="F21" s="2">
+        <v>17</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>127</v>
+        <v>92</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="I21" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="J21" s="2" t="s">
-        <v>128</v>
-      </c>
+        <v>112</v>
+      </c>
+      <c r="I21" s="2">
+        <v>8</v>
+      </c>
+      <c r="J21" s="2"/>
       <c r="K21" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="L21" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="M21" s="2"/>
-      <c r="N21" s="4" t="s">
-        <v>229</v>
-      </c>
+      <c r="L21" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="M21" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="N21" s="5"/>
       <c r="O21" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="P21" s="2" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+      <c r="P21" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="Q21" s="2"/>
+    </row>
+    <row r="22" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>209</v>
+        <v>156</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" s="2" t="s">
-        <v>134</v>
+        <v>155</v>
       </c>
       <c r="D22" s="2">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>207</v>
+        <v>219</v>
       </c>
       <c r="F22" s="6">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="G22" s="2" t="s">
         <v>103</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="I22" s="2">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>133</v>
+        <v>154</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="L22" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="M22" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="N22" s="4" t="s">
-        <v>231</v>
-      </c>
-      <c r="O22" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="P22" s="5" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+      <c r="L22" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="M22" s="2"/>
+      <c r="N22" s="2"/>
+      <c r="O22" s="2"/>
+      <c r="P22" s="2"/>
+      <c r="Q22" s="2"/>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>210</v>
+        <v>152</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" s="2" t="s">
-        <v>137</v>
+        <v>151</v>
       </c>
       <c r="D23" s="2">
-        <v>20</v>
-      </c>
-      <c r="E23" s="6" t="s">
-        <v>206</v>
-      </c>
-      <c r="F23" s="6">
-        <v>15</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
       <c r="G23" s="2" t="s">
         <v>103</v>
       </c>
@@ -3986,232 +4196,272 @@
         <v>109</v>
       </c>
       <c r="I23" s="2">
-        <v>10</v>
-      </c>
-      <c r="J23" s="2" t="s">
-        <v>136</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="J23" s="2"/>
       <c r="K23" s="2" t="s">
-        <v>234</v>
+        <v>81</v>
       </c>
       <c r="L23" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="M23" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="N23" s="4" t="s">
-        <v>230</v>
-      </c>
-      <c r="O23" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="P23" s="5" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+      <c r="M23" s="2"/>
+      <c r="N23" s="2"/>
+      <c r="O23" s="2"/>
+      <c r="P23" s="2"/>
+      <c r="Q23" s="2"/>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>62</v>
+        <v>148</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="D24" s="2">
+        <v>16</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="F24" s="2">
+        <v>7</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="I24" s="2">
         <v>9</v>
       </c>
-      <c r="D24" s="2">
-        <v>5</v>
-      </c>
-      <c r="E24" s="6" t="s">
-        <v>211</v>
-      </c>
-      <c r="F24" s="6">
-        <v>4</v>
-      </c>
-      <c r="G24" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="H24" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="I24" s="2">
-        <v>10</v>
-      </c>
-      <c r="J24" s="2"/>
+      <c r="J24" s="2" t="s">
+        <v>146</v>
+      </c>
       <c r="K24" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="L24" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="M24" s="2"/>
+        <v>234</v>
+      </c>
+      <c r="L24" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="M24" s="2" t="s">
+        <v>103</v>
+      </c>
       <c r="N24" s="2"/>
-      <c r="O24" s="2"/>
-      <c r="P24" s="2"/>
-    </row>
-    <row r="25" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="O24" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="P24" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="Q24" s="2"/>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>57</v>
+        <v>145</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" s="2" t="s">
-        <v>10</v>
+        <v>144</v>
       </c>
       <c r="D25" s="2">
-        <v>6</v>
-      </c>
-      <c r="E25" s="13" t="s">
-        <v>212</v>
-      </c>
-      <c r="F25" s="13">
-        <v>5</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
       <c r="G25" s="2" t="s">
         <v>103</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I25" s="2">
-        <v>10</v>
-      </c>
-      <c r="J25" s="2"/>
+        <v>4</v>
+      </c>
+      <c r="J25" s="2" t="s">
+        <v>143</v>
+      </c>
       <c r="K25" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="L25" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="M25" s="2"/>
+        <v>234</v>
+      </c>
+      <c r="L25" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="M25" s="2" t="s">
+        <v>103</v>
+      </c>
       <c r="N25" s="2"/>
-      <c r="O25" s="2"/>
-      <c r="P25" s="2"/>
-    </row>
-    <row r="26" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="O25" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="P25" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="Q25" s="2"/>
+    </row>
+    <row r="26" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>156</v>
+        <v>210</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" s="2" t="s">
-        <v>155</v>
+        <v>137</v>
       </c>
       <c r="D26" s="2">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>219</v>
+        <v>206</v>
       </c>
       <c r="F26" s="6">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="G26" s="2" t="s">
         <v>103</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I26" s="2">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="K26" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="L26" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="M26" s="2"/>
-      <c r="N26" s="2"/>
-      <c r="O26" s="2"/>
-      <c r="P26" s="2"/>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+        <v>234</v>
+      </c>
+      <c r="L26" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="M26" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="N26" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="O26" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="P26" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="Q26" s="2"/>
+    </row>
+    <row r="27" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>117</v>
+        <v>209</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" s="2" t="s">
-        <v>3</v>
+        <v>134</v>
       </c>
       <c r="D27" s="2">
-        <v>1</v>
-      </c>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
+        <v>27</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="F27" s="6">
+        <v>16</v>
+      </c>
       <c r="G27" s="2" t="s">
         <v>103</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I27" s="2">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>174</v>
+        <v>133</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="L27" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="M27" s="2"/>
-      <c r="N27" s="2"/>
-      <c r="O27" s="2"/>
-      <c r="P27" s="2"/>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+        <v>234</v>
+      </c>
+      <c r="L27" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="M27" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="N27" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="O27" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="P27" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="Q27" s="2"/>
+    </row>
+    <row r="28" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>152</v>
+        <v>131</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" s="2" t="s">
-        <v>151</v>
+        <v>130</v>
       </c>
       <c r="D28" s="2">
+        <v>28</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>208</v>
+      </c>
+      <c r="F28" s="6">
         <v>14</v>
       </c>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
       <c r="G28" s="2" t="s">
-        <v>103</v>
+        <v>127</v>
       </c>
       <c r="H28" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="I28" s="2">
-        <v>2</v>
-      </c>
-      <c r="J28" s="2"/>
+      <c r="I28" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="J28" s="2" t="s">
+        <v>128</v>
+      </c>
       <c r="K28" s="2" t="s">
-        <v>81</v>
+        <v>234</v>
       </c>
       <c r="L28" s="11" t="s">
         <v>87</v>
       </c>
       <c r="M28" s="2"/>
-      <c r="N28" s="2"/>
-      <c r="O28" s="2"/>
-      <c r="P28" s="2"/>
+      <c r="N28" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="O28" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="P28" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q28" s="2"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="L2:L28">
-    <cfRule type="expression" dxfId="3" priority="21">
+    <cfRule type="expression" dxfId="17" priority="21">
       <formula>AND($K2&lt;&gt;"Yes",LEN($L2)=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:F28">
-    <cfRule type="expression" dxfId="2" priority="22">
+    <cfRule type="expression" dxfId="16" priority="22">
       <formula>LEN($D2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:P28">
-    <cfRule type="expression" dxfId="1" priority="5">
+  <conditionalFormatting sqref="A2:Q28">
+    <cfRule type="expression" dxfId="15" priority="5">
       <formula>$K2="Skip"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="23">
+    <cfRule type="expression" dxfId="14" priority="23">
       <formula>$K2="No"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Add optional list of analytical methods
</commit_message>
<xml_diff>
--- a/specs/Coliform-column-definitions.xlsx
+++ b/specs/Coliform-column-definitions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\xl-ese\specs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9212143-0466-47B1-977C-C3F6A85FDE8E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4E895DE-E5DB-4BAE-BC87-4CAC9BFD1B71}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Coliform Sample" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="613" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="617" uniqueCount="270">
   <si>
     <t>Optionality</t>
   </si>
@@ -899,7 +899,10 @@
     <t>[0]</t>
   </si>
   <si>
-    <t>Information</t>
+    <t>None</t>
+  </si>
+  <si>
+    <t>=MethodsList</t>
   </si>
 </sst>
 </file>
@@ -986,7 +989,64 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="60">
+  <dxfs count="46">
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1004,28 +1064,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1037,169 +1076,7 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1266,6 +1143,34 @@
     </dxf>
     <dxf>
       <alignment vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1286,27 +1191,27 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{636125F0-68A9-4682-81D8-01BD3AB67D26}" name="Table1" displayName="Table1" ref="A1:Q33" totalsRowShown="0" headerRowDxfId="59" dataDxfId="58">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{636125F0-68A9-4682-81D8-01BD3AB67D26}" name="Table1" displayName="Table1" ref="A1:Q33" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40">
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Q33">
     <sortCondition ref="B18:B33"/>
   </sortState>
   <tableColumns count="17">
-    <tableColumn id="6" xr3:uid="{57EF6AB6-6C4C-4170-BD9B-BF376C46C5DF}" name="Title" dataDxfId="57"/>
-    <tableColumn id="12" xr3:uid="{BFDB40C3-C9ED-4560-81A1-344ECAE248C8}" name="Excel col #" dataDxfId="56"/>
-    <tableColumn id="1" xr3:uid="{3193A6D3-813B-4494-AEED-01D6509FCA0D}" name="CSV Column Name" dataDxfId="55"/>
-    <tableColumn id="11" xr3:uid="{057EA208-1889-4E3C-A179-F312337D9867}" name="CSV col #" dataDxfId="54"/>
-    <tableColumn id="16" xr3:uid="{1F4E7FF6-264D-41DA-AC14-BAA45F3439C7}" name="XML Element" dataDxfId="53"/>
-    <tableColumn id="10" xr3:uid="{F503FCB6-1F5D-4765-B4AB-F67230BC37A3}" name="XML order #" dataDxfId="52"/>
-    <tableColumn id="2" xr3:uid="{5C52F15D-4AC8-44CE-A401-3402D3CD4152}" name="Data Type" dataDxfId="51"/>
-    <tableColumn id="3" xr3:uid="{FFD71D9C-951A-4BB1-9000-9A1C4C3F71D3}" name="Optionality" dataDxfId="50"/>
-    <tableColumn id="4" xr3:uid="{6FEED7B4-CF3F-4593-BB9F-5CFA5FA5B692}" name="Size" dataDxfId="49"/>
-    <tableColumn id="5" xr3:uid="{563427BF-63BA-491F-9B6F-4E02453C643B}" name="Business Rules" dataDxfId="48"/>
-    <tableColumn id="9" xr3:uid="{A9E34622-C2B4-476B-A018-EABC1256DC10}" name="User Editable" dataDxfId="47"/>
-    <tableColumn id="14" xr3:uid="{9DA3EF2F-E261-414A-B10C-F88F2052640F}" name="Generated" dataDxfId="46"/>
-    <tableColumn id="15" xr3:uid="{AA61284F-4409-4E18-9405-8F2EAA78028A}" name="Format" dataDxfId="45"/>
-    <tableColumn id="13" xr3:uid="{94BA7C53-9CFA-4072-B1A4-7E9CE9D9DDF7}" name="Conditional Formatting" dataDxfId="44"/>
-    <tableColumn id="7" xr3:uid="{22AE72C5-BA89-443A-81AF-BCF4B114454C}" name="Validation" dataDxfId="43"/>
-    <tableColumn id="8" xr3:uid="{5DE66E18-4141-4BDD-B41D-2782AC810F6E}" name="Validation Formula" dataDxfId="42"/>
+    <tableColumn id="6" xr3:uid="{57EF6AB6-6C4C-4170-BD9B-BF376C46C5DF}" name="Title" dataDxfId="39"/>
+    <tableColumn id="12" xr3:uid="{BFDB40C3-C9ED-4560-81A1-344ECAE248C8}" name="Excel col #" dataDxfId="38"/>
+    <tableColumn id="1" xr3:uid="{3193A6D3-813B-4494-AEED-01D6509FCA0D}" name="CSV Column Name" dataDxfId="37"/>
+    <tableColumn id="11" xr3:uid="{057EA208-1889-4E3C-A179-F312337D9867}" name="CSV col #" dataDxfId="36"/>
+    <tableColumn id="16" xr3:uid="{1F4E7FF6-264D-41DA-AC14-BAA45F3439C7}" name="XML Element" dataDxfId="35"/>
+    <tableColumn id="10" xr3:uid="{F503FCB6-1F5D-4765-B4AB-F67230BC37A3}" name="XML order #" dataDxfId="34"/>
+    <tableColumn id="2" xr3:uid="{5C52F15D-4AC8-44CE-A401-3402D3CD4152}" name="Data Type" dataDxfId="33"/>
+    <tableColumn id="3" xr3:uid="{FFD71D9C-951A-4BB1-9000-9A1C4C3F71D3}" name="Optionality" dataDxfId="32"/>
+    <tableColumn id="4" xr3:uid="{6FEED7B4-CF3F-4593-BB9F-5CFA5FA5B692}" name="Size" dataDxfId="31"/>
+    <tableColumn id="5" xr3:uid="{563427BF-63BA-491F-9B6F-4E02453C643B}" name="Business Rules" dataDxfId="30"/>
+    <tableColumn id="9" xr3:uid="{A9E34622-C2B4-476B-A018-EABC1256DC10}" name="User Editable" dataDxfId="29"/>
+    <tableColumn id="14" xr3:uid="{9DA3EF2F-E261-414A-B10C-F88F2052640F}" name="Generated" dataDxfId="28"/>
+    <tableColumn id="15" xr3:uid="{AA61284F-4409-4E18-9405-8F2EAA78028A}" name="Format" dataDxfId="27"/>
+    <tableColumn id="13" xr3:uid="{94BA7C53-9CFA-4072-B1A4-7E9CE9D9DDF7}" name="Conditional Formatting" dataDxfId="26"/>
+    <tableColumn id="7" xr3:uid="{22AE72C5-BA89-443A-81AF-BCF4B114454C}" name="Validation" dataDxfId="25"/>
+    <tableColumn id="8" xr3:uid="{5DE66E18-4141-4BDD-B41D-2782AC810F6E}" name="Validation Formula" dataDxfId="24"/>
     <tableColumn id="17" xr3:uid="{3088A6C0-DDC9-48B3-825B-006B2A52B333}" name="Validation Severity" dataDxfId="23"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1314,28 +1219,28 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{05345577-AC31-4B6D-B899-55D66DEB1874}" name="Table2" displayName="Table2" ref="A1:Q28" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{05345577-AC31-4B6D-B899-55D66DEB1874}" name="Table2" displayName="Table2" ref="A1:Q28" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Q28">
     <sortCondition ref="B25:B28"/>
   </sortState>
   <tableColumns count="17">
-    <tableColumn id="7" xr3:uid="{9E32B24E-F549-442D-B6C5-5B5E67078170}" name="Title" dataDxfId="39"/>
-    <tableColumn id="12" xr3:uid="{023EA1AA-B7DF-4814-BFEF-5AB9B0752B95}" name="Excel col #" dataDxfId="38"/>
-    <tableColumn id="1" xr3:uid="{5687DF61-58A8-463A-A7F7-9B8B474466F3}" name="CSV Column Name" dataDxfId="37"/>
-    <tableColumn id="13" xr3:uid="{9E799E78-81C7-4788-BF70-799894A0FACA}" name="CSV col #" dataDxfId="36"/>
-    <tableColumn id="16" xr3:uid="{6872DDE9-C4EA-4656-AE08-1B51AE6AE7D6}" name="XML Element" dataDxfId="35"/>
-    <tableColumn id="11" xr3:uid="{F0D84552-7E57-4362-9DCD-EDC8E4E51415}" name="XML order #" dataDxfId="34"/>
-    <tableColumn id="2" xr3:uid="{E36A262F-69A4-4276-95F1-0FB7FCE8E2AD}" name="Data Type" dataDxfId="33"/>
-    <tableColumn id="3" xr3:uid="{B4F9F589-759B-40AB-BD12-81562C067103}" name="Optionality" dataDxfId="32"/>
-    <tableColumn id="4" xr3:uid="{29CBFF2E-DC73-4812-9BE8-505CDCED923B}" name="Size" dataDxfId="31"/>
-    <tableColumn id="5" xr3:uid="{2FBE4EBA-0896-4EA8-8E6A-9740D712F4CF}" name="Business Rules" dataDxfId="30"/>
-    <tableColumn id="14" xr3:uid="{F6A291D7-463E-4C10-AE63-F46C62F701F1}" name="User Editable" dataDxfId="29"/>
-    <tableColumn id="6" xr3:uid="{4A3A44E5-9909-437B-9914-BD7AF1AC2439}" name="Generated" dataDxfId="28"/>
-    <tableColumn id="15" xr3:uid="{30410F79-D89B-4BAE-852C-7ADB5287310A}" name="Format" dataDxfId="27"/>
-    <tableColumn id="8" xr3:uid="{23D225B6-A3A4-4446-9AD4-7762B64F46FE}" name="Conditional Formatting" dataDxfId="26"/>
-    <tableColumn id="9" xr3:uid="{27D08B50-8012-49E0-9C10-AEB67B99B91B}" name="Validation" dataDxfId="25"/>
-    <tableColumn id="10" xr3:uid="{A301C8EB-BB2A-4524-AF6E-20714C0D7DD5}" name="Validation Formula" dataDxfId="24"/>
-    <tableColumn id="17" xr3:uid="{BAA62FBF-6DD1-4BE3-944E-A7C12DBF01CD}" name="Validation Severity" dataDxfId="22"/>
+    <tableColumn id="7" xr3:uid="{9E32B24E-F549-442D-B6C5-5B5E67078170}" name="Title" dataDxfId="16"/>
+    <tableColumn id="12" xr3:uid="{023EA1AA-B7DF-4814-BFEF-5AB9B0752B95}" name="Excel col #" dataDxfId="15"/>
+    <tableColumn id="1" xr3:uid="{5687DF61-58A8-463A-A7F7-9B8B474466F3}" name="CSV Column Name" dataDxfId="14"/>
+    <tableColumn id="13" xr3:uid="{9E799E78-81C7-4788-BF70-799894A0FACA}" name="CSV col #" dataDxfId="13"/>
+    <tableColumn id="16" xr3:uid="{6872DDE9-C4EA-4656-AE08-1B51AE6AE7D6}" name="XML Element" dataDxfId="12"/>
+    <tableColumn id="11" xr3:uid="{F0D84552-7E57-4362-9DCD-EDC8E4E51415}" name="XML order #" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{E36A262F-69A4-4276-95F1-0FB7FCE8E2AD}" name="Data Type" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{B4F9F589-759B-40AB-BD12-81562C067103}" name="Optionality" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{29CBFF2E-DC73-4812-9BE8-505CDCED923B}" name="Size" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{2FBE4EBA-0896-4EA8-8E6A-9740D712F4CF}" name="Business Rules" dataDxfId="7"/>
+    <tableColumn id="14" xr3:uid="{F6A291D7-463E-4C10-AE63-F46C62F701F1}" name="User Editable" dataDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{4A3A44E5-9909-437B-9914-BD7AF1AC2439}" name="Generated" dataDxfId="5"/>
+    <tableColumn id="15" xr3:uid="{30410F79-D89B-4BAE-852C-7ADB5287310A}" name="Format" dataDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{23D225B6-A3A4-4446-9AD4-7762B64F46FE}" name="Conditional Formatting" dataDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{27D08B50-8012-49E0-9C10-AEB67B99B91B}" name="Validation" dataDxfId="2"/>
+    <tableColumn id="10" xr3:uid="{A301C8EB-BB2A-4524-AF6E-20714C0D7DD5}" name="Validation Formula" dataDxfId="1"/>
+    <tableColumn id="17" xr3:uid="{BAA62FBF-6DD1-4BE3-944E-A7C12DBF01CD}" name="Validation Severity" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight14" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3102,20 +3007,20 @@
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
   <conditionalFormatting sqref="D2:F33">
-    <cfRule type="expression" dxfId="3" priority="14">
+    <cfRule type="expression" dxfId="45" priority="14">
       <formula>LEN($D2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2:L33">
-    <cfRule type="expression" dxfId="2" priority="13">
+    <cfRule type="expression" dxfId="44" priority="13">
       <formula>AND($K2&lt;&gt;"Yes",LEN($L2)=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:Q33">
-    <cfRule type="expression" dxfId="1" priority="3">
+    <cfRule type="expression" dxfId="43" priority="3">
       <formula>$K2="Skip"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="15">
+    <cfRule type="expression" dxfId="42" priority="15">
       <formula>$K2="No"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3475,8 +3380,12 @@
       <c r="N7" s="5" t="s">
         <v>248</v>
       </c>
-      <c r="O7" s="2"/>
-      <c r="P7" s="2"/>
+      <c r="O7" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="P7" s="5" t="s">
+        <v>269</v>
+      </c>
       <c r="Q7" s="2" t="s">
         <v>268</v>
       </c>
@@ -3751,7 +3660,7 @@
         <v>103</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>249</v>
+        <v>109</v>
       </c>
       <c r="I13" s="2">
         <v>30</v>
@@ -3769,8 +3678,12 @@
       <c r="N13" s="5" t="s">
         <v>258</v>
       </c>
-      <c r="O13" s="2"/>
-      <c r="P13" s="2"/>
+      <c r="O13" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="P13" s="5" t="s">
+        <v>269</v>
+      </c>
       <c r="Q13" s="2" t="s">
         <v>268</v>
       </c>
@@ -4448,20 +4361,20 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="L2:L28">
-    <cfRule type="expression" dxfId="17" priority="21">
+    <cfRule type="expression" dxfId="22" priority="21">
       <formula>AND($K2&lt;&gt;"Yes",LEN($L2)=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:F28">
-    <cfRule type="expression" dxfId="16" priority="22">
+    <cfRule type="expression" dxfId="21" priority="22">
       <formula>LEN($D2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:Q28">
-    <cfRule type="expression" dxfId="15" priority="5">
+    <cfRule type="expression" dxfId="20" priority="5">
       <formula>$K2="Skip"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="23">
+    <cfRule type="expression" dxfId="19" priority="23">
       <formula>$K2="No"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Update data validation for analytical method
</commit_message>
<xml_diff>
--- a/specs/Coliform-column-definitions.xlsx
+++ b/specs/Coliform-column-definitions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\xl-ese\specs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4E895DE-E5DB-4BAE-BC87-4CAC9BFD1B71}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D386671-C2D7-46FA-A97F-E4CFCBE47D6A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Coliform Sample" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="617" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="267">
   <si>
     <t>Optionality</t>
   </si>
@@ -839,12 +839,6 @@
     <t>"3100" or "3014"</t>
   </si>
   <si>
-    <t>=LEN(RC14)=0</t>
-  </si>
-  <si>
-    <t>Required</t>
-  </si>
-  <si>
     <t>=LEN(RC13)=0</t>
   </si>
   <si>
@@ -867,9 +861,6 @@
   </si>
   <si>
     <t>=AND(LEN(RC13)="Present",LEN(RC19)=0)</t>
-  </si>
-  <si>
-    <t>=AND(LEN(RC13)="Present",LEN(RC20)=0)</t>
   </si>
   <si>
     <t>RC3 &lt;= x &lt;= TODAY()</t>
@@ -1593,7 +1584,7 @@
         <v>55</v>
       </c>
       <c r="Q1" s="6" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
     </row>
     <row r="2" spans="1:17" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -1633,7 +1624,7 @@
         <v>103</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="O2" s="2" t="s">
         <v>84</v>
@@ -1642,7 +1633,7 @@
         <v>118</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="30" x14ac:dyDescent="0.25">
@@ -1691,7 +1682,7 @@
         <v>225</v>
       </c>
       <c r="Q3" s="7" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
@@ -1742,7 +1733,7 @@
         <v>203</v>
       </c>
       <c r="Q4" s="2" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
@@ -1793,7 +1784,7 @@
         <v>232</v>
       </c>
       <c r="Q5" s="2" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
@@ -1842,7 +1833,7 @@
         <v>125</v>
       </c>
       <c r="Q6" s="2" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
     </row>
     <row r="7" spans="1:17" ht="30" x14ac:dyDescent="0.25">
@@ -1893,7 +1884,7 @@
         <v>119</v>
       </c>
       <c r="Q7" s="2" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
@@ -1942,7 +1933,7 @@
         <v>97</v>
       </c>
       <c r="Q8" s="2" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
     </row>
     <row r="9" spans="1:17" ht="30" x14ac:dyDescent="0.25">
@@ -1991,7 +1982,7 @@
         <v>98</v>
       </c>
       <c r="Q9" s="2" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
     </row>
     <row r="10" spans="1:17" ht="30" x14ac:dyDescent="0.25">
@@ -2042,7 +2033,7 @@
         <v>121</v>
       </c>
       <c r="Q10" s="2" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
     </row>
     <row r="11" spans="1:17" ht="30" x14ac:dyDescent="0.25">
@@ -2093,7 +2084,7 @@
         <v>123</v>
       </c>
       <c r="Q11" s="2" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
@@ -2139,10 +2130,10 @@
         <v>92</v>
       </c>
       <c r="P12" s="5" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="Q12" s="2" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
     </row>
     <row r="13" spans="1:17" ht="30" x14ac:dyDescent="0.25">
@@ -2191,7 +2182,7 @@
         <v>99</v>
       </c>
       <c r="Q13" s="2" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
@@ -2240,7 +2231,7 @@
         <v>120</v>
       </c>
       <c r="Q14" s="2" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
@@ -3115,7 +3106,7 @@
         <v>55</v>
       </c>
       <c r="Q1" s="6" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="30" x14ac:dyDescent="0.25">
@@ -3123,7 +3114,7 @@
         <v>57</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>10</v>
@@ -3311,7 +3302,7 @@
         <v>103</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="I6" s="2">
         <v>1</v>
@@ -3327,7 +3318,7 @@
         <v>103</v>
       </c>
       <c r="N6" s="5" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="O6" s="2" t="s">
         <v>80</v>
@@ -3336,7 +3327,7 @@
         <v>138</v>
       </c>
       <c r="Q6" s="2" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
     </row>
     <row r="7" spans="1:17" ht="30" x14ac:dyDescent="0.25">
@@ -3362,7 +3353,7 @@
         <v>103</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>249</v>
+        <v>112</v>
       </c>
       <c r="I7" s="2">
         <v>30</v>
@@ -3377,17 +3368,15 @@
       <c r="M7" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="N7" s="5" t="s">
-        <v>248</v>
-      </c>
+      <c r="N7" s="5"/>
       <c r="O7" s="2" t="s">
         <v>80</v>
       </c>
       <c r="P7" s="5" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="Q7" s="2" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
@@ -3433,10 +3422,10 @@
         <v>92</v>
       </c>
       <c r="P8" s="5" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="Q8" s="2" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
@@ -3485,7 +3474,7 @@
         <v>125</v>
       </c>
       <c r="Q9" s="2" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
@@ -3531,10 +3520,10 @@
         <v>92</v>
       </c>
       <c r="P10" s="5" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="Q10" s="2" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
@@ -3583,12 +3572,12 @@
         <v>125</v>
       </c>
       <c r="Q11" s="2" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
     </row>
     <row r="12" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B12" s="2">
         <v>19</v>
@@ -3625,7 +3614,7 @@
         <v>103</v>
       </c>
       <c r="N12" s="5" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="O12" s="2" t="s">
         <v>80</v>
@@ -3634,12 +3623,12 @@
         <v>138</v>
       </c>
       <c r="Q12" s="2" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
     </row>
     <row r="13" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B13" s="2">
         <v>20</v>
@@ -3660,7 +3649,7 @@
         <v>103</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="I13" s="2">
         <v>30</v>
@@ -3675,22 +3664,20 @@
       <c r="M13" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="N13" s="5" t="s">
-        <v>258</v>
-      </c>
+      <c r="N13" s="5"/>
       <c r="O13" s="2" t="s">
         <v>80</v>
       </c>
       <c r="P13" s="5" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="Q13" s="2" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B14" s="2">
         <v>21</v>
@@ -3731,15 +3718,15 @@
         <v>92</v>
       </c>
       <c r="P14" s="5" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="Q14" s="2" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B15" s="2">
         <v>22</v>
@@ -3783,12 +3770,12 @@
         <v>125</v>
       </c>
       <c r="Q15" s="2" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B16" s="2">
         <v>23</v>
@@ -3829,15 +3816,15 @@
         <v>92</v>
       </c>
       <c r="P16" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="Q16" s="2" t="s">
         <v>262</v>
-      </c>
-      <c r="Q16" s="2" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B17" s="2">
         <v>24</v>
@@ -3881,7 +3868,7 @@
         <v>125</v>
       </c>
       <c r="Q17" s="2" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update analytical method lists
</commit_message>
<xml_diff>
--- a/specs/Coliform-column-definitions.xlsx
+++ b/specs/Coliform-column-definitions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\xl-ese\specs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D386671-C2D7-46FA-A97F-E4CFCBE47D6A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3523DA1C-BB3B-4A72-97E8-C7F21B8A5789}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Coliform Sample" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="268">
   <si>
     <t>Optionality</t>
   </si>
@@ -893,7 +893,10 @@
     <t>None</t>
   </si>
   <si>
-    <t>=MethodsList</t>
+    <t>=EColiMethodsList</t>
+  </si>
+  <si>
+    <t>=ColiformMethodsList</t>
   </si>
 </sst>
 </file>
@@ -3373,7 +3376,7 @@
         <v>80</v>
       </c>
       <c r="P7" s="5" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="Q7" s="2" t="s">
         <v>265</v>

</xml_diff>

<commit_message>
Combine the sampling point ID, Type, and Repeat Location fields
</commit_message>
<xml_diff>
--- a/specs/Coliform-column-definitions.xlsx
+++ b/specs/Coliform-column-definitions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\xl-ese\specs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3523DA1C-BB3B-4A72-97E8-C7F21B8A5789}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58DF9957-9F08-4EF8-A1FD-04087ACFFC04}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Coliform Sample" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="263">
   <si>
     <t>Optionality</t>
   </si>
@@ -331,9 +331,6 @@
     <t>=SampleTypesList</t>
   </si>
   <si>
-    <t>=RepeatLocationsList</t>
-  </si>
-  <si>
     <t>&lt;= 40</t>
   </si>
   <si>
@@ -392,9 +389,6 @@
   </si>
   <si>
     <t>1 &lt;= x &lt;= 10</t>
-  </si>
-  <si>
-    <t>1 &lt;= x &lt;= 12</t>
   </si>
   <si>
     <t>Between 0.01 and 99.0</t>
@@ -769,9 +763,6 @@
     <t>=LEN(RC3)=0</t>
   </si>
   <si>
-    <t>=LEN(RC6)=0</t>
-  </si>
-  <si>
     <t>=LEN(RC2)=0</t>
   </si>
   <si>
@@ -815,18 +806,6 @@
     <t>=LEN(RC5)=0</t>
   </si>
   <si>
-    <t>=AND(RC6="Repeat",LEN(RC7)=0)
-=AND(RC6&lt;&gt;"",RC6&lt;&gt;"Repeat")</t>
-  </si>
-  <si>
-    <t>=AND(RC6="Repeat",LEN(RC8)=0)
-=AND(RC6&lt;&gt;"",RC6&lt;&gt;"Repeat")</t>
-  </si>
-  <si>
-    <t>=AND(RC6="Repeat",LEN(RC9)=0)
-=AND(RC6&lt;&gt;"",RC6&lt;&gt;"Repeat")</t>
-  </si>
-  <si>
     <t>[1]</t>
   </si>
   <si>
@@ -897,6 +876,10 @@
   </si>
   <si>
     <t>=ColiformMethodsList</t>
+  </si>
+  <si>
+    <t>=AND(LEFT(RC5,6)="Repeat",LEN(RC)=0)
+=AND(RC5&lt;&gt;"",LEFT(RC5,6)&lt;&gt;"Repeat")</t>
   </si>
 </sst>
 </file>
@@ -1528,7 +1511,7 @@
     <col min="11" max="11" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="26.28515625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="33" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="37" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="48.85546875" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="10.140625" bestFit="1" customWidth="1"/>
@@ -1542,22 +1525,22 @@
         <v>53</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H1" s="6" t="s">
         <v>0</v>
@@ -1569,7 +1552,7 @@
         <v>2</v>
       </c>
       <c r="K1" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="L1" s="6" t="s">
         <v>79</v>
@@ -1587,7 +1570,7 @@
         <v>55</v>
       </c>
       <c r="Q1" s="6" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
     </row>
     <row r="2" spans="1:17" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -1604,16 +1587,16 @@
         <v>7</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="F2" s="13">
         <v>1</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I2" s="3">
         <v>10</v>
@@ -1624,19 +1607,19 @@
       </c>
       <c r="L2" s="2"/>
       <c r="M2" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="O2" s="2" t="s">
         <v>84</v>
       </c>
       <c r="P2" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="30" x14ac:dyDescent="0.25">
@@ -1653,16 +1636,16 @@
         <v>2</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="F3" s="2">
         <v>4</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I3" s="3">
         <v>20</v>
@@ -1673,19 +1656,19 @@
       </c>
       <c r="L3" s="2"/>
       <c r="M3" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="O3" s="2" t="s">
         <v>84</v>
       </c>
       <c r="P3" s="5" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="Q3" s="7" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
@@ -1702,16 +1685,16 @@
         <v>4</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="F4" s="2">
         <v>5</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I4" s="3">
         <v>9</v>
@@ -1724,19 +1707,19 @@
       </c>
       <c r="L4" s="2"/>
       <c r="M4" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="N4" s="5" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="O4" s="2" t="s">
         <v>84</v>
       </c>
       <c r="P4" s="5" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="Q4" s="2" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
@@ -1753,7 +1736,7 @@
         <v>13</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F5" s="7">
         <v>16</v>
@@ -1762,7 +1745,7 @@
         <v>92</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I5" s="3">
         <v>8</v>
@@ -1778,16 +1761,16 @@
         <v>96</v>
       </c>
       <c r="N5" s="5" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="O5" s="2" t="s">
         <v>78</v>
       </c>
       <c r="P5" s="5" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="Q5" s="2" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
@@ -1804,7 +1787,7 @@
         <v>14</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="F6" s="2">
         <v>17</v>
@@ -1813,13 +1796,13 @@
         <v>93</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I6" s="3">
         <v>4</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="K6" s="2" t="s">
         <v>82</v>
@@ -1833,10 +1816,10 @@
         <v>93</v>
       </c>
       <c r="P6" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="Q6" s="2" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
     </row>
     <row r="7" spans="1:17" ht="30" x14ac:dyDescent="0.25">
@@ -1853,16 +1836,16 @@
         <v>9</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="F7" s="13">
         <v>21</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I7" s="3">
         <v>12</v>
@@ -1875,19 +1858,19 @@
       </c>
       <c r="L7" s="2"/>
       <c r="M7" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="N7" s="5" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="O7" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="P7" s="2" t="s">
-        <v>119</v>
+        <v>80</v>
+      </c>
+      <c r="P7" s="5" t="s">
+        <v>97</v>
       </c>
       <c r="Q7" s="2" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
@@ -1895,7 +1878,7 @@
         <v>64</v>
       </c>
       <c r="B8" s="2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>21</v>
@@ -1904,16 +1887,16 @@
         <v>15</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="F8" s="7">
         <v>8</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I8" s="3">
         <v>2</v>
@@ -1924,10 +1907,10 @@
       </c>
       <c r="L8" s="2"/>
       <c r="M8" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="N8" s="5" t="s">
-        <v>227</v>
+        <v>237</v>
       </c>
       <c r="O8" s="2" t="s">
         <v>80</v>
@@ -1936,7 +1919,7 @@
         <v>97</v>
       </c>
       <c r="Q8" s="2" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
     </row>
     <row r="9" spans="1:17" ht="30" x14ac:dyDescent="0.25">
@@ -1944,7 +1927,7 @@
         <v>65</v>
       </c>
       <c r="B9" s="2">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>22</v>
@@ -1953,16 +1936,16 @@
         <v>16</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="F9" s="6">
         <v>22</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I9" s="3">
         <v>2</v>
@@ -1973,27 +1956,27 @@
       </c>
       <c r="L9" s="2"/>
       <c r="M9" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="N9" s="4" t="s">
-        <v>241</v>
+        <v>102</v>
+      </c>
+      <c r="N9" s="5" t="s">
+        <v>237</v>
       </c>
       <c r="O9" s="2" t="s">
         <v>80</v>
       </c>
       <c r="P9" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="Q9" s="2" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
     </row>
     <row r="10" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B10" s="2">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>30</v>
@@ -2002,16 +1985,16 @@
         <v>29</v>
       </c>
       <c r="E10" s="13" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="F10" s="13">
         <v>11</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I10" s="3">
         <v>20</v>
@@ -2024,27 +2007,27 @@
       </c>
       <c r="L10" s="2"/>
       <c r="M10" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="N10" s="4" t="s">
-        <v>242</v>
+        <v>262</v>
       </c>
       <c r="O10" s="2" t="s">
         <v>78</v>
       </c>
       <c r="P10" s="5" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="Q10" s="2" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
     </row>
     <row r="11" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B11" s="2">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>32</v>
@@ -2053,7 +2036,7 @@
         <v>30</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="F11" s="6">
         <v>12</v>
@@ -2062,7 +2045,7 @@
         <v>92</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I11" s="3">
         <v>8</v>
@@ -2078,16 +2061,16 @@
         <v>96</v>
       </c>
       <c r="N11" s="4" t="s">
-        <v>243</v>
+        <v>262</v>
       </c>
       <c r="O11" s="2" t="s">
         <v>78</v>
       </c>
       <c r="P11" s="5" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="Q11" s="2" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
@@ -2095,7 +2078,7 @@
         <v>66</v>
       </c>
       <c r="B12" s="2">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>23</v>
@@ -2104,7 +2087,7 @@
         <v>17</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="F12" s="7">
         <v>18</v>
@@ -2113,7 +2096,7 @@
         <v>92</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I12" s="3">
         <v>8</v>
@@ -2133,18 +2116,18 @@
         <v>92</v>
       </c>
       <c r="P12" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="Q12" s="2" t="s">
         <v>256</v>
-      </c>
-      <c r="Q12" s="2" t="s">
-        <v>262</v>
       </c>
     </row>
     <row r="13" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B13" s="2">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>25</v>
@@ -2153,16 +2136,16 @@
         <v>18</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="F13" s="6">
         <v>15</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I13" s="3">
         <v>40</v>
@@ -2175,25 +2158,25 @@
       </c>
       <c r="L13" s="2"/>
       <c r="M13" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="N13" s="2"/>
       <c r="O13" s="2" t="s">
         <v>84</v>
       </c>
       <c r="P13" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Q13" s="2" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B14" s="2">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>33</v>
@@ -2202,16 +2185,16 @@
         <v>22</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F14" s="7">
         <v>19</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I14" s="3" t="s">
         <v>34</v>
@@ -2224,22 +2207,22 @@
       </c>
       <c r="L14" s="2"/>
       <c r="M14" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="N14" s="2"/>
       <c r="O14" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="P14" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="Q14" s="2" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B15" s="7"/>
       <c r="C15" s="7" t="s">
@@ -2251,10 +2234,10 @@
       <c r="E15" s="7"/>
       <c r="F15" s="7"/>
       <c r="G15" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I15" s="8">
         <v>20</v>
@@ -2286,29 +2269,29 @@
         <v>3</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="F16" s="7">
         <v>3</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I16" s="3">
         <v>20</v>
       </c>
       <c r="J16" s="2"/>
       <c r="K16" s="2" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="L16" s="11" t="s">
         <v>87</v>
       </c>
       <c r="M16" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="N16" s="2"/>
       <c r="O16" s="2" t="s">
@@ -2331,36 +2314,36 @@
         <v>5</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="F17" s="7">
         <v>10</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I17" s="3">
         <v>1</v>
       </c>
       <c r="J17" s="2"/>
       <c r="K17" s="2" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="M17" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="N17" s="5"/>
       <c r="O17" s="2" t="s">
         <v>80</v>
       </c>
       <c r="P17" s="5" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="Q17" s="2"/>
     </row>
@@ -2376,16 +2359,16 @@
         <v>6</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="F18" s="6">
         <v>2</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I18" s="3">
         <v>10</v>
@@ -2415,16 +2398,16 @@
         <v>8</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="F19" s="2">
         <v>6</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I19" s="3">
         <v>10</v>
@@ -2433,26 +2416,26 @@
         <v>52</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="L19" s="5" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="M19" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="N19" s="5"/>
       <c r="O19" s="2" t="s">
         <v>84</v>
       </c>
       <c r="P19" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="Q19" s="2"/>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" s="2" t="s">
@@ -2462,14 +2445,14 @@
         <v>10</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="F20" s="2"/>
       <c r="G20" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I20" s="3">
         <v>40</v>
@@ -2499,16 +2482,16 @@
         <v>11</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="F21" s="7">
         <v>7</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I21" s="3">
         <v>2</v>
@@ -2540,16 +2523,16 @@
         <v>12</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="F22" s="2">
         <v>9</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I22" s="3">
         <v>1</v>
@@ -2558,20 +2541,20 @@
         <v>17</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="L22" s="2" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="M22" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="N22" s="5"/>
       <c r="O22" s="2" t="s">
         <v>80</v>
       </c>
       <c r="P22" s="5" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="Q22" s="2"/>
     </row>
@@ -2587,14 +2570,14 @@
         <v>19</v>
       </c>
       <c r="E23" s="13" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F23" s="13"/>
       <c r="G23" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I23" s="3">
         <v>9</v>
@@ -2624,14 +2607,14 @@
         <v>20</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F24" s="7"/>
       <c r="G24" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I24" s="3">
         <v>2</v>
@@ -2661,14 +2644,14 @@
         <v>21</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F25" s="6"/>
       <c r="G25" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I25" s="3">
         <v>12</v>
@@ -2688,7 +2671,7 @@
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" s="2" t="s">
@@ -2698,16 +2681,16 @@
         <v>23</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F26" s="7">
         <v>20</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I26" s="3" t="s">
         <v>34</v>
@@ -2716,20 +2699,20 @@
         <v>37</v>
       </c>
       <c r="K26" s="2" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="L26" s="11" t="s">
         <v>87</v>
       </c>
       <c r="M26" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="N26" s="2"/>
       <c r="O26" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="P26" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="Q26" s="2"/>
     </row>
@@ -2745,14 +2728,14 @@
         <v>24</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F27" s="7"/>
       <c r="G27" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I27" s="3" t="s">
         <v>39</v>
@@ -2782,14 +2765,14 @@
         <v>25</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F28" s="7"/>
       <c r="G28" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I28" s="3"/>
       <c r="J28" s="2"/>
@@ -2817,14 +2800,14 @@
         <v>26</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F29" s="7"/>
       <c r="G29" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I29" s="3" t="s">
         <v>42</v>
@@ -2854,14 +2837,14 @@
         <v>27</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F30" s="7"/>
       <c r="G30" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I30" s="3" t="s">
         <v>44</v>
@@ -2891,14 +2874,14 @@
         <v>28</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F31" s="7"/>
       <c r="G31" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I31" s="3" t="s">
         <v>46</v>
@@ -2928,16 +2911,16 @@
         <v>31</v>
       </c>
       <c r="E32" s="13" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="F32" s="13">
         <v>13</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I32" s="3">
         <v>10</v>
@@ -2949,7 +2932,7 @@
         <v>81</v>
       </c>
       <c r="L32" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="M32" s="2"/>
       <c r="N32" s="2"/>
@@ -2969,16 +2952,16 @@
         <v>32</v>
       </c>
       <c r="E33" s="13" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F33" s="13">
         <v>14</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I33" s="3">
         <v>10</v>
@@ -2990,7 +2973,7 @@
         <v>81</v>
       </c>
       <c r="L33" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="M33" s="2"/>
       <c r="N33" s="2"/>
@@ -3064,22 +3047,22 @@
         <v>53</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H1" s="6" t="s">
         <v>0</v>
@@ -3091,7 +3074,7 @@
         <v>2</v>
       </c>
       <c r="K1" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="L1" s="6" t="s">
         <v>79</v>
@@ -3109,7 +3092,7 @@
         <v>55</v>
       </c>
       <c r="Q1" s="6" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="30" x14ac:dyDescent="0.25">
@@ -3117,7 +3100,7 @@
         <v>57</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>10</v>
@@ -3126,16 +3109,16 @@
         <v>6</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="F2" s="13">
         <v>5</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I2" s="2">
         <v>10</v>
@@ -3146,7 +3129,7 @@
       </c>
       <c r="L2" s="2"/>
       <c r="M2" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
@@ -3158,7 +3141,7 @@
         <v>56</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>5</v>
@@ -3167,29 +3150,29 @@
         <v>2</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="F3" s="2">
         <v>1</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I3" s="2">
         <v>20</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>82</v>
       </c>
       <c r="L3" s="2"/>
       <c r="M3" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="N3" s="4"/>
       <c r="O3" s="2"/>
@@ -3201,7 +3184,7 @@
         <v>60</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>7</v>
@@ -3210,29 +3193,29 @@
         <v>4</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="F4" s="2">
         <v>2</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I4" s="2">
         <v>9</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>82</v>
       </c>
       <c r="L4" s="2"/>
       <c r="M4" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="N4" s="5"/>
       <c r="O4" s="2"/>
@@ -3244,7 +3227,7 @@
         <v>90</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>18</v>
@@ -3253,7 +3236,7 @@
         <v>3</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F5" s="2">
         <v>3</v>
@@ -3262,13 +3245,13 @@
         <v>92</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I5" s="2">
         <v>8</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="K5" s="2" t="s">
         <v>82</v>
@@ -3284,119 +3267,119 @@
     </row>
     <row r="6" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B6" s="2">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D6" s="2">
         <v>18</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="F6" s="6">
         <v>13</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I6" s="2">
         <v>1</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="K6" s="2" t="s">
         <v>82</v>
       </c>
       <c r="L6" s="2"/>
       <c r="M6" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="N6" s="5" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="O6" s="2" t="s">
         <v>80</v>
       </c>
       <c r="P6" s="5" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="Q6" s="2" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
     </row>
     <row r="7" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B7" s="2">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D7" s="2">
         <v>15</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="F7" s="6">
         <v>6</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I7" s="2">
         <v>30</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="K7" s="2" t="s">
         <v>82</v>
       </c>
       <c r="L7" s="2"/>
       <c r="M7" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="N7" s="5"/>
       <c r="O7" s="2" t="s">
         <v>80</v>
       </c>
       <c r="P7" s="5" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="Q7" s="2" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B8" s="2">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D8" s="2">
         <v>8</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="F8" s="2">
         <v>8</v>
@@ -3405,13 +3388,13 @@
         <v>92</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I8" s="2">
         <v>8</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="K8" s="2" t="s">
         <v>82</v>
@@ -3425,27 +3408,27 @@
         <v>92</v>
       </c>
       <c r="P8" s="5" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="Q8" s="2" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B9" s="2">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D9" s="2">
         <v>9</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="F9" s="2">
         <v>9</v>
@@ -3454,13 +3437,13 @@
         <v>93</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I9" s="2">
         <v>4</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="K9" s="2" t="s">
         <v>82</v>
@@ -3474,27 +3457,27 @@
         <v>93</v>
       </c>
       <c r="P9" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="Q9" s="2" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B10" s="2">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D10" s="2">
         <v>10</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="F10" s="2">
         <v>10</v>
@@ -3503,13 +3486,13 @@
         <v>92</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I10" s="2">
         <v>8</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="K10" s="2" t="s">
         <v>82</v>
@@ -3523,27 +3506,27 @@
         <v>92</v>
       </c>
       <c r="P10" s="5" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="Q10" s="2" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B11" s="2">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D11" s="2">
         <v>11</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F11" s="2">
         <v>11</v>
@@ -3552,13 +3535,13 @@
         <v>93</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I11" s="2">
         <v>4</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="K11" s="2" t="s">
         <v>82</v>
@@ -3572,127 +3555,127 @@
         <v>93</v>
       </c>
       <c r="P11" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="Q11" s="2" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
     </row>
     <row r="12" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="B12" s="2">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D12" s="2">
         <v>18</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="F12" s="6">
         <v>13</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I12" s="2">
         <v>1</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="K12" s="2" t="s">
         <v>82</v>
       </c>
       <c r="L12" s="2"/>
       <c r="M12" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="N12" s="5" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="O12" s="2" t="s">
         <v>80</v>
       </c>
       <c r="P12" s="5" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="Q12" s="2" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
     </row>
     <row r="13" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="B13" s="2">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D13" s="2">
         <v>15</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="F13" s="6">
         <v>6</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I13" s="2">
         <v>30</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="K13" s="2" t="s">
         <v>82</v>
       </c>
       <c r="L13" s="2"/>
       <c r="M13" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="N13" s="5"/>
       <c r="O13" s="2" t="s">
         <v>80</v>
       </c>
       <c r="P13" s="5" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="Q13" s="2" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="B14" s="2">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D14" s="2">
         <v>8</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="F14" s="2">
         <v>8</v>
@@ -3701,13 +3684,13 @@
         <v>92</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I14" s="2">
         <v>8</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="K14" s="2" t="s">
         <v>82</v>
@@ -3721,27 +3704,27 @@
         <v>92</v>
       </c>
       <c r="P14" s="5" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="Q14" s="2" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="B15" s="2">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D15" s="2">
         <v>9</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="F15" s="2">
         <v>9</v>
@@ -3750,13 +3733,13 @@
         <v>93</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I15" s="2">
         <v>4</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="K15" s="2" t="s">
         <v>82</v>
@@ -3770,27 +3753,27 @@
         <v>93</v>
       </c>
       <c r="P15" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="Q15" s="2" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="B16" s="2">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D16" s="2">
         <v>10</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="F16" s="2">
         <v>10</v>
@@ -3799,13 +3782,13 @@
         <v>92</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I16" s="2">
         <v>8</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="K16" s="2" t="s">
         <v>82</v>
@@ -3819,27 +3802,27 @@
         <v>92</v>
       </c>
       <c r="P16" s="5" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="Q16" s="2" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="B17" s="2">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D17" s="2">
         <v>11</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F17" s="2">
         <v>11</v>
@@ -3848,13 +3831,13 @@
         <v>93</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I17" s="2">
         <v>4</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="K17" s="2" t="s">
         <v>82</v>
@@ -3868,15 +3851,15 @@
         <v>93</v>
       </c>
       <c r="P17" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="Q17" s="2" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" s="2" t="s">
@@ -3888,22 +3871,22 @@
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I18" s="2">
         <v>20</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="K18" s="2" t="s">
         <v>81</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="M18" s="2"/>
       <c r="N18" s="2"/>
@@ -3923,16 +3906,16 @@
         <v>5</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="F19" s="6">
         <v>4</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I19" s="2">
         <v>10</v>
@@ -3942,7 +3925,7 @@
         <v>81</v>
       </c>
       <c r="L19" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="M19" s="2"/>
       <c r="N19" s="2"/>
@@ -3952,41 +3935,41 @@
     </row>
     <row r="20" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" s="2" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D20" s="2">
         <v>7</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="F20" s="6">
         <v>12</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I20" s="2">
         <v>4</v>
       </c>
       <c r="J20" s="6" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="K20" s="2" t="s">
         <v>81</v>
       </c>
       <c r="L20" s="2" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="M20" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="N20" s="4"/>
       <c r="O20" s="2"/>
@@ -3995,17 +3978,17 @@
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D21" s="2">
         <v>12</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="F21" s="2">
         <v>17</v>
@@ -4014,17 +3997,17 @@
         <v>92</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I21" s="2">
         <v>8</v>
       </c>
       <c r="J21" s="2"/>
       <c r="K21" s="2" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="L21" s="5" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="M21" s="2" t="s">
         <v>96</v>
@@ -4034,44 +4017,44 @@
         <v>92</v>
       </c>
       <c r="P21" s="5" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="Q21" s="2"/>
     </row>
     <row r="22" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D22" s="2">
         <v>13</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="F22" s="6">
         <v>18</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I22" s="2">
         <v>1</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="K22" s="2" t="s">
         <v>81</v>
       </c>
       <c r="L22" s="2" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="M22" s="2"/>
       <c r="N22" s="2"/>
@@ -4081,11 +4064,11 @@
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D23" s="2">
         <v>14</v>
@@ -4093,10 +4076,10 @@
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
       <c r="G23" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I23" s="2">
         <v>2</v>
@@ -4116,58 +4099,58 @@
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D24" s="2">
         <v>16</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="F24" s="2">
         <v>7</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I24" s="2">
         <v>9</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="K24" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="L24" s="5" t="s">
         <v>234</v>
       </c>
-      <c r="L24" s="5" t="s">
-        <v>237</v>
-      </c>
       <c r="M24" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="N24" s="2"/>
       <c r="O24" s="2" t="s">
         <v>80</v>
       </c>
       <c r="P24" s="5" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="Q24" s="2"/>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D25" s="2">
         <v>17</v>
@@ -4175,177 +4158,177 @@
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
       <c r="G25" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I25" s="2">
         <v>4</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="K25" s="2" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="L25" s="11" t="s">
         <v>87</v>
       </c>
       <c r="M25" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="N25" s="2"/>
       <c r="O25" s="2" t="s">
         <v>80</v>
       </c>
       <c r="P25" s="5" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="Q25" s="2"/>
     </row>
     <row r="26" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D26" s="2">
         <v>20</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="F26" s="6">
         <v>15</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I26" s="2">
         <v>10</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="K26" s="2" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="L26" s="11" t="s">
         <v>87</v>
       </c>
       <c r="M26" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="N26" s="4" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="O26" s="2" t="s">
         <v>80</v>
       </c>
       <c r="P26" s="5" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="Q26" s="2"/>
     </row>
     <row r="27" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" s="2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D27" s="2">
         <v>27</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="F27" s="6">
         <v>16</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I27" s="2">
         <v>9</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="L27" s="11" t="s">
         <v>87</v>
       </c>
       <c r="M27" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="N27" s="4" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="O27" s="2" t="s">
         <v>80</v>
       </c>
       <c r="P27" s="5" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="Q27" s="2"/>
     </row>
     <row r="28" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D28" s="2">
         <v>28</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="F28" s="6">
         <v>14</v>
       </c>
       <c r="G28" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="I28" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="H28" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="I28" s="2" t="s">
-        <v>129</v>
-      </c>
       <c r="J28" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="K28" s="2" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="L28" s="11" t="s">
         <v>87</v>
       </c>
       <c r="M28" s="2"/>
       <c r="N28" s="4" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="O28" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="P28" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="Q28" s="2"/>
     </row>

</xml_diff>

<commit_message>
Add Collection Address field
</commit_message>
<xml_diff>
--- a/specs/Coliform-column-definitions.xlsx
+++ b/specs/Coliform-column-definitions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\xl-ese\specs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58DF9957-9F08-4EF8-A1FD-04087ACFFC04}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E0BE6FA-EC5E-43AD-B2FB-38EFB014F433}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Coliform Sample" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="626" uniqueCount="268">
   <si>
     <t>Optionality</t>
   </si>
@@ -818,9 +818,6 @@
     <t>"3100" or "3014"</t>
   </si>
   <si>
-    <t>=LEN(RC13)=0</t>
-  </si>
-  <si>
     <t>Microbe Presence E</t>
   </si>
   <si>
@@ -837,9 +834,6 @@
   </si>
   <si>
     <t>Analysis End Time E</t>
-  </si>
-  <si>
-    <t>=AND(LEN(RC13)="Present",LEN(RC19)=0)</t>
   </si>
   <si>
     <t>RC3 &lt;= x &lt;= TODAY()</t>
@@ -880,6 +874,29 @@
   <si>
     <t>=AND(LEFT(RC5,6)="Repeat",LEN(RC)=0)
 =AND(RC5&lt;&gt;"",LEFT(RC5,6)&lt;&gt;"Repeat")</t>
+  </si>
+  <si>
+    <t>B_COLLECTION_ADDRS</t>
+  </si>
+  <si>
+    <t>Collection Address</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>SampleLocationIdentification &gt; 
+SampleLocationCollectionAddress</t>
+  </si>
+  <si>
+    <t>&lt;= 200</t>
+  </si>
+  <si>
+    <t>=LEN(RC12)=0</t>
+  </si>
+  <si>
+    <t>=AND(RC12="Present",LEN(RC18)=0)
+=RC12="Absent"</t>
   </si>
 </sst>
 </file>
@@ -966,64 +983,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="46">
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
+  <dxfs count="54">
     <dxf>
       <fill>
         <patternFill>
@@ -1051,6 +1011,147 @@
           <bgColor theme="7" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1120,34 +1221,6 @@
     </dxf>
     <dxf>
       <alignment vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1168,56 +1241,56 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{636125F0-68A9-4682-81D8-01BD3AB67D26}" name="Table1" displayName="Table1" ref="A1:Q33" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40">
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Q33">
-    <sortCondition ref="B18:B33"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{636125F0-68A9-4682-81D8-01BD3AB67D26}" name="Table1" displayName="Table1" ref="A1:Q34" totalsRowShown="0" headerRowDxfId="53" dataDxfId="52">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Q34">
+    <sortCondition ref="B15:B34"/>
   </sortState>
   <tableColumns count="17">
-    <tableColumn id="6" xr3:uid="{57EF6AB6-6C4C-4170-BD9B-BF376C46C5DF}" name="Title" dataDxfId="39"/>
-    <tableColumn id="12" xr3:uid="{BFDB40C3-C9ED-4560-81A1-344ECAE248C8}" name="Excel col #" dataDxfId="38"/>
-    <tableColumn id="1" xr3:uid="{3193A6D3-813B-4494-AEED-01D6509FCA0D}" name="CSV Column Name" dataDxfId="37"/>
-    <tableColumn id="11" xr3:uid="{057EA208-1889-4E3C-A179-F312337D9867}" name="CSV col #" dataDxfId="36"/>
-    <tableColumn id="16" xr3:uid="{1F4E7FF6-264D-41DA-AC14-BAA45F3439C7}" name="XML Element" dataDxfId="35"/>
-    <tableColumn id="10" xr3:uid="{F503FCB6-1F5D-4765-B4AB-F67230BC37A3}" name="XML order #" dataDxfId="34"/>
-    <tableColumn id="2" xr3:uid="{5C52F15D-4AC8-44CE-A401-3402D3CD4152}" name="Data Type" dataDxfId="33"/>
-    <tableColumn id="3" xr3:uid="{FFD71D9C-951A-4BB1-9000-9A1C4C3F71D3}" name="Optionality" dataDxfId="32"/>
-    <tableColumn id="4" xr3:uid="{6FEED7B4-CF3F-4593-BB9F-5CFA5FA5B692}" name="Size" dataDxfId="31"/>
-    <tableColumn id="5" xr3:uid="{563427BF-63BA-491F-9B6F-4E02453C643B}" name="Business Rules" dataDxfId="30"/>
-    <tableColumn id="9" xr3:uid="{A9E34622-C2B4-476B-A018-EABC1256DC10}" name="User Editable" dataDxfId="29"/>
-    <tableColumn id="14" xr3:uid="{9DA3EF2F-E261-414A-B10C-F88F2052640F}" name="Generated" dataDxfId="28"/>
-    <tableColumn id="15" xr3:uid="{AA61284F-4409-4E18-9405-8F2EAA78028A}" name="Format" dataDxfId="27"/>
-    <tableColumn id="13" xr3:uid="{94BA7C53-9CFA-4072-B1A4-7E9CE9D9DDF7}" name="Conditional Formatting" dataDxfId="26"/>
-    <tableColumn id="7" xr3:uid="{22AE72C5-BA89-443A-81AF-BCF4B114454C}" name="Validation" dataDxfId="25"/>
-    <tableColumn id="8" xr3:uid="{5DE66E18-4141-4BDD-B41D-2782AC810F6E}" name="Validation Formula" dataDxfId="24"/>
-    <tableColumn id="17" xr3:uid="{3088A6C0-DDC9-48B3-825B-006B2A52B333}" name="Validation Severity" dataDxfId="23"/>
+    <tableColumn id="6" xr3:uid="{57EF6AB6-6C4C-4170-BD9B-BF376C46C5DF}" name="Title" dataDxfId="51"/>
+    <tableColumn id="12" xr3:uid="{BFDB40C3-C9ED-4560-81A1-344ECAE248C8}" name="Excel col #" dataDxfId="50"/>
+    <tableColumn id="1" xr3:uid="{3193A6D3-813B-4494-AEED-01D6509FCA0D}" name="CSV Column Name" dataDxfId="49"/>
+    <tableColumn id="11" xr3:uid="{057EA208-1889-4E3C-A179-F312337D9867}" name="CSV col #" dataDxfId="48"/>
+    <tableColumn id="16" xr3:uid="{1F4E7FF6-264D-41DA-AC14-BAA45F3439C7}" name="XML Element" dataDxfId="47"/>
+    <tableColumn id="10" xr3:uid="{F503FCB6-1F5D-4765-B4AB-F67230BC37A3}" name="XML order #" dataDxfId="46"/>
+    <tableColumn id="2" xr3:uid="{5C52F15D-4AC8-44CE-A401-3402D3CD4152}" name="Data Type" dataDxfId="45"/>
+    <tableColumn id="3" xr3:uid="{FFD71D9C-951A-4BB1-9000-9A1C4C3F71D3}" name="Optionality" dataDxfId="44"/>
+    <tableColumn id="4" xr3:uid="{6FEED7B4-CF3F-4593-BB9F-5CFA5FA5B692}" name="Size" dataDxfId="43"/>
+    <tableColumn id="5" xr3:uid="{563427BF-63BA-491F-9B6F-4E02453C643B}" name="Business Rules" dataDxfId="42"/>
+    <tableColumn id="9" xr3:uid="{A9E34622-C2B4-476B-A018-EABC1256DC10}" name="User Editable" dataDxfId="41"/>
+    <tableColumn id="14" xr3:uid="{9DA3EF2F-E261-414A-B10C-F88F2052640F}" name="Generated" dataDxfId="40"/>
+    <tableColumn id="15" xr3:uid="{AA61284F-4409-4E18-9405-8F2EAA78028A}" name="Format" dataDxfId="39"/>
+    <tableColumn id="13" xr3:uid="{94BA7C53-9CFA-4072-B1A4-7E9CE9D9DDF7}" name="Conditional Formatting" dataDxfId="38"/>
+    <tableColumn id="7" xr3:uid="{22AE72C5-BA89-443A-81AF-BCF4B114454C}" name="Validation" dataDxfId="37"/>
+    <tableColumn id="8" xr3:uid="{5DE66E18-4141-4BDD-B41D-2782AC810F6E}" name="Validation Formula" dataDxfId="36"/>
+    <tableColumn id="17" xr3:uid="{3088A6C0-DDC9-48B3-825B-006B2A52B333}" name="Validation Severity" dataDxfId="35"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{05345577-AC31-4B6D-B899-55D66DEB1874}" name="Table2" displayName="Table2" ref="A1:Q28" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{05345577-AC31-4B6D-B899-55D66DEB1874}" name="Table2" displayName="Table2" ref="A1:Q28" totalsRowShown="0" headerRowDxfId="34" dataDxfId="33">
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Q28">
-    <sortCondition ref="B25:B28"/>
+    <sortCondition ref="B18:B28"/>
   </sortState>
   <tableColumns count="17">
-    <tableColumn id="7" xr3:uid="{9E32B24E-F549-442D-B6C5-5B5E67078170}" name="Title" dataDxfId="16"/>
-    <tableColumn id="12" xr3:uid="{023EA1AA-B7DF-4814-BFEF-5AB9B0752B95}" name="Excel col #" dataDxfId="15"/>
-    <tableColumn id="1" xr3:uid="{5687DF61-58A8-463A-A7F7-9B8B474466F3}" name="CSV Column Name" dataDxfId="14"/>
-    <tableColumn id="13" xr3:uid="{9E799E78-81C7-4788-BF70-799894A0FACA}" name="CSV col #" dataDxfId="13"/>
-    <tableColumn id="16" xr3:uid="{6872DDE9-C4EA-4656-AE08-1B51AE6AE7D6}" name="XML Element" dataDxfId="12"/>
-    <tableColumn id="11" xr3:uid="{F0D84552-7E57-4362-9DCD-EDC8E4E51415}" name="XML order #" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{E36A262F-69A4-4276-95F1-0FB7FCE8E2AD}" name="Data Type" dataDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{B4F9F589-759B-40AB-BD12-81562C067103}" name="Optionality" dataDxfId="9"/>
-    <tableColumn id="4" xr3:uid="{29CBFF2E-DC73-4812-9BE8-505CDCED923B}" name="Size" dataDxfId="8"/>
-    <tableColumn id="5" xr3:uid="{2FBE4EBA-0896-4EA8-8E6A-9740D712F4CF}" name="Business Rules" dataDxfId="7"/>
-    <tableColumn id="14" xr3:uid="{F6A291D7-463E-4C10-AE63-F46C62F701F1}" name="User Editable" dataDxfId="6"/>
-    <tableColumn id="6" xr3:uid="{4A3A44E5-9909-437B-9914-BD7AF1AC2439}" name="Generated" dataDxfId="5"/>
-    <tableColumn id="15" xr3:uid="{30410F79-D89B-4BAE-852C-7ADB5287310A}" name="Format" dataDxfId="4"/>
-    <tableColumn id="8" xr3:uid="{23D225B6-A3A4-4446-9AD4-7762B64F46FE}" name="Conditional Formatting" dataDxfId="3"/>
-    <tableColumn id="9" xr3:uid="{27D08B50-8012-49E0-9C10-AEB67B99B91B}" name="Validation" dataDxfId="2"/>
-    <tableColumn id="10" xr3:uid="{A301C8EB-BB2A-4524-AF6E-20714C0D7DD5}" name="Validation Formula" dataDxfId="1"/>
-    <tableColumn id="17" xr3:uid="{BAA62FBF-6DD1-4BE3-944E-A7C12DBF01CD}" name="Validation Severity" dataDxfId="0"/>
+    <tableColumn id="7" xr3:uid="{9E32B24E-F549-442D-B6C5-5B5E67078170}" name="Title" dataDxfId="32"/>
+    <tableColumn id="12" xr3:uid="{023EA1AA-B7DF-4814-BFEF-5AB9B0752B95}" name="Excel col #" dataDxfId="31"/>
+    <tableColumn id="1" xr3:uid="{5687DF61-58A8-463A-A7F7-9B8B474466F3}" name="CSV Column Name" dataDxfId="30"/>
+    <tableColumn id="13" xr3:uid="{9E799E78-81C7-4788-BF70-799894A0FACA}" name="CSV col #" dataDxfId="29"/>
+    <tableColumn id="16" xr3:uid="{6872DDE9-C4EA-4656-AE08-1B51AE6AE7D6}" name="XML Element" dataDxfId="28"/>
+    <tableColumn id="11" xr3:uid="{F0D84552-7E57-4362-9DCD-EDC8E4E51415}" name="XML order #" dataDxfId="27"/>
+    <tableColumn id="2" xr3:uid="{E36A262F-69A4-4276-95F1-0FB7FCE8E2AD}" name="Data Type" dataDxfId="26"/>
+    <tableColumn id="3" xr3:uid="{B4F9F589-759B-40AB-BD12-81562C067103}" name="Optionality" dataDxfId="25"/>
+    <tableColumn id="4" xr3:uid="{29CBFF2E-DC73-4812-9BE8-505CDCED923B}" name="Size" dataDxfId="24"/>
+    <tableColumn id="5" xr3:uid="{2FBE4EBA-0896-4EA8-8E6A-9740D712F4CF}" name="Business Rules" dataDxfId="23"/>
+    <tableColumn id="14" xr3:uid="{F6A291D7-463E-4C10-AE63-F46C62F701F1}" name="User Editable" dataDxfId="22"/>
+    <tableColumn id="6" xr3:uid="{4A3A44E5-9909-437B-9914-BD7AF1AC2439}" name="Generated" dataDxfId="21"/>
+    <tableColumn id="15" xr3:uid="{30410F79-D89B-4BAE-852C-7ADB5287310A}" name="Format" dataDxfId="20"/>
+    <tableColumn id="8" xr3:uid="{23D225B6-A3A4-4446-9AD4-7762B64F46FE}" name="Conditional Formatting" dataDxfId="19"/>
+    <tableColumn id="9" xr3:uid="{27D08B50-8012-49E0-9C10-AEB67B99B91B}" name="Validation" dataDxfId="18"/>
+    <tableColumn id="10" xr3:uid="{A301C8EB-BB2A-4524-AF6E-20714C0D7DD5}" name="Validation Formula" dataDxfId="17"/>
+    <tableColumn id="17" xr3:uid="{BAA62FBF-6DD1-4BE3-944E-A7C12DBF01CD}" name="Validation Severity" dataDxfId="16"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight14" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1487,13 +1560,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:Q33"/>
+  <dimension ref="A1:Q34"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1570,7 +1643,7 @@
         <v>55</v>
       </c>
       <c r="Q1" s="6" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="2" spans="1:17" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -1610,7 +1683,7 @@
         <v>102</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="O2" s="2" t="s">
         <v>84</v>
@@ -1619,7 +1692,7 @@
         <v>117</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="30" x14ac:dyDescent="0.25">
@@ -1668,7 +1741,7 @@
         <v>223</v>
       </c>
       <c r="Q3" s="7" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
@@ -1719,7 +1792,7 @@
         <v>201</v>
       </c>
       <c r="Q4" s="2" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
@@ -1770,7 +1843,7 @@
         <v>229</v>
       </c>
       <c r="Q5" s="2" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
@@ -1819,27 +1892,27 @@
         <v>123</v>
       </c>
       <c r="Q6" s="2" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>86</v>
+        <v>64</v>
       </c>
       <c r="B7" s="2">
         <v>5</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="D7" s="7">
-        <v>9</v>
-      </c>
-      <c r="E7" s="13" t="s">
-        <v>195</v>
-      </c>
-      <c r="F7" s="13">
-        <v>21</v>
+        <v>15</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="F7" s="7">
+        <v>8</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>102</v>
@@ -1848,11 +1921,9 @@
         <v>109</v>
       </c>
       <c r="I7" s="3">
-        <v>12</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>51</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="J7" s="2"/>
       <c r="K7" s="2" t="s">
         <v>82</v>
       </c>
@@ -1870,27 +1941,27 @@
         <v>97</v>
       </c>
       <c r="Q7" s="2" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>64</v>
+        <v>86</v>
       </c>
       <c r="B8" s="2">
         <v>5</v>
       </c>
       <c r="C8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="7">
+        <v>9</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>195</v>
+      </c>
+      <c r="F8" s="13">
         <v>21</v>
-      </c>
-      <c r="D8" s="7">
-        <v>15</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>185</v>
-      </c>
-      <c r="F8" s="7">
-        <v>8</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>102</v>
@@ -1899,9 +1970,11 @@
         <v>109</v>
       </c>
       <c r="I8" s="3">
-        <v>2</v>
-      </c>
-      <c r="J8" s="2"/>
+        <v>12</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>51</v>
+      </c>
       <c r="K8" s="2" t="s">
         <v>82</v>
       </c>
@@ -1919,7 +1992,7 @@
         <v>97</v>
       </c>
       <c r="Q8" s="2" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="9" spans="1:17" ht="30" x14ac:dyDescent="0.25">
@@ -1968,40 +2041,38 @@
         <v>97</v>
       </c>
       <c r="Q9" s="2" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="10" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>101</v>
+        <v>262</v>
       </c>
       <c r="B10" s="2">
         <v>6</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D10" s="7">
-        <v>29</v>
+        <v>261</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>263</v>
       </c>
       <c r="E10" s="13" t="s">
-        <v>192</v>
+        <v>264</v>
       </c>
       <c r="F10" s="13">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>102</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="I10" s="3">
-        <v>20</v>
-      </c>
-      <c r="J10" s="2" t="s">
-        <v>31</v>
-      </c>
+        <v>200</v>
+      </c>
+      <c r="J10" s="2"/>
       <c r="K10" s="2" t="s">
         <v>82</v>
       </c>
@@ -2009,46 +2080,44 @@
       <c r="M10" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="N10" s="4" t="s">
-        <v>262</v>
-      </c>
+      <c r="N10" s="2"/>
       <c r="O10" s="2" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="P10" s="5" t="s">
-        <v>119</v>
+        <v>265</v>
       </c>
       <c r="Q10" s="2" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="11" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>120</v>
+        <v>101</v>
       </c>
       <c r="B11" s="2">
         <v>7</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D11" s="2">
         <v>30</v>
       </c>
-      <c r="E11" s="6" t="s">
-        <v>193</v>
-      </c>
-      <c r="F11" s="6">
-        <v>12</v>
+      <c r="D11" s="7">
+        <v>29</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>192</v>
+      </c>
+      <c r="F11" s="13">
+        <v>11</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>92</v>
+        <v>102</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>108</v>
       </c>
       <c r="I11" s="3">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="J11" s="2" t="s">
         <v>31</v>
@@ -2058,51 +2127,51 @@
       </c>
       <c r="L11" s="2"/>
       <c r="M11" s="2" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="N11" s="4" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="O11" s="2" t="s">
         <v>78</v>
       </c>
       <c r="P11" s="5" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="Q11" s="2" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>66</v>
+        <v>120</v>
       </c>
       <c r="B12" s="2">
         <v>8</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D12" s="7">
-        <v>17</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>186</v>
-      </c>
-      <c r="F12" s="7">
-        <v>18</v>
+        <v>32</v>
+      </c>
+      <c r="D12" s="2">
+        <v>30</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="F12" s="6">
+        <v>12</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>92</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="I12" s="3">
         <v>8</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="K12" s="2" t="s">
         <v>82</v>
@@ -2111,258 +2180,266 @@
       <c r="M12" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="N12" s="2"/>
+      <c r="N12" s="4" t="s">
+        <v>260</v>
+      </c>
       <c r="O12" s="2" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="P12" s="5" t="s">
-        <v>250</v>
+        <v>121</v>
       </c>
       <c r="Q12" s="2" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>104</v>
+        <v>66</v>
       </c>
       <c r="B13" s="2">
         <v>9</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D13" s="2">
+        <v>23</v>
+      </c>
+      <c r="D13" s="7">
+        <v>17</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="F13" s="7">
         <v>18</v>
       </c>
-      <c r="E13" s="6" t="s">
-        <v>191</v>
-      </c>
-      <c r="F13" s="6">
-        <v>15</v>
-      </c>
       <c r="G13" s="2" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>111</v>
       </c>
       <c r="I13" s="3">
-        <v>40</v>
+        <v>8</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="K13" s="2" t="s">
         <v>82</v>
       </c>
       <c r="L13" s="2"/>
       <c r="M13" s="2" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="N13" s="2"/>
       <c r="O13" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="P13" s="2" t="s">
-        <v>98</v>
+        <v>92</v>
+      </c>
+      <c r="P13" s="5" t="s">
+        <v>248</v>
       </c>
       <c r="Q13" s="2" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>196</v>
+        <v>104</v>
       </c>
       <c r="B14" s="2">
         <v>10</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D14" s="7">
-        <v>22</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>189</v>
-      </c>
-      <c r="F14" s="7">
-        <v>19</v>
+        <v>25</v>
+      </c>
+      <c r="D14" s="2">
+        <v>18</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="F14" s="6">
+        <v>15</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="H14" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="I14" s="3" t="s">
-        <v>34</v>
+      <c r="I14" s="3">
+        <v>40</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="K14" s="2" t="s">
         <v>82</v>
       </c>
       <c r="L14" s="2"/>
       <c r="M14" s="2" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="N14" s="2"/>
       <c r="O14" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="P14" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q14" s="2" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="B15" s="2">
+        <v>11</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" s="7">
+        <v>22</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="F15" s="7">
+        <v>19</v>
+      </c>
+      <c r="G15" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="P14" s="2" t="s">
+      <c r="H15" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="N15" s="2"/>
+      <c r="O15" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="P15" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="Q14" s="2" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="D15" s="7">
-        <v>1</v>
-      </c>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="H15" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="I15" s="8">
-        <v>20</v>
-      </c>
-      <c r="J15" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="K15" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="L15" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="M15" s="7"/>
-      <c r="N15" s="7"/>
-      <c r="O15" s="7"/>
-      <c r="P15" s="7"/>
-      <c r="Q15" s="2"/>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q15" s="2" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" s="2">
         <v>6</v>
       </c>
-      <c r="D16" s="7">
-        <v>3</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>176</v>
-      </c>
-      <c r="F16" s="7">
-        <v>3</v>
+      <c r="E16" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="F16" s="6">
+        <v>2</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>102</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="I16" s="3">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="J16" s="2"/>
       <c r="K16" s="2" t="s">
-        <v>231</v>
-      </c>
-      <c r="L16" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="M16" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="N16" s="2"/>
-      <c r="O16" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="P16" s="2" t="s">
-        <v>85</v>
-      </c>
+        <v>81</v>
+      </c>
+      <c r="L16" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="M16" s="2"/>
+      <c r="N16" s="5"/>
+      <c r="O16" s="2"/>
+      <c r="P16" s="5"/>
       <c r="Q16" s="2"/>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D17" s="7">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="F17" s="7">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="G17" s="2" t="s">
         <v>102</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="I17" s="3">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="J17" s="2"/>
       <c r="K17" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="L17" s="2" t="s">
-        <v>236</v>
+      <c r="L17" s="11" t="s">
+        <v>87</v>
       </c>
       <c r="M17" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="N17" s="5"/>
+      <c r="N17" s="2"/>
       <c r="O17" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="P17" s="5" t="s">
-        <v>122</v>
+        <v>84</v>
+      </c>
+      <c r="P17" s="2" t="s">
+        <v>85</v>
       </c>
       <c r="Q17" s="2"/>
     </row>
-    <row r="18" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D18" s="2">
+        <v>8</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="F18" s="2">
         <v>6</v>
-      </c>
-      <c r="E18" s="6" t="s">
-        <v>209</v>
-      </c>
-      <c r="F18" s="6">
-        <v>2</v>
       </c>
       <c r="G18" s="2" t="s">
         <v>102</v>
@@ -2373,35 +2450,43 @@
       <c r="I18" s="3">
         <v>10</v>
       </c>
-      <c r="J18" s="2"/>
+      <c r="J18" s="2" t="s">
+        <v>52</v>
+      </c>
       <c r="K18" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="L18" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="M18" s="2"/>
+        <v>231</v>
+      </c>
+      <c r="L18" s="5" t="s">
+        <v>232</v>
+      </c>
+      <c r="M18" s="2" t="s">
+        <v>102</v>
+      </c>
       <c r="N18" s="5"/>
-      <c r="O18" s="2"/>
-      <c r="P18" s="5"/>
+      <c r="O18" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="P18" s="2" t="s">
+        <v>117</v>
+      </c>
       <c r="Q18" s="2"/>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D19" s="7">
         <v>11</v>
       </c>
-      <c r="D19" s="2">
-        <v>8</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="F19" s="2">
-        <v>6</v>
+      <c r="E19" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="F19" s="7">
+        <v>7</v>
       </c>
       <c r="G19" s="2" t="s">
         <v>102</v>
@@ -2410,82 +2495,86 @@
         <v>109</v>
       </c>
       <c r="I19" s="3">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>52</v>
+        <v>15</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>231</v>
-      </c>
-      <c r="L19" s="5" t="s">
-        <v>232</v>
-      </c>
-      <c r="M19" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="N19" s="5"/>
-      <c r="O19" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="P19" s="2" t="s">
-        <v>117</v>
-      </c>
+        <v>81</v>
+      </c>
+      <c r="L19" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="M19" s="2"/>
+      <c r="N19" s="2"/>
+      <c r="O19" s="2"/>
+      <c r="P19" s="2"/>
       <c r="Q19" s="2"/>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>103</v>
+        <v>89</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" s="2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D20" s="2">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="F20" s="2"/>
+        <v>182</v>
+      </c>
+      <c r="F20" s="2">
+        <v>9</v>
+      </c>
       <c r="G20" s="2" t="s">
         <v>102</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I20" s="3">
-        <v>40</v>
-      </c>
-      <c r="J20" s="2"/>
+        <v>1</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>17</v>
+      </c>
       <c r="K20" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="L20" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="M20" s="2"/>
-      <c r="N20" s="2"/>
-      <c r="O20" s="2"/>
-      <c r="P20" s="2"/>
+        <v>231</v>
+      </c>
+      <c r="L20" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="M20" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="N20" s="5"/>
+      <c r="O20" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="P20" s="5" t="s">
+        <v>122</v>
+      </c>
       <c r="Q20" s="2"/>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="2" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="D21" s="7">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="F21" s="7">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="G21" s="2" t="s">
         <v>102</v>
@@ -2494,100 +2583,102 @@
         <v>109</v>
       </c>
       <c r="I21" s="3">
-        <v>2</v>
-      </c>
-      <c r="J21" s="2" t="s">
-        <v>15</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="J21" s="2"/>
       <c r="K21" s="2" t="s">
-        <v>81</v>
+        <v>231</v>
       </c>
       <c r="L21" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="M21" s="2"/>
-      <c r="N21" s="2"/>
-      <c r="O21" s="2"/>
-      <c r="P21" s="2"/>
+        <v>236</v>
+      </c>
+      <c r="M21" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="N21" s="5"/>
+      <c r="O21" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="P21" s="5" t="s">
+        <v>122</v>
+      </c>
       <c r="Q21" s="2"/>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>89</v>
+        <v>74</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D22" s="2">
-        <v>12</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="F22" s="2">
-        <v>9</v>
+        <v>47</v>
+      </c>
+      <c r="D22" s="7">
+        <v>31</v>
+      </c>
+      <c r="E22" s="13" t="s">
+        <v>198</v>
+      </c>
+      <c r="F22" s="13">
+        <v>13</v>
       </c>
       <c r="G22" s="2" t="s">
         <v>102</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I22" s="3">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>17</v>
+        <v>50</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>231</v>
+        <v>81</v>
       </c>
       <c r="L22" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="M22" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="N22" s="5"/>
-      <c r="O22" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="P22" s="5" t="s">
-        <v>122</v>
-      </c>
+        <v>113</v>
+      </c>
+      <c r="M22" s="2"/>
+      <c r="N22" s="2"/>
+      <c r="O22" s="2"/>
+      <c r="P22" s="2"/>
       <c r="Q22" s="2"/>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D23" s="7">
-        <v>19</v>
+        <v>48</v>
+      </c>
+      <c r="D23" s="2">
+        <v>32</v>
       </c>
       <c r="E23" s="13" t="s">
-        <v>188</v>
-      </c>
-      <c r="F23" s="13"/>
+        <v>199</v>
+      </c>
+      <c r="F23" s="13">
+        <v>14</v>
+      </c>
       <c r="G23" s="2" t="s">
         <v>102</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="I23" s="3">
-        <v>9</v>
-      </c>
-      <c r="J23" s="2"/>
+        <v>10</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>49</v>
+      </c>
       <c r="K23" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="L23" s="11" t="s">
-        <v>87</v>
+      <c r="L23" s="2" t="s">
+        <v>107</v>
       </c>
       <c r="M23" s="2"/>
       <c r="N23" s="2"/>
@@ -2597,148 +2688,148 @@
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>68</v>
+        <v>197</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D24" s="7">
+        <v>36</v>
+      </c>
+      <c r="D24" s="2">
+        <v>23</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="F24" s="7">
         <v>20</v>
       </c>
-      <c r="E24" s="7" t="s">
-        <v>187</v>
-      </c>
-      <c r="F24" s="7"/>
       <c r="G24" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="I24" s="3">
-        <v>2</v>
-      </c>
-      <c r="J24" s="2"/>
+        <v>111</v>
+      </c>
+      <c r="I24" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="J24" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="K24" s="2" t="s">
-        <v>81</v>
+        <v>231</v>
       </c>
       <c r="L24" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="M24" s="2"/>
+      <c r="M24" s="2" t="s">
+        <v>99</v>
+      </c>
       <c r="N24" s="2"/>
-      <c r="O24" s="2"/>
-      <c r="P24" s="2"/>
+      <c r="O24" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="P24" s="2" t="s">
+        <v>118</v>
+      </c>
       <c r="Q24" s="2"/>
     </row>
-    <row r="25" spans="1:17" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D25" s="2">
-        <v>21</v>
-      </c>
-      <c r="E25" s="6" t="s">
-        <v>190</v>
-      </c>
-      <c r="F25" s="6"/>
-      <c r="G25" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="H25" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="I25" s="3">
-        <v>12</v>
-      </c>
-      <c r="J25" s="2"/>
-      <c r="K25" s="2" t="s">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A25" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="B25" s="7"/>
+      <c r="C25" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D25" s="7">
+        <v>1</v>
+      </c>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="H25" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="I25" s="8">
+        <v>20</v>
+      </c>
+      <c r="J25" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="K25" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="L25" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="M25" s="2"/>
-      <c r="N25" s="2"/>
-      <c r="O25" s="2"/>
-      <c r="P25" s="2"/>
+      <c r="L25" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="M25" s="7"/>
+      <c r="N25" s="7"/>
+      <c r="O25" s="7"/>
+      <c r="P25" s="7"/>
       <c r="Q25" s="2"/>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>197</v>
+        <v>103</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" s="2" t="s">
-        <v>36</v>
+        <v>13</v>
       </c>
       <c r="D26" s="2">
-        <v>23</v>
-      </c>
-      <c r="E26" s="7" t="s">
-        <v>189</v>
-      </c>
-      <c r="F26" s="7">
-        <v>20</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="F26" s="2"/>
       <c r="G26" s="2" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="I26" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="J26" s="2" t="s">
-        <v>37</v>
-      </c>
+        <v>110</v>
+      </c>
+      <c r="I26" s="3">
+        <v>40</v>
+      </c>
+      <c r="J26" s="2"/>
       <c r="K26" s="2" t="s">
-        <v>231</v>
+        <v>81</v>
       </c>
       <c r="L26" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="M26" s="2" t="s">
-        <v>99</v>
-      </c>
+      <c r="M26" s="2"/>
       <c r="N26" s="2"/>
-      <c r="O26" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="P26" s="2" t="s">
-        <v>118</v>
-      </c>
+      <c r="O26" s="2"/>
+      <c r="P26" s="2"/>
       <c r="Q26" s="2"/>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" s="2" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="D27" s="7">
-        <v>24</v>
-      </c>
-      <c r="E27" s="7" t="s">
-        <v>189</v>
-      </c>
-      <c r="F27" s="7"/>
+        <v>19</v>
+      </c>
+      <c r="E27" s="13" t="s">
+        <v>188</v>
+      </c>
+      <c r="F27" s="13"/>
       <c r="G27" s="2" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="H27" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="I27" s="3" t="s">
-        <v>39</v>
+      <c r="I27" s="3">
+        <v>9</v>
       </c>
       <c r="J27" s="2"/>
       <c r="K27" s="2" t="s">
@@ -2755,17 +2846,17 @@
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D28" s="2">
-        <v>25</v>
+        <v>28</v>
+      </c>
+      <c r="D28" s="7">
+        <v>20</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F28" s="7"/>
       <c r="G28" s="2" t="s">
@@ -2774,7 +2865,9 @@
       <c r="H28" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="I28" s="3"/>
+      <c r="I28" s="3">
+        <v>2</v>
+      </c>
       <c r="J28" s="2"/>
       <c r="K28" s="2" t="s">
         <v>81</v>
@@ -2788,29 +2881,29 @@
       <c r="P28" s="2"/>
       <c r="Q28" s="2"/>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D29" s="7">
-        <v>26</v>
-      </c>
-      <c r="E29" s="7" t="s">
-        <v>189</v>
-      </c>
-      <c r="F29" s="7"/>
+        <v>29</v>
+      </c>
+      <c r="D29" s="2">
+        <v>21</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="F29" s="6"/>
       <c r="G29" s="2" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="H29" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="I29" s="3" t="s">
-        <v>42</v>
+      <c r="I29" s="3">
+        <v>12</v>
       </c>
       <c r="J29" s="2"/>
       <c r="K29" s="2" t="s">
@@ -2827,14 +2920,14 @@
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D30" s="2">
-        <v>27</v>
+        <v>38</v>
+      </c>
+      <c r="D30" s="7">
+        <v>24</v>
       </c>
       <c r="E30" s="7" t="s">
         <v>189</v>
@@ -2847,7 +2940,7 @@
         <v>110</v>
       </c>
       <c r="I30" s="3" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="J30" s="2"/>
       <c r="K30" s="2" t="s">
@@ -2864,28 +2957,26 @@
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D31" s="7">
-        <v>28</v>
+        <v>40</v>
+      </c>
+      <c r="D31" s="2">
+        <v>25</v>
       </c>
       <c r="E31" s="7" t="s">
         <v>189</v>
       </c>
       <c r="F31" s="7"/>
       <c r="G31" s="2" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="H31" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="I31" s="3" t="s">
-        <v>46</v>
-      </c>
+      <c r="I31" s="3"/>
       <c r="J31" s="2"/>
       <c r="K31" s="2" t="s">
         <v>81</v>
@@ -2899,40 +2990,36 @@
       <c r="P31" s="2"/>
       <c r="Q31" s="2"/>
     </row>
-    <row r="32" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" s="2" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D32" s="7">
-        <v>31</v>
-      </c>
-      <c r="E32" s="13" t="s">
-        <v>198</v>
-      </c>
-      <c r="F32" s="13">
-        <v>13</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="E32" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="F32" s="7"/>
       <c r="G32" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="I32" s="3">
-        <v>10</v>
-      </c>
-      <c r="J32" s="2" t="s">
-        <v>50</v>
-      </c>
+        <v>110</v>
+      </c>
+      <c r="I32" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="J32" s="2"/>
       <c r="K32" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="L32" s="2" t="s">
-        <v>113</v>
+      <c r="L32" s="11" t="s">
+        <v>87</v>
       </c>
       <c r="M32" s="2"/>
       <c r="N32" s="2"/>
@@ -2940,40 +3027,36 @@
       <c r="P32" s="2"/>
       <c r="Q32" s="2"/>
     </row>
-    <row r="33" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>58</v>
+        <v>76</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" s="2" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="D33" s="2">
-        <v>32</v>
-      </c>
-      <c r="E33" s="13" t="s">
-        <v>199</v>
-      </c>
-      <c r="F33" s="13">
-        <v>14</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="E33" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="F33" s="7"/>
       <c r="G33" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="I33" s="3">
-        <v>10</v>
-      </c>
-      <c r="J33" s="2" t="s">
-        <v>49</v>
-      </c>
+        <v>110</v>
+      </c>
+      <c r="I33" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="J33" s="2"/>
       <c r="K33" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="L33" s="2" t="s">
-        <v>107</v>
+      <c r="L33" s="11" t="s">
+        <v>87</v>
       </c>
       <c r="M33" s="2"/>
       <c r="N33" s="2"/>
@@ -2981,23 +3064,60 @@
       <c r="P33" s="2"/>
       <c r="Q33" s="2"/>
     </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B34" s="2"/>
+      <c r="C34" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D34" s="7">
+        <v>28</v>
+      </c>
+      <c r="E34" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="F34" s="7"/>
+      <c r="G34" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="I34" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="J34" s="2"/>
+      <c r="K34" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="L34" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="M34" s="2"/>
+      <c r="N34" s="2"/>
+      <c r="O34" s="2"/>
+      <c r="P34" s="2"/>
+      <c r="Q34" s="2"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
-  <conditionalFormatting sqref="D2:F33">
-    <cfRule type="expression" dxfId="45" priority="14">
+  <conditionalFormatting sqref="D2:F34">
+    <cfRule type="expression" dxfId="7" priority="14">
       <formula>LEN($D2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L2:L33">
-    <cfRule type="expression" dxfId="44" priority="13">
+  <conditionalFormatting sqref="L2:L34">
+    <cfRule type="expression" dxfId="6" priority="13">
       <formula>AND($K2&lt;&gt;"Yes",LEN($L2)=0)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:Q33">
-    <cfRule type="expression" dxfId="43" priority="3">
+  <conditionalFormatting sqref="A2:Q34">
+    <cfRule type="expression" dxfId="5" priority="3">
       <formula>$K2="Skip"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="42" priority="15">
+    <cfRule type="expression" dxfId="4" priority="15">
       <formula>$K2="No"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3092,7 +3212,7 @@
         <v>55</v>
       </c>
       <c r="Q1" s="6" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="30" x14ac:dyDescent="0.25">
@@ -3100,7 +3220,7 @@
         <v>57</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>10</v>
@@ -3270,7 +3390,7 @@
         <v>139</v>
       </c>
       <c r="B6" s="2">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>138</v>
@@ -3304,7 +3424,7 @@
         <v>102</v>
       </c>
       <c r="N6" s="5" t="s">
-        <v>242</v>
+        <v>266</v>
       </c>
       <c r="O6" s="2" t="s">
         <v>80</v>
@@ -3313,7 +3433,7 @@
         <v>136</v>
       </c>
       <c r="Q6" s="2" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="7" spans="1:17" ht="30" x14ac:dyDescent="0.25">
@@ -3321,7 +3441,7 @@
         <v>219</v>
       </c>
       <c r="B7" s="2">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>148</v>
@@ -3359,10 +3479,10 @@
         <v>80</v>
       </c>
       <c r="P7" s="5" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="Q7" s="2" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
@@ -3370,7 +3490,7 @@
         <v>165</v>
       </c>
       <c r="B8" s="2">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>164</v>
@@ -3408,10 +3528,10 @@
         <v>92</v>
       </c>
       <c r="P8" s="5" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="Q8" s="2" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
@@ -3419,7 +3539,7 @@
         <v>161</v>
       </c>
       <c r="B9" s="2">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>160</v>
@@ -3460,7 +3580,7 @@
         <v>123</v>
       </c>
       <c r="Q9" s="2" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
@@ -3468,7 +3588,7 @@
         <v>202</v>
       </c>
       <c r="B10" s="2">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>159</v>
@@ -3506,10 +3626,10 @@
         <v>92</v>
       </c>
       <c r="P10" s="5" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="Q10" s="2" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
@@ -3517,7 +3637,7 @@
         <v>203</v>
       </c>
       <c r="B11" s="2">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>157</v>
@@ -3558,15 +3678,15 @@
         <v>123</v>
       </c>
       <c r="Q11" s="2" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="12" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B12" s="2">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>138</v>
@@ -3599,8 +3719,8 @@
       <c r="M12" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="N12" s="5" t="s">
-        <v>249</v>
+      <c r="N12" s="4" t="s">
+        <v>267</v>
       </c>
       <c r="O12" s="2" t="s">
         <v>80</v>
@@ -3609,15 +3729,15 @@
         <v>136</v>
       </c>
       <c r="Q12" s="2" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="13" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B13" s="2">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>148</v>
@@ -3655,18 +3775,18 @@
         <v>80</v>
       </c>
       <c r="P13" s="5" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="Q13" s="2" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B14" s="2">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>164</v>
@@ -3704,18 +3824,18 @@
         <v>92</v>
       </c>
       <c r="P14" s="5" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="Q14" s="2" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B15" s="2">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>160</v>
@@ -3756,15 +3876,15 @@
         <v>123</v>
       </c>
       <c r="Q15" s="2" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B16" s="2">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>159</v>
@@ -3802,18 +3922,18 @@
         <v>92</v>
       </c>
       <c r="P16" s="5" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="Q16" s="2" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B17" s="2">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>157</v>
@@ -3854,22 +3974,26 @@
         <v>123</v>
       </c>
       <c r="Q17" s="2" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>116</v>
+        <v>62</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" s="2" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="D18" s="2">
-        <v>1</v>
-      </c>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
+        <v>5</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="F18" s="6">
+        <v>4</v>
+      </c>
       <c r="G18" s="2" t="s">
         <v>102</v>
       </c>
@@ -3877,16 +4001,14 @@
         <v>109</v>
       </c>
       <c r="I18" s="2">
-        <v>20</v>
-      </c>
-      <c r="J18" s="2" t="s">
-        <v>172</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="J18" s="2"/>
       <c r="K18" s="2" t="s">
         <v>81</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>172</v>
+        <v>114</v>
       </c>
       <c r="M18" s="2"/>
       <c r="N18" s="2"/>
@@ -3894,43 +4016,51 @@
       <c r="P18" s="2"/>
       <c r="Q18" s="2"/>
     </row>
-    <row r="19" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>62</v>
+        <v>146</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="D19" s="2">
+        <v>16</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="F19" s="2">
+        <v>7</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="I19" s="2">
         <v>9</v>
       </c>
-      <c r="D19" s="2">
-        <v>5</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>209</v>
-      </c>
-      <c r="F19" s="6">
-        <v>4</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="H19" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="I19" s="2">
-        <v>10</v>
-      </c>
-      <c r="J19" s="2"/>
+      <c r="J19" s="2" t="s">
+        <v>144</v>
+      </c>
       <c r="K19" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="L19" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="M19" s="2"/>
+        <v>231</v>
+      </c>
+      <c r="L19" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="M19" s="2" t="s">
+        <v>102</v>
+      </c>
       <c r="N19" s="2"/>
-      <c r="O19" s="2"/>
-      <c r="P19" s="2"/>
+      <c r="O19" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="P19" s="5" t="s">
+        <v>130</v>
+      </c>
       <c r="Q19" s="2"/>
     </row>
     <row r="20" spans="1:17" ht="30" x14ac:dyDescent="0.25">
@@ -3976,105 +4106,119 @@
       <c r="P20" s="5"/>
       <c r="Q20" s="2"/>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>156</v>
+        <v>129</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="2" t="s">
-        <v>155</v>
+        <v>128</v>
       </c>
       <c r="D21" s="2">
-        <v>12</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="F21" s="2">
-        <v>17</v>
+        <v>28</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="F21" s="6">
+        <v>14</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>92</v>
+        <v>125</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="I21" s="2">
-        <v>8</v>
-      </c>
-      <c r="J21" s="2"/>
+        <v>108</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>126</v>
+      </c>
       <c r="K21" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="L21" s="5" t="s">
-        <v>235</v>
-      </c>
-      <c r="M21" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="N21" s="5"/>
+      <c r="L21" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="M21" s="2"/>
+      <c r="N21" s="4" t="s">
+        <v>226</v>
+      </c>
       <c r="O21" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="P21" s="5" t="s">
-        <v>162</v>
+        <v>125</v>
+      </c>
+      <c r="P21" s="2" t="s">
+        <v>124</v>
       </c>
       <c r="Q21" s="2"/>
     </row>
     <row r="22" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>154</v>
+        <v>208</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" s="2" t="s">
-        <v>153</v>
+        <v>135</v>
       </c>
       <c r="D22" s="2">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>217</v>
+        <v>204</v>
       </c>
       <c r="F22" s="6">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="G22" s="2" t="s">
         <v>102</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I22" s="2">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>152</v>
+        <v>134</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="L22" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="M22" s="2"/>
-      <c r="N22" s="2"/>
-      <c r="O22" s="2"/>
-      <c r="P22" s="2"/>
+        <v>231</v>
+      </c>
+      <c r="L22" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="M22" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="N22" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="O22" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="P22" s="5" t="s">
+        <v>133</v>
+      </c>
       <c r="Q22" s="2"/>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>150</v>
+        <v>207</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" s="2" t="s">
-        <v>149</v>
+        <v>132</v>
       </c>
       <c r="D23" s="2">
-        <v>14</v>
-      </c>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
+        <v>27</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="F23" s="6">
+        <v>16</v>
+      </c>
       <c r="G23" s="2" t="s">
         <v>102</v>
       </c>
@@ -4082,177 +4226,167 @@
         <v>108</v>
       </c>
       <c r="I23" s="2">
-        <v>2</v>
-      </c>
-      <c r="J23" s="2"/>
+        <v>9</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>131</v>
+      </c>
       <c r="K23" s="2" t="s">
-        <v>81</v>
+        <v>231</v>
       </c>
       <c r="L23" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="M23" s="2"/>
-      <c r="N23" s="2"/>
-      <c r="O23" s="2"/>
-      <c r="P23" s="2"/>
+      <c r="M23" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="N23" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="O23" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="P23" s="5" t="s">
+        <v>130</v>
+      </c>
       <c r="Q23" s="2"/>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>146</v>
+        <v>156</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" s="2" t="s">
-        <v>145</v>
+        <v>155</v>
       </c>
       <c r="D24" s="2">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="F24" s="2">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="H24" s="2" t="s">
         <v>111</v>
       </c>
       <c r="I24" s="2">
-        <v>9</v>
-      </c>
-      <c r="J24" s="2" t="s">
-        <v>144</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="J24" s="2"/>
       <c r="K24" s="2" t="s">
         <v>231</v>
       </c>
       <c r="L24" s="5" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="M24" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="N24" s="2"/>
+        <v>96</v>
+      </c>
+      <c r="N24" s="5"/>
       <c r="O24" s="2" t="s">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="P24" s="5" t="s">
-        <v>130</v>
+        <v>162</v>
       </c>
       <c r="Q24" s="2"/>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>143</v>
+        <v>154</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" s="2" t="s">
-        <v>142</v>
+        <v>153</v>
       </c>
       <c r="D25" s="2">
-        <v>17</v>
-      </c>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
+        <v>13</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="F25" s="6">
+        <v>18</v>
+      </c>
       <c r="G25" s="2" t="s">
         <v>102</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="I25" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>141</v>
+        <v>152</v>
       </c>
       <c r="K25" s="2" t="s">
-        <v>231</v>
-      </c>
-      <c r="L25" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="M25" s="2" t="s">
-        <v>102</v>
-      </c>
+        <v>81</v>
+      </c>
+      <c r="L25" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="M25" s="2"/>
       <c r="N25" s="2"/>
-      <c r="O25" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="P25" s="5" t="s">
-        <v>140</v>
-      </c>
+      <c r="O25" s="2"/>
+      <c r="P25" s="2"/>
       <c r="Q25" s="2"/>
     </row>
-    <row r="26" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>208</v>
+        <v>116</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" s="2" t="s">
-        <v>135</v>
+        <v>3</v>
       </c>
       <c r="D26" s="2">
+        <v>1</v>
+      </c>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="I26" s="2">
         <v>20</v>
       </c>
-      <c r="E26" s="6" t="s">
-        <v>204</v>
-      </c>
-      <c r="F26" s="6">
-        <v>15</v>
-      </c>
-      <c r="G26" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="H26" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="I26" s="2">
-        <v>10</v>
-      </c>
       <c r="J26" s="2" t="s">
-        <v>134</v>
+        <v>172</v>
       </c>
       <c r="K26" s="2" t="s">
-        <v>231</v>
-      </c>
-      <c r="L26" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="M26" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="N26" s="4" t="s">
-        <v>227</v>
-      </c>
-      <c r="O26" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="P26" s="5" t="s">
-        <v>133</v>
-      </c>
+        <v>81</v>
+      </c>
+      <c r="L26" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="M26" s="2"/>
+      <c r="N26" s="2"/>
+      <c r="O26" s="2"/>
+      <c r="P26" s="2"/>
       <c r="Q26" s="2"/>
     </row>
-    <row r="27" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>207</v>
+        <v>150</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" s="2" t="s">
-        <v>132</v>
+        <v>149</v>
       </c>
       <c r="D27" s="2">
-        <v>27</v>
-      </c>
-      <c r="E27" s="6" t="s">
-        <v>205</v>
-      </c>
-      <c r="F27" s="6">
-        <v>16</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
       <c r="G27" s="2" t="s">
         <v>102</v>
       </c>
@@ -4260,59 +4394,45 @@
         <v>108</v>
       </c>
       <c r="I27" s="2">
-        <v>9</v>
-      </c>
-      <c r="J27" s="2" t="s">
-        <v>131</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="J27" s="2"/>
       <c r="K27" s="2" t="s">
-        <v>231</v>
+        <v>81</v>
       </c>
       <c r="L27" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="M27" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="N27" s="4" t="s">
-        <v>228</v>
-      </c>
-      <c r="O27" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="P27" s="5" t="s">
-        <v>130</v>
-      </c>
+      <c r="M27" s="2"/>
+      <c r="N27" s="2"/>
+      <c r="O27" s="2"/>
+      <c r="P27" s="2"/>
       <c r="Q27" s="2"/>
     </row>
-    <row r="28" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>129</v>
+        <v>143</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" s="2" t="s">
-        <v>128</v>
+        <v>142</v>
       </c>
       <c r="D28" s="2">
-        <v>28</v>
-      </c>
-      <c r="E28" s="6" t="s">
-        <v>206</v>
-      </c>
-      <c r="F28" s="6">
-        <v>14</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
       <c r="G28" s="2" t="s">
-        <v>125</v>
+        <v>102</v>
       </c>
       <c r="H28" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="I28" s="2" t="s">
-        <v>127</v>
+      <c r="I28" s="2">
+        <v>4</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>126</v>
+        <v>141</v>
       </c>
       <c r="K28" s="2" t="s">
         <v>231</v>
@@ -4320,34 +4440,34 @@
       <c r="L28" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="M28" s="2"/>
-      <c r="N28" s="4" t="s">
-        <v>226</v>
-      </c>
+      <c r="M28" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="N28" s="2"/>
       <c r="O28" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="P28" s="2" t="s">
-        <v>124</v>
+        <v>80</v>
+      </c>
+      <c r="P28" s="5" t="s">
+        <v>140</v>
       </c>
       <c r="Q28" s="2"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="L2:L28">
-    <cfRule type="expression" dxfId="22" priority="21">
+    <cfRule type="expression" dxfId="3" priority="21">
       <formula>AND($K2&lt;&gt;"Yes",LEN($L2)=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:F28">
-    <cfRule type="expression" dxfId="21" priority="22">
+    <cfRule type="expression" dxfId="2" priority="22">
       <formula>LEN($D2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:Q28">
-    <cfRule type="expression" dxfId="20" priority="5">
+    <cfRule type="expression" dxfId="1" priority="5">
       <formula>$K2="Skip"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="23">
+    <cfRule type="expression" dxfId="0" priority="23">
       <formula>$K2="No"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Make Sample Collection Time required; format time as military time
Also fixed formatting not being applied to new rows
and updated documentation

#19
</commit_message>
<xml_diff>
--- a/specs/Coliform-column-definitions.xlsx
+++ b/specs/Coliform-column-definitions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\xl-ese\specs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E0BE6FA-EC5E-43AD-B2FB-38EFB014F433}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44CB2758-6E15-4923-BCCE-56E13CC85522}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Coliform Sample" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="626" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="627" uniqueCount="269">
   <si>
     <t>Optionality</t>
   </si>
@@ -322,9 +322,6 @@
     <t>Format</t>
   </si>
   <si>
-    <t>[$-en-US]h:mm AM/PM</t>
-  </si>
-  <si>
     <t>[$-en-US]dd-mmm-yyyy;@</t>
   </si>
   <si>
@@ -394,13 +391,7 @@
     <t>Between 0.01 and 99.0</t>
   </si>
   <si>
-    <t>=OR(RC10&lt;&gt;"Repeat",LEN(RC)&gt;0)</t>
-  </si>
-  <si>
     <t>Original Sample Collection Date</t>
-  </si>
-  <si>
-    <t>=OR(RC10&lt;&gt;"Repeat",AND(LEN(RC)&gt;0,RC&lt;=TODAY()))</t>
   </si>
   <si>
     <t>=YesNoList</t>
@@ -897,6 +888,18 @@
   <si>
     <t>=AND(RC12="Present",LEN(RC18)=0)
 =RC12="Absent"</t>
+  </si>
+  <si>
+    <t>[$-en-US]hh:mm</t>
+  </si>
+  <si>
+    <t>=LEN(RC4)=0</t>
+  </si>
+  <si>
+    <t>=OR(LEFT(RC5,6)&lt;&gt;"Repeat",LEN(RC)&gt;0)</t>
+  </si>
+  <si>
+    <t>=OR(LEFT(RC5,6)&lt;&gt;"Repeat",AND(LEN(RC)&gt;0,RC&lt;=TODAY()))</t>
   </si>
 </sst>
 </file>
@@ -1001,6 +1004,119 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor theme="7" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
@@ -1011,147 +1127,6 @@
           <bgColor theme="7" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1221,6 +1196,34 @@
     </dxf>
     <dxf>
       <alignment vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1241,56 +1244,56 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{636125F0-68A9-4682-81D8-01BD3AB67D26}" name="Table1" displayName="Table1" ref="A1:Q34" totalsRowShown="0" headerRowDxfId="53" dataDxfId="52">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{636125F0-68A9-4682-81D8-01BD3AB67D26}" name="Table1" displayName="Table1" ref="A1:Q34" totalsRowShown="0" headerRowDxfId="49" dataDxfId="48">
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Q34">
     <sortCondition ref="B15:B34"/>
   </sortState>
   <tableColumns count="17">
-    <tableColumn id="6" xr3:uid="{57EF6AB6-6C4C-4170-BD9B-BF376C46C5DF}" name="Title" dataDxfId="51"/>
-    <tableColumn id="12" xr3:uid="{BFDB40C3-C9ED-4560-81A1-344ECAE248C8}" name="Excel col #" dataDxfId="50"/>
-    <tableColumn id="1" xr3:uid="{3193A6D3-813B-4494-AEED-01D6509FCA0D}" name="CSV Column Name" dataDxfId="49"/>
-    <tableColumn id="11" xr3:uid="{057EA208-1889-4E3C-A179-F312337D9867}" name="CSV col #" dataDxfId="48"/>
-    <tableColumn id="16" xr3:uid="{1F4E7FF6-264D-41DA-AC14-BAA45F3439C7}" name="XML Element" dataDxfId="47"/>
-    <tableColumn id="10" xr3:uid="{F503FCB6-1F5D-4765-B4AB-F67230BC37A3}" name="XML order #" dataDxfId="46"/>
-    <tableColumn id="2" xr3:uid="{5C52F15D-4AC8-44CE-A401-3402D3CD4152}" name="Data Type" dataDxfId="45"/>
-    <tableColumn id="3" xr3:uid="{FFD71D9C-951A-4BB1-9000-9A1C4C3F71D3}" name="Optionality" dataDxfId="44"/>
-    <tableColumn id="4" xr3:uid="{6FEED7B4-CF3F-4593-BB9F-5CFA5FA5B692}" name="Size" dataDxfId="43"/>
-    <tableColumn id="5" xr3:uid="{563427BF-63BA-491F-9B6F-4E02453C643B}" name="Business Rules" dataDxfId="42"/>
-    <tableColumn id="9" xr3:uid="{A9E34622-C2B4-476B-A018-EABC1256DC10}" name="User Editable" dataDxfId="41"/>
-    <tableColumn id="14" xr3:uid="{9DA3EF2F-E261-414A-B10C-F88F2052640F}" name="Generated" dataDxfId="40"/>
-    <tableColumn id="15" xr3:uid="{AA61284F-4409-4E18-9405-8F2EAA78028A}" name="Format" dataDxfId="39"/>
-    <tableColumn id="13" xr3:uid="{94BA7C53-9CFA-4072-B1A4-7E9CE9D9DDF7}" name="Conditional Formatting" dataDxfId="38"/>
-    <tableColumn id="7" xr3:uid="{22AE72C5-BA89-443A-81AF-BCF4B114454C}" name="Validation" dataDxfId="37"/>
-    <tableColumn id="8" xr3:uid="{5DE66E18-4141-4BDD-B41D-2782AC810F6E}" name="Validation Formula" dataDxfId="36"/>
-    <tableColumn id="17" xr3:uid="{3088A6C0-DDC9-48B3-825B-006B2A52B333}" name="Validation Severity" dataDxfId="35"/>
+    <tableColumn id="6" xr3:uid="{57EF6AB6-6C4C-4170-BD9B-BF376C46C5DF}" name="Title" dataDxfId="47"/>
+    <tableColumn id="12" xr3:uid="{BFDB40C3-C9ED-4560-81A1-344ECAE248C8}" name="Excel col #" dataDxfId="46"/>
+    <tableColumn id="1" xr3:uid="{3193A6D3-813B-4494-AEED-01D6509FCA0D}" name="CSV Column Name" dataDxfId="45"/>
+    <tableColumn id="11" xr3:uid="{057EA208-1889-4E3C-A179-F312337D9867}" name="CSV col #" dataDxfId="44"/>
+    <tableColumn id="16" xr3:uid="{1F4E7FF6-264D-41DA-AC14-BAA45F3439C7}" name="XML Element" dataDxfId="43"/>
+    <tableColumn id="10" xr3:uid="{F503FCB6-1F5D-4765-B4AB-F67230BC37A3}" name="XML order #" dataDxfId="42"/>
+    <tableColumn id="2" xr3:uid="{5C52F15D-4AC8-44CE-A401-3402D3CD4152}" name="Data Type" dataDxfId="41"/>
+    <tableColumn id="3" xr3:uid="{FFD71D9C-951A-4BB1-9000-9A1C4C3F71D3}" name="Optionality" dataDxfId="40"/>
+    <tableColumn id="4" xr3:uid="{6FEED7B4-CF3F-4593-BB9F-5CFA5FA5B692}" name="Size" dataDxfId="39"/>
+    <tableColumn id="5" xr3:uid="{563427BF-63BA-491F-9B6F-4E02453C643B}" name="Business Rules" dataDxfId="38"/>
+    <tableColumn id="9" xr3:uid="{A9E34622-C2B4-476B-A018-EABC1256DC10}" name="User Editable" dataDxfId="37"/>
+    <tableColumn id="14" xr3:uid="{9DA3EF2F-E261-414A-B10C-F88F2052640F}" name="Generated" dataDxfId="36"/>
+    <tableColumn id="15" xr3:uid="{AA61284F-4409-4E18-9405-8F2EAA78028A}" name="Format" dataDxfId="35"/>
+    <tableColumn id="13" xr3:uid="{94BA7C53-9CFA-4072-B1A4-7E9CE9D9DDF7}" name="Conditional Formatting" dataDxfId="34"/>
+    <tableColumn id="7" xr3:uid="{22AE72C5-BA89-443A-81AF-BCF4B114454C}" name="Validation" dataDxfId="33"/>
+    <tableColumn id="8" xr3:uid="{5DE66E18-4141-4BDD-B41D-2782AC810F6E}" name="Validation Formula" dataDxfId="32"/>
+    <tableColumn id="17" xr3:uid="{3088A6C0-DDC9-48B3-825B-006B2A52B333}" name="Validation Severity" dataDxfId="31"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{05345577-AC31-4B6D-B899-55D66DEB1874}" name="Table2" displayName="Table2" ref="A1:Q28" totalsRowShown="0" headerRowDxfId="34" dataDxfId="33">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{05345577-AC31-4B6D-B899-55D66DEB1874}" name="Table2" displayName="Table2" ref="A1:Q28" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25">
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Q28">
     <sortCondition ref="B18:B28"/>
   </sortState>
   <tableColumns count="17">
-    <tableColumn id="7" xr3:uid="{9E32B24E-F549-442D-B6C5-5B5E67078170}" name="Title" dataDxfId="32"/>
-    <tableColumn id="12" xr3:uid="{023EA1AA-B7DF-4814-BFEF-5AB9B0752B95}" name="Excel col #" dataDxfId="31"/>
-    <tableColumn id="1" xr3:uid="{5687DF61-58A8-463A-A7F7-9B8B474466F3}" name="CSV Column Name" dataDxfId="30"/>
-    <tableColumn id="13" xr3:uid="{9E799E78-81C7-4788-BF70-799894A0FACA}" name="CSV col #" dataDxfId="29"/>
-    <tableColumn id="16" xr3:uid="{6872DDE9-C4EA-4656-AE08-1B51AE6AE7D6}" name="XML Element" dataDxfId="28"/>
-    <tableColumn id="11" xr3:uid="{F0D84552-7E57-4362-9DCD-EDC8E4E51415}" name="XML order #" dataDxfId="27"/>
-    <tableColumn id="2" xr3:uid="{E36A262F-69A4-4276-95F1-0FB7FCE8E2AD}" name="Data Type" dataDxfId="26"/>
-    <tableColumn id="3" xr3:uid="{B4F9F589-759B-40AB-BD12-81562C067103}" name="Optionality" dataDxfId="25"/>
-    <tableColumn id="4" xr3:uid="{29CBFF2E-DC73-4812-9BE8-505CDCED923B}" name="Size" dataDxfId="24"/>
-    <tableColumn id="5" xr3:uid="{2FBE4EBA-0896-4EA8-8E6A-9740D712F4CF}" name="Business Rules" dataDxfId="23"/>
-    <tableColumn id="14" xr3:uid="{F6A291D7-463E-4C10-AE63-F46C62F701F1}" name="User Editable" dataDxfId="22"/>
-    <tableColumn id="6" xr3:uid="{4A3A44E5-9909-437B-9914-BD7AF1AC2439}" name="Generated" dataDxfId="21"/>
-    <tableColumn id="15" xr3:uid="{30410F79-D89B-4BAE-852C-7ADB5287310A}" name="Format" dataDxfId="20"/>
-    <tableColumn id="8" xr3:uid="{23D225B6-A3A4-4446-9AD4-7762B64F46FE}" name="Conditional Formatting" dataDxfId="19"/>
-    <tableColumn id="9" xr3:uid="{27D08B50-8012-49E0-9C10-AEB67B99B91B}" name="Validation" dataDxfId="18"/>
-    <tableColumn id="10" xr3:uid="{A301C8EB-BB2A-4524-AF6E-20714C0D7DD5}" name="Validation Formula" dataDxfId="17"/>
-    <tableColumn id="17" xr3:uid="{BAA62FBF-6DD1-4BE3-944E-A7C12DBF01CD}" name="Validation Severity" dataDxfId="16"/>
+    <tableColumn id="7" xr3:uid="{9E32B24E-F549-442D-B6C5-5B5E67078170}" name="Title" dataDxfId="24"/>
+    <tableColumn id="12" xr3:uid="{023EA1AA-B7DF-4814-BFEF-5AB9B0752B95}" name="Excel col #" dataDxfId="23"/>
+    <tableColumn id="1" xr3:uid="{5687DF61-58A8-463A-A7F7-9B8B474466F3}" name="CSV Column Name" dataDxfId="22"/>
+    <tableColumn id="13" xr3:uid="{9E799E78-81C7-4788-BF70-799894A0FACA}" name="CSV col #" dataDxfId="21"/>
+    <tableColumn id="16" xr3:uid="{6872DDE9-C4EA-4656-AE08-1B51AE6AE7D6}" name="XML Element" dataDxfId="20"/>
+    <tableColumn id="11" xr3:uid="{F0D84552-7E57-4362-9DCD-EDC8E4E51415}" name="XML order #" dataDxfId="19"/>
+    <tableColumn id="2" xr3:uid="{E36A262F-69A4-4276-95F1-0FB7FCE8E2AD}" name="Data Type" dataDxfId="18"/>
+    <tableColumn id="3" xr3:uid="{B4F9F589-759B-40AB-BD12-81562C067103}" name="Optionality" dataDxfId="17"/>
+    <tableColumn id="4" xr3:uid="{29CBFF2E-DC73-4812-9BE8-505CDCED923B}" name="Size" dataDxfId="16"/>
+    <tableColumn id="5" xr3:uid="{2FBE4EBA-0896-4EA8-8E6A-9740D712F4CF}" name="Business Rules" dataDxfId="15"/>
+    <tableColumn id="14" xr3:uid="{F6A291D7-463E-4C10-AE63-F46C62F701F1}" name="User Editable" dataDxfId="14"/>
+    <tableColumn id="6" xr3:uid="{4A3A44E5-9909-437B-9914-BD7AF1AC2439}" name="Generated" dataDxfId="13"/>
+    <tableColumn id="15" xr3:uid="{30410F79-D89B-4BAE-852C-7ADB5287310A}" name="Format" dataDxfId="12"/>
+    <tableColumn id="8" xr3:uid="{23D225B6-A3A4-4446-9AD4-7762B64F46FE}" name="Conditional Formatting" dataDxfId="11"/>
+    <tableColumn id="9" xr3:uid="{27D08B50-8012-49E0-9C10-AEB67B99B91B}" name="Validation" dataDxfId="10"/>
+    <tableColumn id="10" xr3:uid="{A301C8EB-BB2A-4524-AF6E-20714C0D7DD5}" name="Validation Formula" dataDxfId="9"/>
+    <tableColumn id="17" xr3:uid="{BAA62FBF-6DD1-4BE3-944E-A7C12DBF01CD}" name="Validation Severity" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight14" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1566,7 +1569,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="N11" sqref="N11"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1598,22 +1601,22 @@
         <v>53</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H1" s="6" t="s">
         <v>0</v>
@@ -1625,7 +1628,7 @@
         <v>2</v>
       </c>
       <c r="K1" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="L1" s="6" t="s">
         <v>79</v>
@@ -1643,7 +1646,7 @@
         <v>55</v>
       </c>
       <c r="Q1" s="6" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
     </row>
     <row r="2" spans="1:17" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -1660,16 +1663,16 @@
         <v>7</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="F2" s="13">
         <v>1</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I2" s="3">
         <v>10</v>
@@ -1680,19 +1683,19 @@
       </c>
       <c r="L2" s="2"/>
       <c r="M2" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="O2" s="2" t="s">
         <v>84</v>
       </c>
       <c r="P2" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="30" x14ac:dyDescent="0.25">
@@ -1709,16 +1712,16 @@
         <v>2</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="F3" s="2">
         <v>4</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I3" s="3">
         <v>20</v>
@@ -1729,19 +1732,19 @@
       </c>
       <c r="L3" s="2"/>
       <c r="M3" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="O3" s="2" t="s">
         <v>84</v>
       </c>
       <c r="P3" s="5" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="Q3" s="7" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
@@ -1758,16 +1761,16 @@
         <v>4</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="F4" s="2">
         <v>5</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I4" s="3">
         <v>9</v>
@@ -1780,19 +1783,19 @@
       </c>
       <c r="L4" s="2"/>
       <c r="M4" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="N4" s="5" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="O4" s="2" t="s">
         <v>84</v>
       </c>
       <c r="P4" s="5" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="Q4" s="2" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
@@ -1809,7 +1812,7 @@
         <v>13</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="F5" s="7">
         <v>16</v>
@@ -1818,7 +1821,7 @@
         <v>92</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I5" s="3">
         <v>8</v>
@@ -1831,19 +1834,19 @@
       </c>
       <c r="L5" s="2"/>
       <c r="M5" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="N5" s="5" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="O5" s="2" t="s">
         <v>78</v>
       </c>
       <c r="P5" s="5" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="Q5" s="2" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
@@ -1860,7 +1863,7 @@
         <v>14</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="F6" s="2">
         <v>17</v>
@@ -1869,30 +1872,32 @@
         <v>93</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="I6" s="3">
         <v>4</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="K6" s="2" t="s">
         <v>82</v>
       </c>
       <c r="L6" s="2"/>
       <c r="M6" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="N6" s="2"/>
+        <v>265</v>
+      </c>
+      <c r="N6" s="5" t="s">
+        <v>266</v>
+      </c>
       <c r="O6" s="2" t="s">
         <v>93</v>
       </c>
       <c r="P6" s="2" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="Q6" s="2" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
@@ -1909,16 +1914,16 @@
         <v>15</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="F7" s="7">
         <v>8</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I7" s="3">
         <v>2</v>
@@ -1929,19 +1934,19 @@
       </c>
       <c r="L7" s="2"/>
       <c r="M7" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="N7" s="5" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="O7" s="2" t="s">
         <v>80</v>
       </c>
       <c r="P7" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="Q7" s="2" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="8" spans="1:17" ht="30" x14ac:dyDescent="0.25">
@@ -1958,16 +1963,16 @@
         <v>9</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="F8" s="13">
         <v>21</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I8" s="3">
         <v>12</v>
@@ -1980,19 +1985,19 @@
       </c>
       <c r="L8" s="2"/>
       <c r="M8" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="N8" s="5" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="O8" s="2" t="s">
         <v>80</v>
       </c>
       <c r="P8" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="Q8" s="2" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="9" spans="1:17" ht="30" x14ac:dyDescent="0.25">
@@ -2009,16 +2014,16 @@
         <v>16</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="F9" s="6">
         <v>22</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I9" s="3">
         <v>2</v>
@@ -2029,45 +2034,45 @@
       </c>
       <c r="L9" s="2"/>
       <c r="M9" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="N9" s="5" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="O9" s="2" t="s">
         <v>80</v>
       </c>
       <c r="P9" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="Q9" s="2" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="10" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="B10" s="2">
         <v>6</v>
       </c>
       <c r="C10" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="E10" s="13" t="s">
         <v>261</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>263</v>
-      </c>
-      <c r="E10" s="13" t="s">
-        <v>264</v>
       </c>
       <c r="F10" s="13">
         <v>23</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I10" s="3">
         <v>200</v>
@@ -2078,22 +2083,22 @@
       </c>
       <c r="L10" s="2"/>
       <c r="M10" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="N10" s="2"/>
       <c r="O10" s="2" t="s">
         <v>84</v>
       </c>
       <c r="P10" s="5" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="Q10" s="2" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
     </row>
     <row r="11" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B11" s="2">
         <v>7</v>
@@ -2105,16 +2110,16 @@
         <v>29</v>
       </c>
       <c r="E11" s="13" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="F11" s="13">
         <v>11</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I11" s="3">
         <v>20</v>
@@ -2127,24 +2132,24 @@
       </c>
       <c r="L11" s="2"/>
       <c r="M11" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="N11" s="4" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="O11" s="2" t="s">
         <v>78</v>
       </c>
       <c r="P11" s="5" t="s">
-        <v>119</v>
+        <v>267</v>
       </c>
       <c r="Q11" s="2" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
     </row>
     <row r="12" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B12" s="2">
         <v>8</v>
@@ -2156,7 +2161,7 @@
         <v>30</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="F12" s="6">
         <v>12</v>
@@ -2165,7 +2170,7 @@
         <v>92</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I12" s="3">
         <v>8</v>
@@ -2178,19 +2183,19 @@
       </c>
       <c r="L12" s="2"/>
       <c r="M12" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="N12" s="4" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="O12" s="2" t="s">
         <v>78</v>
       </c>
       <c r="P12" s="5" t="s">
-        <v>121</v>
+        <v>268</v>
       </c>
       <c r="Q12" s="2" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
@@ -2207,7 +2212,7 @@
         <v>17</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="F13" s="7">
         <v>18</v>
@@ -2216,7 +2221,7 @@
         <v>92</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I13" s="3">
         <v>8</v>
@@ -2229,22 +2234,22 @@
       </c>
       <c r="L13" s="2"/>
       <c r="M13" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="N13" s="2"/>
       <c r="O13" s="2" t="s">
         <v>92</v>
       </c>
       <c r="P13" s="5" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="Q13" s="2" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="14" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B14" s="2">
         <v>10</v>
@@ -2256,16 +2261,16 @@
         <v>18</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="F14" s="6">
         <v>15</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I14" s="3">
         <v>40</v>
@@ -2278,22 +2283,22 @@
       </c>
       <c r="L14" s="2"/>
       <c r="M14" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="N14" s="2"/>
       <c r="O14" s="2" t="s">
         <v>84</v>
       </c>
       <c r="P14" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="Q14" s="2" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B15" s="2">
         <v>11</v>
@@ -2305,16 +2310,16 @@
         <v>22</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="F15" s="7">
         <v>19</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I15" s="3" t="s">
         <v>34</v>
@@ -2327,17 +2332,17 @@
       </c>
       <c r="L15" s="2"/>
       <c r="M15" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="N15" s="2"/>
       <c r="O15" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="P15" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="Q15" s="2" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="16" spans="1:17" ht="30" x14ac:dyDescent="0.25">
@@ -2352,16 +2357,16 @@
         <v>6</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="F16" s="6">
         <v>2</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I16" s="3">
         <v>10</v>
@@ -2391,29 +2396,29 @@
         <v>3</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="F17" s="7">
         <v>3</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I17" s="3">
         <v>20</v>
       </c>
       <c r="J17" s="2"/>
       <c r="K17" s="2" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="L17" s="11" t="s">
         <v>87</v>
       </c>
       <c r="M17" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="N17" s="2"/>
       <c r="O17" s="2" t="s">
@@ -2436,16 +2441,16 @@
         <v>8</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="F18" s="2">
         <v>6</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I18" s="3">
         <v>10</v>
@@ -2454,20 +2459,20 @@
         <v>52</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="L18" s="5" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="M18" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="N18" s="5"/>
       <c r="O18" s="2" t="s">
         <v>84</v>
       </c>
       <c r="P18" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="Q18" s="2"/>
     </row>
@@ -2483,16 +2488,16 @@
         <v>11</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="F19" s="7">
         <v>7</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I19" s="3">
         <v>2</v>
@@ -2524,16 +2529,16 @@
         <v>12</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="F20" s="2">
         <v>9</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I20" s="3">
         <v>1</v>
@@ -2542,20 +2547,20 @@
         <v>17</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="L20" s="2" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="M20" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="N20" s="5"/>
       <c r="O20" s="2" t="s">
         <v>80</v>
       </c>
       <c r="P20" s="5" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="Q20" s="2"/>
     </row>
@@ -2571,36 +2576,36 @@
         <v>5</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="F21" s="7">
         <v>10</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I21" s="3">
         <v>1</v>
       </c>
       <c r="J21" s="2"/>
       <c r="K21" s="2" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="L21" s="2" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="M21" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="N21" s="5"/>
       <c r="O21" s="2" t="s">
         <v>80</v>
       </c>
       <c r="P21" s="5" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="Q21" s="2"/>
     </row>
@@ -2616,16 +2621,16 @@
         <v>31</v>
       </c>
       <c r="E22" s="13" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="F22" s="13">
         <v>13</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I22" s="3">
         <v>10</v>
@@ -2637,7 +2642,7 @@
         <v>81</v>
       </c>
       <c r="L22" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="M22" s="2"/>
       <c r="N22" s="2"/>
@@ -2657,16 +2662,16 @@
         <v>32</v>
       </c>
       <c r="E23" s="13" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="F23" s="13">
         <v>14</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I23" s="3">
         <v>10</v>
@@ -2678,7 +2683,7 @@
         <v>81</v>
       </c>
       <c r="L23" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="M23" s="2"/>
       <c r="N23" s="2"/>
@@ -2688,7 +2693,7 @@
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" s="2" t="s">
@@ -2698,16 +2703,16 @@
         <v>23</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="F24" s="7">
         <v>20</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I24" s="3" t="s">
         <v>34</v>
@@ -2716,26 +2721,26 @@
         <v>37</v>
       </c>
       <c r="K24" s="2" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="L24" s="11" t="s">
         <v>87</v>
       </c>
       <c r="M24" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="N24" s="2"/>
       <c r="O24" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="P24" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="Q24" s="2"/>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B25" s="7"/>
       <c r="C25" s="7" t="s">
@@ -2747,10 +2752,10 @@
       <c r="E25" s="7"/>
       <c r="F25" s="7"/>
       <c r="G25" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H25" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I25" s="8">
         <v>20</v>
@@ -2772,7 +2777,7 @@
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" s="2" t="s">
@@ -2782,14 +2787,14 @@
         <v>10</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="F26" s="2"/>
       <c r="G26" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I26" s="3">
         <v>40</v>
@@ -2819,14 +2824,14 @@
         <v>19</v>
       </c>
       <c r="E27" s="13" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="F27" s="13"/>
       <c r="G27" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I27" s="3">
         <v>9</v>
@@ -2856,14 +2861,14 @@
         <v>20</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="F28" s="7"/>
       <c r="G28" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I28" s="3">
         <v>2</v>
@@ -2893,14 +2898,14 @@
         <v>21</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="F29" s="6"/>
       <c r="G29" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I29" s="3">
         <v>12</v>
@@ -2930,14 +2935,14 @@
         <v>24</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="F30" s="7"/>
       <c r="G30" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I30" s="3" t="s">
         <v>39</v>
@@ -2967,14 +2972,14 @@
         <v>25</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="F31" s="7"/>
       <c r="G31" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I31" s="3"/>
       <c r="J31" s="2"/>
@@ -3002,14 +3007,14 @@
         <v>26</v>
       </c>
       <c r="E32" s="7" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="F32" s="7"/>
       <c r="G32" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I32" s="3" t="s">
         <v>42</v>
@@ -3039,14 +3044,14 @@
         <v>27</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="F33" s="7"/>
       <c r="G33" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I33" s="3" t="s">
         <v>44</v>
@@ -3076,14 +3081,14 @@
         <v>28</v>
       </c>
       <c r="E34" s="7" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="F34" s="7"/>
       <c r="G34" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I34" s="3" t="s">
         <v>46</v>
@@ -3104,20 +3109,20 @@
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
   <conditionalFormatting sqref="D2:F34">
-    <cfRule type="expression" dxfId="7" priority="14">
+    <cfRule type="expression" dxfId="53" priority="14">
       <formula>LEN($D2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2:L34">
-    <cfRule type="expression" dxfId="6" priority="13">
+    <cfRule type="expression" dxfId="52" priority="13">
       <formula>AND($K2&lt;&gt;"Yes",LEN($L2)=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:Q34">
-    <cfRule type="expression" dxfId="5" priority="3">
+    <cfRule type="expression" dxfId="51" priority="3">
       <formula>$K2="Skip"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="15">
+    <cfRule type="expression" dxfId="50" priority="15">
       <formula>$K2="No"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3167,22 +3172,22 @@
         <v>53</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H1" s="6" t="s">
         <v>0</v>
@@ -3194,7 +3199,7 @@
         <v>2</v>
       </c>
       <c r="K1" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="L1" s="6" t="s">
         <v>79</v>
@@ -3212,7 +3217,7 @@
         <v>55</v>
       </c>
       <c r="Q1" s="6" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="30" x14ac:dyDescent="0.25">
@@ -3220,7 +3225,7 @@
         <v>57</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>10</v>
@@ -3229,16 +3234,16 @@
         <v>6</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="F2" s="13">
         <v>5</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I2" s="2">
         <v>10</v>
@@ -3249,7 +3254,7 @@
       </c>
       <c r="L2" s="2"/>
       <c r="M2" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
@@ -3261,7 +3266,7 @@
         <v>56</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>5</v>
@@ -3270,29 +3275,29 @@
         <v>2</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="F3" s="2">
         <v>1</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I3" s="2">
         <v>20</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>82</v>
       </c>
       <c r="L3" s="2"/>
       <c r="M3" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="N3" s="4"/>
       <c r="O3" s="2"/>
@@ -3304,7 +3309,7 @@
         <v>60</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>7</v>
@@ -3313,29 +3318,29 @@
         <v>4</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="F4" s="2">
         <v>2</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I4" s="2">
         <v>9</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>82</v>
       </c>
       <c r="L4" s="2"/>
       <c r="M4" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="N4" s="5"/>
       <c r="O4" s="2"/>
@@ -3347,7 +3352,7 @@
         <v>90</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>18</v>
@@ -3356,7 +3361,7 @@
         <v>3</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="F5" s="2">
         <v>3</v>
@@ -3365,20 +3370,20 @@
         <v>92</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I5" s="2">
         <v>8</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="K5" s="2" t="s">
         <v>82</v>
       </c>
       <c r="L5" s="2"/>
       <c r="M5" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="N5" s="5"/>
       <c r="O5" s="2"/>
@@ -3387,119 +3392,119 @@
     </row>
     <row r="6" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B6" s="2">
         <v>12</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D6" s="2">
         <v>18</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="F6" s="6">
         <v>13</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I6" s="2">
         <v>1</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="K6" s="2" t="s">
         <v>82</v>
       </c>
       <c r="L6" s="2"/>
       <c r="M6" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="N6" s="5" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="O6" s="2" t="s">
         <v>80</v>
       </c>
       <c r="P6" s="5" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="Q6" s="2" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="7" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B7" s="2">
         <v>13</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="D7" s="2">
         <v>15</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="F7" s="6">
         <v>6</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I7" s="2">
         <v>30</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="K7" s="2" t="s">
         <v>82</v>
       </c>
       <c r="L7" s="2"/>
       <c r="M7" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="N7" s="5"/>
       <c r="O7" s="2" t="s">
         <v>80</v>
       </c>
       <c r="P7" s="5" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="Q7" s="2" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B8" s="2">
         <v>14</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="D8" s="2">
         <v>8</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="F8" s="2">
         <v>8</v>
@@ -3508,47 +3513,47 @@
         <v>92</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I8" s="2">
         <v>8</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="K8" s="2" t="s">
         <v>82</v>
       </c>
       <c r="L8" s="2"/>
       <c r="M8" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="N8" s="5"/>
       <c r="O8" s="2" t="s">
         <v>92</v>
       </c>
       <c r="P8" s="5" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="Q8" s="2" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="B9" s="2">
         <v>15</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="D9" s="2">
         <v>9</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="F9" s="2">
         <v>9</v>
@@ -3557,47 +3562,47 @@
         <v>93</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I9" s="2">
         <v>4</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="K9" s="2" t="s">
         <v>82</v>
       </c>
       <c r="L9" s="2"/>
       <c r="M9" s="2" t="s">
-        <v>95</v>
+        <v>265</v>
       </c>
       <c r="N9" s="2"/>
       <c r="O9" s="2" t="s">
         <v>93</v>
       </c>
       <c r="P9" s="2" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="Q9" s="2" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="B10" s="2">
         <v>16</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D10" s="2">
         <v>10</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="F10" s="2">
         <v>10</v>
@@ -3606,47 +3611,47 @@
         <v>92</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I10" s="2">
         <v>8</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="K10" s="2" t="s">
         <v>82</v>
       </c>
       <c r="L10" s="2"/>
       <c r="M10" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="N10" s="5"/>
       <c r="O10" s="2" t="s">
         <v>92</v>
       </c>
       <c r="P10" s="5" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="Q10" s="2" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B11" s="2">
         <v>17</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="D11" s="2">
         <v>11</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="F11" s="2">
         <v>11</v>
@@ -3655,147 +3660,147 @@
         <v>93</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I11" s="2">
         <v>4</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="K11" s="2" t="s">
         <v>82</v>
       </c>
       <c r="L11" s="2"/>
       <c r="M11" s="2" t="s">
-        <v>95</v>
+        <v>265</v>
       </c>
       <c r="N11" s="2"/>
       <c r="O11" s="2" t="s">
         <v>93</v>
       </c>
       <c r="P11" s="2" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="Q11" s="2" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="12" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="B12" s="2">
         <v>18</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D12" s="2">
         <v>18</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="F12" s="6">
         <v>13</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I12" s="2">
         <v>1</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="K12" s="2" t="s">
         <v>82</v>
       </c>
       <c r="L12" s="2"/>
       <c r="M12" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="N12" s="4" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="O12" s="2" t="s">
         <v>80</v>
       </c>
       <c r="P12" s="5" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="Q12" s="2" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="13" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="B13" s="2">
         <v>19</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="D13" s="2">
         <v>15</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="F13" s="6">
         <v>6</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I13" s="2">
         <v>30</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="K13" s="2" t="s">
         <v>82</v>
       </c>
       <c r="L13" s="2"/>
       <c r="M13" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="N13" s="5"/>
       <c r="O13" s="2" t="s">
         <v>80</v>
       </c>
       <c r="P13" s="5" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="Q13" s="2" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="B14" s="2">
         <v>20</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="D14" s="2">
         <v>8</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="F14" s="2">
         <v>8</v>
@@ -3804,47 +3809,47 @@
         <v>92</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I14" s="2">
         <v>8</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="K14" s="2" t="s">
         <v>82</v>
       </c>
       <c r="L14" s="2"/>
       <c r="M14" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="N14" s="5"/>
       <c r="O14" s="2" t="s">
         <v>92</v>
       </c>
       <c r="P14" s="5" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="Q14" s="2" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="B15" s="2">
         <v>21</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="D15" s="2">
         <v>9</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="F15" s="2">
         <v>9</v>
@@ -3853,47 +3858,47 @@
         <v>93</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I15" s="2">
         <v>4</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="K15" s="2" t="s">
         <v>82</v>
       </c>
       <c r="L15" s="2"/>
       <c r="M15" s="2" t="s">
-        <v>95</v>
+        <v>265</v>
       </c>
       <c r="N15" s="2"/>
       <c r="O15" s="2" t="s">
         <v>93</v>
       </c>
       <c r="P15" s="2" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="Q15" s="2" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="B16" s="2">
         <v>22</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D16" s="2">
         <v>10</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="F16" s="2">
         <v>10</v>
@@ -3902,47 +3907,47 @@
         <v>92</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I16" s="2">
         <v>8</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="K16" s="2" t="s">
         <v>82</v>
       </c>
       <c r="L16" s="2"/>
       <c r="M16" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="N16" s="5"/>
       <c r="O16" s="2" t="s">
         <v>92</v>
       </c>
       <c r="P16" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="Q16" s="2" t="s">
         <v>251</v>
-      </c>
-      <c r="Q16" s="2" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="B17" s="2">
         <v>23</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="D17" s="2">
         <v>11</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="F17" s="2">
         <v>11</v>
@@ -3951,30 +3956,30 @@
         <v>93</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I17" s="2">
         <v>4</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="K17" s="2" t="s">
         <v>82</v>
       </c>
       <c r="L17" s="2"/>
       <c r="M17" s="2" t="s">
-        <v>95</v>
+        <v>265</v>
       </c>
       <c r="N17" s="2"/>
       <c r="O17" s="2" t="s">
         <v>93</v>
       </c>
       <c r="P17" s="2" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="Q17" s="2" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="18" spans="1:17" ht="45" x14ac:dyDescent="0.25">
@@ -3989,16 +3994,16 @@
         <v>5</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="F18" s="6">
         <v>4</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I18" s="2">
         <v>10</v>
@@ -4008,7 +4013,7 @@
         <v>81</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="M18" s="2"/>
       <c r="N18" s="2"/>
@@ -4018,88 +4023,88 @@
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" s="2" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="D19" s="2">
         <v>16</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="F19" s="2">
         <v>7</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I19" s="2">
         <v>9</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="K19" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="L19" s="5" t="s">
         <v>231</v>
       </c>
-      <c r="L19" s="5" t="s">
-        <v>234</v>
-      </c>
       <c r="M19" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="N19" s="2"/>
       <c r="O19" s="2" t="s">
         <v>80</v>
       </c>
       <c r="P19" s="5" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="Q19" s="2"/>
     </row>
     <row r="20" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" s="2" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D20" s="2">
         <v>7</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="F20" s="6">
         <v>12</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I20" s="2">
         <v>4</v>
       </c>
       <c r="J20" s="6" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="K20" s="2" t="s">
         <v>81</v>
       </c>
       <c r="L20" s="2" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="M20" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="N20" s="4"/>
       <c r="O20" s="2"/>
@@ -4108,162 +4113,162 @@
     </row>
     <row r="21" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D21" s="2">
         <v>28</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="F21" s="6">
         <v>14</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="L21" s="11" t="s">
         <v>87</v>
       </c>
       <c r="M21" s="2"/>
       <c r="N21" s="4" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="O21" s="2" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="P21" s="2" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="Q21" s="2"/>
     </row>
     <row r="22" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D22" s="2">
         <v>20</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="F22" s="6">
         <v>15</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I22" s="2">
         <v>10</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="L22" s="11" t="s">
         <v>87</v>
       </c>
       <c r="M22" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="N22" s="4" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="O22" s="2" t="s">
         <v>80</v>
       </c>
       <c r="P22" s="5" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="Q22" s="2"/>
     </row>
     <row r="23" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" s="2" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D23" s="2">
         <v>27</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="F23" s="6">
         <v>16</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I23" s="2">
         <v>9</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="L23" s="11" t="s">
         <v>87</v>
       </c>
       <c r="M23" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="N23" s="4" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="O23" s="2" t="s">
         <v>80</v>
       </c>
       <c r="P23" s="5" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="Q23" s="2"/>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" s="2" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="D24" s="2">
         <v>12</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="F24" s="2">
         <v>17</v>
@@ -4272,64 +4277,64 @@
         <v>92</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I24" s="2">
         <v>8</v>
       </c>
       <c r="J24" s="2"/>
       <c r="K24" s="2" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="L24" s="5" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="M24" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="N24" s="5"/>
       <c r="O24" s="2" t="s">
         <v>92</v>
       </c>
       <c r="P24" s="5" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="Q24" s="2"/>
     </row>
     <row r="25" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" s="2" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="D25" s="2">
         <v>13</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="F25" s="6">
         <v>18</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I25" s="2">
         <v>1</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="K25" s="2" t="s">
         <v>81</v>
       </c>
       <c r="L25" s="2" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="M25" s="2"/>
       <c r="N25" s="2"/>
@@ -4339,7 +4344,7 @@
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" s="2" t="s">
@@ -4351,22 +4356,22 @@
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
       <c r="G26" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I26" s="2">
         <v>20</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="K26" s="2" t="s">
         <v>81</v>
       </c>
       <c r="L26" s="2" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="M26" s="2"/>
       <c r="N26" s="2"/>
@@ -4376,11 +4381,11 @@
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" s="2" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="D27" s="2">
         <v>14</v>
@@ -4388,10 +4393,10 @@
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
       <c r="G27" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I27" s="2">
         <v>2</v>
@@ -4411,11 +4416,11 @@
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" s="2" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="D28" s="2">
         <v>17</v>
@@ -4423,52 +4428,84 @@
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
       <c r="G28" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I28" s="2">
         <v>4</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="K28" s="2" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="L28" s="11" t="s">
         <v>87</v>
       </c>
       <c r="M28" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="N28" s="2"/>
       <c r="O28" s="2" t="s">
         <v>80</v>
       </c>
       <c r="P28" s="5" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="Q28" s="2"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="L2:L28">
-    <cfRule type="expression" dxfId="3" priority="21">
+    <cfRule type="expression" dxfId="30" priority="29">
       <formula>AND($K2&lt;&gt;"Yes",LEN($L2)=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:F28">
-    <cfRule type="expression" dxfId="2" priority="22">
+    <cfRule type="expression" dxfId="29" priority="30">
       <formula>LEN($D2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:Q28">
-    <cfRule type="expression" dxfId="1" priority="5">
+  <conditionalFormatting sqref="A2:Q8 A10:Q10 A9:L9 N9:Q9 A12:Q14 A11:L11 N11:Q11 A16:Q16 A15:L15 N15:Q15 A18:Q28 A17:L17 N17:Q17">
+    <cfRule type="expression" dxfId="28" priority="13">
       <formula>$K2="Skip"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="23">
+    <cfRule type="expression" dxfId="27" priority="31">
       <formula>$K2="No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M9">
+    <cfRule type="expression" dxfId="7" priority="7">
+      <formula>$K9="Skip"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="6" priority="8">
+      <formula>$K9="No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M11">
+    <cfRule type="expression" dxfId="5" priority="5">
+      <formula>$K11="Skip"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="4" priority="6">
+      <formula>$K11="No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M15">
+    <cfRule type="expression" dxfId="3" priority="3">
+      <formula>$K15="Skip"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="2" priority="4">
+      <formula>$K15="No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M17">
+    <cfRule type="expression" dxfId="1" priority="1">
+      <formula>$K17="Skip"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="2">
+      <formula>$K17="No"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Make Collection Address required and update description
#19
</commit_message>
<xml_diff>
--- a/specs/Coliform-column-definitions.xlsx
+++ b/specs/Coliform-column-definitions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\xl-ese\specs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44CB2758-6E15-4923-BCCE-56E13CC85522}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABA28300-D74F-4DC5-82A0-06721FB05664}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="627" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="270">
   <si>
     <t>Optionality</t>
   </si>
@@ -900,6 +900,9 @@
   </si>
   <si>
     <t>=OR(LEFT(RC5,6)&lt;&gt;"Repeat",AND(LEN(RC)&gt;0,RC&lt;=TODAY()))</t>
+  </si>
+  <si>
+    <t>=LEN(RC6)=0</t>
   </si>
 </sst>
 </file>
@@ -2072,7 +2075,7 @@
         <v>101</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="I10" s="3">
         <v>200</v>
@@ -2085,7 +2088,9 @@
       <c r="M10" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="N10" s="2"/>
+      <c r="N10" s="5" t="s">
+        <v>269</v>
+      </c>
       <c r="O10" s="2" t="s">
         <v>84</v>
       </c>
@@ -2093,7 +2098,7 @@
         <v>262</v>
       </c>
       <c r="Q10" s="2" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
     </row>
     <row r="11" spans="1:17" ht="30" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Display Routine as "RTOR" and Special as "SPEC"
Users are used to these values

#19
</commit_message>
<xml_diff>
--- a/specs/Coliform-column-definitions.xlsx
+++ b/specs/Coliform-column-definitions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\xl-ese\specs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABA28300-D74F-4DC5-82A0-06721FB05664}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D0F997F-97C7-46F4-BF17-118B07B4EE43}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Coliform Sample" sheetId="1" r:id="rId1"/>
@@ -991,6 +991,63 @@
   </cellStyles>
   <dxfs count="54">
     <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <bgColor theme="0" tint="-0.14996795556505021"/>
@@ -1045,63 +1102,6 @@
           <bgColor theme="5" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <fill>
@@ -1275,28 +1275,28 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{05345577-AC31-4B6D-B899-55D66DEB1874}" name="Table2" displayName="Table2" ref="A1:Q28" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{05345577-AC31-4B6D-B899-55D66DEB1874}" name="Table2" displayName="Table2" ref="A1:Q28" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Q28">
     <sortCondition ref="B18:B28"/>
   </sortState>
   <tableColumns count="17">
-    <tableColumn id="7" xr3:uid="{9E32B24E-F549-442D-B6C5-5B5E67078170}" name="Title" dataDxfId="24"/>
-    <tableColumn id="12" xr3:uid="{023EA1AA-B7DF-4814-BFEF-5AB9B0752B95}" name="Excel col #" dataDxfId="23"/>
-    <tableColumn id="1" xr3:uid="{5687DF61-58A8-463A-A7F7-9B8B474466F3}" name="CSV Column Name" dataDxfId="22"/>
-    <tableColumn id="13" xr3:uid="{9E799E78-81C7-4788-BF70-799894A0FACA}" name="CSV col #" dataDxfId="21"/>
-    <tableColumn id="16" xr3:uid="{6872DDE9-C4EA-4656-AE08-1B51AE6AE7D6}" name="XML Element" dataDxfId="20"/>
-    <tableColumn id="11" xr3:uid="{F0D84552-7E57-4362-9DCD-EDC8E4E51415}" name="XML order #" dataDxfId="19"/>
-    <tableColumn id="2" xr3:uid="{E36A262F-69A4-4276-95F1-0FB7FCE8E2AD}" name="Data Type" dataDxfId="18"/>
-    <tableColumn id="3" xr3:uid="{B4F9F589-759B-40AB-BD12-81562C067103}" name="Optionality" dataDxfId="17"/>
-    <tableColumn id="4" xr3:uid="{29CBFF2E-DC73-4812-9BE8-505CDCED923B}" name="Size" dataDxfId="16"/>
-    <tableColumn id="5" xr3:uid="{2FBE4EBA-0896-4EA8-8E6A-9740D712F4CF}" name="Business Rules" dataDxfId="15"/>
-    <tableColumn id="14" xr3:uid="{F6A291D7-463E-4C10-AE63-F46C62F701F1}" name="User Editable" dataDxfId="14"/>
-    <tableColumn id="6" xr3:uid="{4A3A44E5-9909-437B-9914-BD7AF1AC2439}" name="Generated" dataDxfId="13"/>
-    <tableColumn id="15" xr3:uid="{30410F79-D89B-4BAE-852C-7ADB5287310A}" name="Format" dataDxfId="12"/>
-    <tableColumn id="8" xr3:uid="{23D225B6-A3A4-4446-9AD4-7762B64F46FE}" name="Conditional Formatting" dataDxfId="11"/>
-    <tableColumn id="9" xr3:uid="{27D08B50-8012-49E0-9C10-AEB67B99B91B}" name="Validation" dataDxfId="10"/>
-    <tableColumn id="10" xr3:uid="{A301C8EB-BB2A-4524-AF6E-20714C0D7DD5}" name="Validation Formula" dataDxfId="9"/>
-    <tableColumn id="17" xr3:uid="{BAA62FBF-6DD1-4BE3-944E-A7C12DBF01CD}" name="Validation Severity" dataDxfId="8"/>
+    <tableColumn id="7" xr3:uid="{9E32B24E-F549-442D-B6C5-5B5E67078170}" name="Title" dataDxfId="16"/>
+    <tableColumn id="12" xr3:uid="{023EA1AA-B7DF-4814-BFEF-5AB9B0752B95}" name="Excel col #" dataDxfId="15"/>
+    <tableColumn id="1" xr3:uid="{5687DF61-58A8-463A-A7F7-9B8B474466F3}" name="CSV Column Name" dataDxfId="14"/>
+    <tableColumn id="13" xr3:uid="{9E799E78-81C7-4788-BF70-799894A0FACA}" name="CSV col #" dataDxfId="13"/>
+    <tableColumn id="16" xr3:uid="{6872DDE9-C4EA-4656-AE08-1B51AE6AE7D6}" name="XML Element" dataDxfId="12"/>
+    <tableColumn id="11" xr3:uid="{F0D84552-7E57-4362-9DCD-EDC8E4E51415}" name="XML order #" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{E36A262F-69A4-4276-95F1-0FB7FCE8E2AD}" name="Data Type" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{B4F9F589-759B-40AB-BD12-81562C067103}" name="Optionality" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{29CBFF2E-DC73-4812-9BE8-505CDCED923B}" name="Size" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{2FBE4EBA-0896-4EA8-8E6A-9740D712F4CF}" name="Business Rules" dataDxfId="7"/>
+    <tableColumn id="14" xr3:uid="{F6A291D7-463E-4C10-AE63-F46C62F701F1}" name="User Editable" dataDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{4A3A44E5-9909-437B-9914-BD7AF1AC2439}" name="Generated" dataDxfId="5"/>
+    <tableColumn id="15" xr3:uid="{30410F79-D89B-4BAE-852C-7ADB5287310A}" name="Format" dataDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{23D225B6-A3A4-4446-9AD4-7762B64F46FE}" name="Conditional Formatting" dataDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{27D08B50-8012-49E0-9C10-AEB67B99B91B}" name="Validation" dataDxfId="2"/>
+    <tableColumn id="10" xr3:uid="{A301C8EB-BB2A-4524-AF6E-20714C0D7DD5}" name="Validation Formula" dataDxfId="1"/>
+    <tableColumn id="17" xr3:uid="{BAA62FBF-6DD1-4BE3-944E-A7C12DBF01CD}" name="Validation Severity" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight14" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4482,34 +4482,34 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M9">
-    <cfRule type="expression" dxfId="7" priority="7">
+    <cfRule type="expression" dxfId="26" priority="7">
       <formula>$K9="Skip"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="8">
+    <cfRule type="expression" dxfId="25" priority="8">
       <formula>$K9="No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M11">
-    <cfRule type="expression" dxfId="5" priority="5">
+    <cfRule type="expression" dxfId="24" priority="5">
       <formula>$K11="Skip"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="6">
+    <cfRule type="expression" dxfId="23" priority="6">
       <formula>$K11="No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M15">
-    <cfRule type="expression" dxfId="3" priority="3">
+    <cfRule type="expression" dxfId="22" priority="3">
       <formula>$K15="Skip"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="4">
+    <cfRule type="expression" dxfId="21" priority="4">
       <formula>$K15="No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M17">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="20" priority="1">
       <formula>$K17="Skip"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="2">
+    <cfRule type="expression" dxfId="19" priority="2">
       <formula>$K17="No"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>